<commit_message>
Results for depth 6
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Method</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Java Threads</t>
+  </si>
+  <si>
+    <t>Real Average Move Time (ms)</t>
+  </si>
+  <si>
+    <t>Real Average Game Time (ms)</t>
   </si>
 </sst>
 </file>
@@ -182,8 +188,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="127">
+  <cellStyleXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -349,7 +375,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="127">
+  <cellStyles count="147">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -413,6 +439,16 @@
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -476,6 +512,16 @@
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -805,29 +851,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y13"/>
+  <dimension ref="A1:AA13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="6" max="6" width="12.33203125" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="23" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="25.1640625" customWidth="1"/>
-    <col min="25" max="25" width="8.5" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="25" width="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="25.1640625" customWidth="1"/>
+    <col min="27" max="27" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
-      <c r="L1" s="15" t="s">
+    <row r="1" spans="1:27">
+      <c r="N1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
       <c r="O1" s="15"/>
       <c r="P1" s="15"/>
       <c r="Q1" s="15"/>
@@ -837,8 +883,10 @@
       <c r="U1" s="15"/>
       <c r="V1" s="15"/>
       <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
     </row>
-    <row r="2" spans="1:25" s="1" customFormat="1" ht="56" customHeight="1">
+    <row r="2" spans="1:27" s="1" customFormat="1" ht="56" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -861,61 +909,67 @@
         <v>3</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="M2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="11">
+      <c r="N2" s="11">
         <v>16384</v>
       </c>
-      <c r="M2" s="11">
+      <c r="O2" s="11">
         <v>8192</v>
       </c>
-      <c r="N2" s="11">
+      <c r="P2" s="11">
         <v>4096</v>
       </c>
-      <c r="O2" s="11">
+      <c r="Q2" s="11">
         <v>2048</v>
       </c>
-      <c r="P2" s="11">
+      <c r="R2" s="11">
         <v>1024</v>
       </c>
-      <c r="Q2" s="11">
+      <c r="S2" s="11">
         <v>512</v>
       </c>
-      <c r="R2" s="11">
+      <c r="T2" s="11">
         <v>256</v>
       </c>
-      <c r="S2" s="11">
+      <c r="U2" s="11">
         <v>128</v>
       </c>
-      <c r="T2" s="11">
+      <c r="V2" s="11">
         <v>64</v>
       </c>
-      <c r="U2" s="11">
+      <c r="W2" s="11">
         <v>32</v>
       </c>
-      <c r="V2" s="11">
+      <c r="X2" s="11">
         <v>16</v>
       </c>
-      <c r="W2" s="11">
+      <c r="Y2" s="11">
         <v>8</v>
       </c>
-      <c r="X2" s="14" t="s">
+      <c r="Z2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="Y2" s="14" t="s">
+      <c r="AA2" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:27">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -938,54 +992,62 @@
         <f>E3/C3</f>
         <v>2.1320399999999999</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="3">
+        <f>D3/C3</f>
+        <v>0.49892999999999998</v>
+      </c>
+      <c r="I3" s="7">
         <f>F3/C3</f>
         <v>82.672650000000004</v>
       </c>
-      <c r="I3" s="3">
-        <f>G3/H3</f>
+      <c r="J3" s="3">
+        <f>G3/I3</f>
         <v>2.5788939873101924E-2</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="3">
+        <f>H3/I3</f>
+        <v>6.0350067404395524E-3</v>
+      </c>
+      <c r="L3" s="2">
         <v>889</v>
       </c>
-      <c r="K3" s="2">
+      <c r="M3" s="2">
         <v>4984</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
-      <c r="Q3" s="5">
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="R3" s="5">
+      <c r="T3" s="5">
         <v>5.0369999999999998E-2</v>
       </c>
-      <c r="S3" s="5">
+      <c r="U3" s="5">
         <v>0.45832000000000001</v>
       </c>
-      <c r="T3" s="5">
+      <c r="V3" s="5">
         <v>0.89120999999999995</v>
       </c>
-      <c r="U3" s="5">
+      <c r="W3" s="5">
         <v>0.99451999999999996</v>
       </c>
-      <c r="V3" s="5">
+      <c r="X3" s="5">
         <v>0.99992999999999999</v>
       </c>
-      <c r="W3" s="4">
-        <v>1</v>
-      </c>
-      <c r="X3" t="s">
+      <c r="Y3" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z3" t="s">
         <v>15</v>
       </c>
-      <c r="Y3">
+      <c r="AA3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:27">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1008,56 +1070,64 @@
         <f>E4/C4</f>
         <v>2.2993800000000002</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="3">
+        <f t="shared" ref="H4:H9" si="0">D4/C4</f>
+        <v>0.52159999999999995</v>
+      </c>
+      <c r="I4" s="7">
         <f>F4/C4</f>
         <v>184.41568000000001</v>
       </c>
-      <c r="I4" s="3">
-        <f>G4/H4</f>
+      <c r="J4" s="3">
+        <f>G4/I4</f>
         <v>1.2468462551557438E-2</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="3">
+        <f t="shared" ref="K4:K9" si="1">H4/I4</f>
+        <v>2.8283929002132571E-3</v>
+      </c>
+      <c r="L4" s="2">
         <v>2726</v>
       </c>
-      <c r="K4" s="2">
+      <c r="M4" s="2">
         <v>15568</v>
       </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
-      <c r="P4" s="5">
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5">
         <v>3.3500000000000001E-3</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="S4" s="5">
         <v>0.13125999999999999</v>
       </c>
-      <c r="R4" s="5">
+      <c r="T4" s="5">
         <v>0.58604000000000001</v>
       </c>
-      <c r="S4" s="5">
+      <c r="U4" s="5">
         <v>0.91791</v>
       </c>
-      <c r="T4" s="5">
+      <c r="V4" s="5">
         <v>0.99351999999999996</v>
       </c>
-      <c r="U4" s="5">
+      <c r="W4" s="5">
         <v>0.99995000000000001</v>
       </c>
-      <c r="V4" s="4">
-        <v>1</v>
-      </c>
-      <c r="W4" s="4">
-        <v>1</v>
-      </c>
-      <c r="X4" t="s">
+      <c r="X4" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z4" t="s">
         <v>15</v>
       </c>
-      <c r="Y4">
+      <c r="AA4">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:27">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -1080,60 +1150,68 @@
         <f>E5/C5</f>
         <v>2.6820300000000001</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.55393999999999999</v>
+      </c>
+      <c r="I5" s="7">
         <f>F5/C5</f>
         <v>444.81198999999998</v>
       </c>
-      <c r="I5" s="3">
-        <f>G5/H5</f>
+      <c r="J5" s="3">
+        <f>G5/I5</f>
         <v>6.0295811720363027E-3</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="3">
+        <f t="shared" si="1"/>
+        <v>1.2453351358626822E-3</v>
+      </c>
+      <c r="L5" s="2">
         <v>9129</v>
       </c>
-      <c r="K5" s="2">
+      <c r="M5" s="2">
         <v>66240</v>
       </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5">
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="O5" s="5">
+      <c r="Q5" s="5">
         <v>7.2480000000000003E-2</v>
       </c>
-      <c r="P5" s="5">
+      <c r="R5" s="5">
         <v>0.39942</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="S5" s="5">
         <v>0.76100999999999996</v>
       </c>
-      <c r="R5" s="5">
+      <c r="T5" s="5">
         <v>0.94055</v>
       </c>
-      <c r="S5" s="5">
+      <c r="U5" s="5">
         <v>0.99173</v>
       </c>
-      <c r="T5" s="5">
+      <c r="V5" s="5">
         <v>0.99936000000000003</v>
       </c>
-      <c r="U5" s="5">
+      <c r="W5" s="5">
         <v>0.99997999999999998</v>
       </c>
-      <c r="V5" s="4">
-        <v>1</v>
-      </c>
-      <c r="W5" s="4">
-        <v>1</v>
-      </c>
-      <c r="X5" t="s">
+      <c r="X5" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z5" t="s">
         <v>15</v>
       </c>
-      <c r="Y5">
+      <c r="AA5">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:27">
       <c r="A6" s="6"/>
       <c r="B6">
         <v>2</v>
@@ -1154,60 +1232,68 @@
         <f>E6/C6</f>
         <v>20.84273</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="3">
+        <f t="shared" si="0"/>
+        <v>3.5598399999999999</v>
+      </c>
+      <c r="I6" s="7">
         <f>F6/C6</f>
         <v>634.32843000000003</v>
       </c>
-      <c r="I6" s="3">
-        <f>G6/H6</f>
+      <c r="J6" s="3">
+        <f>G6/I6</f>
         <v>3.2857947104782924E-2</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="3">
+        <f t="shared" si="1"/>
+        <v>5.6119824236791653E-3</v>
+      </c>
+      <c r="L6" s="2">
         <v>14103</v>
       </c>
-      <c r="K6" s="2">
+      <c r="M6" s="2">
         <v>72692</v>
       </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5">
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5">
         <v>7.9699999999999997E-3</v>
       </c>
-      <c r="O6" s="5">
+      <c r="Q6" s="5">
         <v>0.21351000000000001</v>
       </c>
-      <c r="P6" s="5">
+      <c r="R6" s="5">
         <v>0.64770000000000005</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="S6" s="5">
         <v>0.91000999999999999</v>
       </c>
-      <c r="R6" s="5">
+      <c r="T6" s="5">
         <v>0.98502999999999996</v>
       </c>
-      <c r="S6" s="5">
+      <c r="U6" s="5">
         <v>0.99843999999999999</v>
       </c>
-      <c r="T6" s="5">
+      <c r="V6" s="5">
         <v>0.99995000000000001</v>
       </c>
-      <c r="U6" s="4">
-        <v>1</v>
-      </c>
-      <c r="V6" s="4">
-        <v>1</v>
-      </c>
       <c r="W6" s="4">
         <v>1</v>
       </c>
-      <c r="X6" t="s">
+      <c r="X6" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z6" t="s">
         <v>15</v>
       </c>
-      <c r="Y6">
+      <c r="AA6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:27">
       <c r="A7" s="6"/>
       <c r="B7">
         <v>3</v>
@@ -1228,62 +1314,70 @@
         <f>E7/C7</f>
         <v>41.015680000000003</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="3">
+        <f t="shared" si="0"/>
+        <v>6.9243499999999996</v>
+      </c>
+      <c r="I7" s="7">
         <f>F7/C7</f>
         <v>1056.64949</v>
       </c>
-      <c r="I7" s="3">
-        <f>G7/H7</f>
+      <c r="J7" s="3">
+        <f>G7/I7</f>
         <v>3.8816731932554097E-2</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="3">
+        <f t="shared" si="1"/>
+        <v>6.5531191426591228E-3</v>
+      </c>
+      <c r="L7" s="2">
         <v>26232</v>
       </c>
-      <c r="K7" s="2">
+      <c r="M7" s="2">
         <v>121804</v>
       </c>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5">
+      <c r="N7" s="5"/>
+      <c r="O7" s="5">
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="N7" s="5">
+      <c r="P7" s="5">
         <v>0.11705</v>
       </c>
-      <c r="O7" s="5">
+      <c r="Q7" s="5">
         <v>0.63338000000000005</v>
       </c>
-      <c r="P7" s="5">
+      <c r="R7" s="5">
         <v>0.92276000000000002</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="S7" s="5">
         <v>0.98972000000000004</v>
       </c>
-      <c r="R7" s="5">
+      <c r="T7" s="5">
         <v>0.99911000000000005</v>
       </c>
-      <c r="S7" s="5">
+      <c r="U7" s="5">
         <v>0.99999000000000005</v>
       </c>
-      <c r="T7" s="4">
-        <v>1</v>
-      </c>
-      <c r="U7" s="4">
-        <v>1</v>
-      </c>
       <c r="V7" s="4">
         <v>1</v>
       </c>
       <c r="W7" s="4">
         <v>1</v>
       </c>
-      <c r="X7" t="s">
+      <c r="X7" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z7" t="s">
         <v>15</v>
       </c>
-      <c r="Y7">
+      <c r="AA7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:27">
       <c r="A8" s="6"/>
       <c r="B8">
         <v>4</v>
@@ -1304,45 +1398,47 @@
         <f>E8/C8</f>
         <v>847.04769999999996</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="3">
+        <f t="shared" si="0"/>
+        <v>141.2938</v>
+      </c>
+      <c r="I8" s="7">
         <f>F8/C8</f>
         <v>1140.9683</v>
       </c>
-      <c r="I8" s="3">
-        <f>G8/H8</f>
+      <c r="J8" s="3">
+        <f>G8/I8</f>
         <v>0.74239371943988275</v>
       </c>
-      <c r="J8" s="2">
+      <c r="K8" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12383674463173079</v>
+      </c>
+      <c r="L8" s="2">
         <v>28757</v>
       </c>
-      <c r="K8" s="2">
+      <c r="M8" s="2">
         <v>109576</v>
       </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5">
+      <c r="N8" s="5"/>
+      <c r="O8" s="5">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="N8" s="5">
+      <c r="P8" s="5">
         <v>0.16270000000000001</v>
       </c>
-      <c r="O8" s="5">
+      <c r="Q8" s="5">
         <v>0.68689999999999996</v>
       </c>
-      <c r="P8" s="5">
+      <c r="R8" s="5">
         <v>0.94330000000000003</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="S8" s="5">
         <v>0.99390000000000001</v>
       </c>
-      <c r="R8" s="5">
+      <c r="T8" s="5">
         <v>0.99980000000000002</v>
       </c>
-      <c r="S8" s="4">
-        <v>1</v>
-      </c>
-      <c r="T8" s="4">
-        <v>1</v>
-      </c>
       <c r="U8" s="4">
         <v>1</v>
       </c>
@@ -1352,14 +1448,20 @@
       <c r="W8" s="4">
         <v>1</v>
       </c>
-      <c r="X8" t="s">
+      <c r="X8" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z8" t="s">
         <v>15</v>
       </c>
-      <c r="Y8">
+      <c r="AA8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:27">
       <c r="A9" s="6"/>
       <c r="B9">
         <v>5</v>
@@ -1380,44 +1482,46 @@
         <f>E9/C9</f>
         <v>1026.6936000000001</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="3">
+        <f t="shared" si="0"/>
+        <v>171.24250000000001</v>
+      </c>
+      <c r="I9" s="7">
         <f>F9/C9</f>
         <v>1657.7687000000001</v>
       </c>
-      <c r="I9" s="3">
-        <f>G9/H9</f>
+      <c r="J9" s="3">
+        <f>G9/I9</f>
         <v>0.6193225870412441</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="3">
+        <f t="shared" si="1"/>
+        <v>0.10329697985008403</v>
+      </c>
+      <c r="L9" s="2">
         <v>44565</v>
       </c>
-      <c r="K9" s="2">
+      <c r="M9" s="2">
         <v>149960</v>
       </c>
-      <c r="M9" s="5">
+      <c r="O9" s="5">
         <v>1.49E-2</v>
       </c>
-      <c r="N9" s="5">
+      <c r="P9" s="5">
         <v>0.46239999999999998</v>
       </c>
-      <c r="O9" s="5">
+      <c r="Q9" s="5">
         <v>0.90180000000000005</v>
       </c>
-      <c r="P9" s="5">
+      <c r="R9" s="5">
         <v>0.98560000000000003</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="S9" s="5">
         <v>0.99750000000000005</v>
       </c>
-      <c r="R9" s="5">
+      <c r="T9" s="5">
         <v>0.99990000000000001</v>
       </c>
-      <c r="S9" s="4">
-        <v>1</v>
-      </c>
-      <c r="T9" s="4">
-        <v>1</v>
-      </c>
       <c r="U9" s="4">
         <v>1</v>
       </c>
@@ -1427,46 +1531,104 @@
       <c r="W9" s="4">
         <v>1</v>
       </c>
-      <c r="X9" t="s">
+      <c r="X9" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z9" t="s">
         <v>15</v>
       </c>
-      <c r="Y9">
+      <c r="AA9">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:27">
       <c r="A10" s="6"/>
       <c r="B10">
         <v>6</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
+      <c r="C10">
+        <v>5000</v>
+      </c>
+      <c r="D10" s="2">
+        <v>9609433</v>
+      </c>
+      <c r="E10" s="2">
+        <v>19213148</v>
+      </c>
+      <c r="F10" s="2">
+        <v>8870872</v>
+      </c>
+      <c r="G10" s="7">
+        <f>E10/C10</f>
+        <v>3842.6296000000002</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" ref="H10:H11" si="2">D10/C10</f>
+        <v>1921.8866</v>
+      </c>
+      <c r="I10" s="7">
+        <f>F10/C10</f>
+        <v>1774.1744000000001</v>
+      </c>
+      <c r="J10" s="3">
+        <f>G10/I10</f>
+        <v>2.1658691501805007</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" ref="K10:K11" si="3">H10/I10</f>
+        <v>1.0832568658413739</v>
+      </c>
+      <c r="L10" s="2">
+        <v>48152</v>
+      </c>
+      <c r="M10" s="2">
+        <v>152180</v>
+      </c>
       <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" t="s">
+      <c r="O10" s="5">
+        <v>2.1600000000000001E-2</v>
+      </c>
+      <c r="P10" s="5">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>0.9274</v>
+      </c>
+      <c r="R10" s="5">
+        <v>0.99260000000000004</v>
+      </c>
+      <c r="S10" s="5">
+        <v>0.999</v>
+      </c>
+      <c r="T10" s="4">
+        <v>1</v>
+      </c>
+      <c r="U10" s="4">
+        <v>1</v>
+      </c>
+      <c r="V10" s="4">
+        <v>1</v>
+      </c>
+      <c r="W10" s="4">
+        <v>1</v>
+      </c>
+      <c r="X10" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z10" t="s">
         <v>15</v>
       </c>
-      <c r="Y10">
-        <v>6</v>
+      <c r="AA10">
+        <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:27">
       <c r="A11" s="6"/>
       <c r="B11">
         <v>7</v>
@@ -1475,12 +1637,12 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
@@ -1491,8 +1653,13 @@
       <c r="U11" s="5"/>
       <c r="V11" s="5"/>
       <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="AA11">
+        <v>3</v>
+      </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:27">
       <c r="A12" s="6"/>
       <c r="B12">
         <v>8</v>
@@ -1501,12 +1668,12 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
@@ -1517,8 +1684,10 @@
       <c r="U12" s="5"/>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:27">
       <c r="A13" s="6"/>
       <c r="B13">
         <v>9</v>
@@ -1527,12 +1696,12 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
@@ -1543,13 +1712,15 @@
       <c r="U13" s="5"/>
       <c r="V13" s="5"/>
       <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A5:A13"/>
-    <mergeCell ref="L1:W1"/>
+    <mergeCell ref="N1:Y1"/>
   </mergeCells>
-  <conditionalFormatting sqref="L13:W13">
+  <conditionalFormatting sqref="N13:Y13">
     <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
@@ -1571,7 +1742,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L13:W13">
+  <conditionalFormatting sqref="N13:Y13">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1595,7 +1766,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L10:W12 M9:R9 L3:V3 L8:R8 L7:S7 L6:T6 L4:U5">
+  <conditionalFormatting sqref="N11:Y12 O9:T9 N3:X3 N8:T8 N7:U7 N6:V6 N4:W5 N10:S10">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="percent" val="0"/>
@@ -1633,7 +1804,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>L13:W13</xm:sqref>
+          <xm:sqref>N13:Y13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{5780C6F8-193F-7646-97C6-DF03B14611A5}">
@@ -1646,7 +1817,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>L13:W13</xm:sqref>
+          <xm:sqref>N13:Y13</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Results for depth 8
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="13560" windowWidth="49200" windowHeight="13780" tabRatio="500"/>
+    <workbookView xWindow="700" yWindow="13540" windowWidth="49200" windowHeight="13840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="results.prn" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +181,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -206,7 +212,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="159">
+  <cellStyleXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -366,8 +372,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -411,8 +421,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="159">
+  <cellStyles count="163">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -492,6 +507,8 @@
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -571,6 +588,8 @@
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -903,11 +922,12 @@
   <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9"/>
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" customWidth="1"/>
     <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -1034,80 +1054,80 @@
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="19">
         <v>100000</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="20">
         <v>49893</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="20">
         <v>213204</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="20">
         <v>8267265</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="21">
         <f>E3/C3</f>
         <v>2.1320399999999999</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="22">
         <f>D3/C3</f>
         <v>0.49892999999999998</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="21">
         <f>F3/C3</f>
         <v>82.672650000000004</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="22">
         <f>G3/I3</f>
         <v>2.5788939873101924E-2</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K3" s="22">
         <f>H3/I3</f>
         <v>6.0350067404395524E-3</v>
       </c>
-      <c r="L3" s="13">
+      <c r="L3" s="20">
         <v>889</v>
       </c>
-      <c r="M3" s="13">
+      <c r="M3" s="20">
         <v>4984</v>
       </c>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16">
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="T3" s="16">
+      <c r="T3" s="23">
         <v>5.0369999999999998E-2</v>
       </c>
-      <c r="U3" s="16">
+      <c r="U3" s="23">
         <v>0.45832000000000001</v>
       </c>
-      <c r="V3" s="16">
+      <c r="V3" s="23">
         <v>0.89120999999999995</v>
       </c>
-      <c r="W3" s="16">
+      <c r="W3" s="23">
         <v>0.99451999999999996</v>
       </c>
-      <c r="X3" s="16">
+      <c r="X3" s="23">
         <v>0.99992999999999999</v>
       </c>
       <c r="Y3" s="17">
         <v>1</v>
       </c>
-      <c r="Z3" s="12" t="s">
+      <c r="Z3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="AA3" s="12">
+      <c r="AA3" s="19">
         <v>6</v>
       </c>
     </row>
@@ -1195,71 +1215,71 @@
       <c r="A5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="12">
-        <v>1</v>
-      </c>
-      <c r="C5" s="12">
+      <c r="B5" s="19">
+        <v>1</v>
+      </c>
+      <c r="C5" s="19">
         <v>100000</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="20">
         <v>55394</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="20">
         <v>268203</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="20">
         <v>44481199</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="21">
         <f>E5/C5</f>
         <v>2.6820300000000001</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="22">
         <f t="shared" si="0"/>
         <v>0.55393999999999999</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="21">
         <f>F5/C5</f>
         <v>444.81198999999998</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="22">
         <f>G5/I5</f>
         <v>6.0295811720363027E-3</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="22">
         <f t="shared" si="1"/>
         <v>1.2453351358626822E-3</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="20">
         <v>9129</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="20">
         <v>66240</v>
       </c>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16">
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="Q5" s="16">
+      <c r="Q5" s="23">
         <v>7.2480000000000003E-2</v>
       </c>
-      <c r="R5" s="16">
+      <c r="R5" s="23">
         <v>0.39942</v>
       </c>
-      <c r="S5" s="16">
+      <c r="S5" s="23">
         <v>0.76100999999999996</v>
       </c>
-      <c r="T5" s="16">
+      <c r="T5" s="23">
         <v>0.94055</v>
       </c>
-      <c r="U5" s="16">
+      <c r="U5" s="23">
         <v>0.99173</v>
       </c>
-      <c r="V5" s="16">
+      <c r="V5" s="23">
         <v>0.99936000000000003</v>
       </c>
-      <c r="W5" s="16">
+      <c r="W5" s="23">
         <v>0.99997999999999998</v>
       </c>
       <c r="X5" s="17">
@@ -1268,10 +1288,10 @@
       <c r="Y5" s="17">
         <v>1</v>
       </c>
-      <c r="Z5" s="12" t="s">
+      <c r="Z5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="AA5" s="12">
+      <c r="AA5" s="19">
         <v>6</v>
       </c>
     </row>
@@ -1359,67 +1379,67 @@
     </row>
     <row r="7" spans="1:27">
       <c r="A7" s="18"/>
-      <c r="B7" s="12">
+      <c r="B7" s="19">
         <v>3</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="19">
         <v>100000</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="20">
         <v>692435</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="20">
         <v>4101568</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="20">
         <v>105664949</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="21">
         <f>E7/C7</f>
         <v>41.015680000000003</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="22">
         <f t="shared" si="0"/>
         <v>6.9243499999999996</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="21">
         <f>F7/C7</f>
         <v>1056.64949</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="22">
         <f>G7/I7</f>
         <v>3.8816731932554097E-2</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="22">
         <f t="shared" si="1"/>
         <v>6.5531191426591228E-3</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="20">
         <v>26232</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="20">
         <v>121804</v>
       </c>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16">
+      <c r="N7" s="23"/>
+      <c r="O7" s="23">
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="P7" s="16">
+      <c r="P7" s="23">
         <v>0.11705</v>
       </c>
-      <c r="Q7" s="16">
+      <c r="Q7" s="23">
         <v>0.63338000000000005</v>
       </c>
-      <c r="R7" s="16">
+      <c r="R7" s="23">
         <v>0.92276000000000002</v>
       </c>
-      <c r="S7" s="16">
+      <c r="S7" s="23">
         <v>0.98972000000000004</v>
       </c>
-      <c r="T7" s="16">
+      <c r="T7" s="23">
         <v>0.99911000000000005</v>
       </c>
-      <c r="U7" s="16">
+      <c r="U7" s="23">
         <v>0.99999000000000005</v>
       </c>
       <c r="V7" s="17">
@@ -1434,10 +1454,10 @@
       <c r="Y7" s="17">
         <v>1</v>
       </c>
-      <c r="Z7" s="12" t="s">
+      <c r="Z7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="AA7" s="12">
+      <c r="AA7" s="19">
         <v>6</v>
       </c>
     </row>
@@ -1527,64 +1547,64 @@
     </row>
     <row r="9" spans="1:27">
       <c r="A9" s="18"/>
-      <c r="B9" s="12">
+      <c r="B9" s="19">
         <v>5</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="19">
         <v>10000</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="20">
         <v>1712425</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="20">
         <v>10266936</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="20">
         <v>16577687</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="21">
         <f>E9/C9</f>
         <v>1026.6936000000001</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="22">
         <f t="shared" si="0"/>
         <v>171.24250000000001</v>
       </c>
-      <c r="I9" s="14">
+      <c r="I9" s="21">
         <f>F9/C9</f>
         <v>1657.7687000000001</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="22">
         <f>G9/I9</f>
         <v>0.6193225870412441</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9" s="22">
         <f t="shared" si="1"/>
         <v>0.10329697985008403</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="20">
         <v>44565</v>
       </c>
-      <c r="M9" s="13">
+      <c r="M9" s="20">
         <v>149960</v>
       </c>
-      <c r="N9" s="12"/>
-      <c r="O9" s="16">
+      <c r="N9" s="19"/>
+      <c r="O9" s="23">
         <v>1.49E-2</v>
       </c>
-      <c r="P9" s="16">
+      <c r="P9" s="23">
         <v>0.46239999999999998</v>
       </c>
-      <c r="Q9" s="16">
+      <c r="Q9" s="23">
         <v>0.90180000000000005</v>
       </c>
-      <c r="R9" s="16">
+      <c r="R9" s="23">
         <v>0.98560000000000003</v>
       </c>
-      <c r="S9" s="16">
+      <c r="S9" s="23">
         <v>0.99750000000000005</v>
       </c>
-      <c r="T9" s="16">
+      <c r="T9" s="23">
         <v>0.99990000000000001</v>
       </c>
       <c r="U9" s="17">
@@ -1602,10 +1622,10 @@
       <c r="Y9" s="17">
         <v>1</v>
       </c>
-      <c r="Z9" s="12" t="s">
+      <c r="Z9" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="AA9" s="12">
+      <c r="AA9" s="19">
         <v>6</v>
       </c>
     </row>
@@ -1695,58 +1715,58 @@
     </row>
     <row r="11" spans="1:27">
       <c r="A11" s="18"/>
-      <c r="B11" s="12">
+      <c r="B11" s="19">
         <v>7</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="19">
         <v>5000</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="20">
         <v>27113067</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="20">
         <v>81324354</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="20">
         <v>10461163</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="21">
         <f>E11/C11</f>
         <v>16264.870800000001</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="22">
         <f t="shared" ref="H11" si="4">D11/C11</f>
         <v>5422.6134000000002</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="21">
         <f>F11/C11</f>
         <v>2092.2325999999998</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="22">
         <f>G11/I11</f>
         <v>7.7739304893729324</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11" s="22">
         <f t="shared" ref="K11" si="5">H11/I11</f>
         <v>2.5917832462795967</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="20">
         <v>58185</v>
       </c>
-      <c r="M11" s="13">
+      <c r="M11" s="20">
         <v>165452</v>
       </c>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16">
+      <c r="N11" s="23"/>
+      <c r="O11" s="23">
         <v>7.22E-2</v>
       </c>
-      <c r="P11" s="16">
+      <c r="P11" s="23">
         <v>0.67</v>
       </c>
-      <c r="Q11" s="16">
+      <c r="Q11" s="23">
         <v>0.96360000000000001</v>
       </c>
-      <c r="R11" s="16">
+      <c r="R11" s="23">
         <v>0.99580000000000002</v>
       </c>
       <c r="S11" s="17">
@@ -1770,10 +1790,10 @@
       <c r="Y11" s="17">
         <v>1</v>
       </c>
-      <c r="Z11" s="12" t="s">
+      <c r="Z11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="AA11" s="12">
+      <c r="AA11" s="19">
         <v>3</v>
       </c>
     </row>
@@ -1782,66 +1802,100 @@
       <c r="B12" s="12">
         <v>8</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
+      <c r="C12" s="12">
+        <v>608</v>
+      </c>
+      <c r="D12" s="13">
+        <v>20813984</v>
+      </c>
+      <c r="E12" s="13">
+        <v>247712732</v>
+      </c>
+      <c r="F12" s="13">
+        <v>1315687</v>
+      </c>
       <c r="G12" s="14"/>
       <c r="H12" s="15"/>
       <c r="I12" s="14"/>
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
+      <c r="L12" s="13">
+        <v>60275</v>
+      </c>
+      <c r="M12" s="13">
+        <v>150860</v>
+      </c>
       <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="16"/>
-      <c r="U12" s="16"/>
-      <c r="V12" s="16"/>
-      <c r="W12" s="16"/>
-      <c r="X12" s="16"/>
-      <c r="Y12" s="16"/>
+      <c r="O12" s="16">
+        <v>7.0723999999999995E-2</v>
+      </c>
+      <c r="P12" s="16">
+        <v>0.700658</v>
+      </c>
+      <c r="Q12" s="16">
+        <v>0.96052599999999999</v>
+      </c>
+      <c r="R12" s="16">
+        <v>0.99835499999999999</v>
+      </c>
+      <c r="S12" s="17">
+        <v>1</v>
+      </c>
+      <c r="T12" s="17">
+        <v>1</v>
+      </c>
+      <c r="U12" s="17">
+        <v>1</v>
+      </c>
+      <c r="V12" s="17">
+        <v>1</v>
+      </c>
+      <c r="W12" s="17">
+        <v>1</v>
+      </c>
+      <c r="X12" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="17">
+        <v>1</v>
+      </c>
       <c r="Z12" s="12" t="s">
         <v>14</v>
       </c>
       <c r="AA12" s="12">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:27">
       <c r="A13" s="18"/>
-      <c r="B13" s="12">
+      <c r="B13" s="19">
         <v>9</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="16"/>
-      <c r="T13" s="16"/>
-      <c r="U13" s="16"/>
-      <c r="V13" s="16"/>
-      <c r="W13" s="16"/>
-      <c r="X13" s="16"/>
-      <c r="Y13" s="16"/>
-      <c r="Z13" s="12"/>
-      <c r="AA13" s="12"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="23"/>
+      <c r="X13" s="23"/>
+      <c r="Y13" s="23"/>
+      <c r="Z13" s="19"/>
+      <c r="AA13" s="19"/>
     </row>
     <row r="14" spans="1:27">
       <c r="A14" s="1" t="s">
@@ -1928,7 +1982,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N12:Y12 O9:T9 N3:X3 N8:T8 N7:U7 N6:V6 N4:W5 N10:S10 N11:R11">
+  <conditionalFormatting sqref="O9:T9 N3:X3 N8:T8 N7:U7 N6:V6 N4:W5 N10:S10 N11:R12">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="percent" val="0"/>

</xml_diff>

<commit_message>
Refactor out some methods
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="14880" windowWidth="49200" windowHeight="11940" tabRatio="500"/>
+    <workbookView xWindow="180" yWindow="1540" windowWidth="49200" windowHeight="11940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="results.prn" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="22">
   <si>
     <t>Method</t>
   </si>
@@ -257,8 +257,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="245">
+  <cellStyleXfs count="253">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -555,7 +563,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="245">
+  <cellStyles count="253">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -678,6 +686,10 @@
     <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -800,6 +812,10 @@
     <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1131,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2812,31 +2828,84 @@
       <c r="B26" s="9">
         <v>10</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="13"/>
-      <c r="U26" s="13"/>
-      <c r="V26" s="13"/>
-      <c r="W26" s="13"/>
-      <c r="X26" s="13"/>
-      <c r="Y26" s="13"/>
-      <c r="Z26" s="9"/>
-      <c r="AA26" s="9"/>
+      <c r="C26" s="9">
+        <v>34</v>
+      </c>
+      <c r="D26" s="10">
+        <v>24961218</v>
+      </c>
+      <c r="E26" s="10">
+        <v>245091216</v>
+      </c>
+      <c r="F26" s="10">
+        <v>75028</v>
+      </c>
+      <c r="G26" s="10">
+        <v>61876</v>
+      </c>
+      <c r="H26" s="10">
+        <v>126644</v>
+      </c>
+      <c r="I26" s="17">
+        <f t="shared" ref="I26" si="38">E26/C26</f>
+        <v>7208565.176470588</v>
+      </c>
+      <c r="J26" s="18">
+        <f t="shared" ref="J26" si="39">D26/C26</f>
+        <v>734153.4705882353</v>
+      </c>
+      <c r="K26" s="17">
+        <f t="shared" ref="K26" si="40">F26/C26</f>
+        <v>2206.705882352941</v>
+      </c>
+      <c r="L26" s="18">
+        <f t="shared" ref="L26" si="41">I26/K26</f>
+        <v>3266.6633256917421</v>
+      </c>
+      <c r="M26" s="18">
+        <f t="shared" ref="M26" si="42">J26/K26</f>
+        <v>332.69203497360991</v>
+      </c>
+      <c r="N26" s="19"/>
+      <c r="O26" s="13">
+        <v>8.8234999999999994E-2</v>
+      </c>
+      <c r="P26" s="13">
+        <v>0.764706</v>
+      </c>
+      <c r="Q26" s="13">
+        <v>0.94117600000000001</v>
+      </c>
+      <c r="R26" s="13">
+        <v>0.94117600000000001</v>
+      </c>
+      <c r="S26" s="13">
+        <v>1</v>
+      </c>
+      <c r="T26" s="13">
+        <v>1</v>
+      </c>
+      <c r="U26" s="13">
+        <v>1</v>
+      </c>
+      <c r="V26" s="13">
+        <v>1</v>
+      </c>
+      <c r="W26" s="13">
+        <v>1</v>
+      </c>
+      <c r="X26" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA26" s="15">
+        <v>12</v>
+      </c>
     </row>
     <row r="27" spans="1:27">
       <c r="B27" s="15">
@@ -2861,23 +2930,23 @@
         <v>148880</v>
       </c>
       <c r="I27" s="17">
-        <f t="shared" ref="I27" si="38">E27/C27</f>
+        <f t="shared" ref="I27" si="43">E27/C27</f>
         <v>9617603.192307692</v>
       </c>
       <c r="J27" s="18">
-        <f t="shared" ref="J27" si="39">D27/C27</f>
+        <f t="shared" ref="J27" si="44">D27/C27</f>
         <v>898621.69230769225</v>
       </c>
       <c r="K27" s="17">
-        <f t="shared" ref="K27" si="40">F27/C27</f>
+        <f t="shared" ref="K27" si="45">F27/C27</f>
         <v>2705.1923076923076</v>
       </c>
       <c r="L27" s="18">
-        <f t="shared" ref="L27" si="41">I27/K27</f>
+        <f t="shared" ref="L27" si="46">I27/K27</f>
         <v>3555.2382597568776</v>
       </c>
       <c r="M27" s="18">
-        <f t="shared" ref="M27" si="42">J27/K27</f>
+        <f t="shared" ref="M27" si="47">J27/K27</f>
         <v>332.18403355370725</v>
       </c>
       <c r="N27" s="13"/>
@@ -2929,7 +2998,7 @@
     <mergeCell ref="Z1:AA1"/>
   </mergeCells>
   <conditionalFormatting sqref="N13:Y13">
-    <cfRule type="dataBar" priority="67">
+    <cfRule type="dataBar" priority="72">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2941,7 +3010,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="68">
+    <cfRule type="colorScale" priority="73">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>
@@ -2951,7 +3020,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13:Y13">
-    <cfRule type="colorScale" priority="64">
+    <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2961,7 +3030,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="65">
+    <cfRule type="dataBar" priority="70">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2975,7 +3044,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9:T9 N3:X3 N8:T8 N7:U7 N6:V6 N4:W5 N10:S10 N11:R12">
-    <cfRule type="colorScale" priority="69">
+    <cfRule type="colorScale" priority="74">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -2985,7 +3054,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="70">
+    <cfRule type="colorScale" priority="75">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2997,7 +3066,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H13">
-    <cfRule type="colorScale" priority="56">
+    <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3005,7 +3074,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="59">
+    <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3017,7 +3086,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G13">
-    <cfRule type="colorScale" priority="55">
+    <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3027,7 +3096,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N25:Y25">
-    <cfRule type="dataBar" priority="51">
+    <cfRule type="dataBar" priority="56">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3039,7 +3108,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="52">
+    <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>
@@ -3049,7 +3118,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N25:Y25">
-    <cfRule type="colorScale" priority="49">
+    <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3059,7 +3128,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="50">
+    <cfRule type="dataBar" priority="55">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3073,7 +3142,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:V18 O21 N17:W17 N22:S22 N23:R24 Q21:T21 N19:U19 N20:T20">
-    <cfRule type="colorScale" priority="53">
+    <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -3083,7 +3152,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="54">
+    <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3095,7 +3164,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:H25">
-    <cfRule type="colorScale" priority="83">
+    <cfRule type="colorScale" priority="88">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3103,7 +3172,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="84">
+    <cfRule type="colorScale" priority="89">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3115,7 +3184,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17:G25">
-    <cfRule type="colorScale" priority="85">
+    <cfRule type="colorScale" priority="90">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3125,7 +3194,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S24:Y24">
-    <cfRule type="colorScale" priority="44">
+    <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -3135,7 +3204,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="45">
+    <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3147,7 +3216,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S23:Y23">
-    <cfRule type="colorScale" priority="42">
+    <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -3157,7 +3226,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="43">
+    <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3169,7 +3238,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T22:Y22">
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -3179,7 +3248,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="41">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3191,7 +3260,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U20">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -3201,7 +3270,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3213,7 +3282,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N21">
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -3223,7 +3292,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="29">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3235,7 +3304,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P21">
-    <cfRule type="colorScale" priority="24">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -3245,7 +3314,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3257,7 +3326,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17:Y21">
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3269,7 +3338,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17:Y25">
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3281,7 +3350,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:Y12">
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3293,7 +3362,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22">
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -3303,7 +3372,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3315,7 +3384,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3327,7 +3396,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N27:P27">
-    <cfRule type="dataBar" priority="11">
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3339,7 +3408,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>
@@ -3349,7 +3418,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N27:P27">
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3359,7 +3428,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="10">
+    <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3372,8 +3441,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N26:R26">
-    <cfRule type="colorScale" priority="13">
+  <conditionalFormatting sqref="O26:R26">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -3383,7 +3452,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3395,7 +3464,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26:H27">
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3403,7 +3472,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3415,7 +3484,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:G27">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3425,7 +3494,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S26:Y26">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -3435,7 +3504,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3446,8 +3515,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N26:Y26 N27:P27">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="O26:Y26 N27:P27">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3459,7 +3528,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N27">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -3469,7 +3538,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3481,7 +3550,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q27:Y27">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -3491,7 +3560,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3503,6 +3572,64 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q27:Y27">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N26">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{1810DFB6-47F2-F143-8E57-330CA0167153}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFCCFFCC"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N26">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6C763A7F-D732-434C-9477-6DD23E9ECC30}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N26">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3597,6 +3724,32 @@
           </x14:cfRule>
           <xm:sqref>N27:P27</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{1810DFB6-47F2-F143-8E57-330CA0167153}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>N26</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6C763A7F-D732-434C-9477-6DD23E9ECC30}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFFB628"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>N26</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Different game counts for different depths
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="37800" windowHeight="20720" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="32">
   <si>
     <t>Method</t>
   </si>
@@ -112,12 +112,6 @@
   </si>
   <si>
     <t>Close Weight</t>
-  </si>
-  <si>
-    <t>2.6 GHz Intel Core i7</t>
-  </si>
-  <si>
-    <t>2.3.03</t>
   </si>
   <si>
     <t>2.3.4</t>
@@ -305,7 +299,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="335">
+  <cellStyleXfs count="363">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -641,8 +635,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -683,6 +705,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -692,12 +717,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="335">
+  <cellStyles count="363">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -865,6 +886,20 @@
     <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1032,6 +1067,20 @@
     <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1364,7 +1413,7 @@
   <dimension ref="A1:AC43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="W32" sqref="W32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1398,22 +1447,22 @@
       <c r="K1" s="22"/>
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
     </row>
     <row r="2" spans="1:29" s="1" customFormat="1" ht="56" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -1667,7 +1716,7 @@
       <c r="AC4" s="20"/>
     </row>
     <row r="5" spans="1:29">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="27" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="15">
@@ -1754,7 +1803,7 @@
       </c>
     </row>
     <row r="6" spans="1:29">
-      <c r="A6" s="24"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="9">
         <v>2</v>
       </c>
@@ -1839,7 +1888,7 @@
       </c>
     </row>
     <row r="7" spans="1:29">
-      <c r="A7" s="24"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="15">
         <v>3</v>
       </c>
@@ -1926,7 +1975,7 @@
       </c>
     </row>
     <row r="8" spans="1:29">
-      <c r="A8" s="24"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="9">
         <v>4</v>
       </c>
@@ -2013,7 +2062,7 @@
       </c>
     </row>
     <row r="9" spans="1:29">
-      <c r="A9" s="24"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="15">
         <v>5</v>
       </c>
@@ -2100,7 +2149,7 @@
       </c>
     </row>
     <row r="10" spans="1:29">
-      <c r="A10" s="24"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="9">
         <v>6</v>
       </c>
@@ -2187,7 +2236,7 @@
       </c>
     </row>
     <row r="11" spans="1:29">
-      <c r="A11" s="24"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="15">
         <v>7</v>
       </c>
@@ -2274,7 +2323,7 @@
       </c>
     </row>
     <row r="12" spans="1:29">
-      <c r="A12" s="24"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="9">
         <v>8</v>
       </c>
@@ -2361,7 +2410,7 @@
       </c>
     </row>
     <row r="13" spans="1:29">
-      <c r="A13" s="24"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="15">
         <v>9</v>
       </c>
@@ -2485,117 +2534,147 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:29">
-      <c r="A17" s="24" t="s">
+    <row r="17" spans="1:28">
+      <c r="A17" s="27" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="15">
         <v>1</v>
       </c>
       <c r="C17" s="15">
-        <v>96</v>
+        <v>480</v>
       </c>
       <c r="D17" s="16">
-        <v>200</v>
+        <v>381</v>
       </c>
       <c r="E17" s="16">
-        <v>1242</v>
+        <v>3551</v>
       </c>
       <c r="F17" s="16">
-        <v>42060</v>
+        <v>210763</v>
       </c>
       <c r="G17" s="16">
-        <v>8930</v>
+        <v>8975</v>
       </c>
       <c r="H17" s="16">
-        <v>29072</v>
-      </c>
-      <c r="I17" s="17"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
+        <v>34528</v>
+      </c>
+      <c r="I17" s="17">
+        <f t="shared" ref="I17:I23" si="11">E17/C17</f>
+        <v>7.3979166666666663</v>
+      </c>
+      <c r="J17" s="18">
+        <f t="shared" ref="J17:J23" si="12">D17/C17</f>
+        <v>0.79374999999999996</v>
+      </c>
+      <c r="K17" s="17">
+        <f t="shared" ref="K17:K23" si="13">F17/C17</f>
+        <v>439.08958333333334</v>
+      </c>
+      <c r="L17" s="18">
+        <f t="shared" ref="L17:L23" si="14">I17/K17</f>
+        <v>1.6848308289405634E-2</v>
+      </c>
+      <c r="M17" s="18">
+        <f t="shared" ref="M17:M23" si="15">J17/K17</f>
+        <v>1.8077176734056736E-3</v>
+      </c>
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
       <c r="P17" s="19"/>
       <c r="Q17" s="19">
-        <v>5.2082999999999997E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="R17" s="19">
-        <v>0.40625</v>
+        <v>0.375</v>
       </c>
       <c r="S17" s="19">
-        <v>0.79166700000000001</v>
+        <v>0.75833300000000003</v>
       </c>
       <c r="T17" s="19">
-        <v>0.9375</v>
+        <v>0.94374999999999998</v>
       </c>
       <c r="U17" s="19">
         <v>0.98958299999999999</v>
       </c>
-      <c r="V17" s="19">
-        <v>1</v>
-      </c>
-      <c r="W17" s="19">
-        <v>1</v>
-      </c>
-      <c r="X17" s="14">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="14">
+      <c r="V17" s="13">
+        <v>0.99791700000000005</v>
+      </c>
+      <c r="W17" s="13">
+        <v>1</v>
+      </c>
+      <c r="X17" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="13">
         <v>1</v>
       </c>
       <c r="Z17" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA17" s="15">
+        <v>12</v>
+      </c>
+      <c r="AB17" t="s">
         <v>31</v>
       </c>
-      <c r="AA17" s="15">
-        <v>8</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="18" spans="1:29">
-      <c r="A18" s="24"/>
+    <row r="18" spans="1:28">
+      <c r="A18" s="27"/>
       <c r="B18" s="9">
         <v>2</v>
       </c>
       <c r="C18" s="9">
-        <v>96</v>
+        <v>480</v>
       </c>
       <c r="D18" s="10">
-        <v>395</v>
+        <v>956</v>
       </c>
       <c r="E18" s="10">
-        <v>3001</v>
+        <v>10003</v>
       </c>
       <c r="F18" s="10">
-        <v>62985</v>
+        <v>312278</v>
       </c>
       <c r="G18" s="10">
-        <v>14606</v>
+        <v>14505</v>
       </c>
       <c r="H18" s="10">
-        <v>47728</v>
-      </c>
-      <c r="I18" s="17"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
+        <v>53168</v>
+      </c>
+      <c r="I18" s="17">
+        <f t="shared" si="11"/>
+        <v>20.839583333333334</v>
+      </c>
+      <c r="J18" s="18">
+        <f t="shared" si="12"/>
+        <v>1.9916666666666667</v>
+      </c>
+      <c r="K18" s="17">
+        <f t="shared" si="13"/>
+        <v>650.57916666666665</v>
+      </c>
+      <c r="L18" s="18">
+        <f t="shared" si="14"/>
+        <v>3.2032355785550054E-2</v>
+      </c>
+      <c r="M18" s="18">
+        <f t="shared" si="15"/>
+        <v>3.0613748006583876E-3</v>
+      </c>
       <c r="N18" s="13"/>
       <c r="O18" s="13"/>
       <c r="P18" s="13">
-        <v>1.0416999999999999E-2</v>
+        <v>8.3330000000000001E-3</v>
       </c>
       <c r="Q18" s="13">
-        <v>0.22916700000000001</v>
+        <v>0.21875</v>
       </c>
       <c r="R18" s="13">
         <v>0.65625</v>
       </c>
       <c r="S18" s="13">
-        <v>0.92708299999999999</v>
+        <v>0.91249999999999998</v>
       </c>
       <c r="T18" s="13">
         <v>0.98958299999999999</v>
@@ -2606,66 +2685,83 @@
       <c r="V18" s="13">
         <v>1</v>
       </c>
-      <c r="W18" s="14">
-        <v>1</v>
-      </c>
-      <c r="X18" s="14">
-        <v>1</v>
-      </c>
-      <c r="Y18" s="14">
+      <c r="W18" s="13">
+        <v>1</v>
+      </c>
+      <c r="X18" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="13">
         <v>1</v>
       </c>
       <c r="Z18" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA18" s="15">
+        <v>12</v>
+      </c>
+      <c r="AB18" t="s">
         <v>31</v>
       </c>
-      <c r="AA18" s="15">
-        <v>8</v>
-      </c>
-      <c r="AB18" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="19" spans="1:29">
-      <c r="A19" s="24"/>
+    <row r="19" spans="1:28">
+      <c r="A19" s="27"/>
       <c r="B19" s="15">
         <v>3</v>
       </c>
       <c r="C19" s="15">
-        <v>96</v>
+        <v>480</v>
       </c>
       <c r="D19" s="16">
-        <v>1306</v>
+        <v>3392</v>
       </c>
       <c r="E19" s="16">
-        <v>9620</v>
+        <v>38795</v>
       </c>
       <c r="F19" s="16">
-        <v>107551</v>
+        <v>542676</v>
       </c>
       <c r="G19" s="16">
-        <v>28042</v>
+        <v>28357</v>
       </c>
       <c r="H19" s="16">
-        <v>74820</v>
-      </c>
-      <c r="I19" s="17"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
+        <v>99580</v>
+      </c>
+      <c r="I19" s="17">
+        <f t="shared" si="11"/>
+        <v>80.822916666666671</v>
+      </c>
+      <c r="J19" s="18">
+        <f t="shared" si="12"/>
+        <v>7.0666666666666664</v>
+      </c>
+      <c r="K19" s="17">
+        <f t="shared" si="13"/>
+        <v>1130.575</v>
+      </c>
+      <c r="L19" s="18">
+        <f t="shared" si="14"/>
+        <v>7.1488328210571314E-2</v>
+      </c>
+      <c r="M19" s="18">
+        <f t="shared" si="15"/>
+        <v>6.2505067480411883E-3</v>
+      </c>
       <c r="N19" s="13"/>
-      <c r="O19" s="19"/>
+      <c r="O19" s="19">
+        <v>2.0830000000000002E-3</v>
+      </c>
       <c r="P19" s="19">
-        <v>0.125</v>
+        <v>0.13125000000000001</v>
       </c>
       <c r="Q19" s="19">
-        <v>0.6875</v>
+        <v>0.69166700000000003</v>
       </c>
       <c r="R19" s="19">
-        <v>0.94791700000000001</v>
+        <v>0.93958299999999995</v>
       </c>
       <c r="S19" s="19">
-        <v>1</v>
+        <v>0.99375000000000002</v>
       </c>
       <c r="T19" s="19">
         <v>1</v>
@@ -2673,72 +2769,84 @@
       <c r="U19" s="19">
         <v>1</v>
       </c>
-      <c r="V19" s="14">
-        <v>1</v>
-      </c>
-      <c r="W19" s="14">
-        <v>1</v>
-      </c>
-      <c r="X19" s="14">
-        <v>1</v>
-      </c>
-      <c r="Y19" s="14">
-        <v>1</v>
-      </c>
-      <c r="Z19" s="30" t="s">
+      <c r="V19" s="13">
+        <v>1</v>
+      </c>
+      <c r="W19" s="13">
+        <v>1</v>
+      </c>
+      <c r="X19" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA19" s="15">
+        <v>12</v>
+      </c>
+      <c r="AB19" t="s">
         <v>31</v>
       </c>
-      <c r="AA19" s="15">
-        <v>8</v>
-      </c>
-      <c r="AB19" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC19">
-        <v>2.2999999999999998</v>
-      </c>
     </row>
-    <row r="20" spans="1:29">
-      <c r="A20" s="24"/>
+    <row r="20" spans="1:28">
+      <c r="A20" s="27"/>
       <c r="B20" s="9">
         <v>4</v>
       </c>
       <c r="C20" s="9">
-        <v>96</v>
+        <v>480</v>
       </c>
       <c r="D20" s="10">
-        <v>6014</v>
+        <v>39971</v>
       </c>
       <c r="E20" s="10">
-        <v>44977</v>
+        <v>464578</v>
       </c>
       <c r="F20" s="10">
-        <v>117911</v>
+        <v>580794</v>
       </c>
       <c r="G20" s="10">
-        <v>31432</v>
+        <v>30738</v>
       </c>
       <c r="H20" s="10">
-        <v>62972</v>
-      </c>
-      <c r="I20" s="17"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
+        <v>76236</v>
+      </c>
+      <c r="I20" s="17">
+        <f t="shared" si="11"/>
+        <v>967.87083333333328</v>
+      </c>
+      <c r="J20" s="18">
+        <f t="shared" si="12"/>
+        <v>83.27291666666666</v>
+      </c>
+      <c r="K20" s="17">
+        <f t="shared" si="13"/>
+        <v>1209.9875</v>
+      </c>
+      <c r="L20" s="18">
+        <f t="shared" si="14"/>
+        <v>0.79990151413409916</v>
+      </c>
+      <c r="M20" s="18">
+        <f t="shared" si="15"/>
+        <v>6.8821303250377927E-2</v>
+      </c>
       <c r="N20" s="13"/>
       <c r="O20" s="13"/>
       <c r="P20" s="13">
-        <v>0.19791700000000001</v>
+        <v>0.17708299999999999</v>
       </c>
       <c r="Q20" s="13">
-        <v>0.82291700000000001</v>
+        <v>0.75624999999999998</v>
       </c>
       <c r="R20" s="13">
         <v>0.96875</v>
       </c>
       <c r="S20" s="13">
-        <v>1</v>
+        <v>0.99583299999999997</v>
       </c>
       <c r="T20" s="13">
         <v>1</v>
@@ -2746,136 +2854,170 @@
       <c r="U20" s="13">
         <v>1</v>
       </c>
-      <c r="V20" s="14">
-        <v>1</v>
-      </c>
-      <c r="W20" s="14">
-        <v>1</v>
-      </c>
-      <c r="X20" s="14">
-        <v>1</v>
-      </c>
-      <c r="Y20" s="14">
+      <c r="V20" s="13">
+        <v>1</v>
+      </c>
+      <c r="W20" s="13">
+        <v>1</v>
+      </c>
+      <c r="X20" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="13">
         <v>1</v>
       </c>
       <c r="Z20" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA20" s="15">
+        <v>12</v>
+      </c>
+      <c r="AB20" t="s">
         <v>31</v>
       </c>
-      <c r="AA20" s="15">
-        <v>8</v>
-      </c>
-      <c r="AB20" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="21" spans="1:29">
-      <c r="A21" s="24"/>
+    <row r="21" spans="1:28">
+      <c r="A21" s="27"/>
       <c r="B21" s="15">
         <v>5</v>
       </c>
       <c r="C21" s="15">
-        <v>96</v>
+        <v>480</v>
       </c>
       <c r="D21" s="16">
-        <v>39556</v>
+        <v>114748</v>
       </c>
       <c r="E21" s="16">
-        <v>297439</v>
+        <v>1297594</v>
       </c>
       <c r="F21" s="16">
-        <v>171831</v>
+        <v>809567</v>
       </c>
       <c r="G21" s="16">
-        <v>48471</v>
+        <v>45482</v>
       </c>
       <c r="H21" s="16">
-        <v>80416</v>
-      </c>
-      <c r="I21" s="17"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
+        <v>124804</v>
+      </c>
+      <c r="I21" s="17">
+        <f t="shared" si="11"/>
+        <v>2703.3208333333332</v>
+      </c>
+      <c r="J21" s="18">
+        <f t="shared" si="12"/>
+        <v>239.05833333333334</v>
+      </c>
+      <c r="K21" s="17">
+        <f t="shared" si="13"/>
+        <v>1686.5979166666666</v>
+      </c>
+      <c r="L21" s="18">
+        <f t="shared" si="14"/>
+        <v>1.6028247198811216</v>
+      </c>
+      <c r="M21" s="18">
+        <f t="shared" si="15"/>
+        <v>0.14173996716763407</v>
+      </c>
       <c r="N21" s="13"/>
-      <c r="O21" s="19"/>
+      <c r="O21" s="19">
+        <v>1.2500000000000001E-2</v>
+      </c>
       <c r="P21" s="19">
-        <v>0.54166700000000001</v>
+        <v>0.49166700000000002</v>
       </c>
       <c r="Q21" s="19">
-        <v>0.95833299999999999</v>
+        <v>0.9</v>
       </c>
       <c r="R21" s="19">
         <v>0.98958299999999999</v>
       </c>
       <c r="S21" s="19">
-        <v>1</v>
+        <v>0.99791700000000005</v>
       </c>
       <c r="T21" s="19">
         <v>1</v>
       </c>
-      <c r="U21" s="14">
-        <v>1</v>
-      </c>
-      <c r="V21" s="14">
-        <v>1</v>
-      </c>
-      <c r="W21" s="14">
-        <v>1</v>
-      </c>
-      <c r="X21" s="14">
-        <v>1</v>
-      </c>
-      <c r="Y21" s="14">
+      <c r="U21" s="13">
+        <v>1</v>
+      </c>
+      <c r="V21" s="13">
+        <v>1</v>
+      </c>
+      <c r="W21" s="13">
+        <v>1</v>
+      </c>
+      <c r="X21" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="13">
         <v>1</v>
       </c>
       <c r="Z21" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA21" s="15">
+        <v>12</v>
+      </c>
+      <c r="AB21" t="s">
         <v>31</v>
       </c>
-      <c r="AA21" s="15">
-        <v>8</v>
-      </c>
-      <c r="AB21" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="22" spans="1:29">
-      <c r="A22" s="24"/>
+    <row r="22" spans="1:28">
+      <c r="A22" s="27"/>
       <c r="B22" s="9">
         <v>6</v>
       </c>
       <c r="C22" s="9">
-        <v>96</v>
+        <v>480</v>
       </c>
       <c r="D22" s="10">
-        <v>225942</v>
+        <v>1346527</v>
       </c>
       <c r="E22" s="10">
-        <v>1704903</v>
+        <v>15754878</v>
       </c>
       <c r="F22" s="10">
-        <v>170106</v>
+        <v>845904</v>
       </c>
       <c r="G22" s="10">
-        <v>47911</v>
+        <v>47758</v>
       </c>
       <c r="H22" s="10">
-        <v>80468</v>
-      </c>
-      <c r="I22" s="17"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
+        <v>125820</v>
+      </c>
+      <c r="I22" s="17">
+        <f t="shared" si="11"/>
+        <v>32822.662499999999</v>
+      </c>
+      <c r="J22" s="18">
+        <f t="shared" si="12"/>
+        <v>2805.2645833333331</v>
+      </c>
+      <c r="K22" s="17">
+        <f t="shared" si="13"/>
+        <v>1762.3</v>
+      </c>
+      <c r="L22" s="18">
+        <f t="shared" si="14"/>
+        <v>18.624900697951539</v>
+      </c>
+      <c r="M22" s="18">
+        <f t="shared" si="15"/>
+        <v>1.5918201119748812</v>
+      </c>
       <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
+      <c r="O22" s="13">
+        <v>2.0833000000000001E-2</v>
+      </c>
       <c r="P22" s="13">
-        <v>0.55208299999999999</v>
+        <v>0.52291699999999997</v>
       </c>
       <c r="Q22" s="13">
-        <v>0.96875</v>
+        <v>0.91458300000000003</v>
       </c>
       <c r="R22" s="13">
-        <v>1</v>
+        <v>0.98958299999999999</v>
       </c>
       <c r="S22" s="13">
         <v>1</v>
@@ -2899,55 +3041,70 @@
         <v>1</v>
       </c>
       <c r="Z22" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA22" s="15">
+        <v>12</v>
+      </c>
+      <c r="AB22" t="s">
         <v>31</v>
       </c>
-      <c r="AA22" s="15">
-        <v>8</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="23" spans="1:29">
-      <c r="A23" s="24"/>
+    <row r="23" spans="1:28">
+      <c r="A23" s="27"/>
       <c r="B23" s="15">
         <v>7</v>
       </c>
       <c r="C23" s="15">
-        <v>8</v>
+        <v>480</v>
       </c>
       <c r="D23" s="16">
-        <v>113568</v>
+        <v>3209268</v>
       </c>
       <c r="E23" s="16">
-        <v>642553</v>
+        <v>35722453</v>
       </c>
       <c r="F23" s="16">
-        <v>15205</v>
+        <v>1025962</v>
       </c>
       <c r="G23" s="16">
-        <v>52975</v>
+        <v>59808</v>
       </c>
       <c r="H23" s="16">
-        <v>115248</v>
-      </c>
-      <c r="I23" s="17"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
+        <v>154168</v>
+      </c>
+      <c r="I23" s="17">
+        <f t="shared" si="11"/>
+        <v>74421.777083333334</v>
+      </c>
+      <c r="J23" s="18">
+        <f t="shared" si="12"/>
+        <v>6685.9750000000004</v>
+      </c>
+      <c r="K23" s="17">
+        <f t="shared" si="13"/>
+        <v>2137.4208333333331</v>
+      </c>
+      <c r="L23" s="18">
+        <f t="shared" si="14"/>
+        <v>34.818495226918742</v>
+      </c>
+      <c r="M23" s="18">
+        <f t="shared" si="15"/>
+        <v>3.1280573744446678</v>
+      </c>
       <c r="N23" s="13"/>
       <c r="O23" s="19">
-        <v>0.125</v>
+        <v>8.3333000000000004E-2</v>
       </c>
       <c r="P23" s="19">
-        <v>0.5</v>
+        <v>0.70625000000000004</v>
       </c>
       <c r="Q23" s="19">
-        <v>1</v>
+        <v>0.96666700000000005</v>
       </c>
       <c r="R23" s="19">
-        <v>1</v>
+        <v>0.99791700000000005</v>
       </c>
       <c r="S23" s="19">
         <v>1</v>
@@ -2971,70 +3128,70 @@
         <v>1</v>
       </c>
       <c r="Z23" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA23" s="15">
+        <v>12</v>
+      </c>
+      <c r="AB23" t="s">
         <v>31</v>
       </c>
-      <c r="AA23" s="15">
-        <v>8</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="24" spans="1:29">
-      <c r="A24" s="24"/>
+    <row r="24" spans="1:28">
+      <c r="A24" s="27"/>
       <c r="B24" s="9">
         <v>8</v>
       </c>
       <c r="C24" s="9">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="D24" s="10">
-        <v>3401379</v>
+        <v>992266</v>
       </c>
       <c r="E24" s="10">
-        <v>38519590</v>
+        <v>9724819</v>
       </c>
       <c r="F24" s="10">
-        <v>197589</v>
+        <v>26763</v>
       </c>
       <c r="G24" s="10">
-        <v>54404</v>
+        <v>62273</v>
       </c>
       <c r="H24" s="10">
-        <v>125384</v>
+        <v>127184</v>
       </c>
       <c r="I24" s="17">
-        <f t="shared" ref="I17:I27" si="11">E24/C24</f>
-        <v>385195.9</v>
+        <f t="shared" ref="I17:I25" si="16">E24/C24</f>
+        <v>810401.58333333337</v>
       </c>
       <c r="J24" s="18">
-        <f t="shared" ref="J17:J27" si="12">D24/C24</f>
-        <v>34013.79</v>
+        <f t="shared" ref="J17:J25" si="17">D24/C24</f>
+        <v>82688.833333333328</v>
       </c>
       <c r="K24" s="17">
-        <f t="shared" ref="K17:K27" si="13">F24/C24</f>
-        <v>1975.89</v>
+        <f t="shared" ref="K17:K25" si="18">F24/C24</f>
+        <v>2230.25</v>
       </c>
       <c r="L24" s="18">
-        <f t="shared" ref="L17:L27" si="14">I24/K24</f>
-        <v>194.94804872740892</v>
+        <f t="shared" ref="L17:L25" si="19">I24/K24</f>
+        <v>363.36804543586294</v>
       </c>
       <c r="M24" s="18">
-        <f t="shared" ref="M17:M27" si="15">J24/K24</f>
-        <v>17.21441477005299</v>
+        <f t="shared" ref="M17:M25" si="20">J24/K24</f>
+        <v>37.076037813399097</v>
       </c>
       <c r="N24" s="13"/>
       <c r="O24" s="13">
-        <v>0.06</v>
+        <v>8.3333000000000004E-2</v>
       </c>
       <c r="P24" s="13">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="Q24" s="13">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="R24" s="13">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="S24" s="13">
         <v>1</v>
@@ -3057,62 +3214,104 @@
       <c r="Y24" s="13">
         <v>1</v>
       </c>
-      <c r="Z24" s="9"/>
-      <c r="AA24" s="9"/>
-      <c r="AB24">
-        <v>1.5</v>
+      <c r="Z24" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA24" s="9">
+        <v>12</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:29">
-      <c r="A25" s="24"/>
+    <row r="25" spans="1:28">
+      <c r="A25" s="27"/>
       <c r="B25" s="15">
         <v>9</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="17" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J25" s="18" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K25" s="17" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L25" s="18" t="e">
-        <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M25" s="18" t="e">
-        <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
+      <c r="C25" s="15">
+        <v>12</v>
+      </c>
+      <c r="D25" s="16">
+        <v>2883037</v>
+      </c>
+      <c r="E25" s="16">
+        <v>25971860</v>
+      </c>
+      <c r="F25" s="16">
+        <v>32348</v>
+      </c>
+      <c r="G25" s="16">
+        <v>78279</v>
+      </c>
+      <c r="H25" s="16">
+        <v>127256</v>
+      </c>
+      <c r="I25" s="17">
+        <f t="shared" si="16"/>
+        <v>2164321.6666666665</v>
+      </c>
+      <c r="J25" s="18">
+        <f t="shared" si="17"/>
+        <v>240253.08333333334</v>
+      </c>
+      <c r="K25" s="17">
+        <f t="shared" si="18"/>
+        <v>2695.6666666666665</v>
+      </c>
+      <c r="L25" s="18">
+        <f t="shared" si="19"/>
+        <v>802.88920489674786</v>
+      </c>
+      <c r="M25" s="18">
+        <f t="shared" si="20"/>
+        <v>89.125664646964267</v>
       </c>
       <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="19"/>
-      <c r="S25" s="19"/>
-      <c r="T25" s="19"/>
-      <c r="U25" s="19"/>
-      <c r="V25" s="19"/>
-      <c r="W25" s="19"/>
-      <c r="X25" s="19"/>
-      <c r="Y25" s="19"/>
-      <c r="Z25" s="15"/>
-      <c r="AA25" s="15"/>
-      <c r="AB25">
-        <v>1.5</v>
+      <c r="O25" s="19">
+        <v>0.25</v>
+      </c>
+      <c r="P25" s="19">
+        <v>0.91666700000000001</v>
+      </c>
+      <c r="Q25" s="19">
+        <v>1</v>
+      </c>
+      <c r="R25" s="19">
+        <v>1</v>
+      </c>
+      <c r="S25" s="19">
+        <v>1</v>
+      </c>
+      <c r="T25" s="19">
+        <v>1</v>
+      </c>
+      <c r="U25" s="19">
+        <v>1</v>
+      </c>
+      <c r="V25" s="19">
+        <v>1</v>
+      </c>
+      <c r="W25" s="19">
+        <v>1</v>
+      </c>
+      <c r="X25" s="19">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="19">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA25" s="15">
+        <v>12</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:29">
+    <row r="26" spans="1:28">
       <c r="B26" s="9">
         <v>10</v>
       </c>
@@ -3135,23 +3334,23 @@
         <v>126644</v>
       </c>
       <c r="I26" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="I24:I27" si="21">E26/C26</f>
         <v>7208565.176470588</v>
       </c>
       <c r="J26" s="18">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="J24:J27" si="22">D26/C26</f>
         <v>734153.4705882353</v>
       </c>
       <c r="K26" s="17">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="K24:K27" si="23">F26/C26</f>
         <v>2206.705882352941</v>
       </c>
       <c r="L26" s="18">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="L24:L27" si="24">I26/K26</f>
         <v>3266.6633256917421</v>
       </c>
       <c r="M26" s="18">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="M24:M27" si="25">J26/K26</f>
         <v>332.69203497360991</v>
       </c>
       <c r="N26" s="19"/>
@@ -3198,7 +3397,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:29">
+    <row r="27" spans="1:28">
       <c r="B27" s="15">
         <v>11</v>
       </c>
@@ -3221,23 +3420,23 @@
         <v>148880</v>
       </c>
       <c r="I27" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v>9617603.192307692</v>
       </c>
       <c r="J27" s="18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="22"/>
         <v>898621.69230769225</v>
       </c>
       <c r="K27" s="17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="23"/>
         <v>2705.1923076923076</v>
       </c>
       <c r="L27" s="18">
-        <f t="shared" si="14"/>
+        <f t="shared" si="24"/>
         <v>3555.2382597568776</v>
       </c>
       <c r="M27" s="18">
-        <f t="shared" si="15"/>
+        <f t="shared" si="25"/>
         <v>332.18403355370725</v>
       </c>
       <c r="N27" s="13"/>
@@ -3284,51 +3483,47 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="28" spans="1:29">
-      <c r="C28" s="29"/>
+    <row r="28" spans="1:28">
+      <c r="C28" s="26"/>
     </row>
-    <row r="30" spans="1:29">
+    <row r="30" spans="1:28">
       <c r="B30" t="s">
         <v>23</v>
       </c>
-      <c r="G30">
-        <f>D23/D22</f>
-        <v>0.50264227102530734</v>
-      </c>
     </row>
-    <row r="32" spans="1:29">
-      <c r="B32" s="28" t="s">
+    <row r="32" spans="1:28">
+      <c r="B32" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28" t="s">
+      <c r="D32" s="25"/>
+      <c r="E32" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="28" t="s">
+      <c r="F32" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28" t="s">
+      <c r="G32" s="25"/>
+      <c r="H32" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="I32" s="28" t="s">
+      <c r="I32" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28" t="s">
+      <c r="J32" s="25"/>
+      <c r="K32" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="L32" s="28"/>
-      <c r="M32" s="28"/>
-      <c r="N32" s="28" t="s">
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="O32" s="28"/>
+      <c r="O32" s="25"/>
     </row>
-    <row r="33" spans="2:15">
+    <row r="33" spans="2:23">
       <c r="B33">
         <v>1</v>
       </c>
@@ -3359,25 +3554,47 @@
       <c r="O33">
         <v>25639</v>
       </c>
+      <c r="R33">
+        <v>7</v>
+      </c>
+      <c r="S33">
+        <f>D23/1000</f>
+        <v>3209.268</v>
+      </c>
+      <c r="T33">
+        <f>S33/60</f>
+        <v>53.4878</v>
+      </c>
+      <c r="U33">
+        <f>T33/60</f>
+        <v>0.89146333333333339</v>
+      </c>
+      <c r="V33">
+        <v>1</v>
+      </c>
+      <c r="W33">
+        <f>W34*4</f>
+        <v>12582912</v>
+      </c>
     </row>
-    <row r="34" spans="2:15">
+    <row r="34" spans="2:23">
       <c r="B34">
         <v>2</v>
       </c>
       <c r="C34">
         <v>40.4</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="24">
         <f>E33+0.1</f>
         <v>0.2</v>
       </c>
-      <c r="F34" s="27">
+      <c r="F34" s="24">
         <v>79.400000000000006</v>
       </c>
-      <c r="H34" s="27">
-        <v>1</v>
-      </c>
-      <c r="I34" s="27">
+      <c r="H34" s="24">
+        <v>1</v>
+      </c>
+      <c r="I34" s="24">
         <v>78.2</v>
       </c>
       <c r="K34">
@@ -3392,8 +3609,30 @@
       <c r="O34">
         <v>27165</v>
       </c>
+      <c r="R34">
+        <v>8</v>
+      </c>
+      <c r="S34">
+        <f>S33*5</f>
+        <v>16046.34</v>
+      </c>
+      <c r="T34">
+        <f>T33*5</f>
+        <v>267.43900000000002</v>
+      </c>
+      <c r="U34">
+        <f>U33*5</f>
+        <v>4.4573166666666673</v>
+      </c>
+      <c r="V34">
+        <v>2</v>
+      </c>
+      <c r="W34">
+        <f>W35*4</f>
+        <v>3145728</v>
+      </c>
     </row>
-    <row r="35" spans="2:15">
+    <row r="35" spans="2:23">
       <c r="B35">
         <v>3</v>
       </c>
@@ -3401,7 +3640,7 @@
         <v>63.9</v>
       </c>
       <c r="E35">
-        <f t="shared" ref="E35:E42" si="16">E34+0.1</f>
+        <f t="shared" ref="E35:E42" si="26">E34+0.1</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="F35">
@@ -3425,8 +3664,30 @@
       <c r="O35">
         <v>28976</v>
       </c>
+      <c r="R35">
+        <v>9</v>
+      </c>
+      <c r="S35">
+        <f>S34*5</f>
+        <v>80231.7</v>
+      </c>
+      <c r="T35">
+        <f>T34*5</f>
+        <v>1337.1950000000002</v>
+      </c>
+      <c r="U35">
+        <f>U34*5</f>
+        <v>22.286583333333336</v>
+      </c>
+      <c r="V35">
+        <v>3</v>
+      </c>
+      <c r="W35">
+        <f>W36*4</f>
+        <v>786432</v>
+      </c>
     </row>
-    <row r="36" spans="2:15">
+    <row r="36" spans="2:23">
       <c r="B36">
         <v>4</v>
       </c>
@@ -3434,7 +3695,7 @@
         <v>71.099999999999994</v>
       </c>
       <c r="E36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="26"/>
         <v>0.4</v>
       </c>
       <c r="F36">
@@ -3458,8 +3719,30 @@
       <c r="O36">
         <v>27826</v>
       </c>
+      <c r="R36">
+        <v>10</v>
+      </c>
+      <c r="S36">
+        <f>S35*5</f>
+        <v>401158.5</v>
+      </c>
+      <c r="T36">
+        <f>T35*5</f>
+        <v>6685.9750000000004</v>
+      </c>
+      <c r="U36">
+        <f>U35*5</f>
+        <v>111.43291666666669</v>
+      </c>
+      <c r="V36">
+        <v>4</v>
+      </c>
+      <c r="W36">
+        <f>W37*4</f>
+        <v>196608</v>
+      </c>
     </row>
-    <row r="37" spans="2:15">
+    <row r="37" spans="2:23">
       <c r="B37">
         <v>5</v>
       </c>
@@ -3467,7 +3750,7 @@
         <v>70.900000000000006</v>
       </c>
       <c r="E37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="26"/>
         <v>0.5</v>
       </c>
       <c r="F37">
@@ -3488,8 +3771,30 @@
       <c r="N37">
         <v>1.4</v>
       </c>
+      <c r="R37">
+        <v>11</v>
+      </c>
+      <c r="S37">
+        <f>S36*5</f>
+        <v>2005792.5</v>
+      </c>
+      <c r="T37">
+        <f>T36*5</f>
+        <v>33429.875</v>
+      </c>
+      <c r="U37">
+        <f>U36*5</f>
+        <v>557.16458333333344</v>
+      </c>
+      <c r="V37">
+        <v>5</v>
+      </c>
+      <c r="W37">
+        <f>W38*4</f>
+        <v>49152</v>
+      </c>
     </row>
-    <row r="38" spans="2:15">
+    <row r="38" spans="2:23">
       <c r="B38">
         <v>6</v>
       </c>
@@ -3497,7 +3802,7 @@
         <v>75.2</v>
       </c>
       <c r="E38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="26"/>
         <v>0.6</v>
       </c>
       <c r="F38">
@@ -3518,16 +3823,23 @@
       <c r="N38">
         <v>1.5</v>
       </c>
+      <c r="V38">
+        <v>6</v>
+      </c>
+      <c r="W38">
+        <f>W39*4</f>
+        <v>12288</v>
+      </c>
     </row>
-    <row r="39" spans="2:15">
-      <c r="B39" s="27">
+    <row r="39" spans="2:23">
+      <c r="B39" s="24">
         <v>7</v>
       </c>
-      <c r="C39" s="27">
+      <c r="C39" s="24">
         <v>76.7</v>
       </c>
       <c r="E39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="26"/>
         <v>0.7</v>
       </c>
       <c r="F39">
@@ -3542,8 +3854,15 @@
       <c r="N39">
         <v>1.6</v>
       </c>
+      <c r="V39">
+        <v>7</v>
+      </c>
+      <c r="W39">
+        <f>W40*4</f>
+        <v>3072</v>
+      </c>
     </row>
-    <row r="40" spans="2:15">
+    <row r="40" spans="2:23">
       <c r="B40">
         <v>8</v>
       </c>
@@ -3551,7 +3870,7 @@
         <v>76.7</v>
       </c>
       <c r="E40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="26"/>
         <v>0.79999999999999993</v>
       </c>
       <c r="F40">
@@ -3563,8 +3882,15 @@
       <c r="N40">
         <v>1.7</v>
       </c>
+      <c r="V40">
+        <v>8</v>
+      </c>
+      <c r="W40">
+        <f>W41*4</f>
+        <v>768</v>
+      </c>
     </row>
-    <row r="41" spans="2:15">
+    <row r="41" spans="2:23">
       <c r="B41">
         <v>9</v>
       </c>
@@ -3572,7 +3898,7 @@
         <v>74.3</v>
       </c>
       <c r="E41">
-        <f t="shared" si="16"/>
+        <f t="shared" si="26"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="F41">
@@ -3584,8 +3910,15 @@
       <c r="N41">
         <v>1.8</v>
       </c>
+      <c r="V41">
+        <v>9</v>
+      </c>
+      <c r="W41">
+        <f>W42*4</f>
+        <v>192</v>
+      </c>
     </row>
-    <row r="42" spans="2:15">
+    <row r="42" spans="2:23">
       <c r="B42">
         <v>10</v>
       </c>
@@ -3593,7 +3926,7 @@
         <v>76.2</v>
       </c>
       <c r="E42">
-        <f t="shared" si="16"/>
+        <f t="shared" si="26"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="F42">
@@ -3605,8 +3938,15 @@
       <c r="N42">
         <v>1.9</v>
       </c>
+      <c r="V42">
+        <v>10</v>
+      </c>
+      <c r="W42">
+        <f>W43*4</f>
+        <v>48</v>
+      </c>
     </row>
-    <row r="43" spans="2:15">
+    <row r="43" spans="2:23">
       <c r="E43">
         <v>1.1000000000000001</v>
       </c>
@@ -3618,6 +3958,12 @@
       </c>
       <c r="N43">
         <v>2</v>
+      </c>
+      <c r="V43">
+        <v>11</v>
+      </c>
+      <c r="W43">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3628,7 +3974,7 @@
     <mergeCell ref="Z1:AA1"/>
   </mergeCells>
   <conditionalFormatting sqref="N13:Y13">
-    <cfRule type="dataBar" priority="80">
+    <cfRule type="dataBar" priority="87">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3640,7 +3986,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="81">
+    <cfRule type="colorScale" priority="88">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>
@@ -3650,7 +3996,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13:Y13">
-    <cfRule type="colorScale" priority="77">
+    <cfRule type="colorScale" priority="84">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3660,7 +4006,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="78">
+    <cfRule type="dataBar" priority="85">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3674,7 +4020,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9:T9 N3:X3 N8:T8 N7:U7 N6:V6 N4:W5 N10:S10 N11:R12">
-    <cfRule type="colorScale" priority="82">
+    <cfRule type="colorScale" priority="89">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -3684,7 +4030,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="83">
+    <cfRule type="colorScale" priority="90">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3696,7 +4042,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H13">
-    <cfRule type="colorScale" priority="69">
+    <cfRule type="colorScale" priority="76">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3704,7 +4050,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="72">
+    <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3716,7 +4062,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G13">
-    <cfRule type="colorScale" priority="68">
+    <cfRule type="colorScale" priority="75">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3725,76 +4071,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N25:Y25">
-    <cfRule type="dataBar" priority="64">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63C384"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{CCB8BA57-3195-3846-BB2C-7696DAA28184}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-    <cfRule type="colorScale" priority="65">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFCCFFCC"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N25:Y25">
-    <cfRule type="colorScale" priority="62">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="63">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFB628"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{051D336B-17A9-5344-80F7-ED8E7CFBA64F}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N22:S22 O21 Q21:T21 N23:R24 N19:U19 N17:W17 N18:V18 N20:T20">
-    <cfRule type="colorScale" priority="66">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="67">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H17:H25">
-    <cfRule type="colorScale" priority="96">
+    <cfRule type="colorScale" priority="103">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3802,7 +4080,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="97">
+    <cfRule type="colorScale" priority="104">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3814,7 +4092,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17:G25">
-    <cfRule type="colorScale" priority="98">
+    <cfRule type="colorScale" priority="105">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3823,139 +4101,27 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S24:Y24">
-    <cfRule type="colorScale" priority="57">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="58">
+  <conditionalFormatting sqref="N3:Y12">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
+        <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S23:Y23">
-    <cfRule type="colorScale" priority="55">
+  <conditionalFormatting sqref="H26:H27">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="56">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T22:Y22">
-    <cfRule type="colorScale" priority="53">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="54">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U20">
-    <cfRule type="colorScale" priority="51">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="52">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N21">
-    <cfRule type="colorScale" priority="41">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="42">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P21">
-    <cfRule type="colorScale" priority="37">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="38">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N17:Y21">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -3967,154 +4133,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N17:Y25">
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N3:Y12">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N22">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N22">
-    <cfRule type="colorScale" priority="31">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N27:P27">
-    <cfRule type="dataBar" priority="24">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63C384"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{051C1A61-6054-8C4B-AEBC-36C45696833A}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFCCFFCC"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N27:P27">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="23">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFB628"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{AC0C1DD2-A318-F345-A17E-A12FD77B3CA8}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O26:R26">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H26:H27">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G26:G27">
-    <cfRule type="colorScale" priority="30">
+    <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4123,239 +4143,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S26:Y26">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O26:Y26 N27:P27">
-    <cfRule type="colorScale" priority="19">
+  <conditionalFormatting sqref="N17:Y27">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N27">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q27:Y27">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q27:Y27">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N26">
-    <cfRule type="dataBar" priority="12">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63C384"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{1810DFB6-47F2-F143-8E57-330CA0167153}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFCCFFCC"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N26">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="11">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFB628"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6C763A7F-D732-434C-9477-6DD23E9ECC30}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N26">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N23">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N23">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N24">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N24">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N21">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
@@ -4392,84 +4186,6 @@
           </x14:cfRule>
           <xm:sqref>N13:Y13</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{CCB8BA57-3195-3846-BB2C-7696DAA28184}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF63C384"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>N25:Y25</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{051D336B-17A9-5344-80F7-ED8E7CFBA64F}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FFFFB628"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>N25:Y25</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{051C1A61-6054-8C4B-AEBC-36C45696833A}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF63C384"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>N27:P27</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{AC0C1DD2-A318-F345-A17E-A12FD77B3CA8}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FFFFB628"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>N27:P27</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{1810DFB6-47F2-F143-8E57-330CA0167153}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF63C384"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>N26</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6C763A7F-D732-434C-9477-6DD23E9ECC30}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FFFFB628"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>N26</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Change number of runs per depth
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="37">
   <si>
     <t>Method</t>
   </si>
@@ -115,6 +115,21 @@
   </si>
   <si>
     <t>2.3.5</t>
+  </si>
+  <si>
+    <t>Mult for minute</t>
+  </si>
+  <si>
+    <t>Games per minute</t>
+  </si>
+  <si>
+    <t>Games played</t>
+  </si>
+  <si>
+    <t>Desired Minutes</t>
+  </si>
+  <si>
+    <t>Required Games</t>
   </si>
 </sst>
 </file>
@@ -299,8 +314,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="377">
+  <cellStyleXfs count="379">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -732,7 +749,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="377">
+  <cellStyles count="379">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -921,6 +938,7 @@
     <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1109,6 +1127,7 @@
     <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1438,10 +1457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC41"/>
+  <dimension ref="A1:AC44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="T40" sqref="T40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3349,7 +3368,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:28" ht="39" customHeight="1">
       <c r="B30" s="25" t="s">
         <v>25</v>
       </c>
@@ -3380,6 +3399,21 @@
         <v>30</v>
       </c>
       <c r="O30" s="25"/>
+      <c r="Q30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U30" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="31" spans="1:28">
       <c r="B31">
@@ -3423,12 +3457,12 @@
         <f>Q31*R31</f>
         <v>235229.54483083077</v>
       </c>
-      <c r="V31">
-        <v>1</v>
-      </c>
-      <c r="W31">
-        <f>W32*4</f>
-        <v>12582912</v>
+      <c r="T31">
+        <v>1</v>
+      </c>
+      <c r="U31" s="26">
+        <f>S31*T31</f>
+        <v>235229.54483083077</v>
       </c>
     </row>
     <row r="32" spans="1:28">
@@ -3474,15 +3508,15 @@
         <f t="shared" ref="S32:S39" si="17">Q32*R32</f>
         <v>34504.175005175624</v>
       </c>
-      <c r="V32">
-        <v>2</v>
-      </c>
-      <c r="W32">
-        <f>W33*4</f>
-        <v>3145728</v>
+      <c r="T32">
+        <v>3</v>
+      </c>
+      <c r="U32" s="26">
+        <f>S32*T32</f>
+        <v>103512.52501552687</v>
       </c>
     </row>
-    <row r="33" spans="2:23">
+    <row r="33" spans="2:21">
       <c r="B33">
         <v>3</v>
       </c>
@@ -3525,15 +3559,15 @@
         <f t="shared" si="17"/>
         <v>8911.0675458919977</v>
       </c>
-      <c r="V33">
-        <v>3</v>
-      </c>
-      <c r="W33">
-        <f>W34*4</f>
-        <v>786432</v>
+      <c r="T33">
+        <v>5</v>
+      </c>
+      <c r="U33" s="26">
+        <f>S33*T33</f>
+        <v>44555.337729459992</v>
       </c>
     </row>
-    <row r="34" spans="2:23">
+    <row r="34" spans="2:21">
       <c r="B34">
         <v>4</v>
       </c>
@@ -3576,15 +3610,15 @@
         <f t="shared" si="17"/>
         <v>662.35254376494424</v>
       </c>
-      <c r="V34">
-        <v>4</v>
-      </c>
-      <c r="W34">
-        <f>W35*4</f>
-        <v>196608</v>
+      <c r="T34">
+        <v>25</v>
+      </c>
+      <c r="U34" s="26">
+        <f>S34*T34</f>
+        <v>16558.813594123607</v>
       </c>
     </row>
-    <row r="35" spans="2:23">
+    <row r="35" spans="2:21">
       <c r="B35">
         <v>5</v>
       </c>
@@ -3624,15 +3658,15 @@
         <f t="shared" si="17"/>
         <v>278.2131298049726</v>
       </c>
-      <c r="V35">
-        <v>5</v>
-      </c>
-      <c r="W35">
-        <f>W36*4</f>
-        <v>49152</v>
+      <c r="T35">
+        <v>60</v>
+      </c>
+      <c r="U35" s="26">
+        <f t="shared" ref="U35:U39" si="19">S35*T35</f>
+        <v>16692.787788298356</v>
       </c>
     </row>
-    <row r="36" spans="2:23">
+    <row r="36" spans="2:21">
       <c r="B36">
         <v>6</v>
       </c>
@@ -3672,15 +3706,15 @@
         <f t="shared" si="17"/>
         <v>19.588152562979175</v>
       </c>
-      <c r="V36">
-        <v>6</v>
-      </c>
-      <c r="W36">
-        <f>W37*4</f>
-        <v>12288</v>
+      <c r="T36">
+        <v>60</v>
+      </c>
+      <c r="U36" s="26">
+        <f t="shared" si="19"/>
+        <v>1175.2891537787505</v>
       </c>
     </row>
-    <row r="37" spans="2:23">
+    <row r="37" spans="2:21">
       <c r="B37" s="24">
         <v>7</v>
       </c>
@@ -3714,15 +3748,15 @@
         <f t="shared" si="17"/>
         <v>9.5967417142531772</v>
       </c>
-      <c r="V37">
-        <v>7</v>
-      </c>
-      <c r="W37">
-        <f>W38*4</f>
-        <v>3072</v>
+      <c r="T37">
+        <v>120</v>
+      </c>
+      <c r="U37" s="26">
+        <f t="shared" si="19"/>
+        <v>1151.6090057103813</v>
       </c>
     </row>
-    <row r="38" spans="2:23">
+    <row r="38" spans="2:21">
       <c r="B38">
         <v>8</v>
       </c>
@@ -3753,15 +3787,15 @@
         <f t="shared" si="17"/>
         <v>0.67641528399115314</v>
       </c>
-      <c r="V38">
-        <v>8</v>
-      </c>
-      <c r="W38">
-        <f>W39*4</f>
-        <v>768</v>
+      <c r="T38">
+        <v>360</v>
+      </c>
+      <c r="U38" s="26">
+        <f t="shared" si="19"/>
+        <v>243.50950223681514</v>
       </c>
     </row>
-    <row r="39" spans="2:23">
+    <row r="39" spans="2:21">
       <c r="B39">
         <v>9</v>
       </c>
@@ -3792,15 +3826,15 @@
         <f t="shared" si="17"/>
         <v>0.36320122655475551</v>
       </c>
-      <c r="V39">
-        <v>9</v>
-      </c>
-      <c r="W39">
-        <f>W40*4</f>
-        <v>192</v>
+      <c r="T39">
+        <v>720</v>
+      </c>
+      <c r="U39" s="26">
+        <f t="shared" si="19"/>
+        <v>261.50488311942399</v>
       </c>
     </row>
-    <row r="40" spans="2:23">
+    <row r="40" spans="2:21">
       <c r="B40">
         <v>10</v>
       </c>
@@ -3820,15 +3854,8 @@
       <c r="N40">
         <v>1.9</v>
       </c>
-      <c r="V40">
-        <v>10</v>
-      </c>
-      <c r="W40">
-        <f>W41*4</f>
-        <v>48</v>
-      </c>
     </row>
-    <row r="41" spans="2:23">
+    <row r="41" spans="2:21">
       <c r="E41">
         <v>1.1000000000000001</v>
       </c>
@@ -3841,11 +3868,11 @@
       <c r="N41">
         <v>2</v>
       </c>
-      <c r="V41">
-        <v>11</v>
-      </c>
-      <c r="W41">
-        <v>12</v>
+    </row>
+    <row r="44" spans="2:21">
+      <c r="T44">
+        <f>SUM(T31:T39)/60</f>
+        <v>22.566666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version 2.3.7 - minor speed improvements
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="43">
   <si>
     <t>Method</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>EC2 Minutes</t>
-  </si>
-  <si>
-    <t>q</t>
   </si>
 </sst>
 </file>
@@ -335,7 +332,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="421">
+  <cellStyleXfs count="445">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -757,8 +754,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -802,18 +823,26 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="421">
+  <cellStyles count="445">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1024,6 +1053,18 @@
     <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1234,9 +1275,32 @@
     <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
@@ -1563,10 +1627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC44"/>
+  <dimension ref="A1:AC71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1600,22 +1664,22 @@
       <c r="K1" s="22"/>
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
-      <c r="N1" s="28" t="s">
+      <c r="N1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
     </row>
     <row r="2" spans="1:29" s="1" customFormat="1" ht="56" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -1729,7 +1793,7 @@
         <v>4984</v>
       </c>
       <c r="I3" s="17">
-        <f t="shared" ref="I3:I12" si="0">E3/C3</f>
+        <f t="shared" ref="I3:I4" si="0">E3/C3</f>
         <v>2.1320399999999999</v>
       </c>
       <c r="J3" s="18">
@@ -1737,11 +1801,11 @@
         <v>0.49892999999999998</v>
       </c>
       <c r="K3" s="17">
-        <f t="shared" ref="K3:K12" si="1">F3/C3</f>
+        <f t="shared" ref="K3:K4" si="1">F3/C3</f>
         <v>82.672650000000004</v>
       </c>
       <c r="L3" s="18">
-        <f t="shared" ref="L3:L12" si="2">I3/K3</f>
+        <f t="shared" ref="L3:L4" si="2">I3/K3</f>
         <v>2.5788939873101924E-2</v>
       </c>
       <c r="M3" s="18">
@@ -1814,7 +1878,7 @@
         <v>2.2993800000000002</v>
       </c>
       <c r="J4" s="12">
-        <f t="shared" ref="J4:J9" si="3">D4/C4</f>
+        <f t="shared" ref="J4" si="3">D4/C4</f>
         <v>0.52159999999999995</v>
       </c>
       <c r="K4" s="11">
@@ -1826,7 +1890,7 @@
         <v>1.2468462551557438E-2</v>
       </c>
       <c r="M4" s="12">
-        <f t="shared" ref="M4:M9" si="4">J4/K4</f>
+        <f t="shared" ref="M4" si="4">J4/K4</f>
         <v>2.8283929002132571E-3</v>
       </c>
       <c r="N4" s="13"/>
@@ -1868,1067 +1932,1024 @@
       </c>
       <c r="AC4" s="20"/>
     </row>
-    <row r="5" spans="1:29">
-      <c r="A5" s="27" t="s">
+    <row r="5" spans="1:29" ht="17">
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AC5" s="20"/>
+    </row>
+    <row r="6" spans="1:29">
+      <c r="A6" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="36"/>
+      <c r="U6" s="36"/>
+      <c r="V6" s="36"/>
+      <c r="W6" s="36"/>
+      <c r="X6" s="36"/>
+      <c r="Y6" s="36"/>
+      <c r="Z6" s="37"/>
+      <c r="AA6" s="37"/>
+    </row>
+    <row r="7" spans="1:29" s="1" customFormat="1" ht="56" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="7">
+        <v>16384</v>
+      </c>
+      <c r="O7" s="7">
+        <v>8192</v>
+      </c>
+      <c r="P7" s="7">
+        <v>4096</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>2048</v>
+      </c>
+      <c r="R7" s="7">
+        <v>1024</v>
+      </c>
+      <c r="S7" s="7">
+        <v>512</v>
+      </c>
+      <c r="T7" s="7">
+        <v>256</v>
+      </c>
+      <c r="U7" s="7">
+        <v>128</v>
+      </c>
+      <c r="V7" s="7">
+        <v>64</v>
+      </c>
+      <c r="W7" s="7">
+        <v>32</v>
+      </c>
+      <c r="X7" s="7">
+        <v>16</v>
+      </c>
+      <c r="Y7" s="7">
         <v>8</v>
       </c>
-      <c r="B5" s="15">
-        <v>1</v>
-      </c>
-      <c r="C5" s="15">
+      <c r="Z7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB7" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
+      <c r="A8" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="15">
+        <v>1</v>
+      </c>
+      <c r="C8" s="15">
         <v>100000</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D8" s="16">
         <v>55394</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E8" s="16">
         <v>268203</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F8" s="16">
         <v>44481199</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G8" s="16">
         <v>9129</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H8" s="16">
         <v>66240</v>
       </c>
-      <c r="I5" s="17">
-        <f t="shared" si="0"/>
+      <c r="I8" s="17">
+        <f t="shared" ref="I8:I15" si="5">E8/C8</f>
         <v>2.6820300000000001</v>
       </c>
-      <c r="J5" s="18">
-        <f t="shared" si="3"/>
+      <c r="J8" s="18">
+        <f t="shared" ref="J8:J12" si="6">D8/C8</f>
         <v>0.55393999999999999</v>
       </c>
-      <c r="K5" s="17">
-        <f t="shared" si="1"/>
+      <c r="K8" s="17">
+        <f t="shared" ref="K8:K15" si="7">F8/C8</f>
         <v>444.81198999999998</v>
       </c>
-      <c r="L5" s="18">
-        <f t="shared" si="2"/>
+      <c r="L8" s="18">
+        <f t="shared" ref="L8:L15" si="8">I8/K8</f>
         <v>6.0295811720363027E-3</v>
       </c>
-      <c r="M5" s="18">
-        <f t="shared" si="4"/>
+      <c r="M8" s="18">
+        <f t="shared" ref="M8:M12" si="9">J8/K8</f>
         <v>1.2453351358626822E-3</v>
       </c>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19">
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="Q5" s="19">
+      <c r="Q8" s="19">
         <v>7.2480000000000003E-2</v>
       </c>
-      <c r="R5" s="19">
+      <c r="R8" s="19">
         <v>0.39942</v>
       </c>
-      <c r="S5" s="19">
+      <c r="S8" s="19">
         <v>0.76100999999999996</v>
       </c>
-      <c r="T5" s="19">
+      <c r="T8" s="19">
         <v>0.94055</v>
       </c>
-      <c r="U5" s="19">
+      <c r="U8" s="19">
         <v>0.99173</v>
       </c>
-      <c r="V5" s="19">
+      <c r="V8" s="19">
         <v>0.99936000000000003</v>
       </c>
-      <c r="W5" s="19">
+      <c r="W8" s="19">
         <v>0.99997999999999998</v>
       </c>
-      <c r="X5" s="14">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="14">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="15" t="s">
+      <c r="X8" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AA5" s="15">
+      <c r="AA8" s="15">
         <v>6</v>
       </c>
-      <c r="AB5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29">
-      <c r="A6" s="27"/>
-      <c r="B6" s="9">
+      <c r="AB8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
+      <c r="A9" s="38"/>
+      <c r="B9" s="9">
         <v>2</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C9" s="9">
         <v>100000</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D9" s="10">
         <v>355984</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E9" s="10">
         <v>2084273</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F9" s="10">
         <v>63432843</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G9" s="10">
         <v>14103</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H9" s="10">
         <v>72692</v>
       </c>
-      <c r="I6" s="11">
-        <f t="shared" si="0"/>
+      <c r="I9" s="11">
+        <f t="shared" si="5"/>
         <v>20.84273</v>
       </c>
-      <c r="J6" s="12">
-        <f t="shared" si="3"/>
+      <c r="J9" s="12">
+        <f t="shared" si="6"/>
         <v>3.5598399999999999</v>
       </c>
-      <c r="K6" s="11">
-        <f t="shared" si="1"/>
+      <c r="K9" s="11">
+        <f t="shared" si="7"/>
         <v>634.32843000000003</v>
       </c>
-      <c r="L6" s="12">
-        <f t="shared" si="2"/>
+      <c r="L9" s="12">
+        <f t="shared" si="8"/>
         <v>3.2857947104782924E-2</v>
       </c>
-      <c r="M6" s="12">
-        <f t="shared" si="4"/>
+      <c r="M9" s="12">
+        <f t="shared" si="9"/>
         <v>5.6119824236791653E-3</v>
       </c>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13">
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13">
         <v>7.9699999999999997E-3</v>
       </c>
-      <c r="Q6" s="13">
+      <c r="Q9" s="13">
         <v>0.21351000000000001</v>
       </c>
-      <c r="R6" s="13">
+      <c r="R9" s="13">
         <v>0.64770000000000005</v>
       </c>
-      <c r="S6" s="13">
+      <c r="S9" s="13">
         <v>0.91000999999999999</v>
       </c>
-      <c r="T6" s="13">
+      <c r="T9" s="13">
         <v>0.98502999999999996</v>
       </c>
-      <c r="U6" s="13">
+      <c r="U9" s="13">
         <v>0.99843999999999999</v>
       </c>
-      <c r="V6" s="13">
+      <c r="V9" s="13">
         <v>0.99995000000000001</v>
       </c>
-      <c r="W6" s="14">
-        <v>1</v>
-      </c>
-      <c r="X6" s="14">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="14">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="9" t="s">
+      <c r="W9" s="14">
+        <v>1</v>
+      </c>
+      <c r="X9" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AA6" s="9">
+      <c r="AA9" s="9">
         <v>6</v>
       </c>
-      <c r="AB6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29">
-      <c r="A7" s="27"/>
-      <c r="B7" s="15">
+      <c r="AB9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
+      <c r="A10" s="38"/>
+      <c r="B10" s="15">
         <v>3</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C10" s="15">
         <v>100000</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D10" s="16">
         <v>692435</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E10" s="16">
         <v>4101568</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F10" s="16">
         <v>105664949</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G10" s="16">
         <v>26232</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H10" s="16">
         <v>121804</v>
       </c>
-      <c r="I7" s="17">
-        <f t="shared" si="0"/>
+      <c r="I10" s="17">
+        <f t="shared" si="5"/>
         <v>41.015680000000003</v>
       </c>
-      <c r="J7" s="18">
-        <f t="shared" si="3"/>
+      <c r="J10" s="18">
+        <f t="shared" si="6"/>
         <v>6.9243499999999996</v>
       </c>
-      <c r="K7" s="17">
-        <f t="shared" si="1"/>
+      <c r="K10" s="17">
+        <f t="shared" si="7"/>
         <v>1056.64949</v>
       </c>
-      <c r="L7" s="18">
-        <f t="shared" si="2"/>
+      <c r="L10" s="18">
+        <f t="shared" si="8"/>
         <v>3.8816731932554097E-2</v>
       </c>
-      <c r="M7" s="18">
-        <f t="shared" si="4"/>
+      <c r="M10" s="18">
+        <f t="shared" si="9"/>
         <v>6.5531191426591228E-3</v>
       </c>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19">
+      <c r="N10" s="19"/>
+      <c r="O10" s="19">
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="P7" s="19">
+      <c r="P10" s="19">
         <v>0.11705</v>
       </c>
-      <c r="Q7" s="19">
+      <c r="Q10" s="19">
         <v>0.63338000000000005</v>
       </c>
-      <c r="R7" s="19">
+      <c r="R10" s="19">
         <v>0.92276000000000002</v>
       </c>
-      <c r="S7" s="19">
+      <c r="S10" s="19">
         <v>0.98972000000000004</v>
       </c>
-      <c r="T7" s="19">
+      <c r="T10" s="19">
         <v>0.99911000000000005</v>
       </c>
-      <c r="U7" s="19">
+      <c r="U10" s="19">
         <v>0.99999000000000005</v>
       </c>
-      <c r="V7" s="14">
-        <v>1</v>
-      </c>
-      <c r="W7" s="14">
-        <v>1</v>
-      </c>
-      <c r="X7" s="14">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="14">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="15" t="s">
+      <c r="V10" s="14">
+        <v>1</v>
+      </c>
+      <c r="W10" s="14">
+        <v>1</v>
+      </c>
+      <c r="X10" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AA7" s="15">
+      <c r="AA10" s="15">
         <v>6</v>
       </c>
-      <c r="AB7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29">
-      <c r="A8" s="27"/>
-      <c r="B8" s="9">
+      <c r="AB10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
+      <c r="A11" s="38"/>
+      <c r="B11" s="9">
         <v>4</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C11" s="9">
         <v>10000</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D11" s="10">
         <v>1412938</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E11" s="10">
         <v>8470477</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F11" s="10">
         <v>11409683</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G11" s="10">
         <v>28757</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H11" s="10">
         <v>109576</v>
       </c>
-      <c r="I8" s="11">
-        <f t="shared" si="0"/>
+      <c r="I11" s="11">
+        <f t="shared" si="5"/>
         <v>847.04769999999996</v>
       </c>
-      <c r="J8" s="12">
-        <f t="shared" si="3"/>
+      <c r="J11" s="12">
+        <f t="shared" si="6"/>
         <v>141.2938</v>
       </c>
-      <c r="K8" s="11">
-        <f t="shared" si="1"/>
+      <c r="K11" s="11">
+        <f t="shared" si="7"/>
         <v>1140.9683</v>
       </c>
-      <c r="L8" s="12">
-        <f t="shared" si="2"/>
+      <c r="L11" s="12">
+        <f t="shared" si="8"/>
         <v>0.74239371943988275</v>
       </c>
-      <c r="M8" s="12">
-        <f t="shared" si="4"/>
+      <c r="M11" s="12">
+        <f t="shared" si="9"/>
         <v>0.12383674463173079</v>
       </c>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13">
+      <c r="N11" s="13"/>
+      <c r="O11" s="13">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="P8" s="13">
+      <c r="P11" s="13">
         <v>0.16270000000000001</v>
       </c>
-      <c r="Q8" s="13">
+      <c r="Q11" s="13">
         <v>0.68689999999999996</v>
       </c>
-      <c r="R8" s="13">
+      <c r="R11" s="13">
         <v>0.94330000000000003</v>
       </c>
-      <c r="S8" s="13">
+      <c r="S11" s="13">
         <v>0.99390000000000001</v>
       </c>
-      <c r="T8" s="13">
+      <c r="T11" s="13">
         <v>0.99980000000000002</v>
       </c>
-      <c r="U8" s="14">
-        <v>1</v>
-      </c>
-      <c r="V8" s="14">
-        <v>1</v>
-      </c>
-      <c r="W8" s="14">
-        <v>1</v>
-      </c>
-      <c r="X8" s="14">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="14">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="9" t="s">
+      <c r="U11" s="14">
+        <v>1</v>
+      </c>
+      <c r="V11" s="14">
+        <v>1</v>
+      </c>
+      <c r="W11" s="14">
+        <v>1</v>
+      </c>
+      <c r="X11" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AA8" s="9">
+      <c r="AA11" s="9">
         <v>6</v>
       </c>
-      <c r="AB8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29">
-      <c r="A9" s="27"/>
-      <c r="B9" s="15">
+      <c r="AB11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
+      <c r="A12" s="38"/>
+      <c r="B12" s="15">
         <v>5</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C12" s="15">
         <v>10000</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D12" s="16">
         <v>1712425</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E12" s="16">
         <v>10266936</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F12" s="16">
         <v>16577687</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G12" s="16">
         <v>44565</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H12" s="16">
         <v>149960</v>
       </c>
-      <c r="I9" s="17">
-        <f t="shared" si="0"/>
+      <c r="I12" s="17">
+        <f t="shared" si="5"/>
         <v>1026.6936000000001</v>
       </c>
-      <c r="J9" s="18">
-        <f t="shared" si="3"/>
+      <c r="J12" s="18">
+        <f t="shared" si="6"/>
         <v>171.24250000000001</v>
       </c>
-      <c r="K9" s="17">
-        <f t="shared" si="1"/>
+      <c r="K12" s="17">
+        <f t="shared" si="7"/>
         <v>1657.7687000000001</v>
       </c>
-      <c r="L9" s="18">
-        <f t="shared" si="2"/>
+      <c r="L12" s="18">
+        <f t="shared" si="8"/>
         <v>0.6193225870412441</v>
       </c>
-      <c r="M9" s="18">
-        <f t="shared" si="4"/>
+      <c r="M12" s="18">
+        <f t="shared" si="9"/>
         <v>0.10329697985008403</v>
       </c>
-      <c r="N9" s="15"/>
-      <c r="O9" s="19">
+      <c r="N12" s="15"/>
+      <c r="O12" s="19">
         <v>1.49E-2</v>
       </c>
-      <c r="P9" s="19">
+      <c r="P12" s="19">
         <v>0.46239999999999998</v>
       </c>
-      <c r="Q9" s="19">
+      <c r="Q12" s="19">
         <v>0.90180000000000005</v>
       </c>
-      <c r="R9" s="19">
+      <c r="R12" s="19">
         <v>0.98560000000000003</v>
       </c>
-      <c r="S9" s="19">
+      <c r="S12" s="19">
         <v>0.99750000000000005</v>
       </c>
-      <c r="T9" s="19">
+      <c r="T12" s="19">
         <v>0.99990000000000001</v>
       </c>
-      <c r="U9" s="14">
-        <v>1</v>
-      </c>
-      <c r="V9" s="14">
-        <v>1</v>
-      </c>
-      <c r="W9" s="14">
-        <v>1</v>
-      </c>
-      <c r="X9" s="14">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="14">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="15" t="s">
+      <c r="U12" s="14">
+        <v>1</v>
+      </c>
+      <c r="V12" s="14">
+        <v>1</v>
+      </c>
+      <c r="W12" s="14">
+        <v>1</v>
+      </c>
+      <c r="X12" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AA9" s="15">
+      <c r="AA12" s="15">
         <v>6</v>
       </c>
-      <c r="AB9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29">
-      <c r="A10" s="27"/>
-      <c r="B10" s="9">
+      <c r="AB12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
+      <c r="A13" s="38"/>
+      <c r="B13" s="9">
         <v>6</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C13" s="9">
         <v>5000</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D13" s="10">
         <v>9609433</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E13" s="10">
         <v>19213148</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F13" s="10">
         <v>8870872</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G13" s="10">
         <v>48152</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H13" s="10">
         <v>152180</v>
       </c>
-      <c r="I10" s="11">
-        <f t="shared" si="0"/>
+      <c r="I13" s="11">
+        <f t="shared" si="5"/>
         <v>3842.6296000000002</v>
       </c>
-      <c r="J10" s="12">
-        <f t="shared" ref="J10" si="5">D10/C10</f>
+      <c r="J13" s="12">
+        <f t="shared" ref="J13" si="10">D13/C13</f>
         <v>1921.8866</v>
       </c>
-      <c r="K10" s="11">
-        <f t="shared" si="1"/>
+      <c r="K13" s="11">
+        <f t="shared" si="7"/>
         <v>1774.1744000000001</v>
       </c>
-      <c r="L10" s="12">
-        <f t="shared" si="2"/>
+      <c r="L13" s="12">
+        <f t="shared" si="8"/>
         <v>2.1658691501805007</v>
       </c>
-      <c r="M10" s="12">
-        <f t="shared" ref="M10" si="6">J10/K10</f>
+      <c r="M13" s="12">
+        <f t="shared" ref="M13" si="11">J13/K13</f>
         <v>1.0832568658413739</v>
       </c>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13">
+      <c r="N13" s="13"/>
+      <c r="O13" s="13">
         <v>2.1600000000000001E-2</v>
       </c>
-      <c r="P10" s="13">
+      <c r="P13" s="13">
         <v>0.52800000000000002</v>
       </c>
-      <c r="Q10" s="13">
+      <c r="Q13" s="13">
         <v>0.9274</v>
       </c>
-      <c r="R10" s="13">
+      <c r="R13" s="13">
         <v>0.99260000000000004</v>
       </c>
-      <c r="S10" s="13">
+      <c r="S13" s="13">
         <v>0.999</v>
       </c>
-      <c r="T10" s="14">
-        <v>1</v>
-      </c>
-      <c r="U10" s="14">
-        <v>1</v>
-      </c>
-      <c r="V10" s="14">
-        <v>1</v>
-      </c>
-      <c r="W10" s="14">
-        <v>1</v>
-      </c>
-      <c r="X10" s="14">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="14">
-        <v>1</v>
-      </c>
-      <c r="Z10" s="9" t="s">
+      <c r="T13" s="14">
+        <v>1</v>
+      </c>
+      <c r="U13" s="14">
+        <v>1</v>
+      </c>
+      <c r="V13" s="14">
+        <v>1</v>
+      </c>
+      <c r="W13" s="14">
+        <v>1</v>
+      </c>
+      <c r="X13" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AA10" s="9">
+      <c r="AA13" s="9">
         <v>2</v>
       </c>
-      <c r="AB10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29">
-      <c r="A11" s="27"/>
-      <c r="B11" s="15">
+      <c r="AB13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
+      <c r="A14" s="38"/>
+      <c r="B14" s="15">
         <v>7</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C14" s="15">
         <v>5000</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D14" s="16">
         <v>27113067</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E14" s="16">
         <v>81324354</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F14" s="16">
         <v>10461163</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G14" s="16">
         <v>58185</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H14" s="16">
         <v>165452</v>
       </c>
-      <c r="I11" s="17">
-        <f t="shared" si="0"/>
+      <c r="I14" s="17">
+        <f t="shared" si="5"/>
         <v>16264.870800000001</v>
       </c>
-      <c r="J11" s="18">
-        <f t="shared" ref="J11" si="7">D11/C11</f>
+      <c r="J14" s="18">
+        <f t="shared" ref="J14" si="12">D14/C14</f>
         <v>5422.6134000000002</v>
       </c>
-      <c r="K11" s="17">
-        <f t="shared" si="1"/>
+      <c r="K14" s="17">
+        <f t="shared" si="7"/>
         <v>2092.2325999999998</v>
       </c>
-      <c r="L11" s="18">
-        <f t="shared" si="2"/>
+      <c r="L14" s="18">
+        <f t="shared" si="8"/>
         <v>7.7739304893729324</v>
       </c>
-      <c r="M11" s="18">
-        <f t="shared" ref="M11" si="8">J11/K11</f>
+      <c r="M14" s="18">
+        <f t="shared" ref="M14" si="13">J14/K14</f>
         <v>2.5917832462795967</v>
       </c>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19">
+      <c r="N14" s="19"/>
+      <c r="O14" s="19">
         <v>7.22E-2</v>
       </c>
-      <c r="P11" s="19">
+      <c r="P14" s="19">
         <v>0.67</v>
       </c>
-      <c r="Q11" s="19">
+      <c r="Q14" s="19">
         <v>0.96360000000000001</v>
       </c>
-      <c r="R11" s="19">
+      <c r="R14" s="19">
         <v>0.99580000000000002</v>
       </c>
-      <c r="S11" s="14">
-        <v>1</v>
-      </c>
-      <c r="T11" s="14">
-        <v>1</v>
-      </c>
-      <c r="U11" s="14">
-        <v>1</v>
-      </c>
-      <c r="V11" s="14">
-        <v>1</v>
-      </c>
-      <c r="W11" s="14">
-        <v>1</v>
-      </c>
-      <c r="X11" s="14">
-        <v>1</v>
-      </c>
-      <c r="Y11" s="14">
-        <v>1</v>
-      </c>
-      <c r="Z11" s="15" t="s">
+      <c r="S14" s="14">
+        <v>1</v>
+      </c>
+      <c r="T14" s="14">
+        <v>1</v>
+      </c>
+      <c r="U14" s="14">
+        <v>1</v>
+      </c>
+      <c r="V14" s="14">
+        <v>1</v>
+      </c>
+      <c r="W14" s="14">
+        <v>1</v>
+      </c>
+      <c r="X14" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AA11" s="15">
+      <c r="AA14" s="15">
         <v>3</v>
       </c>
-      <c r="AB11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29">
-      <c r="A12" s="27"/>
-      <c r="B12" s="9">
+      <c r="AB14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
+      <c r="A15" s="38"/>
+      <c r="B15" s="9">
         <v>8</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C15" s="9">
         <v>608</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D15" s="10">
         <v>20813984</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E15" s="10">
         <v>247712732</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F15" s="10">
         <v>1315687</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G15" s="10">
         <v>60275</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H15" s="10">
         <v>150860</v>
       </c>
-      <c r="I12" s="17">
-        <f t="shared" si="0"/>
+      <c r="I15" s="17">
+        <f t="shared" si="5"/>
         <v>407422.25657894736</v>
       </c>
-      <c r="J12" s="18">
-        <f t="shared" ref="J12" si="9">D12/C12</f>
+      <c r="J15" s="18">
+        <f t="shared" ref="J15" si="14">D15/C15</f>
         <v>34233.526315789473</v>
       </c>
-      <c r="K12" s="17">
-        <f t="shared" si="1"/>
+      <c r="K15" s="17">
+        <f t="shared" si="7"/>
         <v>2163.9588815789475</v>
       </c>
-      <c r="L12" s="18">
-        <f t="shared" si="2"/>
+      <c r="L15" s="18">
+        <f t="shared" si="8"/>
         <v>188.27633928130322</v>
       </c>
-      <c r="M12" s="18">
-        <f t="shared" ref="M12" si="10">J12/K12</f>
+      <c r="M15" s="18">
+        <f t="shared" ref="M15" si="15">J15/K15</f>
         <v>15.819859890688285</v>
       </c>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13">
+      <c r="N15" s="13"/>
+      <c r="O15" s="13">
         <v>7.0723999999999995E-2</v>
       </c>
-      <c r="P12" s="13">
+      <c r="P15" s="13">
         <v>0.700658</v>
       </c>
-      <c r="Q12" s="13">
+      <c r="Q15" s="13">
         <v>0.96052599999999999</v>
       </c>
-      <c r="R12" s="13">
+      <c r="R15" s="13">
         <v>0.99835499999999999</v>
       </c>
-      <c r="S12" s="14">
-        <v>1</v>
-      </c>
-      <c r="T12" s="14">
-        <v>1</v>
-      </c>
-      <c r="U12" s="14">
-        <v>1</v>
-      </c>
-      <c r="V12" s="14">
-        <v>1</v>
-      </c>
-      <c r="W12" s="14">
-        <v>1</v>
-      </c>
-      <c r="X12" s="14">
-        <v>1</v>
-      </c>
-      <c r="Y12" s="14">
-        <v>1</v>
-      </c>
-      <c r="Z12" s="9" t="s">
+      <c r="S15" s="14">
+        <v>1</v>
+      </c>
+      <c r="T15" s="14">
+        <v>1</v>
+      </c>
+      <c r="U15" s="14">
+        <v>1</v>
+      </c>
+      <c r="V15" s="14">
+        <v>1</v>
+      </c>
+      <c r="W15" s="14">
+        <v>1</v>
+      </c>
+      <c r="X15" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AA12" s="9">
+      <c r="AA15" s="9">
         <v>12</v>
       </c>
-      <c r="AB12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29">
-      <c r="A13" s="27"/>
-      <c r="B13" s="15">
+      <c r="AB15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="N17" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="36"/>
+      <c r="U17" s="36"/>
+      <c r="V17" s="36"/>
+      <c r="W17" s="36"/>
+      <c r="X17" s="36"/>
+      <c r="Y17" s="36"/>
+    </row>
+    <row r="18" spans="1:28" ht="45">
+      <c r="A18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
-      <c r="S13" s="19"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="19"/>
-      <c r="V13" s="19"/>
-      <c r="W13" s="19"/>
-      <c r="X13" s="19"/>
-      <c r="Y13" s="19"/>
-      <c r="Z13" s="15"/>
-      <c r="AA13" s="15"/>
-      <c r="AB13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" ht="45">
-      <c r="A16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="I18" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="J18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="M18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N16" s="7">
+      <c r="N18" s="7">
         <v>16384</v>
       </c>
-      <c r="O16" s="7">
+      <c r="O18" s="7">
         <v>8192</v>
       </c>
-      <c r="P16" s="7">
+      <c r="P18" s="7">
         <v>4096</v>
       </c>
-      <c r="Q16" s="7">
+      <c r="Q18" s="7">
         <v>2048</v>
       </c>
-      <c r="R16" s="7">
+      <c r="R18" s="7">
         <v>1024</v>
       </c>
-      <c r="S16" s="7">
+      <c r="S18" s="7">
         <v>512</v>
       </c>
-      <c r="T16" s="7">
+      <c r="T18" s="7">
         <v>256</v>
       </c>
-      <c r="U16" s="7">
+      <c r="U18" s="7">
         <v>128</v>
       </c>
-      <c r="V16" s="7">
+      <c r="V18" s="7">
         <v>64</v>
       </c>
-      <c r="W16" s="7">
+      <c r="W18" s="7">
         <v>32</v>
       </c>
-      <c r="X16" s="7">
+      <c r="X18" s="7">
         <v>16</v>
       </c>
-      <c r="Y16" s="7">
+      <c r="Y18" s="7">
         <v>8</v>
       </c>
-      <c r="Z16" s="8" t="s">
+      <c r="Z18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="AA16" s="8" t="s">
+      <c r="AA18" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="AB16" s="8" t="s">
+      <c r="AB18" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:28">
-      <c r="A17" s="27" t="s">
+    <row r="19" spans="1:28">
+      <c r="A19" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="15">
-        <v>1</v>
-      </c>
-      <c r="C17" s="15">
+      <c r="B19" s="15">
+        <v>1</v>
+      </c>
+      <c r="C19" s="15">
         <v>249984</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D19" s="16">
         <v>51212</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E19" s="16">
         <v>1556550</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F19" s="16">
         <v>111284135</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G19" s="16">
         <v>9136</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H19" s="16">
         <v>57652</v>
       </c>
-      <c r="I17" s="17">
-        <f t="shared" ref="I17:I23" si="11">E17/C17</f>
+      <c r="I19" s="17">
+        <f t="shared" ref="I19:I26" si="16">E19/C19</f>
         <v>6.2265985023041477</v>
       </c>
-      <c r="J17" s="18">
-        <f t="shared" ref="J17:J23" si="12">D17/C17</f>
+      <c r="J19" s="18">
+        <f t="shared" ref="J19:J26" si="17">D19/C19</f>
         <v>0.2048611111111111</v>
       </c>
-      <c r="K17" s="17">
-        <f t="shared" ref="K17:K23" si="13">F17/C17</f>
+      <c r="K19" s="17">
+        <f t="shared" ref="K19:K26" si="18">F19/C19</f>
         <v>445.16503056195597</v>
       </c>
-      <c r="L17" s="18">
-        <f t="shared" ref="L17:L23" si="14">I17/K17</f>
+      <c r="L19" s="18">
+        <f t="shared" ref="L19:L26" si="19">I19/K19</f>
         <v>1.3987168970671336E-2</v>
       </c>
-      <c r="M17" s="18">
-        <f t="shared" ref="M17:M23" si="15">J17/K17</f>
+      <c r="M19" s="18">
+        <f t="shared" ref="M19:M26" si="20">J19/K19</f>
         <v>4.6019138307540423E-4</v>
       </c>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="19">
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="19">
         <v>4.64E-4</v>
       </c>
-      <c r="Q17" s="19">
+      <c r="Q19" s="19">
         <v>7.2497000000000006E-2</v>
       </c>
-      <c r="R17" s="19">
+      <c r="R19" s="19">
         <v>0.40044999999999997</v>
       </c>
-      <c r="S17" s="19">
+      <c r="S19" s="19">
         <v>0.76200900000000005</v>
       </c>
-      <c r="T17" s="19">
+      <c r="T19" s="19">
         <v>0.94154000000000004</v>
       </c>
-      <c r="U17" s="19">
+      <c r="U19" s="19">
         <v>0.99202299999999999</v>
       </c>
-      <c r="V17" s="13">
+      <c r="V19" s="13">
         <v>0.99945600000000001</v>
       </c>
-      <c r="W17" s="13">
+      <c r="W19" s="13">
         <v>0.99997199999999997</v>
-      </c>
-      <c r="X17" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="13">
-        <v>1</v>
-      </c>
-      <c r="Z17" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA17" s="15">
-        <v>36</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28">
-      <c r="A18" s="27"/>
-      <c r="B18" s="9">
-        <v>2</v>
-      </c>
-      <c r="C18" s="9">
-        <v>99972</v>
-      </c>
-      <c r="D18" s="10">
-        <v>148219</v>
-      </c>
-      <c r="E18" s="10">
-        <v>4842872</v>
-      </c>
-      <c r="F18" s="10">
-        <v>63652157</v>
-      </c>
-      <c r="G18" s="10">
-        <v>14152</v>
-      </c>
-      <c r="H18" s="10">
-        <v>73056</v>
-      </c>
-      <c r="I18" s="17">
-        <f t="shared" si="11"/>
-        <v>48.442283839475053</v>
-      </c>
-      <c r="J18" s="18">
-        <f t="shared" si="12"/>
-        <v>1.4826051294362421</v>
-      </c>
-      <c r="K18" s="17">
-        <f t="shared" si="13"/>
-        <v>636.69984595686788</v>
-      </c>
-      <c r="L18" s="18">
-        <f t="shared" si="14"/>
-        <v>7.6083391800846598E-2</v>
-      </c>
-      <c r="M18" s="18">
-        <f t="shared" si="15"/>
-        <v>2.3285778045196489E-3</v>
-      </c>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13">
-        <v>6.3619999999999996E-3</v>
-      </c>
-      <c r="Q18" s="13">
-        <v>0.21117900000000001</v>
-      </c>
-      <c r="R18" s="13">
-        <v>0.65922499999999995</v>
-      </c>
-      <c r="S18" s="13">
-        <v>0.91756700000000002</v>
-      </c>
-      <c r="T18" s="13">
-        <v>0.98738599999999999</v>
-      </c>
-      <c r="U18" s="13">
-        <v>0.99868999999999997</v>
-      </c>
-      <c r="V18" s="13">
-        <v>0.99995999999999996</v>
-      </c>
-      <c r="W18" s="13">
-        <v>1</v>
-      </c>
-      <c r="X18" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y18" s="13">
-        <v>1</v>
-      </c>
-      <c r="Z18" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA18" s="15">
-        <v>36</v>
-      </c>
-      <c r="AB18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28">
-      <c r="A19" s="27"/>
-      <c r="B19" s="15">
-        <v>3</v>
-      </c>
-      <c r="C19" s="15">
-        <v>49968</v>
-      </c>
-      <c r="D19" s="16">
-        <v>147254</v>
-      </c>
-      <c r="E19" s="16">
-        <v>5082335</v>
-      </c>
-      <c r="F19" s="16">
-        <v>56231514</v>
-      </c>
-      <c r="G19" s="16">
-        <v>28288</v>
-      </c>
-      <c r="H19" s="16">
-        <v>128680</v>
-      </c>
-      <c r="I19" s="17">
-        <f t="shared" si="11"/>
-        <v>101.71179554915146</v>
-      </c>
-      <c r="J19" s="18">
-        <f t="shared" si="12"/>
-        <v>2.9469660582772974</v>
-      </c>
-      <c r="K19" s="17">
-        <f t="shared" si="13"/>
-        <v>1125.3505043227665</v>
-      </c>
-      <c r="L19" s="18">
-        <f t="shared" si="14"/>
-        <v>9.0382325469664584E-2</v>
-      </c>
-      <c r="M19" s="18">
-        <f t="shared" si="15"/>
-        <v>2.6187095015794883E-3</v>
-      </c>
-      <c r="N19" s="13"/>
-      <c r="O19" s="19">
-        <v>3.2000000000000003E-4</v>
-      </c>
-      <c r="P19" s="19">
-        <v>0.146814</v>
-      </c>
-      <c r="Q19" s="19">
-        <v>0.69306400000000001</v>
-      </c>
-      <c r="R19" s="19">
-        <v>0.94448399999999999</v>
-      </c>
-      <c r="S19" s="19">
-        <v>0.99393600000000004</v>
-      </c>
-      <c r="T19" s="19">
-        <v>0.99963999999999997</v>
-      </c>
-      <c r="U19" s="19">
-        <v>0.99997999999999998</v>
-      </c>
-      <c r="V19" s="13">
-        <v>1</v>
-      </c>
-      <c r="W19" s="13">
-        <v>1</v>
       </c>
       <c r="X19" s="13">
         <v>1</v>
@@ -2947,72 +2968,70 @@
       </c>
     </row>
     <row r="20" spans="1:28">
-      <c r="A20" s="27"/>
+      <c r="A20" s="38"/>
       <c r="B20" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C20" s="9">
-        <v>14976</v>
+        <v>99972</v>
       </c>
       <c r="D20" s="10">
-        <v>990499</v>
+        <v>148219</v>
       </c>
       <c r="E20" s="10">
-        <v>34757265</v>
+        <v>4842872</v>
       </c>
       <c r="F20" s="10">
-        <v>18367864</v>
+        <v>63652157</v>
       </c>
       <c r="G20" s="10">
-        <v>31331</v>
+        <v>14152</v>
       </c>
       <c r="H20" s="10">
-        <v>120120</v>
+        <v>73056</v>
       </c>
       <c r="I20" s="17">
-        <f t="shared" si="11"/>
-        <v>2320.8643830128203</v>
+        <f t="shared" si="16"/>
+        <v>48.442283839475053</v>
       </c>
       <c r="J20" s="18">
-        <f t="shared" si="12"/>
-        <v>66.139089209401703</v>
+        <f t="shared" si="17"/>
+        <v>1.4826051294362421</v>
       </c>
       <c r="K20" s="17">
-        <f t="shared" si="13"/>
-        <v>1226.4866452991453</v>
+        <f t="shared" si="18"/>
+        <v>636.69984595686788</v>
       </c>
       <c r="L20" s="18">
-        <f t="shared" si="14"/>
-        <v>1.8922867133598114</v>
+        <f t="shared" si="19"/>
+        <v>7.6083391800846598E-2</v>
       </c>
       <c r="M20" s="18">
-        <f t="shared" si="15"/>
-        <v>5.3925649710821026E-2</v>
+        <f t="shared" si="20"/>
+        <v>2.3285778045196489E-3</v>
       </c>
       <c r="N20" s="13"/>
-      <c r="O20" s="13">
-        <v>6.6799999999999997E-4</v>
-      </c>
+      <c r="O20" s="13"/>
       <c r="P20" s="13">
-        <v>0.20058799999999999</v>
+        <v>6.3619999999999996E-3</v>
       </c>
       <c r="Q20" s="13">
-        <v>0.75928200000000001</v>
+        <v>0.21117900000000001</v>
       </c>
       <c r="R20" s="13">
-        <v>0.96387599999999996</v>
+        <v>0.65922499999999995</v>
       </c>
       <c r="S20" s="13">
-        <v>0.99712900000000004</v>
+        <v>0.91756700000000002</v>
       </c>
       <c r="T20" s="13">
-        <v>0.99993299999999996</v>
+        <v>0.98738599999999999</v>
       </c>
       <c r="U20" s="13">
-        <v>1</v>
+        <v>0.99868999999999997</v>
       </c>
       <c r="V20" s="13">
-        <v>1</v>
+        <v>0.99995999999999996</v>
       </c>
       <c r="W20" s="13">
         <v>1</v>
@@ -3034,69 +3053,69 @@
       </c>
     </row>
     <row r="21" spans="1:28">
-      <c r="A21" s="27"/>
+      <c r="A21" s="38"/>
       <c r="B21" s="15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C21" s="15">
-        <v>14976</v>
+        <v>49968</v>
       </c>
       <c r="D21" s="16">
-        <v>1667438</v>
+        <v>147254</v>
       </c>
       <c r="E21" s="16">
-        <v>59045390</v>
+        <v>5082335</v>
       </c>
       <c r="F21" s="16">
-        <v>25263890</v>
+        <v>56231514</v>
       </c>
       <c r="G21" s="16">
-        <v>45422</v>
+        <v>28288</v>
       </c>
       <c r="H21" s="16">
-        <v>150108</v>
+        <v>128680</v>
       </c>
       <c r="I21" s="17">
-        <f t="shared" si="11"/>
-        <v>3942.6676014957266</v>
+        <f t="shared" si="16"/>
+        <v>101.71179554915146</v>
       </c>
       <c r="J21" s="18">
-        <f t="shared" si="12"/>
-        <v>111.34067841880342</v>
+        <f t="shared" si="17"/>
+        <v>2.9469660582772974</v>
       </c>
       <c r="K21" s="17">
-        <f t="shared" si="13"/>
-        <v>1686.9584668803418</v>
+        <f t="shared" si="18"/>
+        <v>1125.3505043227665</v>
       </c>
       <c r="L21" s="18">
-        <f t="shared" si="14"/>
-        <v>2.3371456256340575</v>
+        <f t="shared" si="19"/>
+        <v>9.0382325469664584E-2</v>
       </c>
       <c r="M21" s="18">
-        <f t="shared" si="15"/>
-        <v>6.6000841517280195E-2</v>
+        <f t="shared" si="20"/>
+        <v>2.6187095015794883E-3</v>
       </c>
       <c r="N21" s="13"/>
       <c r="O21" s="19">
-        <v>1.5091E-2</v>
+        <v>3.2000000000000003E-4</v>
       </c>
       <c r="P21" s="19">
-        <v>0.466947</v>
+        <v>0.146814</v>
       </c>
       <c r="Q21" s="19">
-        <v>0.92040599999999995</v>
+        <v>0.69306400000000001</v>
       </c>
       <c r="R21" s="19">
-        <v>0.99118600000000001</v>
+        <v>0.94448399999999999</v>
       </c>
       <c r="S21" s="19">
-        <v>0.99939900000000004</v>
+        <v>0.99393600000000004</v>
       </c>
       <c r="T21" s="19">
-        <v>0.99993299999999996</v>
-      </c>
-      <c r="U21" s="13">
-        <v>1</v>
+        <v>0.99963999999999997</v>
+      </c>
+      <c r="U21" s="19">
+        <v>0.99997999999999998</v>
       </c>
       <c r="V21" s="13">
         <v>1</v>
@@ -3121,66 +3140,66 @@
       </c>
     </row>
     <row r="22" spans="1:28">
-      <c r="A22" s="27"/>
+      <c r="A22" s="38"/>
       <c r="B22" s="9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C22" s="9">
-        <v>972</v>
+        <v>14976</v>
       </c>
       <c r="D22" s="10">
-        <v>2210411</v>
+        <v>990499</v>
       </c>
       <c r="E22" s="10">
-        <v>76277073</v>
+        <v>34757265</v>
       </c>
       <c r="F22" s="10">
-        <v>1781573</v>
+        <v>18367864</v>
       </c>
       <c r="G22" s="10">
-        <v>50018</v>
+        <v>31331</v>
       </c>
       <c r="H22" s="10">
-        <v>127492</v>
+        <v>120120</v>
       </c>
       <c r="I22" s="17">
-        <f t="shared" si="11"/>
-        <v>78474.354938271601</v>
+        <f t="shared" si="16"/>
+        <v>2320.8643830128203</v>
       </c>
       <c r="J22" s="18">
-        <f t="shared" si="12"/>
-        <v>2274.0853909465022</v>
+        <f t="shared" si="17"/>
+        <v>66.139089209401703</v>
       </c>
       <c r="K22" s="17">
-        <f t="shared" si="13"/>
-        <v>1832.8940329218108</v>
+        <f t="shared" si="18"/>
+        <v>1226.4866452991453</v>
       </c>
       <c r="L22" s="18">
-        <f t="shared" si="14"/>
-        <v>42.814452733623597</v>
+        <f t="shared" si="19"/>
+        <v>1.8922867133598114</v>
       </c>
       <c r="M22" s="18">
-        <f t="shared" si="15"/>
-        <v>1.2407075095996629</v>
+        <f t="shared" si="20"/>
+        <v>5.3925649710821026E-2</v>
       </c>
       <c r="N22" s="13"/>
       <c r="O22" s="13">
-        <v>2.572E-2</v>
+        <v>6.6799999999999997E-4</v>
       </c>
       <c r="P22" s="13">
-        <v>0.56172800000000001</v>
+        <v>0.20058799999999999</v>
       </c>
       <c r="Q22" s="13">
-        <v>0.94855999999999996</v>
+        <v>0.75928200000000001</v>
       </c>
       <c r="R22" s="13">
-        <v>0.99382700000000002</v>
+        <v>0.96387599999999996</v>
       </c>
       <c r="S22" s="13">
-        <v>1</v>
+        <v>0.99712900000000004</v>
       </c>
       <c r="T22" s="13">
-        <v>1</v>
+        <v>0.99993299999999996</v>
       </c>
       <c r="U22" s="13">
         <v>1</v>
@@ -3208,80 +3227,80 @@
       </c>
     </row>
     <row r="23" spans="1:28">
-      <c r="A23" s="27"/>
+      <c r="A23" s="38"/>
       <c r="B23" s="15">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C23" s="15">
-        <v>972</v>
+        <v>14976</v>
       </c>
       <c r="D23" s="16">
-        <v>3128628</v>
+        <v>1667438</v>
       </c>
       <c r="E23" s="16">
-        <v>107046544</v>
+        <v>59045390</v>
       </c>
       <c r="F23" s="16">
-        <v>2057564</v>
+        <v>25263890</v>
       </c>
       <c r="G23" s="16">
-        <v>59012</v>
+        <v>45422</v>
       </c>
       <c r="H23" s="16">
-        <v>160728</v>
+        <v>150108</v>
       </c>
       <c r="I23" s="17">
-        <f t="shared" si="11"/>
-        <v>110130.18930041153</v>
+        <f t="shared" si="16"/>
+        <v>3942.6676014957266</v>
       </c>
       <c r="J23" s="18">
-        <f t="shared" si="12"/>
-        <v>3218.7530864197529</v>
+        <f t="shared" si="17"/>
+        <v>111.34067841880342</v>
       </c>
       <c r="K23" s="17">
-        <f t="shared" si="13"/>
-        <v>2116.8353909465022</v>
+        <f t="shared" si="18"/>
+        <v>1686.9584668803418</v>
       </c>
       <c r="L23" s="18">
-        <f t="shared" si="14"/>
-        <v>52.025863594036437</v>
+        <f t="shared" si="19"/>
+        <v>2.3371456256340575</v>
       </c>
       <c r="M23" s="18">
-        <f t="shared" si="15"/>
-        <v>1.5205495430518805</v>
+        <f t="shared" si="20"/>
+        <v>6.6000841517280195E-2</v>
       </c>
       <c r="N23" s="13"/>
       <c r="O23" s="19">
-        <v>6.8930000000000005E-2</v>
+        <v>1.5091E-2</v>
       </c>
       <c r="P23" s="19">
-        <v>0.69135800000000003</v>
+        <v>0.466947</v>
       </c>
       <c r="Q23" s="19">
-        <v>0.96707799999999999</v>
+        <v>0.92040599999999995</v>
       </c>
       <c r="R23" s="19">
-        <v>0.99691399999999997</v>
+        <v>0.99118600000000001</v>
       </c>
       <c r="S23" s="19">
-        <v>1</v>
+        <v>0.99939900000000004</v>
       </c>
       <c r="T23" s="19">
-        <v>1</v>
-      </c>
-      <c r="U23" s="19">
-        <v>1</v>
-      </c>
-      <c r="V23" s="19">
-        <v>1</v>
-      </c>
-      <c r="W23" s="19">
-        <v>1</v>
-      </c>
-      <c r="X23" s="19">
-        <v>1</v>
-      </c>
-      <c r="Y23" s="19">
+        <v>0.99993299999999996</v>
+      </c>
+      <c r="U23" s="13">
+        <v>1</v>
+      </c>
+      <c r="V23" s="13">
+        <v>1</v>
+      </c>
+      <c r="W23" s="13">
+        <v>1</v>
+      </c>
+      <c r="X23" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="13">
         <v>1</v>
       </c>
       <c r="Z23" s="15" t="s">
@@ -3295,60 +3314,60 @@
       </c>
     </row>
     <row r="24" spans="1:28">
-      <c r="A24" s="27"/>
+      <c r="A24" s="38"/>
       <c r="B24" s="9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C24" s="9">
-        <v>240</v>
+        <v>972</v>
       </c>
       <c r="D24" s="10">
-        <v>22175726</v>
+        <v>2210411</v>
       </c>
       <c r="E24" s="10">
-        <v>257899674</v>
+        <v>76277073</v>
       </c>
       <c r="F24" s="10">
-        <v>535885</v>
+        <v>1781573</v>
       </c>
       <c r="G24" s="10">
-        <v>62807</v>
+        <v>50018</v>
       </c>
       <c r="H24" s="10">
-        <v>141604</v>
+        <v>127492</v>
       </c>
       <c r="I24" s="17">
-        <f t="shared" ref="I17:I25" si="16">E24/C24</f>
-        <v>1074581.9750000001</v>
+        <f t="shared" si="16"/>
+        <v>78474.354938271601</v>
       </c>
       <c r="J24" s="18">
-        <f t="shared" ref="J17:J25" si="17">D24/C24</f>
-        <v>92398.858333333337</v>
+        <f t="shared" si="17"/>
+        <v>2274.0853909465022</v>
       </c>
       <c r="K24" s="17">
-        <f t="shared" ref="K17:K25" si="18">F24/C24</f>
-        <v>2232.8541666666665</v>
+        <f t="shared" si="18"/>
+        <v>1832.8940329218108</v>
       </c>
       <c r="L24" s="18">
-        <f t="shared" ref="L17:L25" si="19">I24/K24</f>
-        <v>481.25936348283687</v>
+        <f t="shared" si="19"/>
+        <v>42.814452733623597</v>
       </c>
       <c r="M24" s="18">
-        <f t="shared" ref="M17:M25" si="20">J24/K24</f>
-        <v>41.381501628147838</v>
+        <f t="shared" si="20"/>
+        <v>1.2407075095996629</v>
       </c>
       <c r="N24" s="13"/>
       <c r="O24" s="13">
-        <v>9.5833000000000002E-2</v>
+        <v>2.572E-2</v>
       </c>
       <c r="P24" s="13">
-        <v>0.74166699999999997</v>
+        <v>0.56172800000000001</v>
       </c>
       <c r="Q24" s="13">
-        <v>0.99166699999999997</v>
+        <v>0.94855999999999996</v>
       </c>
       <c r="R24" s="13">
-        <v>0.99583299999999997</v>
+        <v>0.99382700000000002</v>
       </c>
       <c r="S24" s="13">
         <v>1</v>
@@ -3372,807 +3391,1751 @@
         <v>1</v>
       </c>
       <c r="Z24" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA24" s="9">
-        <v>12</v>
+        <v>40</v>
+      </c>
+      <c r="AA24" s="15">
+        <v>36</v>
       </c>
       <c r="AB24" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:28">
-      <c r="A25" s="27"/>
+      <c r="A25" s="38"/>
       <c r="B25" s="15">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C25" s="15">
-        <v>96</v>
+        <v>972</v>
       </c>
       <c r="D25" s="16">
-        <v>16519768</v>
+        <v>3128628</v>
       </c>
       <c r="E25" s="16">
-        <v>185926000</v>
+        <v>107046544</v>
       </c>
       <c r="F25" s="16">
-        <v>241615</v>
+        <v>2057564</v>
       </c>
       <c r="G25" s="16">
-        <v>71699</v>
+        <v>59012</v>
       </c>
       <c r="H25" s="16">
-        <v>149712</v>
+        <v>160728</v>
       </c>
       <c r="I25" s="17">
         <f t="shared" si="16"/>
-        <v>1936729.1666666667</v>
+        <v>110130.18930041153</v>
       </c>
       <c r="J25" s="18">
         <f t="shared" si="17"/>
-        <v>172080.91666666666</v>
+        <v>3218.7530864197529</v>
       </c>
       <c r="K25" s="17">
         <f t="shared" si="18"/>
-        <v>2516.8229166666665</v>
+        <v>2116.8353909465022</v>
       </c>
       <c r="L25" s="18">
         <f t="shared" si="19"/>
-        <v>769.51348219274473</v>
+        <v>52.025863594036437</v>
       </c>
       <c r="M25" s="18">
         <f t="shared" si="20"/>
+        <v>1.5205495430518805</v>
+      </c>
+      <c r="N25" s="13"/>
+      <c r="O25" s="19">
+        <v>6.8930000000000005E-2</v>
+      </c>
+      <c r="P25" s="19">
+        <v>0.69135800000000003</v>
+      </c>
+      <c r="Q25" s="19">
+        <v>0.96707799999999999</v>
+      </c>
+      <c r="R25" s="19">
+        <v>0.99691399999999997</v>
+      </c>
+      <c r="S25" s="19">
+        <v>1</v>
+      </c>
+      <c r="T25" s="19">
+        <v>1</v>
+      </c>
+      <c r="U25" s="19">
+        <v>1</v>
+      </c>
+      <c r="V25" s="19">
+        <v>1</v>
+      </c>
+      <c r="W25" s="19">
+        <v>1</v>
+      </c>
+      <c r="X25" s="19">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="19">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA25" s="15">
+        <v>36</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28">
+      <c r="A26" s="38"/>
+      <c r="B26" s="9">
+        <v>8</v>
+      </c>
+      <c r="C26" s="9">
+        <v>216</v>
+      </c>
+      <c r="D26" s="10">
+        <v>13924965</v>
+      </c>
+      <c r="E26" s="10">
+        <v>466802010</v>
+      </c>
+      <c r="F26" s="10">
+        <v>491023</v>
+      </c>
+      <c r="G26" s="10">
+        <v>64108</v>
+      </c>
+      <c r="H26" s="10">
+        <v>126972</v>
+      </c>
+      <c r="I26" s="17">
+        <f t="shared" si="16"/>
+        <v>2161120.4166666665</v>
+      </c>
+      <c r="J26" s="18">
+        <f t="shared" si="17"/>
+        <v>64467.430555555555</v>
+      </c>
+      <c r="K26" s="17">
+        <f t="shared" si="18"/>
+        <v>2273.2546296296296</v>
+      </c>
+      <c r="L26" s="18">
+        <f t="shared" si="19"/>
+        <v>950.67239212827099</v>
+      </c>
+      <c r="M26" s="18">
+        <f t="shared" si="20"/>
+        <v>28.35908908543999</v>
+      </c>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13">
+        <v>9.2592999999999995E-2</v>
+      </c>
+      <c r="P26" s="13">
+        <v>0.796296</v>
+      </c>
+      <c r="Q26" s="13">
+        <v>0.98148100000000005</v>
+      </c>
+      <c r="R26" s="13">
+        <v>1</v>
+      </c>
+      <c r="S26" s="13">
+        <v>1</v>
+      </c>
+      <c r="T26" s="13">
+        <v>1</v>
+      </c>
+      <c r="U26" s="13">
+        <v>1</v>
+      </c>
+      <c r="V26" s="13">
+        <v>1</v>
+      </c>
+      <c r="W26" s="13">
+        <v>1</v>
+      </c>
+      <c r="X26" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA26" s="9">
+        <v>36</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28">
+      <c r="A27" s="38"/>
+      <c r="B27" s="15">
+        <v>9</v>
+      </c>
+      <c r="C27" s="15">
+        <v>96</v>
+      </c>
+      <c r="D27" s="16">
+        <v>16519768</v>
+      </c>
+      <c r="E27" s="16">
+        <v>185926000</v>
+      </c>
+      <c r="F27" s="16">
+        <v>241615</v>
+      </c>
+      <c r="G27" s="16">
+        <v>71699</v>
+      </c>
+      <c r="H27" s="16">
+        <v>149712</v>
+      </c>
+      <c r="I27" s="17">
+        <f t="shared" ref="I26:I27" si="21">E27/C27</f>
+        <v>1936729.1666666667</v>
+      </c>
+      <c r="J27" s="18">
+        <f t="shared" ref="J26:J27" si="22">D27/C27</f>
+        <v>172080.91666666666</v>
+      </c>
+      <c r="K27" s="17">
+        <f t="shared" ref="K26:K27" si="23">F27/C27</f>
+        <v>2516.8229166666665</v>
+      </c>
+      <c r="L27" s="18">
+        <f t="shared" ref="L26:L27" si="24">I27/K27</f>
+        <v>769.51348219274473</v>
+      </c>
+      <c r="M27" s="18">
+        <f t="shared" ref="M26:M27" si="25">J27/K27</f>
         <v>68.372278211203778</v>
       </c>
-      <c r="N25" s="19"/>
-      <c r="O25" s="19">
+      <c r="N27" s="19"/>
+      <c r="O27" s="19">
         <v>0.14583299999999999</v>
       </c>
-      <c r="P25" s="19">
+      <c r="P27" s="19">
         <v>0.84375</v>
       </c>
-      <c r="Q25" s="19">
-        <v>1</v>
-      </c>
-      <c r="R25" s="19">
-        <v>1</v>
-      </c>
-      <c r="S25" s="19">
-        <v>1</v>
-      </c>
-      <c r="T25" s="19">
-        <v>1</v>
-      </c>
-      <c r="U25" s="19">
-        <v>1</v>
-      </c>
-      <c r="V25" s="19">
-        <v>1</v>
-      </c>
-      <c r="W25" s="19">
-        <v>1</v>
-      </c>
-      <c r="X25" s="19">
-        <v>1</v>
-      </c>
-      <c r="Y25" s="19">
-        <v>1</v>
-      </c>
-      <c r="Z25" s="15" t="s">
+      <c r="Q27" s="19">
+        <v>1</v>
+      </c>
+      <c r="R27" s="19">
+        <v>1</v>
+      </c>
+      <c r="S27" s="19">
+        <v>1</v>
+      </c>
+      <c r="T27" s="19">
+        <v>1</v>
+      </c>
+      <c r="U27" s="19">
+        <v>1</v>
+      </c>
+      <c r="V27" s="19">
+        <v>1</v>
+      </c>
+      <c r="W27" s="19">
+        <v>1</v>
+      </c>
+      <c r="X27" s="19">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="19">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AA25" s="15">
+      <c r="AA27" s="15">
         <v>12</v>
       </c>
-      <c r="AB25" t="s">
+      <c r="AB27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:28">
-      <c r="C26" s="26"/>
-    </row>
     <row r="28" spans="1:28">
-      <c r="B28" t="s">
+      <c r="C28" s="26"/>
+    </row>
+    <row r="30" spans="1:28">
+      <c r="B30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="39" customHeight="1">
-      <c r="B30" s="25" t="s">
+    <row r="32" spans="1:28" ht="39" customHeight="1">
+      <c r="B32" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C32" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25" t="s">
+      <c r="D32" s="25"/>
+      <c r="E32" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="25" t="s">
+      <c r="F32" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25" t="s">
+      <c r="G32" s="25"/>
+      <c r="H32" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="I30" s="25" t="s">
+      <c r="I32" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J30" s="25"/>
-      <c r="K30" s="25" t="s">
+      <c r="J32" s="25"/>
+      <c r="K32" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="25" t="s">
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="O30" s="25"/>
-      <c r="Q30" s="1" t="s">
+      <c r="O32" s="25"/>
+      <c r="Q32" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="R30" s="1" t="s">
+      <c r="R32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="S30" s="1" t="s">
+      <c r="S32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="T30" s="1" t="s">
+      <c r="T32" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U30" s="1" t="s">
+      <c r="U32" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="V30" s="1" t="s">
+      <c r="V32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="W30" s="1" t="s">
+      <c r="W32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="X30" s="1" t="s">
+      <c r="X32" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Y30" s="1" t="s">
+      <c r="Y32" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28">
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>32.6</v>
-      </c>
-      <c r="E31">
-        <v>0.1</v>
-      </c>
-      <c r="F31">
-        <v>78.400000000000006</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <v>74</v>
-      </c>
-      <c r="K31">
-        <v>1</v>
-      </c>
-      <c r="L31">
-        <v>50</v>
-      </c>
-      <c r="N31">
-        <v>1</v>
-      </c>
-      <c r="O31">
-        <v>25639</v>
-      </c>
-      <c r="Q31">
-        <v>100000</v>
-      </c>
-      <c r="R31">
-        <f>60000/D17</f>
-        <v>1.1716004061548075</v>
-      </c>
-      <c r="S31" s="30">
-        <f>Q31*R31</f>
-        <v>117160.04061548076</v>
-      </c>
-      <c r="T31">
-        <v>1</v>
-      </c>
-      <c r="U31" s="26">
-        <f>S31*T31</f>
-        <v>117160.04061548076</v>
-      </c>
-      <c r="V31" s="26">
-        <v>250000</v>
-      </c>
-      <c r="W31" s="30">
-        <f>V31/S31</f>
-        <v>2.133833333333333</v>
-      </c>
-      <c r="X31" s="30">
-        <f>D17/60000</f>
-        <v>0.85353333333333337</v>
-      </c>
-      <c r="Y31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28">
-      <c r="B32">
-        <v>2</v>
-      </c>
-      <c r="C32">
-        <v>40.4</v>
-      </c>
-      <c r="E32" s="24">
-        <f>E31+0.1</f>
-        <v>0.2</v>
-      </c>
-      <c r="F32" s="24">
-        <v>79.400000000000006</v>
-      </c>
-      <c r="H32" s="24">
-        <v>1</v>
-      </c>
-      <c r="I32" s="24">
-        <v>78.2</v>
-      </c>
-      <c r="K32">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="L32">
-        <v>76.599999999999994</v>
-      </c>
-      <c r="N32">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="O32">
-        <v>27165</v>
-      </c>
-      <c r="Q32">
-        <v>25000</v>
-      </c>
-      <c r="R32">
-        <f t="shared" ref="R32:R39" si="21">60000/D18</f>
-        <v>0.40480640133855983</v>
-      </c>
-      <c r="S32" s="30">
-        <f t="shared" ref="S32:S39" si="22">Q32*R32</f>
-        <v>10120.160033463995</v>
-      </c>
-      <c r="T32">
-        <v>3</v>
-      </c>
-      <c r="U32" s="26">
-        <f>S32*T32</f>
-        <v>30360.480100391986</v>
-      </c>
-      <c r="V32" s="26">
-        <v>100000</v>
-      </c>
-      <c r="W32" s="30">
-        <f t="shared" ref="W32:W39" si="23">V32/S32</f>
-        <v>9.8812666666666669</v>
-      </c>
-      <c r="X32" s="30">
-        <f t="shared" ref="X32:X39" si="24">D18/60000</f>
-        <v>2.4703166666666667</v>
-      </c>
-      <c r="Y32">
-        <v>2</v>
       </c>
     </row>
     <row r="33" spans="2:25">
       <c r="B33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C33">
-        <v>63.9</v>
+        <v>32.6</v>
       </c>
       <c r="E33">
-        <f t="shared" ref="E33:E40" si="25">E32+0.1</f>
-        <v>0.30000000000000004</v>
+        <v>0.1</v>
       </c>
       <c r="F33">
-        <v>78</v>
+        <v>78.400000000000006</v>
       </c>
       <c r="H33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I33">
-        <v>66.400000000000006</v>
+        <v>74</v>
       </c>
       <c r="K33">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="L33">
-        <v>76.8</v>
+        <v>50</v>
       </c>
       <c r="N33">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="O33">
-        <v>28976</v>
+        <v>25639</v>
       </c>
       <c r="Q33">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="R33">
-        <f t="shared" si="21"/>
-        <v>0.40745922012305269</v>
-      </c>
-      <c r="S33" s="30">
-        <f t="shared" si="22"/>
-        <v>4074.5922012305268</v>
+        <f>60000/D19</f>
+        <v>1.1716004061548075</v>
+      </c>
+      <c r="S33" s="27">
+        <f>Q33*R33</f>
+        <v>117160.04061548076</v>
       </c>
       <c r="T33">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U33" s="26">
         <f>S33*T33</f>
-        <v>20372.961006152633</v>
+        <v>117160.04061548076</v>
       </c>
       <c r="V33" s="26">
-        <v>50000</v>
-      </c>
-      <c r="W33" s="30">
-        <f t="shared" si="23"/>
-        <v>12.271166666666666</v>
-      </c>
-      <c r="X33" s="30">
-        <f t="shared" si="24"/>
-        <v>2.4542333333333333</v>
+        <v>250000</v>
+      </c>
+      <c r="W33" s="27">
+        <f>V33/S33</f>
+        <v>2.133833333333333</v>
+      </c>
+      <c r="X33" s="27">
+        <f>D19/60000</f>
+        <v>0.85353333333333337</v>
       </c>
       <c r="Y33">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:25">
       <c r="B34">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C34">
-        <v>71.099999999999994</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="25"/>
-        <v>0.4</v>
-      </c>
-      <c r="F34">
-        <v>77</v>
-      </c>
-      <c r="H34">
+        <v>40.4</v>
+      </c>
+      <c r="E34" s="24">
+        <f>E33+0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="F34" s="24">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="H34" s="24">
+        <v>1</v>
+      </c>
+      <c r="I34" s="24">
+        <v>78.2</v>
+      </c>
+      <c r="K34">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L34">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="N34">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O34">
+        <v>27165</v>
+      </c>
+      <c r="Q34">
+        <v>25000</v>
+      </c>
+      <c r="R34">
+        <f t="shared" ref="R34:R41" si="26">60000/D20</f>
+        <v>0.40480640133855983</v>
+      </c>
+      <c r="S34" s="27">
+        <f t="shared" ref="S34:S41" si="27">Q34*R34</f>
+        <v>10120.160033463995</v>
+      </c>
+      <c r="T34">
         <v>3</v>
-      </c>
-      <c r="I34">
-        <v>70.8</v>
-      </c>
-      <c r="K34">
-        <v>1.3</v>
-      </c>
-      <c r="L34">
-        <v>75.8</v>
-      </c>
-      <c r="N34">
-        <v>1.3</v>
-      </c>
-      <c r="O34">
-        <v>27826</v>
-      </c>
-      <c r="Q34">
-        <v>5000</v>
-      </c>
-      <c r="R34">
-        <f t="shared" si="21"/>
-        <v>6.0575528092405947E-2</v>
-      </c>
-      <c r="S34" s="30">
-        <f t="shared" si="22"/>
-        <v>302.87764046202972</v>
-      </c>
-      <c r="T34">
-        <v>25</v>
       </c>
       <c r="U34" s="26">
         <f>S34*T34</f>
-        <v>7571.9410115507426</v>
+        <v>30360.480100391986</v>
       </c>
       <c r="V34" s="26">
-        <v>15000</v>
-      </c>
-      <c r="W34" s="30">
-        <f t="shared" si="23"/>
-        <v>49.524950000000004</v>
-      </c>
-      <c r="X34" s="30">
-        <f t="shared" si="24"/>
-        <v>16.508316666666666</v>
+        <v>100000</v>
+      </c>
+      <c r="W34" s="27">
+        <f t="shared" ref="W34:W41" si="28">V34/S34</f>
+        <v>9.8812666666666669</v>
+      </c>
+      <c r="X34" s="27">
+        <f t="shared" ref="X34:X41" si="29">D20/60000</f>
+        <v>2.4703166666666667</v>
       </c>
       <c r="Y34">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="2:25">
       <c r="B35">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C35">
-        <v>70.900000000000006</v>
+        <v>63.9</v>
       </c>
       <c r="E35">
-        <f t="shared" si="25"/>
-        <v>0.5</v>
+        <f t="shared" ref="E35:E42" si="30">E34+0.1</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="F35">
         <v>78</v>
       </c>
       <c r="H35">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I35">
-        <v>68.8</v>
+        <v>66.400000000000006</v>
       </c>
       <c r="K35">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="L35">
-        <v>72.599999999999994</v>
+        <v>76.8</v>
       </c>
       <c r="N35">
-        <v>1.4</v>
+        <v>1.2</v>
+      </c>
+      <c r="O35">
+        <v>28976</v>
       </c>
       <c r="Q35">
-        <v>2500</v>
+        <v>10000</v>
       </c>
       <c r="R35">
-        <f t="shared" si="21"/>
-        <v>3.5983346907051419E-2</v>
-      </c>
-      <c r="S35" s="30">
-        <f t="shared" si="22"/>
-        <v>89.958367267628546</v>
+        <f t="shared" si="26"/>
+        <v>0.40745922012305269</v>
+      </c>
+      <c r="S35" s="27">
+        <f t="shared" si="27"/>
+        <v>4074.5922012305268</v>
       </c>
       <c r="T35">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="U35" s="26">
-        <f t="shared" ref="U35:U39" si="26">S35*T35</f>
-        <v>5397.5020360577128</v>
+        <f>S35*T35</f>
+        <v>20372.961006152633</v>
       </c>
       <c r="V35" s="26">
-        <v>15000</v>
-      </c>
-      <c r="W35" s="30">
-        <f t="shared" si="23"/>
-        <v>166.74379999999999</v>
-      </c>
-      <c r="X35" s="30">
-        <f t="shared" si="24"/>
-        <v>27.790633333333332</v>
+        <v>50000</v>
+      </c>
+      <c r="W35" s="27">
+        <f t="shared" si="28"/>
+        <v>12.271166666666666</v>
+      </c>
+      <c r="X35" s="27">
+        <f t="shared" si="29"/>
+        <v>2.4542333333333333</v>
       </c>
       <c r="Y35">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="2:25">
       <c r="B36">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C36">
-        <v>75.2</v>
+        <v>71.099999999999994</v>
       </c>
       <c r="E36">
-        <f t="shared" si="25"/>
-        <v>0.6</v>
+        <f t="shared" si="30"/>
+        <v>0.4</v>
       </c>
       <c r="F36">
-        <v>77.599999999999994</v>
+        <v>77</v>
       </c>
       <c r="H36">
+        <v>3</v>
+      </c>
+      <c r="I36">
+        <v>70.8</v>
+      </c>
+      <c r="K36">
+        <v>1.3</v>
+      </c>
+      <c r="L36">
+        <v>75.8</v>
+      </c>
+      <c r="N36">
+        <v>1.3</v>
+      </c>
+      <c r="O36">
+        <v>27826</v>
+      </c>
+      <c r="Q36">
+        <v>5000</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="26"/>
+        <v>6.0575528092405947E-2</v>
+      </c>
+      <c r="S36" s="27">
+        <f t="shared" si="27"/>
+        <v>302.87764046202972</v>
+      </c>
+      <c r="T36">
+        <v>25</v>
+      </c>
+      <c r="U36" s="26">
+        <f>S36*T36</f>
+        <v>7571.9410115507426</v>
+      </c>
+      <c r="V36" s="26">
+        <v>15000</v>
+      </c>
+      <c r="W36" s="27">
+        <f t="shared" si="28"/>
+        <v>49.524950000000004</v>
+      </c>
+      <c r="X36" s="27">
+        <f t="shared" si="29"/>
+        <v>16.508316666666666</v>
+      </c>
+      <c r="Y36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:25">
+      <c r="B37">
         <v>5</v>
       </c>
-      <c r="I36">
-        <v>66.599999999999994</v>
-      </c>
-      <c r="K36">
-        <v>1.5</v>
-      </c>
-      <c r="L36">
-        <v>74.8</v>
-      </c>
-      <c r="N36">
-        <v>1.5</v>
-      </c>
-      <c r="Q36">
-        <v>1000</v>
-      </c>
-      <c r="R36">
-        <f t="shared" si="21"/>
-        <v>2.7144273169107464E-2</v>
-      </c>
-      <c r="S36" s="30">
-        <f t="shared" si="22"/>
-        <v>27.144273169107464</v>
-      </c>
-      <c r="T36">
+      <c r="C37">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="30"/>
+        <v>0.5</v>
+      </c>
+      <c r="F37">
+        <v>78</v>
+      </c>
+      <c r="H37">
+        <v>4</v>
+      </c>
+      <c r="I37">
+        <v>68.8</v>
+      </c>
+      <c r="K37">
+        <v>1.4</v>
+      </c>
+      <c r="L37">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="N37">
+        <v>1.4</v>
+      </c>
+      <c r="Q37">
+        <v>2500</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="26"/>
+        <v>3.5983346907051419E-2</v>
+      </c>
+      <c r="S37" s="27">
+        <f t="shared" si="27"/>
+        <v>89.958367267628546</v>
+      </c>
+      <c r="T37">
         <v>60</v>
       </c>
-      <c r="U36" s="26">
-        <f t="shared" si="26"/>
-        <v>1628.6563901464478</v>
-      </c>
-      <c r="V36" s="26">
-        <v>1000</v>
-      </c>
-      <c r="W36" s="30">
-        <f t="shared" si="23"/>
-        <v>36.840183333333336</v>
-      </c>
-      <c r="X36" s="30">
-        <f t="shared" si="24"/>
-        <v>36.840183333333336</v>
-      </c>
-      <c r="Y36">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="2:25">
-      <c r="B37" s="24">
-        <v>7</v>
-      </c>
-      <c r="C37" s="24">
-        <v>76.7</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="25"/>
-        <v>0.7</v>
-      </c>
-      <c r="F37">
-        <v>76.8</v>
-      </c>
-      <c r="K37">
-        <v>1.6</v>
-      </c>
-      <c r="L37">
-        <v>73.599999999999994</v>
-      </c>
-      <c r="N37">
-        <v>1.6</v>
-      </c>
-      <c r="Q37">
-        <v>500</v>
-      </c>
-      <c r="R37">
-        <f t="shared" si="21"/>
-        <v>1.9177735416291104E-2</v>
-      </c>
-      <c r="S37" s="30">
-        <f t="shared" si="22"/>
-        <v>9.5888677081455516</v>
-      </c>
-      <c r="T37">
-        <v>120</v>
-      </c>
       <c r="U37" s="26">
-        <f t="shared" si="26"/>
-        <v>1150.6641249774661</v>
+        <f t="shared" ref="U37:U41" si="31">S37*T37</f>
+        <v>5397.5020360577128</v>
       </c>
       <c r="V37" s="26">
-        <v>1000</v>
-      </c>
-      <c r="W37" s="30">
-        <f t="shared" si="23"/>
-        <v>104.2876</v>
-      </c>
-      <c r="X37" s="30">
-        <f t="shared" si="24"/>
-        <v>52.143799999999999</v>
+        <v>5000</v>
+      </c>
+      <c r="W37" s="27">
+        <f t="shared" si="28"/>
+        <v>55.581266666666664</v>
+      </c>
+      <c r="X37" s="27">
+        <f t="shared" si="29"/>
+        <v>27.790633333333332</v>
       </c>
       <c r="Y37">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="2:25">
       <c r="B38">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C38">
+        <v>75.2</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="30"/>
+        <v>0.6</v>
+      </c>
+      <c r="F38">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="H38">
+        <v>5</v>
+      </c>
+      <c r="I38">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="K38">
+        <v>1.5</v>
+      </c>
+      <c r="L38">
+        <v>74.8</v>
+      </c>
+      <c r="N38">
+        <v>1.5</v>
+      </c>
+      <c r="Q38">
+        <v>1000</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="26"/>
+        <v>2.7144273169107464E-2</v>
+      </c>
+      <c r="S38" s="27">
+        <f t="shared" si="27"/>
+        <v>27.144273169107464</v>
+      </c>
+      <c r="T38">
+        <v>60</v>
+      </c>
+      <c r="U38" s="26">
+        <f t="shared" si="31"/>
+        <v>1628.6563901464478</v>
+      </c>
+      <c r="V38" s="26">
+        <v>1000</v>
+      </c>
+      <c r="W38" s="27">
+        <f t="shared" si="28"/>
+        <v>36.840183333333336</v>
+      </c>
+      <c r="X38" s="27">
+        <f t="shared" si="29"/>
+        <v>36.840183333333336</v>
+      </c>
+      <c r="Y38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="2:25">
+      <c r="B39" s="24">
+        <v>7</v>
+      </c>
+      <c r="C39" s="24">
         <v>76.7</v>
       </c>
-      <c r="E38">
-        <f t="shared" si="25"/>
-        <v>0.79999999999999993</v>
-      </c>
-      <c r="F38">
+      <c r="E39">
+        <f t="shared" si="30"/>
+        <v>0.7</v>
+      </c>
+      <c r="F39">
+        <v>76.8</v>
+      </c>
+      <c r="K39">
+        <v>1.6</v>
+      </c>
+      <c r="L39">
         <v>73.599999999999994</v>
       </c>
-      <c r="K38">
-        <v>1.7</v>
-      </c>
-      <c r="N38">
-        <v>1.7</v>
-      </c>
-      <c r="Q38">
-        <v>250</v>
-      </c>
-      <c r="R38">
-        <f t="shared" si="21"/>
-        <v>2.7056611359646127E-3</v>
-      </c>
-      <c r="S38" s="30">
-        <f t="shared" si="22"/>
-        <v>0.67641528399115314</v>
-      </c>
-      <c r="T38">
-        <v>360</v>
-      </c>
-      <c r="U38" s="26">
+      <c r="N39">
+        <v>1.6</v>
+      </c>
+      <c r="Q39">
+        <v>500</v>
+      </c>
+      <c r="R39">
         <f t="shared" si="26"/>
-        <v>243.50950223681514</v>
-      </c>
-      <c r="V38" s="26">
-        <v>250</v>
-      </c>
-      <c r="W38" s="30">
-        <f t="shared" si="23"/>
-        <v>369.59543333333335</v>
-      </c>
-      <c r="X38" s="30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="2:25">
-      <c r="B39">
-        <v>9</v>
-      </c>
-      <c r="C39">
-        <v>74.3</v>
-      </c>
-      <c r="E39">
-        <f t="shared" si="25"/>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="F39">
-        <v>74.8</v>
-      </c>
-      <c r="K39">
-        <v>1.8</v>
-      </c>
-      <c r="N39">
-        <v>1.8</v>
-      </c>
-      <c r="Q39">
-        <v>100</v>
-      </c>
-      <c r="R39">
-        <f t="shared" si="21"/>
-        <v>3.6320122655475549E-3</v>
-      </c>
-      <c r="S39" s="30">
-        <f t="shared" si="22"/>
-        <v>0.36320122655475551</v>
+        <v>1.9177735416291104E-2</v>
+      </c>
+      <c r="S39" s="27">
+        <f t="shared" si="27"/>
+        <v>9.5888677081455516</v>
       </c>
       <c r="T39">
-        <v>720</v>
+        <v>120</v>
       </c>
       <c r="U39" s="26">
-        <f t="shared" si="26"/>
-        <v>261.50488311942399</v>
+        <f t="shared" si="31"/>
+        <v>1150.6641249774661</v>
       </c>
       <c r="V39" s="26">
-        <v>250</v>
-      </c>
-      <c r="W39" s="30">
-        <f t="shared" si="23"/>
-        <v>688.32366666666667</v>
-      </c>
-      <c r="X39" s="30"/>
+        <v>1000</v>
+      </c>
+      <c r="W39" s="27">
+        <f t="shared" si="28"/>
+        <v>104.2876</v>
+      </c>
+      <c r="X39" s="27">
+        <f t="shared" si="29"/>
+        <v>52.143799999999999</v>
+      </c>
+      <c r="Y39">
+        <v>7</v>
+      </c>
     </row>
     <row r="40" spans="2:25">
       <c r="B40">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>76.7</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="30"/>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="F40">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="K40">
+        <v>1.7</v>
+      </c>
+      <c r="N40">
+        <v>1.7</v>
+      </c>
+      <c r="Q40">
+        <v>250</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="26"/>
+        <v>4.3088079575065363E-3</v>
+      </c>
+      <c r="S40" s="27">
+        <f t="shared" si="27"/>
+        <v>1.077201989376634</v>
+      </c>
+      <c r="T40">
+        <v>360</v>
+      </c>
+      <c r="U40" s="26">
+        <f t="shared" si="31"/>
+        <v>387.79271617558823</v>
+      </c>
+      <c r="V40" s="26">
+        <v>250</v>
+      </c>
+      <c r="W40" s="27">
+        <f t="shared" si="28"/>
+        <v>232.08274999999998</v>
+      </c>
+      <c r="X40" s="27">
+        <f t="shared" si="29"/>
+        <v>232.08275</v>
+      </c>
+    </row>
+    <row r="41" spans="2:25">
+      <c r="B41">
+        <v>9</v>
+      </c>
+      <c r="C41">
+        <v>74.3</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="30"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="F41">
+        <v>74.8</v>
+      </c>
+      <c r="K41">
+        <v>1.8</v>
+      </c>
+      <c r="N41">
+        <v>1.8</v>
+      </c>
+      <c r="Q41">
+        <v>100</v>
+      </c>
+      <c r="R41">
+        <f t="shared" si="26"/>
+        <v>3.6320122655475549E-3</v>
+      </c>
+      <c r="S41" s="27">
+        <f t="shared" si="27"/>
+        <v>0.36320122655475551</v>
+      </c>
+      <c r="T41">
+        <v>720</v>
+      </c>
+      <c r="U41" s="26">
+        <f t="shared" si="31"/>
+        <v>261.50488311942399</v>
+      </c>
+      <c r="V41" s="26">
+        <v>250</v>
+      </c>
+      <c r="W41" s="27">
+        <f t="shared" si="28"/>
+        <v>688.32366666666667</v>
+      </c>
+      <c r="X41" s="27">
+        <f t="shared" si="29"/>
+        <v>275.32946666666669</v>
+      </c>
+    </row>
+    <row r="42" spans="2:25">
+      <c r="B42">
         <v>10</v>
       </c>
-      <c r="C40">
+      <c r="C42">
         <v>76.2</v>
       </c>
-      <c r="E40">
-        <f t="shared" si="25"/>
+      <c r="E42">
+        <f t="shared" si="30"/>
         <v>0.99999999999999989</v>
       </c>
-      <c r="F40">
+      <c r="F42">
         <v>59.4</v>
       </c>
-      <c r="K40">
+      <c r="K42">
         <v>1.9</v>
       </c>
-      <c r="N40">
+      <c r="N42">
         <v>1.9</v>
       </c>
     </row>
-    <row r="41" spans="2:25">
-      <c r="E41">
+    <row r="43" spans="2:25">
+      <c r="E43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F41">
+      <c r="F43">
         <v>0.2</v>
       </c>
-      <c r="K41">
+      <c r="K43">
         <v>2</v>
       </c>
-      <c r="N41">
+      <c r="N43">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="2:25">
-      <c r="T44">
-        <f>SUM(T31:T39)/60</f>
+    <row r="46" spans="2:25">
+      <c r="T46">
+        <f>SUM(T33:T41)/60</f>
         <v>22.566666666666666</v>
       </c>
-      <c r="V44" t="s">
+      <c r="V46" t="s">
         <v>39</v>
       </c>
-      <c r="W44">
-        <f>SUM(W31:W39)/60</f>
-        <v>23.993365000000001</v>
+      <c r="W46">
+        <f>SUM(W33:W41)/60</f>
+        <v>19.848778055555556</v>
+      </c>
+      <c r="X46" s="27">
+        <f>SUM(X33:X39)</f>
+        <v>139.06101666666666</v>
+      </c>
+    </row>
+    <row r="48" spans="2:25">
+      <c r="G48">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>2496</v>
+      </c>
+      <c r="C49">
+        <v>1560</v>
+      </c>
+      <c r="D49">
+        <v>16461</v>
+      </c>
+      <c r="E49">
+        <v>1544761</v>
+      </c>
+      <c r="F49">
+        <v>13771</v>
+      </c>
+      <c r="G49">
+        <v>58068</v>
+      </c>
+      <c r="O49" s="34">
+        <v>6.0099999999999997E-3</v>
+      </c>
+      <c r="P49" s="34">
+        <v>0.213141</v>
+      </c>
+      <c r="Q49" s="34">
+        <v>0.66987200000000002</v>
+      </c>
+      <c r="R49" s="34">
+        <v>0.91947100000000004</v>
+      </c>
+      <c r="S49" s="34">
+        <v>0.98116999999999999</v>
+      </c>
+      <c r="T49" s="34">
+        <v>0.996394</v>
+      </c>
+      <c r="U49" s="34">
+        <v>0.99959900000000002</v>
+      </c>
+      <c r="V49" s="35">
+        <v>1</v>
+      </c>
+      <c r="W49" s="35">
+        <v>1</v>
+      </c>
+      <c r="X49" s="35">
+        <v>1</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z49">
+        <v>12</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50">
+        <v>996</v>
+      </c>
+      <c r="C50">
+        <v>2037</v>
+      </c>
+      <c r="D50">
+        <v>23437</v>
+      </c>
+      <c r="E50">
+        <v>748306</v>
+      </c>
+      <c r="F50">
+        <v>17352</v>
+      </c>
+      <c r="G50">
+        <v>68220</v>
+      </c>
+      <c r="O50" s="34">
+        <v>1.506E-2</v>
+      </c>
+      <c r="P50" s="34">
+        <v>0.34638600000000003</v>
+      </c>
+      <c r="Q50" s="34">
+        <v>0.77710800000000002</v>
+      </c>
+      <c r="R50" s="34">
+        <v>0.96586300000000003</v>
+      </c>
+      <c r="S50" s="34">
+        <v>0.99598399999999998</v>
+      </c>
+      <c r="T50" s="34">
+        <v>1</v>
+      </c>
+      <c r="U50" s="35">
+        <v>1</v>
+      </c>
+      <c r="V50" s="35">
+        <v>1</v>
+      </c>
+      <c r="W50" s="35">
+        <v>1</v>
+      </c>
+      <c r="X50" s="35">
+        <v>1</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z50">
+        <v>12</v>
+      </c>
+      <c r="AA50" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51">
+        <v>492</v>
+      </c>
+      <c r="C51">
+        <v>3740</v>
+      </c>
+      <c r="D51">
+        <v>42771</v>
+      </c>
+      <c r="E51">
+        <v>604808</v>
+      </c>
+      <c r="F51">
+        <v>31494</v>
+      </c>
+      <c r="G51">
+        <v>95616</v>
+      </c>
+      <c r="N51" s="34">
+        <v>2.0330000000000001E-3</v>
+      </c>
+      <c r="O51" s="34">
+        <v>0.21138199999999999</v>
+      </c>
+      <c r="P51" s="34">
+        <v>0.75</v>
+      </c>
+      <c r="Q51" s="34">
+        <v>0.95121999999999995</v>
+      </c>
+      <c r="R51" s="34">
+        <v>0.99187000000000003</v>
+      </c>
+      <c r="S51" s="35">
+        <v>1</v>
+      </c>
+      <c r="T51" s="35">
+        <v>1</v>
+      </c>
+      <c r="U51" s="35">
+        <v>1</v>
+      </c>
+      <c r="V51" s="35">
+        <v>1</v>
+      </c>
+      <c r="W51" s="35">
+        <v>1</v>
+      </c>
+      <c r="X51" s="35">
+        <v>1</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z51">
+        <v>12</v>
+      </c>
+      <c r="AA51" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27">
+      <c r="A52">
+        <v>4</v>
+      </c>
+      <c r="B52">
+        <v>144</v>
+      </c>
+      <c r="C52">
+        <v>14360</v>
+      </c>
+      <c r="D52">
+        <v>165255</v>
+      </c>
+      <c r="E52">
+        <v>191797</v>
+      </c>
+      <c r="F52">
+        <v>34747</v>
+      </c>
+      <c r="G52">
+        <v>99580</v>
+      </c>
+      <c r="N52" s="34">
+        <v>6.9439999999999997E-3</v>
+      </c>
+      <c r="O52" s="34">
+        <v>0.29166700000000001</v>
+      </c>
+      <c r="P52" s="34">
+        <v>0.81944399999999995</v>
+      </c>
+      <c r="Q52" s="34">
+        <v>0.97222200000000003</v>
+      </c>
+      <c r="R52" s="34">
+        <v>1</v>
+      </c>
+      <c r="S52" s="35">
+        <v>1</v>
+      </c>
+      <c r="T52" s="35">
+        <v>1</v>
+      </c>
+      <c r="U52" s="35">
+        <v>1</v>
+      </c>
+      <c r="V52" s="35">
+        <v>1</v>
+      </c>
+      <c r="W52" s="35">
+        <v>1</v>
+      </c>
+      <c r="X52" s="35">
+        <v>1</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z52">
+        <v>12</v>
+      </c>
+      <c r="AA52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27">
+      <c r="A53">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>48</v>
+      </c>
+      <c r="C53">
+        <v>12409</v>
+      </c>
+      <c r="D53">
+        <v>123020</v>
+      </c>
+      <c r="E53">
+        <v>89344</v>
+      </c>
+      <c r="F53">
+        <v>51621</v>
+      </c>
+      <c r="G53">
+        <v>120188</v>
+      </c>
+      <c r="N53" s="34">
+        <v>8.3333000000000004E-2</v>
+      </c>
+      <c r="O53" s="34">
+        <v>0.54166700000000001</v>
+      </c>
+      <c r="P53" s="34">
+        <v>1</v>
+      </c>
+      <c r="Q53" s="35">
+        <v>1</v>
+      </c>
+      <c r="R53" s="35">
+        <v>1</v>
+      </c>
+      <c r="S53" s="35">
+        <v>1</v>
+      </c>
+      <c r="T53" s="35">
+        <v>1</v>
+      </c>
+      <c r="U53" s="35">
+        <v>1</v>
+      </c>
+      <c r="V53" s="35">
+        <v>1</v>
+      </c>
+      <c r="W53" s="35">
+        <v>1</v>
+      </c>
+      <c r="X53" s="35">
+        <v>1</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z53">
+        <v>12</v>
+      </c>
+      <c r="AA53" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27">
+      <c r="A54">
+        <v>6</v>
+      </c>
+      <c r="B54">
+        <v>12</v>
+      </c>
+      <c r="C54">
+        <v>31152</v>
+      </c>
+      <c r="D54">
+        <v>321625</v>
+      </c>
+      <c r="E54">
+        <v>19695</v>
+      </c>
+      <c r="F54">
+        <v>44731</v>
+      </c>
+      <c r="G54">
+        <v>73020</v>
+      </c>
+      <c r="N54" s="34"/>
+      <c r="O54" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="P54" s="34">
+        <v>0.91666700000000001</v>
+      </c>
+      <c r="Q54" s="35">
+        <v>1</v>
+      </c>
+      <c r="R54" s="35">
+        <v>1</v>
+      </c>
+      <c r="S54" s="35">
+        <v>1</v>
+      </c>
+      <c r="T54" s="35">
+        <v>1</v>
+      </c>
+      <c r="U54" s="35">
+        <v>1</v>
+      </c>
+      <c r="V54" s="35">
+        <v>1</v>
+      </c>
+      <c r="W54" s="35">
+        <v>1</v>
+      </c>
+      <c r="X54" s="35">
+        <v>1</v>
+      </c>
+      <c r="Y54" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z54">
+        <v>12</v>
+      </c>
+      <c r="AA54" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>2496</v>
+      </c>
+      <c r="C57">
+        <v>1560</v>
+      </c>
+      <c r="D57">
+        <v>16461</v>
+      </c>
+      <c r="E57">
+        <v>1544761</v>
+      </c>
+      <c r="F57">
+        <v>13771</v>
+      </c>
+      <c r="G57">
+        <v>58068</v>
+      </c>
+      <c r="O57" s="34">
+        <v>6.0099999999999997E-3</v>
+      </c>
+      <c r="P57" s="34">
+        <v>0.213141</v>
+      </c>
+      <c r="Q57" s="34">
+        <v>0.66987200000000002</v>
+      </c>
+      <c r="R57" s="34">
+        <v>0.91947100000000004</v>
+      </c>
+      <c r="S57" s="34">
+        <v>0.98116999999999999</v>
+      </c>
+      <c r="T57" s="34">
+        <v>0.996394</v>
+      </c>
+      <c r="U57" s="34">
+        <v>0.99959900000000002</v>
+      </c>
+      <c r="V57" s="35">
+        <v>1</v>
+      </c>
+      <c r="W57" s="35">
+        <v>1</v>
+      </c>
+      <c r="X57" s="35">
+        <v>1</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z57">
+        <v>12</v>
+      </c>
+      <c r="AA57" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27">
+      <c r="A58">
+        <v>2</v>
+      </c>
+      <c r="B58">
+        <v>996</v>
+      </c>
+      <c r="C58">
+        <v>2037</v>
+      </c>
+      <c r="D58">
+        <v>23437</v>
+      </c>
+      <c r="E58">
+        <v>748306</v>
+      </c>
+      <c r="F58">
+        <v>17352</v>
+      </c>
+      <c r="G58">
+        <v>68220</v>
+      </c>
+      <c r="O58" s="34">
+        <v>1.506E-2</v>
+      </c>
+      <c r="P58" s="34">
+        <v>0.34638600000000003</v>
+      </c>
+      <c r="Q58" s="34">
+        <v>0.77710800000000002</v>
+      </c>
+      <c r="R58" s="34">
+        <v>0.96586300000000003</v>
+      </c>
+      <c r="S58" s="34">
+        <v>0.99598399999999998</v>
+      </c>
+      <c r="T58" s="34">
+        <v>1</v>
+      </c>
+      <c r="U58" s="35">
+        <v>1</v>
+      </c>
+      <c r="V58" s="35">
+        <v>1</v>
+      </c>
+      <c r="W58" s="35">
+        <v>1</v>
+      </c>
+      <c r="X58" s="35">
+        <v>1</v>
+      </c>
+      <c r="Y58" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z58">
+        <v>12</v>
+      </c>
+      <c r="AA58" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="B59">
+        <v>492</v>
+      </c>
+      <c r="C59">
+        <v>3740</v>
+      </c>
+      <c r="D59">
+        <v>42771</v>
+      </c>
+      <c r="E59">
+        <v>604808</v>
+      </c>
+      <c r="F59">
+        <v>31494</v>
+      </c>
+      <c r="G59">
+        <v>95616</v>
+      </c>
+      <c r="N59" s="34">
+        <v>2.0330000000000001E-3</v>
+      </c>
+      <c r="O59" s="34">
+        <v>0.21138199999999999</v>
+      </c>
+      <c r="P59" s="34">
+        <v>0.75</v>
+      </c>
+      <c r="Q59" s="34">
+        <v>0.95121999999999995</v>
+      </c>
+      <c r="R59" s="34">
+        <v>0.99187000000000003</v>
+      </c>
+      <c r="S59" s="35">
+        <v>1</v>
+      </c>
+      <c r="T59" s="35">
+        <v>1</v>
+      </c>
+      <c r="U59" s="35">
+        <v>1</v>
+      </c>
+      <c r="V59" s="35">
+        <v>1</v>
+      </c>
+      <c r="W59" s="35">
+        <v>1</v>
+      </c>
+      <c r="X59" s="35">
+        <v>1</v>
+      </c>
+      <c r="Y59" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z59">
+        <v>12</v>
+      </c>
+      <c r="AA59" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27">
+      <c r="A60">
+        <v>4</v>
+      </c>
+      <c r="B60">
+        <v>144</v>
+      </c>
+      <c r="C60">
+        <v>14360</v>
+      </c>
+      <c r="D60">
+        <v>165255</v>
+      </c>
+      <c r="E60">
+        <v>191797</v>
+      </c>
+      <c r="F60">
+        <v>34747</v>
+      </c>
+      <c r="G60">
+        <v>99580</v>
+      </c>
+      <c r="N60" s="34">
+        <v>6.9439999999999997E-3</v>
+      </c>
+      <c r="O60" s="34">
+        <v>0.29166700000000001</v>
+      </c>
+      <c r="P60" s="34">
+        <v>0.81944399999999995</v>
+      </c>
+      <c r="Q60" s="34">
+        <v>0.97222200000000003</v>
+      </c>
+      <c r="R60" s="35">
+        <v>1</v>
+      </c>
+      <c r="S60" s="35">
+        <v>1</v>
+      </c>
+      <c r="T60" s="35">
+        <v>1</v>
+      </c>
+      <c r="U60" s="35">
+        <v>1</v>
+      </c>
+      <c r="V60" s="35">
+        <v>1</v>
+      </c>
+      <c r="W60" s="35">
+        <v>1</v>
+      </c>
+      <c r="X60" s="35">
+        <v>1</v>
+      </c>
+      <c r="Y60" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z60">
+        <v>12</v>
+      </c>
+      <c r="AA60" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27">
+      <c r="A61">
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <v>48</v>
+      </c>
+      <c r="C61">
+        <v>12409</v>
+      </c>
+      <c r="D61">
+        <v>123020</v>
+      </c>
+      <c r="E61">
+        <v>89344</v>
+      </c>
+      <c r="F61">
+        <v>51621</v>
+      </c>
+      <c r="G61">
+        <v>120188</v>
+      </c>
+      <c r="N61" s="34">
+        <v>8.3333000000000004E-2</v>
+      </c>
+      <c r="O61" s="34">
+        <v>0.54166700000000001</v>
+      </c>
+      <c r="P61" s="34">
+        <v>1</v>
+      </c>
+      <c r="Q61" s="35">
+        <v>1</v>
+      </c>
+      <c r="R61" s="35">
+        <v>1</v>
+      </c>
+      <c r="S61" s="35">
+        <v>1</v>
+      </c>
+      <c r="T61" s="35">
+        <v>1</v>
+      </c>
+      <c r="U61" s="35">
+        <v>1</v>
+      </c>
+      <c r="V61" s="35">
+        <v>1</v>
+      </c>
+      <c r="W61" s="35">
+        <v>1</v>
+      </c>
+      <c r="X61" s="35">
+        <v>1</v>
+      </c>
+      <c r="Y61" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z61">
+        <v>12</v>
+      </c>
+      <c r="AA61" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27">
+      <c r="A62">
+        <v>6</v>
+      </c>
+      <c r="B62">
+        <v>12</v>
+      </c>
+      <c r="C62">
+        <v>31152</v>
+      </c>
+      <c r="D62">
+        <v>321625</v>
+      </c>
+      <c r="E62">
+        <v>19695</v>
+      </c>
+      <c r="F62">
+        <v>44731</v>
+      </c>
+      <c r="G62">
+        <v>73020</v>
+      </c>
+      <c r="N62" s="34"/>
+      <c r="O62" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="P62" s="35">
+        <v>0.91666700000000001</v>
+      </c>
+      <c r="Q62" s="35">
+        <v>1</v>
+      </c>
+      <c r="R62" s="35">
+        <v>1</v>
+      </c>
+      <c r="S62" s="35">
+        <v>1</v>
+      </c>
+      <c r="T62" s="35">
+        <v>1</v>
+      </c>
+      <c r="U62" s="35">
+        <v>1</v>
+      </c>
+      <c r="V62" s="35">
+        <v>1</v>
+      </c>
+      <c r="W62" s="35">
+        <v>1</v>
+      </c>
+      <c r="X62" s="35">
+        <v>1</v>
+      </c>
+      <c r="Y62" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z62">
+        <v>12</v>
+      </c>
+      <c r="AA62" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="6:6">
+      <c r="F66">
+        <f>F57-F49</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="6:6">
+      <c r="F67">
+        <f t="shared" ref="F67:F71" si="32">F58-F50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="6:6">
+      <c r="F68">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="6:6">
+      <c r="F69">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="6:6">
+      <c r="F70">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="6:6">
+      <c r="F71">
+        <f t="shared" si="32"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A17:A25"/>
-    <mergeCell ref="A5:A13"/>
+  <mergeCells count="7">
     <mergeCell ref="N1:Y1"/>
     <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="A19:A27"/>
+    <mergeCell ref="A8:A15"/>
+    <mergeCell ref="N6:Y6"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="N17:Y17"/>
   </mergeCells>
-  <conditionalFormatting sqref="N13:Y13">
-    <cfRule type="dataBar" priority="87">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63C384"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8824DAEE-3449-1F47-B7EB-0F4232F6041D}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-    <cfRule type="colorScale" priority="88">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFCCFFCC"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N13:Y13">
-    <cfRule type="colorScale" priority="84">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="85">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFB628"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5780C6F8-193F-7646-97C6-DF03B14611A5}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O9:T9 N3:X3 N8:T8 N7:U7 N6:V6 N4:W5 N10:S10 N11:R12">
-    <cfRule type="colorScale" priority="89">
+  <conditionalFormatting sqref="O12:T12 N11:T11 N10:U10 N9:V9 N8:W8 N13:S13 N14:R15">
+    <cfRule type="colorScale" priority="101">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -4182,7 +5145,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="90">
+    <cfRule type="colorScale" priority="102">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4193,8 +5156,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H13">
-    <cfRule type="colorScale" priority="76">
+  <conditionalFormatting sqref="H19:H27">
+    <cfRule type="colorScale" priority="115">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4202,7 +5165,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="79">
+    <cfRule type="colorScale" priority="116">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4213,8 +5176,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G13">
-    <cfRule type="colorScale" priority="75">
+  <conditionalFormatting sqref="G19:G27">
+    <cfRule type="colorScale" priority="117">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4223,8 +5186,54 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H17:H25">
-    <cfRule type="colorScale" priority="103">
+  <conditionalFormatting sqref="N19:Y27">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:X3 N4:W5">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:Y5">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H5">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4232,7 +5241,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="104">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4243,8 +5252,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G17:G25">
-    <cfRule type="colorScale" priority="105">
+  <conditionalFormatting sqref="G3:G5">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4253,8 +5262,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:Y12">
-    <cfRule type="colorScale" priority="41">
+  <conditionalFormatting sqref="N8:Y15">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4265,8 +5274,38 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N17:Y25">
-    <cfRule type="colorScale" priority="106">
+  <conditionalFormatting sqref="H8:H15">
+    <cfRule type="colorScale" priority="135">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="136">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8:G15">
+    <cfRule type="colorScale" priority="137">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N8:Y15 N19:Y27 N3:Y4">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4277,39 +5316,36 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="X5:Y5">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F66:F71">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8824DAEE-3449-1F47-B7EB-0F4232F6041D}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF63C384"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>N13:Y13</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5780C6F8-193F-7646-97C6-DF03B14611A5}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FFFFB628"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>N13:Y13</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>

</xml_diff>

<commit_message>
Update to version 2.3.12
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="47020" windowHeight="18620" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="results.prn" sheetId="1" r:id="rId1"/>
+    <sheet name="Random7" sheetId="1" r:id="rId1"/>
+    <sheet name="Random4" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="25">
   <si>
     <t>Method</t>
   </si>
@@ -92,6 +93,9 @@
   <si>
     <t>2.3.9</t>
   </si>
+  <si>
+    <t>2.3.11</t>
+  </si>
 </sst>
 </file>
 
@@ -102,7 +106,7 @@
     <numFmt numFmtId="165" formatCode="0.0000%"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -139,8 +143,15 @@
       <color theme="1"/>
       <name val="Helvetica Neue"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +210,18 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFABF8F"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -283,7 +306,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="485">
+  <cellStyleXfs count="519">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -769,8 +792,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -813,6 +870,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -826,8 +884,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="485">
+  <cellStyles count="519">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1070,6 +1136,23 @@
     <cellStyle name="Followed Hyperlink" xfId="480" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="482" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="484" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="486" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="488" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="490" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="492" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="494" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="496" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="498" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="500" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="502" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="504" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="506" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="508" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="510" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="512" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="516" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="518" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1312,6 +1395,23 @@
     <cellStyle name="Hyperlink" xfId="479" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="481" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="483" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="485" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="487" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="489" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="491" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="493" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="495" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="497" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="499" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="501" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="503" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="505" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="507" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="509" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="511" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="515" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="517" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -1665,7 +1765,7 @@
   <dimension ref="A1:AC61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+      <selection activeCell="I27" sqref="I27:M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1699,22 +1799,22 @@
       <c r="K1" s="22"/>
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
     </row>
     <row r="2" spans="1:29" s="1" customFormat="1" ht="56" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -1765,7 +1865,7 @@
       <c r="P2" s="7">
         <v>4096</v>
       </c>
-      <c r="Q2" s="7">
+      <c r="Q2" s="34">
         <v>2048</v>
       </c>
       <c r="R2" s="7">
@@ -1971,20 +2071,20 @@
       <c r="C5" s="24"/>
     </row>
     <row r="6" spans="1:29">
-      <c r="N6" s="27" t="s">
+      <c r="N6" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="27"/>
-      <c r="S6" s="27"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="27"/>
-      <c r="V6" s="27"/>
-      <c r="W6" s="27"/>
-      <c r="X6" s="27"/>
-      <c r="Y6" s="27"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="28"/>
+      <c r="V6" s="28"/>
+      <c r="W6" s="28"/>
+      <c r="X6" s="28"/>
+      <c r="Y6" s="28"/>
     </row>
     <row r="7" spans="1:29" ht="45">
       <c r="A7" s="2" t="s">
@@ -2035,7 +2135,7 @@
       <c r="P7" s="7">
         <v>4096</v>
       </c>
-      <c r="Q7" s="7">
+      <c r="Q7" s="34">
         <v>2048</v>
       </c>
       <c r="R7" s="7">
@@ -2073,7 +2173,7 @@
       </c>
     </row>
     <row r="8" spans="1:29">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="15">
@@ -2160,7 +2260,7 @@
       </c>
     </row>
     <row r="9" spans="1:29">
-      <c r="A9" s="30"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="9">
         <v>2</v>
       </c>
@@ -2245,7 +2345,7 @@
       </c>
     </row>
     <row r="10" spans="1:29">
-      <c r="A10" s="30"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="15">
         <v>3</v>
       </c>
@@ -2332,7 +2432,7 @@
       </c>
     </row>
     <row r="11" spans="1:29">
-      <c r="A11" s="30"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="9">
         <v>4</v>
       </c>
@@ -2419,7 +2519,7 @@
       </c>
     </row>
     <row r="12" spans="1:29">
-      <c r="A12" s="30"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="15">
         <v>5</v>
       </c>
@@ -2506,7 +2606,7 @@
       </c>
     </row>
     <row r="13" spans="1:29">
-      <c r="A13" s="30"/>
+      <c r="A13" s="31"/>
       <c r="B13" s="9">
         <v>6</v>
       </c>
@@ -2593,7 +2693,7 @@
       </c>
     </row>
     <row r="14" spans="1:29">
-      <c r="A14" s="30"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="15">
         <v>7</v>
       </c>
@@ -2680,7 +2780,7 @@
       </c>
     </row>
     <row r="15" spans="1:29">
-      <c r="A15" s="30"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="9">
         <v>8</v>
       </c>
@@ -2767,20 +2867,20 @@
       </c>
     </row>
     <row r="16" spans="1:29">
-      <c r="N16" s="27" t="s">
+      <c r="N16" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="27"/>
-      <c r="T16" s="27"/>
-      <c r="U16" s="27"/>
-      <c r="V16" s="27"/>
-      <c r="W16" s="27"/>
-      <c r="X16" s="27"/>
-      <c r="Y16" s="27"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
+      <c r="W16" s="28"/>
+      <c r="X16" s="28"/>
+      <c r="Y16" s="28"/>
     </row>
     <row r="17" spans="1:29" ht="45">
       <c r="A17" s="2" t="s">
@@ -2831,7 +2931,7 @@
       <c r="P17" s="7">
         <v>4096</v>
       </c>
-      <c r="Q17" s="7">
+      <c r="Q17" s="34">
         <v>2048</v>
       </c>
       <c r="R17" s="7">
@@ -3034,7 +3134,7 @@
       <c r="AC19" s="20"/>
     </row>
     <row r="20" spans="1:29">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="15">
@@ -3121,7 +3221,7 @@
       </c>
     </row>
     <row r="21" spans="1:29">
-      <c r="A21" s="30"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="9">
         <v>2</v>
       </c>
@@ -3208,7 +3308,7 @@
       </c>
     </row>
     <row r="22" spans="1:29">
-      <c r="A22" s="30"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="15">
         <v>3</v>
       </c>
@@ -3295,7 +3395,7 @@
       </c>
     </row>
     <row r="23" spans="1:29">
-      <c r="A23" s="30"/>
+      <c r="A23" s="31"/>
       <c r="B23" s="9">
         <v>4</v>
       </c>
@@ -3382,7 +3482,7 @@
       </c>
     </row>
     <row r="24" spans="1:29">
-      <c r="A24" s="30"/>
+      <c r="A24" s="31"/>
       <c r="B24" s="15">
         <v>5</v>
       </c>
@@ -3469,7 +3569,7 @@
       </c>
     </row>
     <row r="25" spans="1:29">
-      <c r="A25" s="30"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="9">
         <v>6</v>
       </c>
@@ -3556,7 +3656,7 @@
       </c>
     </row>
     <row r="26" spans="1:29">
-      <c r="A26" s="30"/>
+      <c r="A26" s="31"/>
       <c r="B26" s="15">
         <v>7</v>
       </c>
@@ -3643,36 +3743,159 @@
       </c>
     </row>
     <row r="27" spans="1:29">
-      <c r="A27" s="30"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="9">
+        <v>8</v>
+      </c>
+      <c r="C27" s="9">
+        <v>216</v>
+      </c>
+      <c r="D27" s="10">
+        <v>13705246</v>
+      </c>
+      <c r="E27" s="10">
+        <v>461706935</v>
+      </c>
+      <c r="F27" s="10">
+        <v>499707</v>
+      </c>
+      <c r="G27" s="10">
+        <v>65570</v>
+      </c>
+      <c r="H27" s="10">
+        <v>160608</v>
+      </c>
+      <c r="I27" s="11">
+        <f t="shared" ref="I27" si="25">E27/C27</f>
+        <v>2137532.1064814813</v>
+      </c>
+      <c r="J27" s="12">
+        <f t="shared" ref="J27" si="26">D27/C27</f>
+        <v>63450.212962962964</v>
+      </c>
+      <c r="K27" s="11">
+        <f t="shared" ref="K27" si="27">F27/C27</f>
+        <v>2313.4583333333335</v>
+      </c>
+      <c r="L27" s="12">
+        <f t="shared" ref="L27" si="28">I27/K27</f>
+        <v>923.95530781037678</v>
+      </c>
+      <c r="M27" s="12">
+        <f t="shared" ref="M27" si="29">J27/K27</f>
+        <v>27.426563966484359</v>
+      </c>
       <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
-      <c r="U27" s="13"/>
-      <c r="V27" s="13"/>
-      <c r="W27" s="13"/>
-      <c r="X27" s="13"/>
-      <c r="Y27" s="13"/>
-      <c r="Z27" s="15"/>
-      <c r="AA27" s="9"/>
+      <c r="O27" s="13">
+        <v>0.125</v>
+      </c>
+      <c r="P27" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="Q27" s="13">
+        <v>0.97685200000000005</v>
+      </c>
+      <c r="R27" s="13">
+        <v>1</v>
+      </c>
+      <c r="S27" s="13">
+        <v>1</v>
+      </c>
+      <c r="T27" s="13">
+        <v>1</v>
+      </c>
+      <c r="U27" s="13">
+        <v>1</v>
+      </c>
+      <c r="V27" s="13">
+        <v>1</v>
+      </c>
+      <c r="W27" s="13">
+        <v>1</v>
+      </c>
+      <c r="X27" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA27" s="9">
+        <v>36</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29">
+      <c r="D28">
+        <f>D27/60000/60</f>
+        <v>3.807012777777778</v>
+      </c>
     </row>
     <row r="29" spans="1:29">
-      <c r="I29" s="24"/>
+      <c r="G29" s="24">
+        <f>SUM(G22:G27)</f>
+        <v>291237</v>
+      </c>
+      <c r="H29" s="24">
+        <f>SUM(H22:H27)</f>
+        <v>842960</v>
+      </c>
+      <c r="M29" s="32">
+        <f>SUM(M22:M27)</f>
+        <v>30.268235706279171</v>
+      </c>
+      <c r="N29" s="26">
+        <f>SUM(N8:N13)/6</f>
+        <v>0</v>
+      </c>
+      <c r="O29" s="26">
+        <f t="shared" ref="O29:Y29" si="30">SUM(O8:O13)/6</f>
+        <v>7.0016666666666673E-3</v>
+      </c>
+      <c r="P29" s="26">
+        <f t="shared" si="30"/>
+        <v>0.26971283333333335</v>
+      </c>
+      <c r="Q29" s="26">
+        <f t="shared" si="30"/>
+        <v>0.66943366666666682</v>
+      </c>
+      <c r="R29" s="26">
+        <f t="shared" si="30"/>
+        <v>0.90011999999999992</v>
+      </c>
+      <c r="S29" s="26">
+        <f t="shared" si="30"/>
+        <v>0.97983483333333343</v>
+      </c>
+      <c r="T29" s="26">
+        <f t="shared" si="30"/>
+        <v>0.99700216666666674</v>
+      </c>
+      <c r="U29" s="26">
+        <f t="shared" si="30"/>
+        <v>0.99968533333333331</v>
+      </c>
+      <c r="V29" s="26">
+        <f t="shared" si="30"/>
+        <v>0.99998333333333334</v>
+      </c>
+      <c r="W29" s="26">
+        <f t="shared" si="30"/>
+        <v>0.99999933333333324</v>
+      </c>
+      <c r="X29" s="26">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="Y29" s="26">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:29" ht="18" customHeight="1">
       <c r="W31" s="1"/>
@@ -3683,88 +3906,96 @@
       <c r="W32" s="25"/>
       <c r="X32" s="25"/>
     </row>
-    <row r="33" spans="23:24">
+    <row r="33" spans="4:24">
       <c r="W33" s="25"/>
       <c r="X33" s="25"/>
     </row>
-    <row r="34" spans="23:24">
+    <row r="34" spans="4:24">
+      <c r="D34">
+        <f>D11/3600000</f>
+        <v>0.40771000000000002</v>
+      </c>
+      <c r="L34">
+        <f>L14/6.3</f>
+        <v>5.2441018595631634</v>
+      </c>
       <c r="W34" s="25"/>
       <c r="X34" s="25"/>
     </row>
-    <row r="35" spans="23:24">
+    <row r="35" spans="4:24">
       <c r="W35" s="25"/>
       <c r="X35" s="25"/>
     </row>
-    <row r="36" spans="23:24">
+    <row r="36" spans="4:24">
       <c r="W36" s="25"/>
       <c r="X36" s="25"/>
     </row>
-    <row r="37" spans="23:24">
+    <row r="37" spans="4:24">
       <c r="W37" s="25"/>
       <c r="X37" s="25"/>
     </row>
-    <row r="38" spans="23:24">
+    <row r="38" spans="4:24">
       <c r="W38" s="25"/>
       <c r="X38" s="25"/>
     </row>
-    <row r="39" spans="23:24">
+    <row r="39" spans="4:24">
       <c r="W39" s="25"/>
       <c r="X39" s="25"/>
     </row>
-    <row r="40" spans="23:24">
+    <row r="40" spans="4:24">
       <c r="W40" s="25"/>
       <c r="X40" s="25"/>
     </row>
-    <row r="45" spans="23:24">
+    <row r="45" spans="4:24">
       <c r="X45" s="25"/>
     </row>
-    <row r="48" spans="23:24">
-      <c r="W48" s="26"/>
-      <c r="X48" s="26"/>
+    <row r="48" spans="4:24">
+      <c r="W48" s="27"/>
+      <c r="X48" s="27"/>
     </row>
     <row r="49" spans="23:24">
-      <c r="W49" s="26"/>
-      <c r="X49" s="26"/>
+      <c r="W49" s="27"/>
+      <c r="X49" s="27"/>
     </row>
     <row r="50" spans="23:24">
-      <c r="W50" s="26"/>
-      <c r="X50" s="26"/>
+      <c r="W50" s="27"/>
+      <c r="X50" s="27"/>
     </row>
     <row r="51" spans="23:24">
-      <c r="W51" s="26"/>
-      <c r="X51" s="26"/>
+      <c r="W51" s="27"/>
+      <c r="X51" s="27"/>
     </row>
     <row r="52" spans="23:24">
-      <c r="W52" s="26"/>
-      <c r="X52" s="26"/>
+      <c r="W52" s="27"/>
+      <c r="X52" s="27"/>
     </row>
     <row r="53" spans="23:24">
-      <c r="W53" s="26"/>
-      <c r="X53" s="26"/>
+      <c r="W53" s="27"/>
+      <c r="X53" s="27"/>
     </row>
     <row r="56" spans="23:24">
-      <c r="W56" s="26"/>
-      <c r="X56" s="26"/>
+      <c r="W56" s="27"/>
+      <c r="X56" s="27"/>
     </row>
     <row r="57" spans="23:24">
-      <c r="W57" s="26"/>
-      <c r="X57" s="26"/>
+      <c r="W57" s="27"/>
+      <c r="X57" s="27"/>
     </row>
     <row r="58" spans="23:24">
-      <c r="W58" s="26"/>
-      <c r="X58" s="26"/>
+      <c r="W58" s="27"/>
+      <c r="X58" s="27"/>
     </row>
     <row r="59" spans="23:24">
-      <c r="W59" s="26"/>
-      <c r="X59" s="26"/>
+      <c r="W59" s="27"/>
+      <c r="X59" s="27"/>
     </row>
     <row r="60" spans="23:24">
-      <c r="W60" s="26"/>
-      <c r="X60" s="26"/>
+      <c r="W60" s="27"/>
+      <c r="X60" s="27"/>
     </row>
     <row r="61" spans="23:24">
-      <c r="W61" s="26"/>
-      <c r="X61" s="26"/>
+      <c r="W61" s="27"/>
+      <c r="X61" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3776,7 +4007,7 @@
     <mergeCell ref="Z1:AA1"/>
   </mergeCells>
   <conditionalFormatting sqref="F65:F70">
-    <cfRule type="cellIs" dxfId="1" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="28" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4144,4 +4375,779 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" customWidth="1"/>
+    <col min="26" max="26" width="27.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28">
+      <c r="N1" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+    </row>
+    <row r="2" spans="1:28" ht="60">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="7">
+        <v>16384</v>
+      </c>
+      <c r="O2" s="7">
+        <v>8192</v>
+      </c>
+      <c r="P2" s="7">
+        <v>4096</v>
+      </c>
+      <c r="Q2" s="35">
+        <v>2048</v>
+      </c>
+      <c r="R2" s="7">
+        <v>1024</v>
+      </c>
+      <c r="S2" s="7">
+        <v>512</v>
+      </c>
+      <c r="T2" s="7">
+        <v>256</v>
+      </c>
+      <c r="U2" s="7">
+        <v>128</v>
+      </c>
+      <c r="V2" s="7">
+        <v>64</v>
+      </c>
+      <c r="W2" s="7">
+        <v>32</v>
+      </c>
+      <c r="X2" s="7">
+        <v>16</v>
+      </c>
+      <c r="Y2" s="7">
+        <v>8</v>
+      </c>
+      <c r="Z2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB2" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28">
+      <c r="A3" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="15">
+        <v>6</v>
+      </c>
+      <c r="C3" s="15">
+        <v>1</v>
+      </c>
+      <c r="D3" s="16">
+        <v>7854</v>
+      </c>
+      <c r="E3" s="16">
+        <v>7851</v>
+      </c>
+      <c r="F3" s="16">
+        <v>2471</v>
+      </c>
+      <c r="G3" s="16">
+        <v>71156</v>
+      </c>
+      <c r="H3" s="16">
+        <v>71156</v>
+      </c>
+      <c r="I3" s="17">
+        <f t="shared" ref="I3" si="0">E3/C3</f>
+        <v>7851</v>
+      </c>
+      <c r="J3" s="18">
+        <f t="shared" ref="J3" si="1">D3/C3</f>
+        <v>7854</v>
+      </c>
+      <c r="K3" s="17">
+        <f t="shared" ref="K3" si="2">F3/C3</f>
+        <v>2471</v>
+      </c>
+      <c r="L3" s="18">
+        <f t="shared" ref="L3" si="3">I3/K3</f>
+        <v>3.1772561715904493</v>
+      </c>
+      <c r="M3" s="18">
+        <f t="shared" ref="M3" si="4">J3/K3</f>
+        <v>3.178470254957507</v>
+      </c>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="19">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="19">
+        <v>1</v>
+      </c>
+      <c r="R3" s="19">
+        <v>1</v>
+      </c>
+      <c r="S3" s="19">
+        <v>1</v>
+      </c>
+      <c r="T3" s="19">
+        <v>1</v>
+      </c>
+      <c r="U3" s="19">
+        <v>1</v>
+      </c>
+      <c r="V3" s="13">
+        <v>1</v>
+      </c>
+      <c r="W3" s="13">
+        <v>1</v>
+      </c>
+      <c r="X3" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA3" s="15">
+        <v>12</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28">
+      <c r="A4" s="31"/>
+      <c r="B4" s="9">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9">
+        <v>99996</v>
+      </c>
+      <c r="D4" s="10">
+        <v>231291</v>
+      </c>
+      <c r="E4" s="10">
+        <v>2716871</v>
+      </c>
+      <c r="F4" s="10">
+        <v>77935377</v>
+      </c>
+      <c r="G4" s="10">
+        <v>18183</v>
+      </c>
+      <c r="H4" s="10">
+        <v>77308</v>
+      </c>
+      <c r="I4" s="17"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13">
+        <v>2.3361E-2</v>
+      </c>
+      <c r="Q4" s="13">
+        <v>0.37146499999999999</v>
+      </c>
+      <c r="R4" s="13">
+        <v>0.80790200000000001</v>
+      </c>
+      <c r="S4" s="13">
+        <v>0.96798899999999999</v>
+      </c>
+      <c r="T4" s="13">
+        <v>0.99651999999999996</v>
+      </c>
+      <c r="U4" s="13">
+        <v>0.99968000000000001</v>
+      </c>
+      <c r="V4" s="13">
+        <v>1</v>
+      </c>
+      <c r="W4" s="13">
+        <v>1</v>
+      </c>
+      <c r="X4" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA4" s="15">
+        <v>12</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28">
+      <c r="A5" s="31"/>
+      <c r="B5" s="15">
+        <v>3</v>
+      </c>
+      <c r="C5" s="15">
+        <v>49992</v>
+      </c>
+      <c r="D5" s="16">
+        <v>207777</v>
+      </c>
+      <c r="E5" s="16">
+        <v>2441857</v>
+      </c>
+      <c r="F5" s="16">
+        <v>54203332</v>
+      </c>
+      <c r="G5" s="16">
+        <v>27234</v>
+      </c>
+      <c r="H5" s="16">
+        <v>118628</v>
+      </c>
+      <c r="I5" s="17"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="19">
+        <v>6.2E-4</v>
+      </c>
+      <c r="P5" s="19">
+        <v>0.14582300000000001</v>
+      </c>
+      <c r="Q5" s="19">
+        <v>0.64876400000000001</v>
+      </c>
+      <c r="R5" s="19">
+        <v>0.91672699999999996</v>
+      </c>
+      <c r="S5" s="19">
+        <v>0.98629800000000001</v>
+      </c>
+      <c r="T5" s="19">
+        <v>0.99883999999999995</v>
+      </c>
+      <c r="U5" s="19">
+        <v>0.99995999999999996</v>
+      </c>
+      <c r="V5" s="13">
+        <v>1</v>
+      </c>
+      <c r="W5" s="13">
+        <v>1</v>
+      </c>
+      <c r="X5" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA5" s="15">
+        <v>12</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28">
+      <c r="A6" s="31"/>
+      <c r="B6" s="9">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9">
+        <v>15000</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1467756</v>
+      </c>
+      <c r="E6" s="10">
+        <v>17534709</v>
+      </c>
+      <c r="F6" s="10">
+        <v>19805266</v>
+      </c>
+      <c r="G6" s="10">
+        <v>34284</v>
+      </c>
+      <c r="H6" s="10">
+        <v>126740</v>
+      </c>
+      <c r="I6" s="17">
+        <f t="shared" ref="I3:I8" si="5">E6/C6</f>
+        <v>1168.9806000000001</v>
+      </c>
+      <c r="J6" s="18">
+        <f t="shared" ref="J3:J8" si="6">D6/C6</f>
+        <v>97.850399999999993</v>
+      </c>
+      <c r="K6" s="17">
+        <f t="shared" ref="K3:K8" si="7">F6/C6</f>
+        <v>1320.3510666666666</v>
+      </c>
+      <c r="L6" s="18">
+        <f t="shared" ref="L3:L8" si="8">I6/K6</f>
+        <v>0.88535589474031817</v>
+      </c>
+      <c r="M6" s="18">
+        <f t="shared" ref="M3:M8" si="9">J6/K6</f>
+        <v>7.410938080811437E-2</v>
+      </c>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13">
+        <v>2.0669999999999998E-3</v>
+      </c>
+      <c r="P6" s="13">
+        <v>0.266067</v>
+      </c>
+      <c r="Q6" s="13">
+        <v>0.80320000000000003</v>
+      </c>
+      <c r="R6" s="13">
+        <v>0.97426699999999999</v>
+      </c>
+      <c r="S6" s="13">
+        <v>0.99760000000000004</v>
+      </c>
+      <c r="T6" s="13">
+        <v>0.99993299999999996</v>
+      </c>
+      <c r="U6" s="13">
+        <v>1</v>
+      </c>
+      <c r="V6" s="13">
+        <v>1</v>
+      </c>
+      <c r="W6" s="13">
+        <v>1</v>
+      </c>
+      <c r="X6" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA6" s="15">
+        <v>12</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28">
+      <c r="A7" s="31"/>
+      <c r="B7" s="15">
+        <v>5</v>
+      </c>
+      <c r="C7" s="15">
+        <v>4992</v>
+      </c>
+      <c r="D7" s="16">
+        <v>1102944</v>
+      </c>
+      <c r="E7" s="16">
+        <v>13103064</v>
+      </c>
+      <c r="F7" s="16">
+        <v>8837876</v>
+      </c>
+      <c r="G7" s="16">
+        <v>48138</v>
+      </c>
+      <c r="H7" s="16">
+        <v>156316</v>
+      </c>
+      <c r="I7" s="17">
+        <f t="shared" si="5"/>
+        <v>2624.8125</v>
+      </c>
+      <c r="J7" s="18">
+        <f t="shared" si="6"/>
+        <v>220.94230769230768</v>
+      </c>
+      <c r="K7" s="17">
+        <f t="shared" si="7"/>
+        <v>1770.4078525641025</v>
+      </c>
+      <c r="L7" s="18">
+        <f t="shared" si="8"/>
+        <v>1.4826032861289296</v>
+      </c>
+      <c r="M7" s="18">
+        <f t="shared" si="9"/>
+        <v>0.124797406073586</v>
+      </c>
+      <c r="N7" s="13"/>
+      <c r="O7" s="19">
+        <v>2.1635000000000001E-2</v>
+      </c>
+      <c r="P7" s="19">
+        <v>0.52443899999999999</v>
+      </c>
+      <c r="Q7" s="19">
+        <v>0.93309299999999995</v>
+      </c>
+      <c r="R7" s="19">
+        <v>0.99338899999999997</v>
+      </c>
+      <c r="S7" s="19">
+        <v>0.99899800000000005</v>
+      </c>
+      <c r="T7" s="19">
+        <v>1</v>
+      </c>
+      <c r="U7" s="13">
+        <v>1</v>
+      </c>
+      <c r="V7" s="13">
+        <v>1</v>
+      </c>
+      <c r="W7" s="13">
+        <v>1</v>
+      </c>
+      <c r="X7" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA7" s="15">
+        <v>12</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28">
+      <c r="A8" s="31"/>
+      <c r="B8" s="9">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9">
+        <v>996</v>
+      </c>
+      <c r="D8" s="10">
+        <v>3164522</v>
+      </c>
+      <c r="E8" s="10">
+        <v>37381349</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1866432</v>
+      </c>
+      <c r="G8" s="10">
+        <v>51163</v>
+      </c>
+      <c r="H8" s="10">
+        <v>129084</v>
+      </c>
+      <c r="I8" s="17">
+        <f t="shared" si="5"/>
+        <v>37531.47489959839</v>
+      </c>
+      <c r="J8" s="18">
+        <f t="shared" si="6"/>
+        <v>3177.230923694779</v>
+      </c>
+      <c r="K8" s="17">
+        <f t="shared" si="7"/>
+        <v>1873.9277108433735</v>
+      </c>
+      <c r="L8" s="18">
+        <f t="shared" si="8"/>
+        <v>20.028240514521823</v>
+      </c>
+      <c r="M8" s="18">
+        <f t="shared" si="9"/>
+        <v>1.695492790522237</v>
+      </c>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13">
+        <v>1.7068E-2</v>
+      </c>
+      <c r="P8" s="13">
+        <v>0.59036100000000002</v>
+      </c>
+      <c r="Q8" s="13">
+        <v>0.94779100000000005</v>
+      </c>
+      <c r="R8" s="13">
+        <v>0.99497999999999998</v>
+      </c>
+      <c r="S8" s="13">
+        <v>1</v>
+      </c>
+      <c r="T8" s="13">
+        <v>1</v>
+      </c>
+      <c r="U8" s="13">
+        <v>1</v>
+      </c>
+      <c r="V8" s="13">
+        <v>1</v>
+      </c>
+      <c r="W8" s="13">
+        <v>1</v>
+      </c>
+      <c r="X8" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA8" s="15">
+        <v>12</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28">
+      <c r="G10" s="24">
+        <f>SUM(G3:G8)</f>
+        <v>250158</v>
+      </c>
+      <c r="H10" s="24">
+        <f>SUM(H3:H8)</f>
+        <v>679232</v>
+      </c>
+      <c r="M10" s="32">
+        <f>SUM(M3:M8)</f>
+        <v>5.0728698323614445</v>
+      </c>
+      <c r="N10" s="26">
+        <f>SUM(N3:N8)/6</f>
+        <v>0</v>
+      </c>
+      <c r="O10" s="26">
+        <f>SUM(O3:O8)/6</f>
+        <v>6.8983333333333327E-3</v>
+      </c>
+      <c r="P10" s="26">
+        <f t="shared" ref="P10:Y10" si="10">SUM(P3:P8)/6</f>
+        <v>0.42500850000000007</v>
+      </c>
+      <c r="Q10" s="33">
+        <f t="shared" si="10"/>
+        <v>0.78405216666666666</v>
+      </c>
+      <c r="R10" s="26">
+        <f t="shared" si="10"/>
+        <v>0.94787749999999982</v>
+      </c>
+      <c r="S10" s="26">
+        <f t="shared" si="10"/>
+        <v>0.99181416666666677</v>
+      </c>
+      <c r="T10" s="26">
+        <f t="shared" si="10"/>
+        <v>0.99921550000000003</v>
+      </c>
+      <c r="U10" s="26">
+        <f t="shared" si="10"/>
+        <v>0.99994000000000005</v>
+      </c>
+      <c r="V10" s="26">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="W10" s="26">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="X10" s="26">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="Y10" s="26">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28">
+      <c r="L11">
+        <f>L8/L3</f>
+        <v>6.3036278577739679</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="N1:Y1"/>
+    <mergeCell ref="A3:A8"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H3:H6">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G6">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:Y6">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7:H8">
+    <cfRule type="colorScale" priority="187">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="188">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7:G8">
+    <cfRule type="colorScale" priority="189">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N7:Y8">
+    <cfRule type="colorScale" priority="190">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update to version 2.3.15
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="26">
   <si>
     <t>Method</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>2.3.12</t>
+  </si>
+  <si>
+    <t>2.3.13</t>
   </si>
 </sst>
 </file>
@@ -306,8 +309,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="523">
+  <cellStyleXfs count="531">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -897,7 +908,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="523">
+  <cellStyles count="531">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1159,6 +1170,10 @@
     <cellStyle name="Followed Hyperlink" xfId="518" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="520" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="522" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="524" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="526" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="528" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="530" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1420,6 +1435,10 @@
     <cellStyle name="Hyperlink" xfId="517" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="519" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="521" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="523" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="525" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="527" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="529" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -1773,7 +1792,7 @@
   <dimension ref="A1:AC61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+      <selection activeCell="I8" sqref="I8:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4387,10 +4406,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB20"/>
+  <dimension ref="A1:AB22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="I7" sqref="I7:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4528,11 +4547,26 @@
       <c r="H3" s="16">
         <v>77880</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="I3" s="17">
+        <f t="shared" ref="I3:I6" si="0">E3/C3</f>
+        <v>4.0631850109601757</v>
+      </c>
+      <c r="J3" s="18">
+        <f t="shared" ref="J3:J6" si="1">D3/C3</f>
+        <v>0.38225411606585707</v>
+      </c>
+      <c r="K3" s="17">
+        <f t="shared" ref="K3:K6" si="2">F3/C3</f>
+        <v>670.88369413910618</v>
+      </c>
+      <c r="L3" s="18">
+        <f t="shared" ref="L3:L6" si="3">I3/K3</f>
+        <v>6.0564670843195117E-3</v>
+      </c>
+      <c r="M3" s="18">
+        <f t="shared" ref="M3:M6" si="4">J3/K3</f>
+        <v>5.6977702604081712E-4</v>
+      </c>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
       <c r="P3" s="19">
@@ -4598,11 +4632,26 @@
       <c r="H4" s="10">
         <v>79056</v>
       </c>
-      <c r="I4" s="17"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
+      <c r="I4" s="17">
+        <f t="shared" si="0"/>
+        <v>27.087903516140646</v>
+      </c>
+      <c r="J4" s="18">
+        <f t="shared" si="1"/>
+        <v>2.3077723108924357</v>
+      </c>
+      <c r="K4" s="17">
+        <f t="shared" si="2"/>
+        <v>819.17063682547303</v>
+      </c>
+      <c r="L4" s="18">
+        <f t="shared" si="3"/>
+        <v>3.306747373308476E-2</v>
+      </c>
+      <c r="M4" s="18">
+        <f t="shared" si="4"/>
+        <v>2.8172058508294825E-3</v>
+      </c>
       <c r="N4" s="13"/>
       <c r="O4" s="13"/>
       <c r="P4" s="13">
@@ -4668,11 +4717,26 @@
       <c r="H5" s="16">
         <v>136476</v>
       </c>
-      <c r="I5" s="17"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
+      <c r="I5" s="17">
+        <f t="shared" si="0"/>
+        <v>84.49401904304689</v>
+      </c>
+      <c r="J5" s="18">
+        <f t="shared" si="1"/>
+        <v>7.1347215554488717</v>
+      </c>
+      <c r="K5" s="17">
+        <f t="shared" si="2"/>
+        <v>1228.6998719795167</v>
+      </c>
+      <c r="L5" s="18">
+        <f t="shared" si="3"/>
+        <v>6.8767012164591051E-2</v>
+      </c>
+      <c r="M5" s="18">
+        <f t="shared" si="4"/>
+        <v>5.8067244232347512E-3</v>
+      </c>
       <c r="N5" s="13"/>
       <c r="O5" s="19">
         <v>2.1800000000000001E-3</v>
@@ -4740,11 +4804,26 @@
       <c r="H6" s="10">
         <v>139612</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
+      <c r="I6" s="17">
+        <f t="shared" si="0"/>
+        <v>1222.5109333333332</v>
+      </c>
+      <c r="J6" s="18">
+        <f t="shared" si="1"/>
+        <v>102.41306666666667</v>
+      </c>
+      <c r="K6" s="17">
+        <f t="shared" si="2"/>
+        <v>1317.6448666666668</v>
+      </c>
+      <c r="L6" s="18">
+        <f t="shared" si="3"/>
+        <v>0.92780001976253279</v>
+      </c>
+      <c r="M6" s="18">
+        <f t="shared" si="4"/>
+        <v>7.772433169018278E-2</v>
+      </c>
       <c r="N6" s="13"/>
       <c r="O6" s="13">
         <v>3.2000000000000002E-3</v>
@@ -4812,11 +4891,26 @@
       <c r="H7" s="16">
         <v>159256</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
+      <c r="I7" s="17">
+        <f t="shared" ref="I7:I8" si="5">E7/C7</f>
+        <v>2719.1973157051284</v>
+      </c>
+      <c r="J7" s="18">
+        <f t="shared" ref="J7:J8" si="6">D7/C7</f>
+        <v>229.22215544871796</v>
+      </c>
+      <c r="K7" s="17">
+        <f t="shared" ref="K7:K8" si="7">F7/C7</f>
+        <v>1864.8782051282051</v>
+      </c>
+      <c r="L7" s="18">
+        <f t="shared" ref="L7:L8" si="8">I7/K7</f>
+        <v>1.4581098691741059</v>
+      </c>
+      <c r="M7" s="18">
+        <f t="shared" ref="M7:M8" si="9">J7/K7</f>
+        <v>0.12291534901227481</v>
+      </c>
       <c r="N7" s="13"/>
       <c r="O7" s="19">
         <v>4.2067E-2</v>
@@ -4884,11 +4978,26 @@
       <c r="H8" s="10">
         <v>153196</v>
       </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
+      <c r="I8" s="17">
+        <f t="shared" si="5"/>
+        <v>38520.626506024098</v>
+      </c>
+      <c r="J8" s="18">
+        <f t="shared" si="6"/>
+        <v>3284.5833333333335</v>
+      </c>
+      <c r="K8" s="17">
+        <f t="shared" si="7"/>
+        <v>1950.2720883534137</v>
+      </c>
+      <c r="L8" s="18">
+        <f t="shared" si="8"/>
+        <v>19.751411475383673</v>
+      </c>
+      <c r="M8" s="18">
+        <f t="shared" si="9"/>
+        <v>1.6841667134284115</v>
+      </c>
       <c r="N8" s="13"/>
       <c r="O8" s="13">
         <v>5.5220999999999999E-2</v>
@@ -4944,7 +5053,7 @@
       </c>
       <c r="M10" s="32">
         <f>SUM(M3:M8)</f>
-        <v>0</v>
+        <v>1.8940001014309742</v>
       </c>
       <c r="N10" s="26">
         <f>SUM(N3:N8)/6</f>
@@ -4955,50 +5064,50 @@
         <v>1.7111333333333336E-2</v>
       </c>
       <c r="P10" s="26">
-        <f t="shared" ref="P10:Y10" si="0">SUM(P3:P8)/6</f>
+        <f t="shared" ref="P10:Y10" si="10">SUM(P3:P8)/6</f>
         <v>0.28283700000000001</v>
       </c>
       <c r="Q10" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>0.68294349999999993</v>
       </c>
       <c r="R10" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>0.91362733333333335</v>
       </c>
       <c r="S10" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>0.98375866666666667</v>
       </c>
       <c r="T10" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>0.99782850000000012</v>
       </c>
       <c r="U10" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>0.99978166666666668</v>
       </c>
       <c r="V10" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>0.99999033333333331</v>
       </c>
       <c r="W10" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="X10" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="Y10" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:28">
-      <c r="L11" t="e">
+      <c r="L11">
         <f>L8/L3</f>
-        <v>#DIV/0!</v>
+        <v>3261.2100751807998</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="60">
@@ -5092,65 +5201,65 @@
         <v>249996</v>
       </c>
       <c r="D15" s="16">
-        <v>90724</v>
+        <v>103529</v>
       </c>
       <c r="E15" s="16">
-        <v>956340</v>
+        <v>1103921</v>
       </c>
       <c r="F15" s="16">
-        <v>157127969</v>
+        <v>167078359</v>
       </c>
       <c r="G15" s="16">
-        <v>14041</v>
+        <v>15094</v>
       </c>
       <c r="H15" s="16">
-        <v>74592</v>
+        <v>76776</v>
       </c>
       <c r="I15" s="17">
-        <f t="shared" ref="I15:I20" si="1">E15/C15</f>
-        <v>3.8254212067393079</v>
+        <f t="shared" ref="I15:I18" si="11">E15/C15</f>
+        <v>4.4157546520744333</v>
       </c>
       <c r="J15" s="18">
-        <f t="shared" ref="J15:J20" si="2">D15/C15</f>
-        <v>0.36290180642890285</v>
+        <f t="shared" ref="J15:J18" si="12">D15/C15</f>
+        <v>0.41412262596201538</v>
       </c>
       <c r="K15" s="17">
-        <f t="shared" ref="K15:K20" si="3">F15/C15</f>
-        <v>628.52193235091761</v>
+        <f t="shared" ref="K15:K18" si="13">F15/C15</f>
+        <v>668.32412918606701</v>
       </c>
       <c r="L15" s="18">
-        <f t="shared" ref="L15:L20" si="4">I15/K15</f>
-        <v>6.0863766399220755E-3</v>
+        <f t="shared" ref="L15:L18" si="14">I15/K15</f>
+        <v>6.6072051856817674E-3</v>
       </c>
       <c r="M15" s="18">
-        <f t="shared" ref="M15:M20" si="5">J15/K15</f>
-        <v>5.7738924888668295E-4</v>
+        <f t="shared" ref="M15:M18" si="15">J15/K15</f>
+        <v>6.1964338541294864E-4</v>
       </c>
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
       <c r="P15" s="19">
-        <v>5.5960000000000003E-3</v>
+        <v>8.5400000000000007E-3</v>
       </c>
       <c r="Q15" s="19">
-        <v>0.22456400000000001</v>
+        <v>0.25731599999999999</v>
       </c>
       <c r="R15" s="19">
-        <v>0.67955900000000002</v>
+        <v>0.720804</v>
       </c>
       <c r="S15" s="19">
-        <v>0.92228299999999996</v>
+        <v>0.93848299999999996</v>
       </c>
       <c r="T15" s="19">
-        <v>0.98658000000000001</v>
+        <v>0.99029199999999995</v>
       </c>
       <c r="U15" s="19">
-        <v>0.99839199999999995</v>
+        <v>0.99894400000000005</v>
       </c>
       <c r="V15" s="13">
-        <v>0.99992000000000003</v>
+        <v>0.99996399999999996</v>
       </c>
       <c r="W15" s="13">
-        <v>0.999996</v>
+        <v>1</v>
       </c>
       <c r="X15" s="13">
         <v>1</v>
@@ -5165,7 +5274,7 @@
         <v>12</v>
       </c>
       <c r="AB15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:28">
@@ -5176,62 +5285,62 @@
         <v>99996</v>
       </c>
       <c r="D16" s="10">
-        <v>209020</v>
+        <v>216248</v>
       </c>
       <c r="E16" s="10">
-        <v>2450523</v>
+        <v>2535625</v>
       </c>
       <c r="F16" s="10">
-        <v>77155678</v>
+        <v>81413133</v>
       </c>
       <c r="G16" s="10">
-        <v>17973</v>
+        <v>19173</v>
       </c>
       <c r="H16" s="10">
-        <v>76316</v>
+        <v>76940</v>
       </c>
       <c r="I16" s="17">
-        <f t="shared" si="1"/>
-        <v>24.506210248409936</v>
+        <f t="shared" si="11"/>
+        <v>25.357264290571624</v>
       </c>
       <c r="J16" s="18">
-        <f t="shared" si="2"/>
-        <v>2.0902836113444536</v>
+        <f t="shared" si="12"/>
+        <v>2.1625665026601064</v>
       </c>
       <c r="K16" s="17">
-        <f t="shared" si="3"/>
-        <v>771.58764350574017</v>
+        <f t="shared" si="13"/>
+        <v>814.16389655586227</v>
       </c>
       <c r="L16" s="18">
-        <f t="shared" si="4"/>
-        <v>3.176076036814815E-2</v>
+        <f t="shared" si="14"/>
+        <v>3.1145159344254693E-2</v>
       </c>
       <c r="M16" s="18">
-        <f t="shared" si="5"/>
-        <v>2.7090682814037356E-3</v>
+        <f t="shared" si="15"/>
+        <v>2.656180790880508E-3</v>
       </c>
       <c r="N16" s="13"/>
       <c r="O16" s="13"/>
       <c r="P16" s="13">
-        <v>2.2641000000000001E-2</v>
+        <v>2.9940999999999999E-2</v>
       </c>
       <c r="Q16" s="13">
-        <v>0.36367500000000003</v>
+        <v>0.40700599999999998</v>
       </c>
       <c r="R16" s="13">
-        <v>0.80291199999999996</v>
+        <v>0.83407299999999995</v>
       </c>
       <c r="S16" s="13">
-        <v>0.96508899999999997</v>
+        <v>0.97155899999999995</v>
       </c>
       <c r="T16" s="13">
-        <v>0.99582000000000004</v>
+        <v>0.99673</v>
       </c>
       <c r="U16" s="13">
-        <v>0.99972000000000005</v>
+        <v>0.99977000000000005</v>
       </c>
       <c r="V16" s="13">
-        <v>0.99997999999999998</v>
+        <v>1</v>
       </c>
       <c r="W16" s="13">
         <v>1</v>
@@ -5249,7 +5358,7 @@
         <v>12</v>
       </c>
       <c r="AB16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="2:28">
@@ -5260,58 +5369,58 @@
         <v>49992</v>
       </c>
       <c r="D17" s="16">
-        <v>353406</v>
+        <v>369062</v>
       </c>
       <c r="E17" s="16">
-        <v>4193112</v>
+        <v>4370251</v>
       </c>
       <c r="F17" s="16">
-        <v>60678611</v>
+        <v>60425721</v>
       </c>
       <c r="G17" s="16">
-        <v>31088</v>
+        <v>30969</v>
       </c>
       <c r="H17" s="16">
-        <v>126976</v>
+        <v>126820</v>
       </c>
       <c r="I17" s="17">
-        <f t="shared" si="1"/>
-        <v>83.875660105616902</v>
+        <f t="shared" si="11"/>
+        <v>87.419007041126576</v>
       </c>
       <c r="J17" s="18">
-        <f t="shared" si="2"/>
-        <v>7.0692510801728279</v>
+        <f t="shared" si="12"/>
+        <v>7.3824211873899825</v>
       </c>
       <c r="K17" s="17">
-        <f t="shared" si="3"/>
-        <v>1213.7664226276204</v>
+        <f t="shared" si="13"/>
+        <v>1208.7078132501201</v>
       </c>
       <c r="L17" s="18">
-        <f t="shared" si="4"/>
-        <v>6.9103625328536283E-2</v>
+        <f t="shared" si="14"/>
+        <v>7.2324350089260817E-2</v>
       </c>
       <c r="M17" s="18">
-        <f t="shared" si="5"/>
-        <v>5.8242269256954483E-3</v>
+        <f t="shared" si="15"/>
+        <v>6.1076970848225375E-3</v>
       </c>
       <c r="N17" s="13"/>
       <c r="O17" s="19">
-        <v>1.24E-3</v>
+        <v>1.8400000000000001E-3</v>
       </c>
       <c r="P17" s="19">
-        <v>0.209173</v>
+        <v>0.208313</v>
       </c>
       <c r="Q17" s="19">
-        <v>0.74427900000000002</v>
+        <v>0.73457799999999995</v>
       </c>
       <c r="R17" s="19">
-        <v>0.95561300000000005</v>
+        <v>0.95361300000000004</v>
       </c>
       <c r="S17" s="19">
-        <v>0.99503900000000001</v>
+        <v>0.995479</v>
       </c>
       <c r="T17" s="19">
-        <v>0.99968000000000001</v>
+        <v>0.99960000000000004</v>
       </c>
       <c r="U17" s="19">
         <v>1</v>
@@ -5335,7 +5444,7 @@
         <v>12</v>
       </c>
       <c r="AB17" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:28">
@@ -5346,58 +5455,58 @@
         <v>15000</v>
       </c>
       <c r="D18" s="10">
-        <v>1467756</v>
+        <v>1587241</v>
       </c>
       <c r="E18" s="10">
-        <v>17534709</v>
+        <v>18981224</v>
       </c>
       <c r="F18" s="10">
-        <v>19805266</v>
+        <v>19499363</v>
       </c>
       <c r="G18" s="10">
-        <v>34284</v>
+        <v>33687</v>
       </c>
       <c r="H18" s="10">
-        <v>126740</v>
+        <v>140860</v>
       </c>
       <c r="I18" s="17">
-        <f t="shared" si="1"/>
-        <v>1168.9806000000001</v>
+        <f t="shared" si="11"/>
+        <v>1265.4149333333332</v>
       </c>
       <c r="J18" s="18">
-        <f t="shared" si="2"/>
-        <v>97.850399999999993</v>
+        <f t="shared" si="12"/>
+        <v>105.81606666666667</v>
       </c>
       <c r="K18" s="17">
-        <f t="shared" si="3"/>
-        <v>1320.3510666666666</v>
+        <f t="shared" si="13"/>
+        <v>1299.9575333333332</v>
       </c>
       <c r="L18" s="18">
-        <f t="shared" si="4"/>
-        <v>0.88535589474031817</v>
+        <f t="shared" si="14"/>
+        <v>0.97342790120887535</v>
       </c>
       <c r="M18" s="18">
-        <f t="shared" si="5"/>
-        <v>7.410938080811437E-2</v>
+        <f t="shared" si="15"/>
+        <v>8.1399633413665878E-2</v>
       </c>
       <c r="N18" s="13"/>
       <c r="O18" s="13">
-        <v>2.0669999999999998E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="P18" s="13">
-        <v>0.266067</v>
+        <v>0.25640000000000002</v>
       </c>
       <c r="Q18" s="13">
-        <v>0.80320000000000003</v>
+        <v>0.78226700000000005</v>
       </c>
       <c r="R18" s="13">
-        <v>0.97426699999999999</v>
+        <v>0.97246699999999997</v>
       </c>
       <c r="S18" s="13">
-        <v>0.99760000000000004</v>
+        <v>0.99746699999999999</v>
       </c>
       <c r="T18" s="13">
-        <v>0.99993299999999996</v>
+        <v>1</v>
       </c>
       <c r="U18" s="13">
         <v>1</v>
@@ -5421,7 +5530,7 @@
         <v>12</v>
       </c>
       <c r="AB18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:28">
@@ -5432,58 +5541,43 @@
         <v>4992</v>
       </c>
       <c r="D19" s="16">
-        <v>1102944</v>
+        <v>1144277</v>
       </c>
       <c r="E19" s="16">
-        <v>13103064</v>
+        <v>13574233</v>
       </c>
       <c r="F19" s="16">
-        <v>8837876</v>
+        <v>9309472</v>
       </c>
       <c r="G19" s="16">
-        <v>48138</v>
+        <v>51209</v>
       </c>
       <c r="H19" s="16">
-        <v>156316</v>
-      </c>
-      <c r="I19" s="17">
-        <f t="shared" si="1"/>
-        <v>2624.8125</v>
-      </c>
-      <c r="J19" s="18">
-        <f t="shared" si="2"/>
-        <v>220.94230769230768</v>
-      </c>
-      <c r="K19" s="17">
-        <f t="shared" si="3"/>
-        <v>1770.4078525641025</v>
-      </c>
-      <c r="L19" s="18">
-        <f t="shared" si="4"/>
-        <v>1.4826032861289296</v>
-      </c>
-      <c r="M19" s="18">
-        <f t="shared" si="5"/>
-        <v>0.124797406073586</v>
-      </c>
+        <v>159256</v>
+      </c>
+      <c r="I19" s="17"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
       <c r="N19" s="13"/>
       <c r="O19" s="19">
-        <v>2.1635000000000001E-2</v>
+        <v>4.2067E-2</v>
       </c>
       <c r="P19" s="19">
-        <v>0.52443899999999999</v>
+        <v>0.57211500000000004</v>
       </c>
       <c r="Q19" s="19">
-        <v>0.93309299999999995</v>
+        <v>0.93429499999999999</v>
       </c>
       <c r="R19" s="19">
-        <v>0.99338899999999997</v>
+        <v>0.99419100000000005</v>
       </c>
       <c r="S19" s="19">
-        <v>0.99899800000000005</v>
+        <v>0.99859799999999999</v>
       </c>
       <c r="T19" s="19">
-        <v>1</v>
+        <v>0.99980000000000002</v>
       </c>
       <c r="U19" s="13">
         <v>1</v>
@@ -5507,7 +5601,7 @@
         <v>12</v>
       </c>
       <c r="AB19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="2:28">
@@ -5518,52 +5612,37 @@
         <v>996</v>
       </c>
       <c r="D20" s="10">
-        <v>3164522</v>
+        <v>3271445</v>
       </c>
       <c r="E20" s="10">
-        <v>37381349</v>
+        <v>38366544</v>
       </c>
       <c r="F20" s="10">
-        <v>1866432</v>
+        <v>1942471</v>
       </c>
       <c r="G20" s="10">
-        <v>51163</v>
+        <v>53842</v>
       </c>
       <c r="H20" s="10">
-        <v>129084</v>
-      </c>
-      <c r="I20" s="17">
-        <f t="shared" si="1"/>
-        <v>37531.47489959839</v>
-      </c>
-      <c r="J20" s="18">
-        <f t="shared" si="2"/>
-        <v>3177.230923694779</v>
-      </c>
-      <c r="K20" s="17">
-        <f t="shared" si="3"/>
-        <v>1873.9277108433735</v>
-      </c>
-      <c r="L20" s="18">
-        <f t="shared" si="4"/>
-        <v>20.028240514521823</v>
-      </c>
-      <c r="M20" s="18">
-        <f t="shared" si="5"/>
-        <v>1.695492790522237</v>
-      </c>
+        <v>153196</v>
+      </c>
+      <c r="I20" s="17"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
       <c r="N20" s="13"/>
       <c r="O20" s="13">
-        <v>1.7068E-2</v>
+        <v>5.5220999999999999E-2</v>
       </c>
       <c r="P20" s="13">
-        <v>0.59036100000000002</v>
+        <v>0.59738999999999998</v>
       </c>
       <c r="Q20" s="13">
-        <v>0.94779100000000005</v>
+        <v>0.95281099999999996</v>
       </c>
       <c r="R20" s="13">
-        <v>0.99497999999999998</v>
+        <v>0.998996</v>
       </c>
       <c r="S20" s="13">
         <v>1</v>
@@ -5593,7 +5672,69 @@
         <v>12</v>
       </c>
       <c r="AB20" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:28">
+      <c r="G22" s="24">
+        <f>SUM(G15:G20)</f>
+        <v>203974</v>
+      </c>
+      <c r="H22" s="24">
+        <f>SUM(H15:H20)</f>
+        <v>733848</v>
+      </c>
+      <c r="M22" s="32">
+        <f>SUM(M15:M20)</f>
+        <v>9.0783154674781874E-2</v>
+      </c>
+      <c r="N22" s="26">
+        <f>SUM(N15:N20)/6</f>
+        <v>0</v>
+      </c>
+      <c r="O22" s="26">
+        <f>SUM(O15:O20)/6</f>
+        <v>1.7021333333333333E-2</v>
+      </c>
+      <c r="P22" s="26">
+        <f t="shared" ref="P22:Y22" si="16">SUM(P15:P20)/6</f>
+        <v>0.27878316666666669</v>
+      </c>
+      <c r="Q22" s="33">
+        <f t="shared" si="16"/>
+        <v>0.67804549999999997</v>
+      </c>
+      <c r="R22" s="26">
+        <f t="shared" si="16"/>
+        <v>0.91235733333333335</v>
+      </c>
+      <c r="S22" s="26">
+        <f t="shared" si="16"/>
+        <v>0.9835976666666667</v>
+      </c>
+      <c r="T22" s="26">
+        <f t="shared" si="16"/>
+        <v>0.99773699999999999</v>
+      </c>
+      <c r="U22" s="26">
+        <f t="shared" si="16"/>
+        <v>0.99978566666666657</v>
+      </c>
+      <c r="V22" s="26">
+        <f t="shared" si="16"/>
+        <v>0.99999400000000005</v>
+      </c>
+      <c r="W22" s="26">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="X22" s="26">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="Y22" s="26">
+        <f t="shared" si="16"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to version 2.3.16
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="47020" windowHeight="18620" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="47020" windowHeight="18620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Random7" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="27">
   <si>
     <t>Method</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>2.3.13</t>
+  </si>
+  <si>
+    <t>2.3.15</t>
   </si>
 </sst>
 </file>
@@ -309,7 +312,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="531">
+  <cellStyleXfs count="539">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -841,8 +844,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -893,6 +904,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -907,8 +926,17 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="531">
+  <cellStyles count="539">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1174,6 +1202,10 @@
     <cellStyle name="Followed Hyperlink" xfId="526" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="528" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="530" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="532" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="534" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="536" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="538" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1439,19 +1471,13 @@
     <cellStyle name="Hyperlink" xfId="525" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="527" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="529" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="531" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="533" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="535" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="537" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1789,10 +1815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC61"/>
+  <dimension ref="A1:AE62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1804,13 +1830,13 @@
     <col min="8" max="8" width="10.6640625" customWidth="1"/>
     <col min="10" max="10" width="14.6640625" customWidth="1"/>
     <col min="12" max="12" width="13.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12.1640625" customWidth="1"/>
-    <col min="14" max="25" width="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="25.1640625" customWidth="1"/>
-    <col min="27" max="27" width="8.5" customWidth="1"/>
+    <col min="13" max="15" width="12.1640625" customWidth="1"/>
+    <col min="16" max="27" width="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="25.1640625" customWidth="1"/>
+    <col min="29" max="29" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:31">
       <c r="A1" s="21" t="s">
         <v>18</v>
       </c>
@@ -1826,24 +1852,26 @@
       <c r="K1" s="22"/>
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
-      <c r="N1" s="28" t="s">
+      <c r="N1" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-    </row>
-    <row r="2" spans="1:29" s="1" customFormat="1" ht="56" customHeight="1">
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="42"/>
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+    </row>
+    <row r="2" spans="1:31" s="1" customFormat="1" ht="56" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1884,52 +1912,60 @@
         <v>19</v>
       </c>
       <c r="N2" s="7">
+        <f>O2*2</f>
+        <v>65536</v>
+      </c>
+      <c r="O2" s="7">
+        <f>P2*2</f>
+        <v>32768</v>
+      </c>
+      <c r="P2" s="7">
         <v>16384</v>
       </c>
-      <c r="O2" s="7">
+      <c r="Q2" s="7">
         <v>8192</v>
       </c>
-      <c r="P2" s="7">
+      <c r="R2" s="7">
         <v>4096</v>
       </c>
-      <c r="Q2" s="34">
+      <c r="S2" s="40">
         <v>2048</v>
       </c>
-      <c r="R2" s="7">
+      <c r="T2" s="7">
         <v>1024</v>
       </c>
-      <c r="S2" s="7">
+      <c r="U2" s="7">
         <v>512</v>
       </c>
-      <c r="T2" s="7">
+      <c r="V2" s="7">
         <v>256</v>
       </c>
-      <c r="U2" s="7">
+      <c r="W2" s="7">
         <v>128</v>
       </c>
-      <c r="V2" s="7">
+      <c r="X2" s="7">
         <v>64</v>
       </c>
-      <c r="W2" s="7">
+      <c r="Y2" s="7">
         <v>32</v>
       </c>
-      <c r="X2" s="7">
+      <c r="Z2" s="7">
         <v>16</v>
       </c>
-      <c r="Y2" s="7">
+      <c r="AA2" s="7">
         <v>8</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="AB2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="AA2" s="8" t="s">
+      <c r="AC2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="AB2" s="8" t="s">
+      <c r="AD2" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:31">
       <c r="A3" s="15" t="s">
         <v>6</v>
       </c>
@@ -1974,43 +2010,45 @@
         <f>J3/K3</f>
         <v>6.0350067404395524E-3</v>
       </c>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
       <c r="P3" s="19"/>
       <c r="Q3" s="19"/>
       <c r="R3" s="19"/>
-      <c r="S3" s="19">
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="19">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="T3" s="19">
+      <c r="V3" s="19">
         <v>5.0369999999999998E-2</v>
       </c>
-      <c r="U3" s="19">
+      <c r="W3" s="19">
         <v>0.45832000000000001</v>
       </c>
-      <c r="V3" s="19">
+      <c r="X3" s="19">
         <v>0.89120999999999995</v>
       </c>
-      <c r="W3" s="19">
+      <c r="Y3" s="19">
         <v>0.99451999999999996</v>
       </c>
-      <c r="X3" s="19">
+      <c r="Z3" s="19">
         <v>0.99992999999999999</v>
       </c>
-      <c r="Y3" s="14">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="15" t="s">
+      <c r="AA3" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AA3" s="15">
+      <c r="AC3" s="15">
         <v>6</v>
       </c>
-      <c r="AB3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" ht="17">
+      <c r="AD3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" ht="17">
       <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
@@ -2055,65 +2093,69 @@
         <f t="shared" ref="M4" si="4">J4/K4</f>
         <v>2.8283929002132571E-3</v>
       </c>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
-      <c r="R4" s="13">
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13">
         <v>3.3500000000000001E-3</v>
       </c>
-      <c r="S4" s="13">
+      <c r="U4" s="13">
         <v>0.13125999999999999</v>
       </c>
-      <c r="T4" s="13">
+      <c r="V4" s="13">
         <v>0.58604000000000001</v>
       </c>
-      <c r="U4" s="13">
+      <c r="W4" s="13">
         <v>0.91791</v>
       </c>
-      <c r="V4" s="13">
+      <c r="X4" s="13">
         <v>0.99351999999999996</v>
       </c>
-      <c r="W4" s="13">
+      <c r="Y4" s="13">
         <v>0.99995000000000001</v>
       </c>
-      <c r="X4" s="14">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="14">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="9" t="s">
+      <c r="Z4" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AA4" s="9">
+      <c r="AC4" s="9">
         <v>6</v>
       </c>
-      <c r="AB4">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="20"/>
-    </row>
-    <row r="5" spans="1:29">
+      <c r="AD4">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="20"/>
+    </row>
+    <row r="5" spans="1:31">
       <c r="C5" s="24"/>
     </row>
-    <row r="6" spans="1:29">
-      <c r="N6" s="28" t="s">
+    <row r="6" spans="1:31">
+      <c r="N6" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="28"/>
-      <c r="U6" s="28"/>
-      <c r="V6" s="28"/>
-      <c r="W6" s="28"/>
-      <c r="X6" s="28"/>
-      <c r="Y6" s="28"/>
-    </row>
-    <row r="7" spans="1:29" ht="45">
+      <c r="O6" s="42"/>
+      <c r="P6" s="42"/>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="42"/>
+      <c r="S6" s="42"/>
+      <c r="T6" s="42"/>
+      <c r="U6" s="42"/>
+      <c r="V6" s="42"/>
+      <c r="W6" s="42"/>
+      <c r="X6" s="42"/>
+      <c r="Y6" s="42"/>
+      <c r="Z6" s="42"/>
+      <c r="AA6" s="43"/>
+    </row>
+    <row r="7" spans="1:31" ht="45">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -2154,53 +2196,61 @@
         <v>19</v>
       </c>
       <c r="N7" s="7">
+        <f>O7*2</f>
+        <v>65536</v>
+      </c>
+      <c r="O7" s="7">
+        <f>P7*2</f>
+        <v>32768</v>
+      </c>
+      <c r="P7" s="7">
         <v>16384</v>
       </c>
-      <c r="O7" s="7">
+      <c r="Q7" s="7">
         <v>8192</v>
       </c>
-      <c r="P7" s="7">
+      <c r="R7" s="7">
         <v>4096</v>
       </c>
-      <c r="Q7" s="34">
+      <c r="S7" s="40">
         <v>2048</v>
       </c>
-      <c r="R7" s="7">
+      <c r="T7" s="7">
         <v>1024</v>
       </c>
-      <c r="S7" s="7">
+      <c r="U7" s="7">
         <v>512</v>
       </c>
-      <c r="T7" s="7">
+      <c r="V7" s="7">
         <v>256</v>
       </c>
-      <c r="U7" s="7">
+      <c r="W7" s="7">
         <v>128</v>
       </c>
-      <c r="V7" s="7">
+      <c r="X7" s="7">
         <v>64</v>
       </c>
-      <c r="W7" s="7">
+      <c r="Y7" s="7">
         <v>32</v>
       </c>
-      <c r="X7" s="7">
+      <c r="Z7" s="7">
         <v>16</v>
       </c>
-      <c r="Y7" s="7">
+      <c r="AA7" s="7">
         <v>8</v>
       </c>
-      <c r="Z7" s="8" t="s">
+      <c r="AB7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="AA7" s="8" t="s">
+      <c r="AC7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="AB7" s="8" t="s">
+      <c r="AD7" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:31">
+      <c r="A8" s="36" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="15">
@@ -2210,84 +2260,71 @@
         <v>249996</v>
       </c>
       <c r="D8" s="16">
-        <v>90724</v>
+        <v>103529</v>
       </c>
       <c r="E8" s="16">
-        <v>956340</v>
+        <v>1103921</v>
       </c>
       <c r="F8" s="16">
-        <v>157127969</v>
+        <v>167078359</v>
       </c>
       <c r="G8" s="16">
-        <v>14041</v>
+        <v>15094</v>
       </c>
       <c r="H8" s="16">
-        <v>74592</v>
-      </c>
-      <c r="I8" s="17">
-        <f t="shared" ref="I8:I15" si="5">E8/C8</f>
-        <v>3.8254212067393079</v>
-      </c>
-      <c r="J8" s="18">
-        <f t="shared" ref="J8:J15" si="6">D8/C8</f>
-        <v>0.36290180642890285</v>
-      </c>
-      <c r="K8" s="17">
-        <f t="shared" ref="K8:K15" si="7">F8/C8</f>
-        <v>628.52193235091761</v>
-      </c>
-      <c r="L8" s="18">
-        <f t="shared" ref="L8:L15" si="8">I8/K8</f>
-        <v>6.0863766399220755E-3</v>
-      </c>
-      <c r="M8" s="18">
-        <f t="shared" ref="M8:M15" si="9">J8/K8</f>
-        <v>5.7738924888668295E-4</v>
-      </c>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="19">
-        <v>5.5960000000000003E-3</v>
-      </c>
-      <c r="Q8" s="19">
-        <v>0.22456400000000001</v>
-      </c>
+        <v>76776</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
       <c r="R8" s="19">
-        <v>0.67955900000000002</v>
+        <v>8.5400000000000007E-3</v>
       </c>
       <c r="S8" s="19">
-        <v>0.92228299999999996</v>
+        <v>0.25731599999999999</v>
       </c>
       <c r="T8" s="19">
-        <v>0.98658000000000001</v>
+        <v>0.720804</v>
       </c>
       <c r="U8" s="19">
-        <v>0.99839199999999995</v>
-      </c>
-      <c r="V8" s="13">
-        <v>0.99992000000000003</v>
-      </c>
-      <c r="W8" s="13">
-        <v>0.999996</v>
+        <v>0.93848299999999996</v>
+      </c>
+      <c r="V8" s="19">
+        <v>0.99029199999999995</v>
+      </c>
+      <c r="W8" s="19">
+        <v>0.99894400000000005</v>
       </c>
       <c r="X8" s="13">
-        <v>1</v>
+        <v>0.99996399999999996</v>
       </c>
       <c r="Y8" s="13">
         <v>1</v>
       </c>
-      <c r="Z8" s="15" t="s">
+      <c r="Z8" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AA8" s="15">
+      <c r="AC8" s="15">
         <v>12</v>
       </c>
-      <c r="AB8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29">
-      <c r="A9" s="31"/>
+      <c r="AD8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31">
+      <c r="A9" s="37"/>
       <c r="B9" s="9">
         <v>2</v>
       </c>
@@ -2295,65 +2332,46 @@
         <v>99996</v>
       </c>
       <c r="D9" s="10">
-        <v>209020</v>
+        <v>216248</v>
       </c>
       <c r="E9" s="10">
-        <v>2450523</v>
+        <v>2535625</v>
       </c>
       <c r="F9" s="10">
-        <v>77155678</v>
+        <v>81413133</v>
       </c>
       <c r="G9" s="10">
-        <v>17973</v>
+        <v>19173</v>
       </c>
       <c r="H9" s="10">
-        <v>76316</v>
-      </c>
-      <c r="I9" s="17">
-        <f t="shared" si="5"/>
-        <v>24.506210248409936</v>
-      </c>
-      <c r="J9" s="18">
-        <f t="shared" si="6"/>
-        <v>2.0902836113444536</v>
-      </c>
-      <c r="K9" s="17">
-        <f t="shared" si="7"/>
-        <v>771.58764350574017</v>
-      </c>
-      <c r="L9" s="18">
-        <f t="shared" si="8"/>
-        <v>3.176076036814815E-2</v>
-      </c>
-      <c r="M9" s="18">
-        <f t="shared" si="9"/>
-        <v>2.7090682814037356E-3</v>
-      </c>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13">
-        <v>2.2641000000000001E-2</v>
-      </c>
-      <c r="Q9" s="13">
-        <v>0.36367500000000003</v>
-      </c>
+        <v>76940</v>
+      </c>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
       <c r="R9" s="13">
-        <v>0.80291199999999996</v>
+        <v>2.9940999999999999E-2</v>
       </c>
       <c r="S9" s="13">
-        <v>0.96508899999999997</v>
+        <v>0.40700599999999998</v>
       </c>
       <c r="T9" s="13">
-        <v>0.99582000000000004</v>
+        <v>0.83407299999999995</v>
       </c>
       <c r="U9" s="13">
-        <v>0.99972000000000005</v>
+        <v>0.97155899999999995</v>
       </c>
       <c r="V9" s="13">
-        <v>0.99997999999999998</v>
+        <v>0.99673</v>
       </c>
       <c r="W9" s="13">
-        <v>1</v>
+        <v>0.99977000000000005</v>
       </c>
       <c r="X9" s="13">
         <v>1</v>
@@ -2361,18 +2379,24 @@
       <c r="Y9" s="13">
         <v>1</v>
       </c>
-      <c r="Z9" s="15" t="s">
+      <c r="Z9" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AA9" s="15">
+      <c r="AC9" s="15">
         <v>12</v>
       </c>
-      <c r="AB9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29">
-      <c r="A10" s="31"/>
+      <c r="AD9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31">
+      <c r="A10" s="37"/>
       <c r="B10" s="15">
         <v>3</v>
       </c>
@@ -2380,66 +2404,47 @@
         <v>49992</v>
       </c>
       <c r="D10" s="16">
-        <v>353406</v>
+        <v>369062</v>
       </c>
       <c r="E10" s="16">
-        <v>4193112</v>
+        <v>4370251</v>
       </c>
       <c r="F10" s="16">
-        <v>60678611</v>
+        <v>60425721</v>
       </c>
       <c r="G10" s="16">
-        <v>31088</v>
+        <v>30969</v>
       </c>
       <c r="H10" s="16">
-        <v>126976</v>
-      </c>
-      <c r="I10" s="17">
-        <f t="shared" si="5"/>
-        <v>83.875660105616902</v>
-      </c>
-      <c r="J10" s="18">
-        <f t="shared" si="6"/>
-        <v>7.0692510801728279</v>
-      </c>
-      <c r="K10" s="17">
-        <f t="shared" si="7"/>
-        <v>1213.7664226276204</v>
-      </c>
-      <c r="L10" s="18">
-        <f t="shared" si="8"/>
-        <v>6.9103625328536283E-2</v>
-      </c>
-      <c r="M10" s="18">
-        <f t="shared" si="9"/>
-        <v>5.8242269256954483E-3</v>
-      </c>
-      <c r="N10" s="13"/>
-      <c r="O10" s="19">
-        <v>1.24E-3</v>
-      </c>
-      <c r="P10" s="19">
-        <v>0.209173</v>
-      </c>
+        <v>126820</v>
+      </c>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="13"/>
       <c r="Q10" s="19">
-        <v>0.74427900000000002</v>
+        <v>1.8400000000000001E-3</v>
       </c>
       <c r="R10" s="19">
-        <v>0.95561300000000005</v>
+        <v>0.208313</v>
       </c>
       <c r="S10" s="19">
-        <v>0.99503900000000001</v>
+        <v>0.73457799999999995</v>
       </c>
       <c r="T10" s="19">
-        <v>0.99968000000000001</v>
+        <v>0.95361300000000004</v>
       </c>
       <c r="U10" s="19">
-        <v>1</v>
-      </c>
-      <c r="V10" s="13">
-        <v>1</v>
-      </c>
-      <c r="W10" s="13">
+        <v>0.995479</v>
+      </c>
+      <c r="V10" s="19">
+        <v>0.99960000000000004</v>
+      </c>
+      <c r="W10" s="19">
         <v>1</v>
       </c>
       <c r="X10" s="13">
@@ -2448,18 +2453,24 @@
       <c r="Y10" s="13">
         <v>1</v>
       </c>
-      <c r="Z10" s="15" t="s">
+      <c r="Z10" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AA10" s="15">
+      <c r="AC10" s="15">
         <v>12</v>
       </c>
-      <c r="AB10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29">
-      <c r="A11" s="31"/>
+      <c r="AD10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31">
+      <c r="A11" s="37"/>
       <c r="B11" s="9">
         <v>4</v>
       </c>
@@ -2467,61 +2478,42 @@
         <v>15000</v>
       </c>
       <c r="D11" s="10">
-        <v>1467756</v>
+        <v>1587241</v>
       </c>
       <c r="E11" s="10">
-        <v>17534709</v>
+        <v>18981224</v>
       </c>
       <c r="F11" s="10">
-        <v>19805266</v>
+        <v>19499363</v>
       </c>
       <c r="G11" s="10">
-        <v>34284</v>
+        <v>33687</v>
       </c>
       <c r="H11" s="10">
-        <v>126740</v>
-      </c>
-      <c r="I11" s="17">
-        <f t="shared" si="5"/>
-        <v>1168.9806000000001</v>
-      </c>
-      <c r="J11" s="18">
-        <f t="shared" si="6"/>
-        <v>97.850399999999993</v>
-      </c>
-      <c r="K11" s="17">
-        <f t="shared" si="7"/>
-        <v>1320.3510666666666</v>
-      </c>
-      <c r="L11" s="18">
-        <f t="shared" si="8"/>
-        <v>0.88535589474031817</v>
-      </c>
-      <c r="M11" s="18">
-        <f t="shared" si="9"/>
-        <v>7.410938080811437E-2</v>
-      </c>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13">
-        <v>2.0669999999999998E-3</v>
-      </c>
-      <c r="P11" s="13">
-        <v>0.266067</v>
-      </c>
+        <v>140860</v>
+      </c>
+      <c r="I11" s="17"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="13"/>
       <c r="Q11" s="13">
-        <v>0.80320000000000003</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="R11" s="13">
-        <v>0.97426699999999999</v>
+        <v>0.25640000000000002</v>
       </c>
       <c r="S11" s="13">
-        <v>0.99760000000000004</v>
+        <v>0.78226700000000005</v>
       </c>
       <c r="T11" s="13">
-        <v>0.99993299999999996</v>
+        <v>0.97246699999999997</v>
       </c>
       <c r="U11" s="13">
-        <v>1</v>
+        <v>0.99746699999999999</v>
       </c>
       <c r="V11" s="13">
         <v>1</v>
@@ -2535,18 +2527,24 @@
       <c r="Y11" s="13">
         <v>1</v>
       </c>
-      <c r="Z11" s="15" t="s">
+      <c r="Z11" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AA11" s="15">
+      <c r="AC11" s="15">
         <v>12</v>
       </c>
-      <c r="AB11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29">
-      <c r="A12" s="31"/>
+      <c r="AD11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31">
+      <c r="A12" s="37"/>
       <c r="B12" s="15">
         <v>5</v>
       </c>
@@ -2554,63 +2552,44 @@
         <v>4992</v>
       </c>
       <c r="D12" s="16">
-        <v>1102944</v>
+        <v>1218639</v>
       </c>
       <c r="E12" s="16">
-        <v>13103064</v>
+        <v>14236601</v>
       </c>
       <c r="F12" s="16">
-        <v>8837876</v>
+        <v>9266692</v>
       </c>
       <c r="G12" s="16">
-        <v>48138</v>
+        <v>50922</v>
       </c>
       <c r="H12" s="16">
-        <v>156316</v>
-      </c>
-      <c r="I12" s="17">
-        <f t="shared" si="5"/>
-        <v>2624.8125</v>
-      </c>
-      <c r="J12" s="18">
-        <f t="shared" si="6"/>
-        <v>220.94230769230768</v>
-      </c>
-      <c r="K12" s="17">
-        <f t="shared" si="7"/>
-        <v>1770.4078525641025</v>
-      </c>
-      <c r="L12" s="18">
-        <f t="shared" si="8"/>
-        <v>1.4826032861289296</v>
-      </c>
-      <c r="M12" s="18">
-        <f t="shared" si="9"/>
-        <v>0.124797406073586</v>
-      </c>
-      <c r="N12" s="13"/>
-      <c r="O12" s="19">
-        <v>2.1635000000000001E-2</v>
-      </c>
-      <c r="P12" s="19">
-        <v>0.52443899999999999</v>
-      </c>
+        <v>163604</v>
+      </c>
+      <c r="I12" s="17"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="13"/>
       <c r="Q12" s="19">
-        <v>0.93309299999999995</v>
+        <v>4.0264000000000001E-2</v>
       </c>
       <c r="R12" s="19">
-        <v>0.99338899999999997</v>
+        <v>0.56630599999999998</v>
       </c>
       <c r="S12" s="19">
-        <v>0.99899800000000005</v>
+        <v>0.93429499999999999</v>
       </c>
       <c r="T12" s="19">
-        <v>1</v>
-      </c>
-      <c r="U12" s="13">
-        <v>1</v>
-      </c>
-      <c r="V12" s="13">
+        <v>0.99378999999999995</v>
+      </c>
+      <c r="U12" s="19">
+        <v>0.99959900000000002</v>
+      </c>
+      <c r="V12" s="19">
         <v>1</v>
       </c>
       <c r="W12" s="13">
@@ -2622,18 +2601,24 @@
       <c r="Y12" s="13">
         <v>1</v>
       </c>
-      <c r="Z12" s="15" t="s">
+      <c r="Z12" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AA12" s="15">
+      <c r="AC12" s="15">
         <v>12</v>
       </c>
-      <c r="AB12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29">
-      <c r="A13" s="31"/>
+      <c r="AD12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31">
+      <c r="A13" s="37"/>
       <c r="B13" s="9">
         <v>6</v>
       </c>
@@ -2641,58 +2626,39 @@
         <v>996</v>
       </c>
       <c r="D13" s="10">
-        <v>3164522</v>
+        <v>2518431</v>
       </c>
       <c r="E13" s="10">
-        <v>37381349</v>
+        <v>29063720</v>
       </c>
       <c r="F13" s="10">
-        <v>1866432</v>
+        <v>1956400</v>
       </c>
       <c r="G13" s="10">
-        <v>51163</v>
+        <v>54162</v>
       </c>
       <c r="H13" s="10">
-        <v>129084</v>
-      </c>
-      <c r="I13" s="17">
-        <f t="shared" si="5"/>
-        <v>37531.47489959839</v>
-      </c>
-      <c r="J13" s="18">
-        <f t="shared" si="6"/>
-        <v>3177.230923694779</v>
-      </c>
-      <c r="K13" s="17">
-        <f t="shared" si="7"/>
-        <v>1873.9277108433735</v>
-      </c>
-      <c r="L13" s="18">
-        <f t="shared" si="8"/>
-        <v>20.028240514521823</v>
-      </c>
-      <c r="M13" s="18">
-        <f t="shared" si="9"/>
-        <v>1.695492790522237</v>
-      </c>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13">
-        <v>1.7068E-2</v>
-      </c>
-      <c r="P13" s="13">
-        <v>0.59036100000000002</v>
-      </c>
+        <v>156328</v>
+      </c>
+      <c r="I13" s="17"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="13"/>
       <c r="Q13" s="13">
-        <v>0.94779100000000005</v>
+        <v>4.7189000000000002E-2</v>
       </c>
       <c r="R13" s="13">
-        <v>0.99497999999999998</v>
+        <v>0.61746999999999996</v>
       </c>
       <c r="S13" s="13">
-        <v>1</v>
+        <v>0.95582299999999998</v>
       </c>
       <c r="T13" s="13">
-        <v>1</v>
+        <v>0.998996</v>
       </c>
       <c r="U13" s="13">
         <v>1</v>
@@ -2709,18 +2675,24 @@
       <c r="Y13" s="13">
         <v>1</v>
       </c>
-      <c r="Z13" s="15" t="s">
+      <c r="Z13" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AA13" s="15">
+      <c r="AC13" s="15">
         <v>12</v>
       </c>
-      <c r="AB13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29">
-      <c r="A14" s="31"/>
+      <c r="AD13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31">
+      <c r="A14" s="37"/>
       <c r="B14" s="15">
         <v>7</v>
       </c>
@@ -2728,59 +2700,42 @@
         <v>744</v>
       </c>
       <c r="D14" s="16">
-        <v>4750574</v>
+        <v>9122650</v>
       </c>
       <c r="E14" s="16">
-        <v>54347580</v>
+        <v>108421688</v>
       </c>
       <c r="F14" s="16">
-        <v>1645010</v>
+        <v>1744569</v>
       </c>
       <c r="G14" s="16">
-        <v>62015</v>
+        <v>66689</v>
       </c>
       <c r="H14" s="16">
-        <v>158724</v>
-      </c>
-      <c r="I14" s="17">
-        <f t="shared" si="5"/>
-        <v>73047.822580645166</v>
-      </c>
-      <c r="J14" s="18">
-        <f t="shared" si="6"/>
-        <v>6385.1801075268813</v>
-      </c>
-      <c r="K14" s="17">
-        <f t="shared" si="7"/>
-        <v>2211.0349462365593</v>
-      </c>
-      <c r="L14" s="18">
-        <f t="shared" si="8"/>
-        <v>33.037841715247929</v>
-      </c>
-      <c r="M14" s="18">
-        <f t="shared" si="9"/>
-        <v>2.8878693746542572</v>
-      </c>
-      <c r="N14" s="13"/>
-      <c r="O14" s="19">
-        <v>8.7365999999999999E-2</v>
-      </c>
-      <c r="P14" s="19">
-        <v>0.72177400000000003</v>
+        <v>252016</v>
+      </c>
+      <c r="I14" s="17"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="13">
+        <v>1.3439999999999999E-3</v>
       </c>
       <c r="Q14" s="19">
-        <v>0.97983900000000002</v>
+        <v>0.13978499999999999</v>
       </c>
       <c r="R14" s="19">
+        <v>0.77688199999999996</v>
+      </c>
+      <c r="S14" s="19">
+        <v>0.97715099999999999</v>
+      </c>
+      <c r="T14" s="19">
         <v>0.99865599999999999</v>
       </c>
-      <c r="S14" s="19">
-        <v>1</v>
-      </c>
-      <c r="T14" s="19">
-        <v>1</v>
-      </c>
       <c r="U14" s="19">
         <v>1</v>
       </c>
@@ -2796,18 +2751,24 @@
       <c r="Y14" s="19">
         <v>1</v>
       </c>
-      <c r="Z14" s="15" t="s">
+      <c r="Z14" s="19">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="19">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AA14" s="15">
+      <c r="AC14" s="15">
         <v>12</v>
       </c>
-      <c r="AB14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29">
-      <c r="A15" s="31"/>
+      <c r="AD14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31">
+      <c r="A15" s="37"/>
       <c r="B15" s="9">
         <v>8</v>
       </c>
@@ -2815,1225 +2776,1275 @@
         <v>240</v>
       </c>
       <c r="D15" s="10">
-        <v>22500122</v>
+        <v>21558313</v>
       </c>
       <c r="E15" s="10">
-        <v>262990345</v>
+        <v>249134375</v>
       </c>
       <c r="F15" s="10">
-        <v>554197</v>
+        <v>565306</v>
       </c>
       <c r="G15" s="10">
-        <v>65360</v>
+        <v>66546</v>
       </c>
       <c r="H15" s="10">
-        <v>141960</v>
-      </c>
-      <c r="I15" s="17">
+        <v>164996</v>
+      </c>
+      <c r="I15" s="17"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13">
+        <v>9.5833000000000002E-2</v>
+      </c>
+      <c r="R15" s="13">
+        <v>0.80833299999999997</v>
+      </c>
+      <c r="S15" s="13">
+        <v>0.98333300000000001</v>
+      </c>
+      <c r="T15" s="13">
+        <v>1</v>
+      </c>
+      <c r="U15" s="13">
+        <v>1</v>
+      </c>
+      <c r="V15" s="13">
+        <v>1</v>
+      </c>
+      <c r="W15" s="13">
+        <v>1</v>
+      </c>
+      <c r="X15" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC15" s="9">
+        <v>12</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31">
+      <c r="A16" s="30"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="44"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
+      <c r="T16" s="45"/>
+      <c r="U16" s="45"/>
+      <c r="V16" s="45"/>
+      <c r="W16" s="45"/>
+      <c r="X16" s="45"/>
+      <c r="Y16" s="45"/>
+      <c r="Z16" s="45"/>
+      <c r="AA16" s="46"/>
+      <c r="AB16" s="35"/>
+      <c r="AC16" s="31"/>
+    </row>
+    <row r="17" spans="1:31">
+      <c r="N17" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="O17" s="42"/>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="42"/>
+      <c r="R17" s="42"/>
+      <c r="S17" s="42"/>
+      <c r="T17" s="42"/>
+      <c r="U17" s="42"/>
+      <c r="V17" s="42"/>
+      <c r="W17" s="42"/>
+      <c r="X17" s="42"/>
+      <c r="Y17" s="42"/>
+      <c r="Z17" s="42"/>
+      <c r="AA17" s="43"/>
+    </row>
+    <row r="18" spans="1:31" ht="45">
+      <c r="A18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N18" s="7">
+        <f>O18*2</f>
+        <v>65536</v>
+      </c>
+      <c r="O18" s="7">
+        <f>P18*2</f>
+        <v>32768</v>
+      </c>
+      <c r="P18" s="7">
+        <v>16384</v>
+      </c>
+      <c r="Q18" s="7">
+        <v>8192</v>
+      </c>
+      <c r="R18" s="7">
+        <v>4096</v>
+      </c>
+      <c r="S18" s="40">
+        <v>2048</v>
+      </c>
+      <c r="T18" s="7">
+        <v>1024</v>
+      </c>
+      <c r="U18" s="7">
+        <v>512</v>
+      </c>
+      <c r="V18" s="7">
+        <v>256</v>
+      </c>
+      <c r="W18" s="7">
+        <v>128</v>
+      </c>
+      <c r="X18" s="7">
+        <v>64</v>
+      </c>
+      <c r="Y18" s="7">
+        <v>32</v>
+      </c>
+      <c r="Z18" s="7">
+        <v>16</v>
+      </c>
+      <c r="AA18" s="7">
+        <v>8</v>
+      </c>
+      <c r="AB18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD18" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31">
+      <c r="A19" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="15">
+        <v>100000</v>
+      </c>
+      <c r="D19" s="16">
+        <v>49893</v>
+      </c>
+      <c r="E19" s="16">
+        <v>213204</v>
+      </c>
+      <c r="F19" s="16">
+        <v>8267265</v>
+      </c>
+      <c r="G19" s="16">
+        <v>889</v>
+      </c>
+      <c r="H19" s="16">
+        <v>4984</v>
+      </c>
+      <c r="I19" s="17">
+        <f t="shared" ref="I19:I20" si="5">E19/C19</f>
+        <v>2.1320399999999999</v>
+      </c>
+      <c r="J19" s="18">
+        <f>D19/C19</f>
+        <v>0.49892999999999998</v>
+      </c>
+      <c r="K19" s="17">
+        <f t="shared" ref="K19:K20" si="6">F19/C19</f>
+        <v>82.672650000000004</v>
+      </c>
+      <c r="L19" s="18">
+        <f t="shared" ref="L19:L20" si="7">I19/K19</f>
+        <v>2.5788939873101924E-2</v>
+      </c>
+      <c r="M19" s="18">
+        <f>J19/K19</f>
+        <v>6.0350067404395524E-3</v>
+      </c>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="19">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="V19" s="19">
+        <v>5.0369999999999998E-2</v>
+      </c>
+      <c r="W19" s="19">
+        <v>0.45832000000000001</v>
+      </c>
+      <c r="X19" s="19">
+        <v>0.89120999999999995</v>
+      </c>
+      <c r="Y19" s="19">
+        <v>0.99451999999999996</v>
+      </c>
+      <c r="Z19" s="19">
+        <v>0.99992999999999999</v>
+      </c>
+      <c r="AA19" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB19" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC19" s="15">
+        <v>6</v>
+      </c>
+      <c r="AD19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" ht="17">
+      <c r="A20" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="9">
+        <v>100000</v>
+      </c>
+      <c r="D20" s="10">
+        <v>52160</v>
+      </c>
+      <c r="E20" s="10">
+        <v>229938</v>
+      </c>
+      <c r="F20" s="10">
+        <v>18441568</v>
+      </c>
+      <c r="G20" s="10">
+        <v>2726</v>
+      </c>
+      <c r="H20" s="10">
+        <v>15568</v>
+      </c>
+      <c r="I20" s="11">
         <f t="shared" si="5"/>
-        <v>1095793.1041666667</v>
-      </c>
-      <c r="J15" s="18">
+        <v>2.2993800000000002</v>
+      </c>
+      <c r="J20" s="12">
+        <f t="shared" ref="J20" si="8">D20/C20</f>
+        <v>0.52159999999999995</v>
+      </c>
+      <c r="K20" s="11">
         <f t="shared" si="6"/>
-        <v>93750.508333333331</v>
-      </c>
-      <c r="K15" s="17">
+        <v>184.41568000000001</v>
+      </c>
+      <c r="L20" s="12">
         <f t="shared" si="7"/>
-        <v>2309.1541666666667</v>
-      </c>
-      <c r="L15" s="18">
-        <f t="shared" si="8"/>
-        <v>474.5430686200034</v>
-      </c>
-      <c r="M15" s="18">
-        <f t="shared" si="9"/>
-        <v>40.599501621264636</v>
-      </c>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13">
-        <v>0.129167</v>
-      </c>
-      <c r="P15" s="13">
+        <v>1.2468462551557438E-2</v>
+      </c>
+      <c r="M20" s="12">
+        <f t="shared" ref="M20" si="9">J20/K20</f>
+        <v>2.8283929002132571E-3</v>
+      </c>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13">
+        <v>3.3500000000000001E-3</v>
+      </c>
+      <c r="U20" s="13">
+        <v>0.13125999999999999</v>
+      </c>
+      <c r="V20" s="13">
+        <v>0.58604000000000001</v>
+      </c>
+      <c r="W20" s="13">
+        <v>0.91791</v>
+      </c>
+      <c r="X20" s="13">
+        <v>0.99351999999999996</v>
+      </c>
+      <c r="Y20" s="13">
+        <v>0.99995000000000001</v>
+      </c>
+      <c r="Z20" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC20" s="9">
+        <v>6</v>
+      </c>
+      <c r="AD20">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="20"/>
+    </row>
+    <row r="21" spans="1:31">
+      <c r="A21" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="15">
+        <v>1</v>
+      </c>
+      <c r="C21" s="15">
+        <v>249984</v>
+      </c>
+      <c r="D21" s="16">
+        <v>75882</v>
+      </c>
+      <c r="E21" s="16">
+        <v>2266088</v>
+      </c>
+      <c r="F21" s="16">
+        <v>157011609</v>
+      </c>
+      <c r="G21" s="16">
+        <v>14025</v>
+      </c>
+      <c r="H21" s="16">
+        <v>73536</v>
+      </c>
+      <c r="I21" s="11">
+        <f t="shared" ref="I21:I26" si="10">E21/C21</f>
+        <v>9.0649321556579618</v>
+      </c>
+      <c r="J21" s="12">
+        <f t="shared" ref="J21:J26" si="11">D21/C21</f>
+        <v>0.30354742703533028</v>
+      </c>
+      <c r="K21" s="11">
+        <f t="shared" ref="K21:K26" si="12">F21/C21</f>
+        <v>628.08663354454688</v>
+      </c>
+      <c r="L21" s="12">
+        <f t="shared" ref="L21:L26" si="13">I21/K21</f>
+        <v>1.4432614342548389E-2</v>
+      </c>
+      <c r="M21" s="12">
+        <f t="shared" ref="M21:M26" si="14">J21/K21</f>
+        <v>4.8328910507502667E-4</v>
+      </c>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="19">
+        <v>5.9319999999999998E-3</v>
+      </c>
+      <c r="S21" s="19">
+        <v>0.221474</v>
+      </c>
+      <c r="T21" s="19">
+        <v>0.68030000000000002</v>
+      </c>
+      <c r="U21" s="19">
+        <v>0.92280300000000004</v>
+      </c>
+      <c r="V21" s="19">
+        <v>0.98709899999999995</v>
+      </c>
+      <c r="W21" s="19">
+        <v>0.99846800000000002</v>
+      </c>
+      <c r="X21" s="13">
+        <v>0.99994400000000006</v>
+      </c>
+      <c r="Y21" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC21" s="15">
+        <v>36</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31">
+      <c r="A22" s="37"/>
+      <c r="B22" s="9">
+        <v>2</v>
+      </c>
+      <c r="C22" s="9">
+        <v>99972</v>
+      </c>
+      <c r="D22" s="10">
+        <v>190395</v>
+      </c>
+      <c r="E22" s="10">
+        <v>6286075</v>
+      </c>
+      <c r="F22" s="10">
+        <v>77198157</v>
+      </c>
+      <c r="G22" s="10">
+        <v>17990</v>
+      </c>
+      <c r="H22" s="10">
+        <v>96020</v>
+      </c>
+      <c r="I22" s="11">
+        <f t="shared" si="10"/>
+        <v>62.878355939663109</v>
+      </c>
+      <c r="J22" s="12">
+        <f t="shared" si="11"/>
+        <v>1.9044832553114872</v>
+      </c>
+      <c r="K22" s="11">
+        <f t="shared" si="12"/>
+        <v>772.19778537990635</v>
+      </c>
+      <c r="L22" s="12">
+        <f t="shared" si="13"/>
+        <v>8.1427785899085656E-2</v>
+      </c>
+      <c r="M22" s="12">
+        <f t="shared" si="14"/>
+        <v>2.4663153551709792E-3</v>
+      </c>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R22" s="13">
+        <v>2.2556E-2</v>
+      </c>
+      <c r="S22" s="13">
+        <v>0.36591200000000002</v>
+      </c>
+      <c r="T22" s="13">
+        <v>0.80297499999999999</v>
+      </c>
+      <c r="U22" s="13">
+        <v>0.96620099999999998</v>
+      </c>
+      <c r="V22" s="13">
+        <v>0.99589899999999998</v>
+      </c>
+      <c r="W22" s="13">
+        <v>0.99960000000000004</v>
+      </c>
+      <c r="X22" s="13">
+        <v>0.99999000000000005</v>
+      </c>
+      <c r="Y22" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z22" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB22" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC22" s="15">
+        <v>36</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31">
+      <c r="A23" s="37"/>
+      <c r="B23" s="15">
+        <v>3</v>
+      </c>
+      <c r="C23" s="15">
+        <v>49968</v>
+      </c>
+      <c r="D23" s="16">
+        <v>156411</v>
+      </c>
+      <c r="E23" s="16">
+        <v>5427374</v>
+      </c>
+      <c r="F23" s="16">
+        <v>61104521</v>
+      </c>
+      <c r="G23" s="16">
+        <v>31364</v>
+      </c>
+      <c r="H23" s="16">
+        <v>124480</v>
+      </c>
+      <c r="I23" s="11">
+        <f t="shared" si="10"/>
+        <v>108.61699487672111</v>
+      </c>
+      <c r="J23" s="12">
+        <f t="shared" si="11"/>
+        <v>3.1302233429394812</v>
+      </c>
+      <c r="K23" s="11">
+        <f t="shared" si="12"/>
+        <v>1222.8730587576049</v>
+      </c>
+      <c r="L23" s="12">
+        <f t="shared" si="13"/>
+        <v>8.8821152857085653E-2</v>
+      </c>
+      <c r="M23" s="12">
+        <f t="shared" si="14"/>
+        <v>2.5597287637685595E-3</v>
+      </c>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="19">
+        <v>1.2409999999999999E-3</v>
+      </c>
+      <c r="R23" s="19">
+        <v>0.21503800000000001</v>
+      </c>
+      <c r="S23" s="19">
+        <v>0.74697800000000003</v>
+      </c>
+      <c r="T23" s="19">
+        <v>0.95771300000000004</v>
+      </c>
+      <c r="U23" s="19">
+        <v>0.99611799999999995</v>
+      </c>
+      <c r="V23" s="19">
+        <v>0.99975999999999998</v>
+      </c>
+      <c r="W23" s="19">
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="X23" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA23" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB23" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC23" s="15">
+        <v>36</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31">
+      <c r="A24" s="37"/>
+      <c r="B24" s="9">
+        <v>4</v>
+      </c>
+      <c r="C24" s="9">
+        <v>14976</v>
+      </c>
+      <c r="D24" s="10">
+        <v>1118075</v>
+      </c>
+      <c r="E24" s="10">
+        <v>39265635</v>
+      </c>
+      <c r="F24" s="10">
+        <v>19678039</v>
+      </c>
+      <c r="G24" s="10">
+        <v>34082</v>
+      </c>
+      <c r="H24" s="10">
+        <v>125044</v>
+      </c>
+      <c r="I24" s="11">
+        <f t="shared" si="10"/>
+        <v>2621.9040464743589</v>
+      </c>
+      <c r="J24" s="12">
+        <f t="shared" si="11"/>
+        <v>74.657785790598297</v>
+      </c>
+      <c r="K24" s="11">
+        <f t="shared" si="12"/>
+        <v>1313.9716212606838</v>
+      </c>
+      <c r="L24" s="12">
+        <f t="shared" si="13"/>
+        <v>1.9954038611266089</v>
+      </c>
+      <c r="M24" s="12">
+        <f t="shared" si="14"/>
+        <v>5.6818415696808004E-2</v>
+      </c>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13">
+        <v>2.003E-3</v>
+      </c>
+      <c r="R24" s="13">
+        <v>0.26155200000000001</v>
+      </c>
+      <c r="S24" s="13">
+        <v>0.79720899999999995</v>
+      </c>
+      <c r="T24" s="13">
+        <v>0.96975199999999995</v>
+      </c>
+      <c r="U24" s="13">
+        <v>0.99766299999999997</v>
+      </c>
+      <c r="V24" s="13">
+        <v>0.99993299999999996</v>
+      </c>
+      <c r="W24" s="13">
+        <v>1</v>
+      </c>
+      <c r="X24" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA24" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB24" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC24" s="15">
+        <v>36</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31">
+      <c r="A25" s="37"/>
+      <c r="B25" s="15">
+        <v>5</v>
+      </c>
+      <c r="C25" s="15">
+        <v>4968</v>
+      </c>
+      <c r="D25" s="16">
+        <v>569724</v>
+      </c>
+      <c r="E25" s="16">
+        <v>19821757</v>
+      </c>
+      <c r="F25" s="16">
+        <v>8705130</v>
+      </c>
+      <c r="G25" s="16">
+        <v>47595</v>
+      </c>
+      <c r="H25" s="16">
+        <v>129668</v>
+      </c>
+      <c r="I25" s="11">
+        <f t="shared" si="10"/>
+        <v>3989.8866747181964</v>
+      </c>
+      <c r="J25" s="12">
+        <f t="shared" si="11"/>
+        <v>114.67874396135265</v>
+      </c>
+      <c r="K25" s="11">
+        <f t="shared" si="12"/>
+        <v>1752.2403381642512</v>
+      </c>
+      <c r="L25" s="12">
+        <f t="shared" si="13"/>
+        <v>2.2770202168146829</v>
+      </c>
+      <c r="M25" s="12">
+        <f t="shared" si="14"/>
+        <v>6.5446926122872368E-2</v>
+      </c>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="19">
+        <v>2.5361999999999999E-2</v>
+      </c>
+      <c r="R25" s="19">
+        <v>0.51308399999999998</v>
+      </c>
+      <c r="S25" s="19">
+        <v>0.92290700000000003</v>
+      </c>
+      <c r="T25" s="19">
+        <v>0.99335700000000005</v>
+      </c>
+      <c r="U25" s="19">
+        <v>0.99939599999999995</v>
+      </c>
+      <c r="V25" s="19">
+        <v>1</v>
+      </c>
+      <c r="W25" s="13">
+        <v>1</v>
+      </c>
+      <c r="X25" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC25" s="15">
+        <v>36</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31">
+      <c r="A26" s="37"/>
+      <c r="B26" s="9">
+        <v>6</v>
+      </c>
+      <c r="C26" s="9">
+        <v>972</v>
+      </c>
+      <c r="D26" s="10">
+        <v>2332749</v>
+      </c>
+      <c r="E26" s="10">
+        <v>80957852</v>
+      </c>
+      <c r="F26" s="10">
+        <v>1827081</v>
+      </c>
+      <c r="G26" s="10">
+        <v>51563</v>
+      </c>
+      <c r="H26" s="10">
+        <v>142088</v>
+      </c>
+      <c r="I26" s="11">
+        <f t="shared" si="10"/>
+        <v>83289.971193415637</v>
+      </c>
+      <c r="J26" s="12">
+        <f t="shared" si="11"/>
+        <v>2399.9475308641977</v>
+      </c>
+      <c r="K26" s="11">
+        <f t="shared" si="12"/>
+        <v>1879.712962962963</v>
+      </c>
+      <c r="L26" s="12">
+        <f t="shared" si="13"/>
+        <v>44.309941376435965</v>
+      </c>
+      <c r="M26" s="12">
+        <f t="shared" si="14"/>
+        <v>1.2767627707802773</v>
+      </c>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13">
+        <v>3.0863999999999999E-2</v>
+      </c>
+      <c r="R26" s="13">
+        <v>0.58539099999999999</v>
+      </c>
+      <c r="S26" s="13">
+        <v>0.95987699999999998</v>
+      </c>
+      <c r="T26" s="13">
+        <v>0.99382700000000002</v>
+      </c>
+      <c r="U26" s="13">
+        <v>1</v>
+      </c>
+      <c r="V26" s="13">
+        <v>1</v>
+      </c>
+      <c r="W26" s="13">
+        <v>1</v>
+      </c>
+      <c r="X26" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA26" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC26" s="15">
+        <v>36</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31">
+      <c r="A27" s="37"/>
+      <c r="B27" s="15">
+        <v>7</v>
+      </c>
+      <c r="C27" s="15">
+        <v>720</v>
+      </c>
+      <c r="D27" s="16">
+        <v>2256803</v>
+      </c>
+      <c r="E27" s="16">
+        <v>77021819</v>
+      </c>
+      <c r="F27" s="16">
+        <v>1567133</v>
+      </c>
+      <c r="G27" s="16">
+        <v>61063</v>
+      </c>
+      <c r="H27" s="16">
+        <v>161072</v>
+      </c>
+      <c r="I27" s="11">
+        <f t="shared" ref="I27" si="15">E27/C27</f>
+        <v>106974.74861111111</v>
+      </c>
+      <c r="J27" s="12">
+        <f t="shared" ref="J27" si="16">D27/C27</f>
+        <v>3134.4486111111109</v>
+      </c>
+      <c r="K27" s="11">
+        <f t="shared" ref="K27" si="17">F27/C27</f>
+        <v>2176.5736111111109</v>
+      </c>
+      <c r="L27" s="12">
+        <f t="shared" ref="L27" si="18">I27/K27</f>
+        <v>49.148233749145732</v>
+      </c>
+      <c r="M27" s="12">
+        <f t="shared" ref="M27" si="19">J27/K27</f>
+        <v>1.440083898431084</v>
+      </c>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="19">
+        <v>8.6110999999999993E-2</v>
+      </c>
+      <c r="R27" s="19">
+        <v>0.72638899999999995</v>
+      </c>
+      <c r="S27" s="19">
+        <v>0.97916700000000001</v>
+      </c>
+      <c r="T27" s="19">
+        <v>1</v>
+      </c>
+      <c r="U27" s="19">
+        <v>1</v>
+      </c>
+      <c r="V27" s="19">
+        <v>1</v>
+      </c>
+      <c r="W27" s="19">
+        <v>1</v>
+      </c>
+      <c r="X27" s="19">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="19">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="19">
+        <v>1</v>
+      </c>
+      <c r="AA27" s="19">
+        <v>1</v>
+      </c>
+      <c r="AB27" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC27" s="15">
+        <v>36</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31">
+      <c r="A28" s="37"/>
+      <c r="B28" s="9">
+        <v>8</v>
+      </c>
+      <c r="C28" s="9">
+        <v>216</v>
+      </c>
+      <c r="D28" s="10">
+        <v>13705246</v>
+      </c>
+      <c r="E28" s="10">
+        <v>461706935</v>
+      </c>
+      <c r="F28" s="10">
+        <v>499707</v>
+      </c>
+      <c r="G28" s="10">
+        <v>65570</v>
+      </c>
+      <c r="H28" s="10">
+        <v>160608</v>
+      </c>
+      <c r="I28" s="11">
+        <f t="shared" ref="I28" si="20">E28/C28</f>
+        <v>2137532.1064814813</v>
+      </c>
+      <c r="J28" s="12">
+        <f t="shared" ref="J28" si="21">D28/C28</f>
+        <v>63450.212962962964</v>
+      </c>
+      <c r="K28" s="11">
+        <f t="shared" ref="K28" si="22">F28/C28</f>
+        <v>2313.4583333333335</v>
+      </c>
+      <c r="L28" s="12">
+        <f t="shared" ref="L28" si="23">I28/K28</f>
+        <v>923.95530781037678</v>
+      </c>
+      <c r="M28" s="12">
+        <f t="shared" ref="M28" si="24">J28/K28</f>
+        <v>27.426563966484359</v>
+      </c>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13">
+        <v>0.125</v>
+      </c>
+      <c r="R28" s="13">
         <v>0.75</v>
       </c>
-      <c r="Q15" s="13">
-        <v>0.98750000000000004</v>
-      </c>
-      <c r="R15" s="13">
-        <v>1</v>
-      </c>
-      <c r="S15" s="13">
-        <v>1</v>
-      </c>
-      <c r="T15" s="13">
-        <v>1</v>
-      </c>
-      <c r="U15" s="13">
-        <v>1</v>
-      </c>
-      <c r="V15" s="13">
-        <v>1</v>
-      </c>
-      <c r="W15" s="13">
-        <v>1</v>
-      </c>
-      <c r="X15" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y15" s="13">
-        <v>1</v>
-      </c>
-      <c r="Z15" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA15" s="9">
-        <v>12</v>
-      </c>
-      <c r="AB15" t="s">
+      <c r="S28" s="13">
+        <v>0.97685200000000005</v>
+      </c>
+      <c r="T28" s="13">
+        <v>1</v>
+      </c>
+      <c r="U28" s="13">
+        <v>1</v>
+      </c>
+      <c r="V28" s="13">
+        <v>1</v>
+      </c>
+      <c r="W28" s="13">
+        <v>1</v>
+      </c>
+      <c r="X28" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA28" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB28" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC28" s="9">
+        <v>36</v>
+      </c>
+      <c r="AD28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
-      <c r="N16" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="28"/>
-      <c r="R16" s="28"/>
-      <c r="S16" s="28"/>
-      <c r="T16" s="28"/>
-      <c r="U16" s="28"/>
-      <c r="V16" s="28"/>
-      <c r="W16" s="28"/>
-      <c r="X16" s="28"/>
-      <c r="Y16" s="28"/>
-    </row>
-    <row r="17" spans="1:29" ht="45">
-      <c r="A17" s="2" t="s">
+    <row r="29" spans="1:31">
+      <c r="D29">
+        <f>D28/60000/60</f>
+        <v>3.807012777777778</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31">
+      <c r="G30" s="24">
+        <f>SUM(G23:G28)</f>
+        <v>291237</v>
+      </c>
+      <c r="H30" s="24">
+        <f>SUM(H23:H28)</f>
+        <v>842960</v>
+      </c>
+      <c r="M30" s="38">
+        <f>SUM(M23:M28)</f>
+        <v>30.268235706279171</v>
+      </c>
+      <c r="N30" s="38"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="26">
+        <f>SUM(P8:P13)/6</f>
         <v>0</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="N17" s="7">
-        <v>16384</v>
-      </c>
-      <c r="O17" s="7">
-        <v>8192</v>
-      </c>
-      <c r="P17" s="7">
-        <v>4096</v>
-      </c>
-      <c r="Q17" s="34">
-        <v>2048</v>
-      </c>
-      <c r="R17" s="7">
-        <v>1024</v>
-      </c>
-      <c r="S17" s="7">
-        <v>512</v>
-      </c>
-      <c r="T17" s="7">
-        <v>256</v>
-      </c>
-      <c r="U17" s="7">
-        <v>128</v>
-      </c>
-      <c r="V17" s="7">
-        <v>64</v>
-      </c>
-      <c r="W17" s="7">
-        <v>32</v>
-      </c>
-      <c r="X17" s="7">
-        <v>16</v>
-      </c>
-      <c r="Y17" s="7">
-        <v>8</v>
-      </c>
-      <c r="Z17" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA17" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB17" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:29">
-      <c r="A18" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="15">
-        <v>100000</v>
-      </c>
-      <c r="D18" s="16">
-        <v>49893</v>
-      </c>
-      <c r="E18" s="16">
-        <v>213204</v>
-      </c>
-      <c r="F18" s="16">
-        <v>8267265</v>
-      </c>
-      <c r="G18" s="16">
-        <v>889</v>
-      </c>
-      <c r="H18" s="16">
-        <v>4984</v>
-      </c>
-      <c r="I18" s="17">
-        <f t="shared" ref="I18:I19" si="10">E18/C18</f>
-        <v>2.1320399999999999</v>
-      </c>
-      <c r="J18" s="18">
-        <f>D18/C18</f>
-        <v>0.49892999999999998</v>
-      </c>
-      <c r="K18" s="17">
-        <f t="shared" ref="K18:K19" si="11">F18/C18</f>
-        <v>82.672650000000004</v>
-      </c>
-      <c r="L18" s="18">
-        <f t="shared" ref="L18:L19" si="12">I18/K18</f>
-        <v>2.5788939873101924E-2</v>
-      </c>
-      <c r="M18" s="18">
-        <f>J18/K18</f>
-        <v>6.0350067404395524E-3</v>
-      </c>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19"/>
-      <c r="S18" s="19">
-        <v>5.0000000000000002E-5</v>
-      </c>
-      <c r="T18" s="19">
-        <v>5.0369999999999998E-2</v>
-      </c>
-      <c r="U18" s="19">
-        <v>0.45832000000000001</v>
-      </c>
-      <c r="V18" s="19">
-        <v>0.89120999999999995</v>
-      </c>
-      <c r="W18" s="19">
-        <v>0.99451999999999996</v>
-      </c>
-      <c r="X18" s="19">
-        <v>0.99992999999999999</v>
-      </c>
-      <c r="Y18" s="14">
-        <v>1</v>
-      </c>
-      <c r="Z18" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA18" s="15">
-        <v>6</v>
-      </c>
-      <c r="AB18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29" ht="17">
-      <c r="A19" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="9">
-        <v>100000</v>
-      </c>
-      <c r="D19" s="10">
-        <v>52160</v>
-      </c>
-      <c r="E19" s="10">
-        <v>229938</v>
-      </c>
-      <c r="F19" s="10">
-        <v>18441568</v>
-      </c>
-      <c r="G19" s="10">
-        <v>2726</v>
-      </c>
-      <c r="H19" s="10">
-        <v>15568</v>
-      </c>
-      <c r="I19" s="11">
-        <f t="shared" si="10"/>
-        <v>2.2993800000000002</v>
-      </c>
-      <c r="J19" s="12">
-        <f t="shared" ref="J19" si="13">D19/C19</f>
-        <v>0.52159999999999995</v>
-      </c>
-      <c r="K19" s="11">
-        <f t="shared" si="11"/>
-        <v>184.41568000000001</v>
-      </c>
-      <c r="L19" s="12">
-        <f t="shared" si="12"/>
-        <v>1.2468462551557438E-2</v>
-      </c>
-      <c r="M19" s="12">
-        <f t="shared" ref="M19" si="14">J19/K19</f>
-        <v>2.8283929002132571E-3</v>
-      </c>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13">
-        <v>3.3500000000000001E-3</v>
-      </c>
-      <c r="S19" s="13">
-        <v>0.13125999999999999</v>
-      </c>
-      <c r="T19" s="13">
-        <v>0.58604000000000001</v>
-      </c>
-      <c r="U19" s="13">
-        <v>0.91791</v>
-      </c>
-      <c r="V19" s="13">
-        <v>0.99351999999999996</v>
-      </c>
-      <c r="W19" s="13">
-        <v>0.99995000000000001</v>
-      </c>
-      <c r="X19" s="14">
-        <v>1</v>
-      </c>
-      <c r="Y19" s="14">
-        <v>1</v>
-      </c>
-      <c r="Z19" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA19" s="9">
-        <v>6</v>
-      </c>
-      <c r="AB19">
-        <v>1</v>
-      </c>
-      <c r="AC19" s="20"/>
-    </row>
-    <row r="20" spans="1:29">
-      <c r="A20" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="15">
-        <v>1</v>
-      </c>
-      <c r="C20" s="15">
-        <v>249984</v>
-      </c>
-      <c r="D20" s="16">
-        <v>75882</v>
-      </c>
-      <c r="E20" s="16">
-        <v>2266088</v>
-      </c>
-      <c r="F20" s="16">
-        <v>157011609</v>
-      </c>
-      <c r="G20" s="16">
-        <v>14025</v>
-      </c>
-      <c r="H20" s="16">
-        <v>73536</v>
-      </c>
-      <c r="I20" s="11">
-        <f t="shared" ref="I20:I25" si="15">E20/C20</f>
-        <v>9.0649321556579618</v>
-      </c>
-      <c r="J20" s="12">
-        <f t="shared" ref="J20:J25" si="16">D20/C20</f>
-        <v>0.30354742703533028</v>
-      </c>
-      <c r="K20" s="11">
-        <f t="shared" ref="K20:K25" si="17">F20/C20</f>
-        <v>628.08663354454688</v>
-      </c>
-      <c r="L20" s="12">
-        <f t="shared" ref="L20:L25" si="18">I20/K20</f>
-        <v>1.4432614342548389E-2</v>
-      </c>
-      <c r="M20" s="12">
-        <f t="shared" ref="M20:M25" si="19">J20/K20</f>
-        <v>4.8328910507502667E-4</v>
-      </c>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="19">
-        <v>5.9319999999999998E-3</v>
-      </c>
-      <c r="Q20" s="19">
-        <v>0.221474</v>
-      </c>
-      <c r="R20" s="19">
-        <v>0.68030000000000002</v>
-      </c>
-      <c r="S20" s="19">
-        <v>0.92280300000000004</v>
-      </c>
-      <c r="T20" s="19">
-        <v>0.98709899999999995</v>
-      </c>
-      <c r="U20" s="19">
-        <v>0.99846800000000002</v>
-      </c>
-      <c r="V20" s="13">
-        <v>0.99994400000000006</v>
-      </c>
-      <c r="W20" s="13">
-        <v>1</v>
-      </c>
-      <c r="X20" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y20" s="13">
-        <v>1</v>
-      </c>
-      <c r="Z20" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA20" s="15">
-        <v>36</v>
-      </c>
-      <c r="AB20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29">
-      <c r="A21" s="31"/>
-      <c r="B21" s="9">
-        <v>2</v>
-      </c>
-      <c r="C21" s="9">
-        <v>99972</v>
-      </c>
-      <c r="D21" s="10">
-        <v>190395</v>
-      </c>
-      <c r="E21" s="10">
-        <v>6286075</v>
-      </c>
-      <c r="F21" s="10">
-        <v>77198157</v>
-      </c>
-      <c r="G21" s="10">
-        <v>17990</v>
-      </c>
-      <c r="H21" s="10">
-        <v>96020</v>
-      </c>
-      <c r="I21" s="11">
-        <f t="shared" si="15"/>
-        <v>62.878355939663109</v>
-      </c>
-      <c r="J21" s="12">
-        <f t="shared" si="16"/>
-        <v>1.9044832553114872</v>
-      </c>
-      <c r="K21" s="11">
-        <f t="shared" si="17"/>
-        <v>772.19778537990635</v>
-      </c>
-      <c r="L21" s="12">
-        <f t="shared" si="18"/>
-        <v>8.1427785899085656E-2</v>
-      </c>
-      <c r="M21" s="12">
-        <f t="shared" si="19"/>
-        <v>2.4663153551709792E-3</v>
-      </c>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="P21" s="13">
-        <v>2.2556E-2</v>
-      </c>
-      <c r="Q21" s="13">
-        <v>0.36591200000000002</v>
-      </c>
-      <c r="R21" s="13">
-        <v>0.80297499999999999</v>
-      </c>
-      <c r="S21" s="13">
-        <v>0.96620099999999998</v>
-      </c>
-      <c r="T21" s="13">
-        <v>0.99589899999999998</v>
-      </c>
-      <c r="U21" s="13">
-        <v>0.99960000000000004</v>
-      </c>
-      <c r="V21" s="13">
-        <v>0.99999000000000005</v>
-      </c>
-      <c r="W21" s="13">
-        <v>1</v>
-      </c>
-      <c r="X21" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y21" s="13">
-        <v>1</v>
-      </c>
-      <c r="Z21" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA21" s="15">
-        <v>36</v>
-      </c>
-      <c r="AB21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:29">
-      <c r="A22" s="31"/>
-      <c r="B22" s="15">
-        <v>3</v>
-      </c>
-      <c r="C22" s="15">
-        <v>49968</v>
-      </c>
-      <c r="D22" s="16">
-        <v>156411</v>
-      </c>
-      <c r="E22" s="16">
-        <v>5427374</v>
-      </c>
-      <c r="F22" s="16">
-        <v>61104521</v>
-      </c>
-      <c r="G22" s="16">
-        <v>31364</v>
-      </c>
-      <c r="H22" s="16">
-        <v>124480</v>
-      </c>
-      <c r="I22" s="11">
-        <f t="shared" si="15"/>
-        <v>108.61699487672111</v>
-      </c>
-      <c r="J22" s="12">
-        <f t="shared" si="16"/>
-        <v>3.1302233429394812</v>
-      </c>
-      <c r="K22" s="11">
-        <f t="shared" si="17"/>
-        <v>1222.8730587576049</v>
-      </c>
-      <c r="L22" s="12">
-        <f t="shared" si="18"/>
-        <v>8.8821152857085653E-2</v>
-      </c>
-      <c r="M22" s="12">
-        <f t="shared" si="19"/>
-        <v>2.5597287637685595E-3</v>
-      </c>
-      <c r="N22" s="13"/>
-      <c r="O22" s="19">
-        <v>1.2409999999999999E-3</v>
-      </c>
-      <c r="P22" s="19">
-        <v>0.21503800000000001</v>
-      </c>
-      <c r="Q22" s="19">
-        <v>0.74697800000000003</v>
-      </c>
-      <c r="R22" s="19">
-        <v>0.95771300000000004</v>
-      </c>
-      <c r="S22" s="19">
-        <v>0.99611799999999995</v>
-      </c>
-      <c r="T22" s="19">
-        <v>0.99975999999999998</v>
-      </c>
-      <c r="U22" s="19">
-        <v>0.99997999999999998</v>
-      </c>
-      <c r="V22" s="13">
-        <v>1</v>
-      </c>
-      <c r="W22" s="13">
-        <v>1</v>
-      </c>
-      <c r="X22" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y22" s="13">
-        <v>1</v>
-      </c>
-      <c r="Z22" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA22" s="15">
-        <v>36</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:29">
-      <c r="A23" s="31"/>
-      <c r="B23" s="9">
-        <v>4</v>
-      </c>
-      <c r="C23" s="9">
-        <v>14976</v>
-      </c>
-      <c r="D23" s="10">
-        <v>1118075</v>
-      </c>
-      <c r="E23" s="10">
-        <v>39265635</v>
-      </c>
-      <c r="F23" s="10">
-        <v>19678039</v>
-      </c>
-      <c r="G23" s="10">
-        <v>34082</v>
-      </c>
-      <c r="H23" s="10">
-        <v>125044</v>
-      </c>
-      <c r="I23" s="11">
-        <f t="shared" si="15"/>
-        <v>2621.9040464743589</v>
-      </c>
-      <c r="J23" s="12">
-        <f t="shared" si="16"/>
-        <v>74.657785790598297</v>
-      </c>
-      <c r="K23" s="11">
-        <f t="shared" si="17"/>
-        <v>1313.9716212606838</v>
-      </c>
-      <c r="L23" s="12">
-        <f t="shared" si="18"/>
-        <v>1.9954038611266089</v>
-      </c>
-      <c r="M23" s="12">
-        <f t="shared" si="19"/>
-        <v>5.6818415696808004E-2</v>
-      </c>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13">
-        <v>2.003E-3</v>
-      </c>
-      <c r="P23" s="13">
-        <v>0.26155200000000001</v>
-      </c>
-      <c r="Q23" s="13">
-        <v>0.79720899999999995</v>
-      </c>
-      <c r="R23" s="13">
-        <v>0.96975199999999995</v>
-      </c>
-      <c r="S23" s="13">
-        <v>0.99766299999999997</v>
-      </c>
-      <c r="T23" s="13">
-        <v>0.99993299999999996</v>
-      </c>
-      <c r="U23" s="13">
-        <v>1</v>
-      </c>
-      <c r="V23" s="13">
-        <v>1</v>
-      </c>
-      <c r="W23" s="13">
-        <v>1</v>
-      </c>
-      <c r="X23" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y23" s="13">
-        <v>1</v>
-      </c>
-      <c r="Z23" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA23" s="15">
-        <v>36</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:29">
-      <c r="A24" s="31"/>
-      <c r="B24" s="15">
-        <v>5</v>
-      </c>
-      <c r="C24" s="15">
-        <v>4968</v>
-      </c>
-      <c r="D24" s="16">
-        <v>569724</v>
-      </c>
-      <c r="E24" s="16">
-        <v>19821757</v>
-      </c>
-      <c r="F24" s="16">
-        <v>8705130</v>
-      </c>
-      <c r="G24" s="16">
-        <v>47595</v>
-      </c>
-      <c r="H24" s="16">
-        <v>129668</v>
-      </c>
-      <c r="I24" s="11">
-        <f t="shared" si="15"/>
-        <v>3989.8866747181964</v>
-      </c>
-      <c r="J24" s="12">
-        <f t="shared" si="16"/>
-        <v>114.67874396135265</v>
-      </c>
-      <c r="K24" s="11">
-        <f t="shared" si="17"/>
-        <v>1752.2403381642512</v>
-      </c>
-      <c r="L24" s="12">
-        <f t="shared" si="18"/>
-        <v>2.2770202168146829</v>
-      </c>
-      <c r="M24" s="12">
-        <f t="shared" si="19"/>
-        <v>6.5446926122872368E-2</v>
-      </c>
-      <c r="N24" s="13"/>
-      <c r="O24" s="19">
-        <v>2.5361999999999999E-2</v>
-      </c>
-      <c r="P24" s="19">
-        <v>0.51308399999999998</v>
-      </c>
-      <c r="Q24" s="19">
-        <v>0.92290700000000003</v>
-      </c>
-      <c r="R24" s="19">
-        <v>0.99335700000000005</v>
-      </c>
-      <c r="S24" s="19">
-        <v>0.99939599999999995</v>
-      </c>
-      <c r="T24" s="19">
-        <v>1</v>
-      </c>
-      <c r="U24" s="13">
-        <v>1</v>
-      </c>
-      <c r="V24" s="13">
-        <v>1</v>
-      </c>
-      <c r="W24" s="13">
-        <v>1</v>
-      </c>
-      <c r="X24" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y24" s="13">
-        <v>1</v>
-      </c>
-      <c r="Z24" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA24" s="15">
-        <v>36</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:29">
-      <c r="A25" s="31"/>
-      <c r="B25" s="9">
-        <v>6</v>
-      </c>
-      <c r="C25" s="9">
-        <v>972</v>
-      </c>
-      <c r="D25" s="10">
-        <v>2332749</v>
-      </c>
-      <c r="E25" s="10">
-        <v>80957852</v>
-      </c>
-      <c r="F25" s="10">
-        <v>1827081</v>
-      </c>
-      <c r="G25" s="10">
-        <v>51563</v>
-      </c>
-      <c r="H25" s="10">
-        <v>142088</v>
-      </c>
-      <c r="I25" s="11">
-        <f t="shared" si="15"/>
-        <v>83289.971193415637</v>
-      </c>
-      <c r="J25" s="12">
-        <f t="shared" si="16"/>
-        <v>2399.9475308641977</v>
-      </c>
-      <c r="K25" s="11">
-        <f t="shared" si="17"/>
-        <v>1879.712962962963</v>
-      </c>
-      <c r="L25" s="12">
-        <f t="shared" si="18"/>
-        <v>44.309941376435965</v>
-      </c>
-      <c r="M25" s="12">
-        <f t="shared" si="19"/>
-        <v>1.2767627707802773</v>
-      </c>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13">
-        <v>3.0863999999999999E-2</v>
-      </c>
-      <c r="P25" s="13">
-        <v>0.58539099999999999</v>
-      </c>
-      <c r="Q25" s="13">
-        <v>0.95987699999999998</v>
-      </c>
-      <c r="R25" s="13">
-        <v>0.99382700000000002</v>
-      </c>
-      <c r="S25" s="13">
-        <v>1</v>
-      </c>
-      <c r="T25" s="13">
-        <v>1</v>
-      </c>
-      <c r="U25" s="13">
-        <v>1</v>
-      </c>
-      <c r="V25" s="13">
-        <v>1</v>
-      </c>
-      <c r="W25" s="13">
-        <v>1</v>
-      </c>
-      <c r="X25" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y25" s="13">
-        <v>1</v>
-      </c>
-      <c r="Z25" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA25" s="15">
-        <v>36</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:29">
-      <c r="A26" s="31"/>
-      <c r="B26" s="15">
-        <v>7</v>
-      </c>
-      <c r="C26" s="15">
-        <v>720</v>
-      </c>
-      <c r="D26" s="16">
-        <v>2256803</v>
-      </c>
-      <c r="E26" s="16">
-        <v>77021819</v>
-      </c>
-      <c r="F26" s="16">
-        <v>1567133</v>
-      </c>
-      <c r="G26" s="16">
-        <v>61063</v>
-      </c>
-      <c r="H26" s="16">
-        <v>161072</v>
-      </c>
-      <c r="I26" s="11">
-        <f t="shared" ref="I26" si="20">E26/C26</f>
-        <v>106974.74861111111</v>
-      </c>
-      <c r="J26" s="12">
-        <f t="shared" ref="J26" si="21">D26/C26</f>
-        <v>3134.4486111111109</v>
-      </c>
-      <c r="K26" s="11">
-        <f t="shared" ref="K26" si="22">F26/C26</f>
-        <v>2176.5736111111109</v>
-      </c>
-      <c r="L26" s="12">
-        <f t="shared" ref="L26" si="23">I26/K26</f>
-        <v>49.148233749145732</v>
-      </c>
-      <c r="M26" s="12">
-        <f t="shared" ref="M26" si="24">J26/K26</f>
-        <v>1.440083898431084</v>
-      </c>
-      <c r="N26" s="13"/>
-      <c r="O26" s="19">
-        <v>8.6110999999999993E-2</v>
-      </c>
-      <c r="P26" s="19">
-        <v>0.72638899999999995</v>
-      </c>
-      <c r="Q26" s="19">
-        <v>0.97916700000000001</v>
-      </c>
-      <c r="R26" s="19">
-        <v>1</v>
-      </c>
-      <c r="S26" s="19">
-        <v>1</v>
-      </c>
-      <c r="T26" s="19">
-        <v>1</v>
-      </c>
-      <c r="U26" s="19">
-        <v>1</v>
-      </c>
-      <c r="V26" s="19">
-        <v>1</v>
-      </c>
-      <c r="W26" s="19">
-        <v>1</v>
-      </c>
-      <c r="X26" s="19">
-        <v>1</v>
-      </c>
-      <c r="Y26" s="19">
-        <v>1</v>
-      </c>
-      <c r="Z26" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA26" s="15">
-        <v>36</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29">
-      <c r="A27" s="31"/>
-      <c r="B27" s="9">
-        <v>8</v>
-      </c>
-      <c r="C27" s="9">
-        <v>216</v>
-      </c>
-      <c r="D27" s="10">
-        <v>13705246</v>
-      </c>
-      <c r="E27" s="10">
-        <v>461706935</v>
-      </c>
-      <c r="F27" s="10">
-        <v>499707</v>
-      </c>
-      <c r="G27" s="10">
-        <v>65570</v>
-      </c>
-      <c r="H27" s="10">
-        <v>160608</v>
-      </c>
-      <c r="I27" s="11">
-        <f t="shared" ref="I27" si="25">E27/C27</f>
-        <v>2137532.1064814813</v>
-      </c>
-      <c r="J27" s="12">
-        <f t="shared" ref="J27" si="26">D27/C27</f>
-        <v>63450.212962962964</v>
-      </c>
-      <c r="K27" s="11">
-        <f t="shared" ref="K27" si="27">F27/C27</f>
-        <v>2313.4583333333335</v>
-      </c>
-      <c r="L27" s="12">
-        <f t="shared" ref="L27" si="28">I27/K27</f>
-        <v>923.95530781037678</v>
-      </c>
-      <c r="M27" s="12">
-        <f t="shared" ref="M27" si="29">J27/K27</f>
-        <v>27.426563966484359</v>
-      </c>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13">
-        <v>0.125</v>
-      </c>
-      <c r="P27" s="13">
-        <v>0.75</v>
-      </c>
-      <c r="Q27" s="13">
-        <v>0.97685200000000005</v>
-      </c>
-      <c r="R27" s="13">
-        <v>1</v>
-      </c>
-      <c r="S27" s="13">
-        <v>1</v>
-      </c>
-      <c r="T27" s="13">
-        <v>1</v>
-      </c>
-      <c r="U27" s="13">
-        <v>1</v>
-      </c>
-      <c r="V27" s="13">
-        <v>1</v>
-      </c>
-      <c r="W27" s="13">
-        <v>1</v>
-      </c>
-      <c r="X27" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y27" s="13">
-        <v>1</v>
-      </c>
-      <c r="Z27" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA27" s="9">
-        <v>36</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29">
-      <c r="D28">
-        <f>D27/60000/60</f>
-        <v>3.807012777777778</v>
-      </c>
-    </row>
-    <row r="29" spans="1:29">
-      <c r="G29" s="24">
-        <f>SUM(G22:G27)</f>
-        <v>291237</v>
-      </c>
-      <c r="H29" s="24">
-        <f>SUM(H22:H27)</f>
-        <v>842960</v>
-      </c>
-      <c r="M29" s="32">
-        <f>SUM(M22:M27)</f>
-        <v>30.268235706279171</v>
-      </c>
-      <c r="N29" s="26">
-        <f>SUM(N8:N13)/6</f>
+      <c r="Q30" s="26">
+        <f t="shared" ref="Q30:AA30" si="25">SUM(Q8:Q13)/6</f>
+        <v>1.5382166666666669E-2</v>
+      </c>
+      <c r="R30" s="26">
+        <f t="shared" si="25"/>
+        <v>0.2811616666666667</v>
+      </c>
+      <c r="S30" s="26">
+        <f t="shared" si="25"/>
+        <v>0.67854749999999997</v>
+      </c>
+      <c r="T30" s="26">
+        <f t="shared" si="25"/>
+        <v>0.9122905</v>
+      </c>
+      <c r="U30" s="26">
+        <f t="shared" si="25"/>
+        <v>0.98376449999999993</v>
+      </c>
+      <c r="V30" s="26">
+        <f t="shared" si="25"/>
+        <v>0.99777033333333343</v>
+      </c>
+      <c r="W30" s="26">
+        <f t="shared" si="25"/>
+        <v>0.99978566666666657</v>
+      </c>
+      <c r="X30" s="26">
+        <f t="shared" si="25"/>
+        <v>0.99999400000000005</v>
+      </c>
+      <c r="Y30" s="26">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="Z30" s="26">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="AA30" s="26">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" ht="18" customHeight="1">
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
+    </row>
+    <row r="33" spans="4:26" ht="17" customHeight="1">
+      <c r="Y33" s="25"/>
+      <c r="Z33" s="25"/>
+    </row>
+    <row r="34" spans="4:26">
+      <c r="Y34" s="25"/>
+      <c r="Z34" s="25"/>
+    </row>
+    <row r="35" spans="4:26">
+      <c r="D35">
+        <f>D11/3600000</f>
+        <v>0.44090027777777779</v>
+      </c>
+      <c r="L35">
+        <f>L14/6.3</f>
         <v>0</v>
       </c>
-      <c r="O29" s="26">
-        <f t="shared" ref="O29:Y29" si="30">SUM(O8:O13)/6</f>
-        <v>7.0016666666666673E-3</v>
-      </c>
-      <c r="P29" s="26">
-        <f t="shared" si="30"/>
-        <v>0.26971283333333335</v>
-      </c>
-      <c r="Q29" s="26">
-        <f t="shared" si="30"/>
-        <v>0.66943366666666682</v>
-      </c>
-      <c r="R29" s="26">
-        <f t="shared" si="30"/>
-        <v>0.90011999999999992</v>
-      </c>
-      <c r="S29" s="26">
-        <f t="shared" si="30"/>
-        <v>0.97983483333333343</v>
-      </c>
-      <c r="T29" s="26">
-        <f t="shared" si="30"/>
-        <v>0.99700216666666674</v>
-      </c>
-      <c r="U29" s="26">
-        <f t="shared" si="30"/>
-        <v>0.99968533333333331</v>
-      </c>
-      <c r="V29" s="26">
-        <f t="shared" si="30"/>
-        <v>0.99998333333333334</v>
-      </c>
-      <c r="W29" s="26">
-        <f t="shared" si="30"/>
-        <v>0.99999933333333324</v>
-      </c>
-      <c r="X29" s="26">
-        <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="Y29" s="26">
-        <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:29" ht="18" customHeight="1">
-      <c r="W31" s="1"/>
-      <c r="X31" s="1"/>
-      <c r="Y31" s="1"/>
-    </row>
-    <row r="32" spans="1:29" ht="17" customHeight="1">
-      <c r="W32" s="25"/>
-      <c r="X32" s="25"/>
-    </row>
-    <row r="33" spans="4:24">
-      <c r="W33" s="25"/>
-      <c r="X33" s="25"/>
-    </row>
-    <row r="34" spans="4:24">
-      <c r="D34">
-        <f>D11/3600000</f>
-        <v>0.40771000000000002</v>
-      </c>
-      <c r="L34">
-        <f>L14/6.3</f>
-        <v>5.2441018595631634</v>
-      </c>
-      <c r="W34" s="25"/>
-      <c r="X34" s="25"/>
-    </row>
-    <row r="35" spans="4:24">
-      <c r="W35" s="25"/>
-      <c r="X35" s="25"/>
-    </row>
-    <row r="36" spans="4:24">
-      <c r="W36" s="25"/>
-      <c r="X36" s="25"/>
-    </row>
-    <row r="37" spans="4:24">
-      <c r="W37" s="25"/>
-      <c r="X37" s="25"/>
-    </row>
-    <row r="38" spans="4:24">
-      <c r="W38" s="25"/>
-      <c r="X38" s="25"/>
-    </row>
-    <row r="39" spans="4:24">
-      <c r="W39" s="25"/>
-      <c r="X39" s="25"/>
-    </row>
-    <row r="40" spans="4:24">
-      <c r="W40" s="25"/>
-      <c r="X40" s="25"/>
-    </row>
-    <row r="45" spans="4:24">
-      <c r="X45" s="25"/>
-    </row>
-    <row r="48" spans="4:24">
-      <c r="W48" s="27"/>
-      <c r="X48" s="27"/>
-    </row>
-    <row r="49" spans="23:24">
-      <c r="W49" s="27"/>
-      <c r="X49" s="27"/>
-    </row>
-    <row r="50" spans="23:24">
-      <c r="W50" s="27"/>
-      <c r="X50" s="27"/>
-    </row>
-    <row r="51" spans="23:24">
-      <c r="W51" s="27"/>
-      <c r="X51" s="27"/>
-    </row>
-    <row r="52" spans="23:24">
-      <c r="W52" s="27"/>
-      <c r="X52" s="27"/>
-    </row>
-    <row r="53" spans="23:24">
-      <c r="W53" s="27"/>
-      <c r="X53" s="27"/>
-    </row>
-    <row r="56" spans="23:24">
-      <c r="W56" s="27"/>
-      <c r="X56" s="27"/>
-    </row>
-    <row r="57" spans="23:24">
-      <c r="W57" s="27"/>
-      <c r="X57" s="27"/>
-    </row>
-    <row r="58" spans="23:24">
-      <c r="W58" s="27"/>
-      <c r="X58" s="27"/>
-    </row>
-    <row r="59" spans="23:24">
-      <c r="W59" s="27"/>
-      <c r="X59" s="27"/>
-    </row>
-    <row r="60" spans="23:24">
-      <c r="W60" s="27"/>
-      <c r="X60" s="27"/>
-    </row>
-    <row r="61" spans="23:24">
-      <c r="W61" s="27"/>
-      <c r="X61" s="27"/>
+      <c r="Y35" s="25"/>
+      <c r="Z35" s="25"/>
+    </row>
+    <row r="36" spans="4:26">
+      <c r="Y36" s="25"/>
+      <c r="Z36" s="25"/>
+    </row>
+    <row r="37" spans="4:26">
+      <c r="Y37" s="25"/>
+      <c r="Z37" s="25"/>
+    </row>
+    <row r="38" spans="4:26">
+      <c r="Y38" s="25"/>
+      <c r="Z38" s="25"/>
+    </row>
+    <row r="39" spans="4:26">
+      <c r="Y39" s="25"/>
+      <c r="Z39" s="25"/>
+    </row>
+    <row r="40" spans="4:26">
+      <c r="Y40" s="25"/>
+      <c r="Z40" s="25"/>
+    </row>
+    <row r="41" spans="4:26">
+      <c r="Y41" s="25"/>
+      <c r="Z41" s="25"/>
+    </row>
+    <row r="46" spans="4:26">
+      <c r="Z46" s="25"/>
+    </row>
+    <row r="49" spans="25:26">
+      <c r="Y49" s="27"/>
+      <c r="Z49" s="27"/>
+    </row>
+    <row r="50" spans="25:26">
+      <c r="Y50" s="27"/>
+      <c r="Z50" s="27"/>
+    </row>
+    <row r="51" spans="25:26">
+      <c r="Y51" s="27"/>
+      <c r="Z51" s="27"/>
+    </row>
+    <row r="52" spans="25:26">
+      <c r="Y52" s="27"/>
+      <c r="Z52" s="27"/>
+    </row>
+    <row r="53" spans="25:26">
+      <c r="Y53" s="27"/>
+      <c r="Z53" s="27"/>
+    </row>
+    <row r="54" spans="25:26">
+      <c r="Y54" s="27"/>
+      <c r="Z54" s="27"/>
+    </row>
+    <row r="57" spans="25:26">
+      <c r="Y57" s="27"/>
+      <c r="Z57" s="27"/>
+    </row>
+    <row r="58" spans="25:26">
+      <c r="Y58" s="27"/>
+      <c r="Z58" s="27"/>
+    </row>
+    <row r="59" spans="25:26">
+      <c r="Y59" s="27"/>
+      <c r="Z59" s="27"/>
+    </row>
+    <row r="60" spans="25:26">
+      <c r="Y60" s="27"/>
+      <c r="Z60" s="27"/>
+    </row>
+    <row r="61" spans="25:26">
+      <c r="Y61" s="27"/>
+      <c r="Z61" s="27"/>
+    </row>
+    <row r="62" spans="25:26">
+      <c r="Y62" s="27"/>
+      <c r="Z62" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="N6:Y6"/>
     <mergeCell ref="A8:A15"/>
-    <mergeCell ref="A20:A27"/>
-    <mergeCell ref="N16:Y16"/>
-    <mergeCell ref="N1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="A21:A28"/>
+    <mergeCell ref="N1:AA1"/>
+    <mergeCell ref="N6:AA6"/>
+    <mergeCell ref="N17:AA17"/>
+    <mergeCell ref="AB1:AC1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F65:F70">
+  <conditionalFormatting sqref="F66:F71">
     <cfRule type="cellIs" dxfId="0" priority="28" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -4068,7 +4079,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N8:Y11">
+  <conditionalFormatting sqref="P8:AA11">
     <cfRule type="colorScale" priority="177">
       <colorScale>
         <cfvo type="min"/>
@@ -4080,7 +4091,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12:H15">
+  <conditionalFormatting sqref="H12:H16">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -4100,7 +4111,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G12:G15">
+  <conditionalFormatting sqref="G12:G16">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -4110,7 +4121,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N12:Y15">
+  <conditionalFormatting sqref="P12:AA16">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -4122,7 +4133,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N12:Y15">
+  <conditionalFormatting sqref="P12:AA16">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -4134,7 +4145,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H20:H23">
+  <conditionalFormatting sqref="H21:H24">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -4154,7 +4165,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20:G23">
+  <conditionalFormatting sqref="G21:G24">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -4164,7 +4175,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N20:Y23">
+  <conditionalFormatting sqref="P21:AA24">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -4176,7 +4187,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24:H27">
+  <conditionalFormatting sqref="H25:H28">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -4196,7 +4207,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G24:G27">
+  <conditionalFormatting sqref="G25:G28">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -4206,7 +4217,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N24:Y27">
+  <conditionalFormatting sqref="P25:AA28">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -4218,7 +4229,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N24:Y27">
+  <conditionalFormatting sqref="P25:AA28">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -4230,7 +4241,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:X3 N4:W4">
+  <conditionalFormatting sqref="P3:Z3 P4:Y4">
     <cfRule type="colorScale" priority="178">
       <colorScale>
         <cfvo type="percent" val="0"/>
@@ -4252,7 +4263,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:Y4">
+  <conditionalFormatting sqref="P3:AA4">
     <cfRule type="colorScale" priority="182">
       <colorScale>
         <cfvo type="min"/>
@@ -4294,7 +4305,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:Y4">
+  <conditionalFormatting sqref="P3:AA4">
     <cfRule type="colorScale" priority="186">
       <colorScale>
         <cfvo type="min"/>
@@ -4306,7 +4317,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N18:X18 N19:W19">
+  <conditionalFormatting sqref="P19:Z19 P20:Y20">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="percent" val="0"/>
@@ -4328,7 +4339,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N18:Y19">
+  <conditionalFormatting sqref="P19:AA20">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -4340,7 +4351,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H18:H19">
+  <conditionalFormatting sqref="H19:H20">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -4360,7 +4371,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G18:G19">
+  <conditionalFormatting sqref="G19:G20">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -4370,7 +4381,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N18:Y19">
+  <conditionalFormatting sqref="P19:AA20">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -4382,7 +4393,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N18:Y26">
+  <conditionalFormatting sqref="P19:AA27">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -4408,8 +4419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:M8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4485,7 +4496,7 @@
       <c r="P2" s="7">
         <v>4096</v>
       </c>
-      <c r="Q2" s="35">
+      <c r="Q2" s="41">
         <v>2048</v>
       </c>
       <c r="R2" s="7">
@@ -4523,7 +4534,7 @@
       </c>
     </row>
     <row r="3" spans="1:28">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="36" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="15">
@@ -4610,7 +4621,7 @@
       </c>
     </row>
     <row r="4" spans="1:28">
-      <c r="A4" s="31"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="9">
         <v>2</v>
       </c>
@@ -4695,7 +4706,7 @@
       </c>
     </row>
     <row r="5" spans="1:28">
-      <c r="A5" s="31"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="15">
         <v>3</v>
       </c>
@@ -4782,7 +4793,7 @@
       </c>
     </row>
     <row r="6" spans="1:28">
-      <c r="A6" s="31"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="9">
         <v>4</v>
       </c>
@@ -4869,7 +4880,7 @@
       </c>
     </row>
     <row r="7" spans="1:28">
-      <c r="A7" s="31"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="15">
         <v>5</v>
       </c>
@@ -4956,7 +4967,7 @@
       </c>
     </row>
     <row r="8" spans="1:28">
-      <c r="A8" s="31"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="9">
         <v>6</v>
       </c>
@@ -5051,7 +5062,7 @@
         <f>SUM(H3:H8)</f>
         <v>745476</v>
       </c>
-      <c r="M10" s="32">
+      <c r="M10" s="38">
         <f>SUM(M3:M8)</f>
         <v>1.8940001014309742</v>
       </c>
@@ -5067,7 +5078,7 @@
         <f t="shared" ref="P10:Y10" si="10">SUM(P3:P8)/6</f>
         <v>0.28283700000000001</v>
       </c>
-      <c r="Q10" s="33">
+      <c r="Q10" s="39">
         <f t="shared" si="10"/>
         <v>0.68294349999999993</v>
       </c>
@@ -5156,7 +5167,7 @@
       <c r="P14" s="7">
         <v>4096</v>
       </c>
-      <c r="Q14" s="34">
+      <c r="Q14" s="40">
         <v>2048</v>
       </c>
       <c r="R14" s="7">
@@ -5201,62 +5212,47 @@
         <v>249996</v>
       </c>
       <c r="D15" s="16">
-        <v>103529</v>
+        <v>192677</v>
       </c>
       <c r="E15" s="16">
-        <v>1103921</v>
+        <v>2067800</v>
       </c>
       <c r="F15" s="16">
-        <v>167078359</v>
+        <v>166103240</v>
       </c>
       <c r="G15" s="16">
-        <v>15094</v>
+        <v>14973</v>
       </c>
       <c r="H15" s="16">
-        <v>76776</v>
-      </c>
-      <c r="I15" s="17">
-        <f t="shared" ref="I15:I18" si="11">E15/C15</f>
-        <v>4.4157546520744333</v>
-      </c>
-      <c r="J15" s="18">
-        <f t="shared" ref="J15:J18" si="12">D15/C15</f>
-        <v>0.41412262596201538</v>
-      </c>
-      <c r="K15" s="17">
-        <f t="shared" ref="K15:K18" si="13">F15/C15</f>
-        <v>668.32412918606701</v>
-      </c>
-      <c r="L15" s="18">
-        <f t="shared" ref="L15:L18" si="14">I15/K15</f>
-        <v>6.6072051856817674E-3</v>
-      </c>
-      <c r="M15" s="18">
-        <f t="shared" ref="M15:M18" si="15">J15/K15</f>
-        <v>6.1964338541294864E-4</v>
-      </c>
+        <v>76800</v>
+      </c>
+      <c r="I15" s="17"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
       <c r="P15" s="19">
-        <v>8.5400000000000007E-3</v>
+        <v>8.2000000000000007E-3</v>
       </c>
       <c r="Q15" s="19">
-        <v>0.25731599999999999</v>
+        <v>0.24967600000000001</v>
       </c>
       <c r="R15" s="19">
-        <v>0.720804</v>
+        <v>0.71625499999999998</v>
       </c>
       <c r="S15" s="19">
-        <v>0.93848299999999996</v>
+        <v>0.93696699999999999</v>
       </c>
       <c r="T15" s="19">
-        <v>0.99029199999999995</v>
+        <v>0.99006799999999995</v>
       </c>
       <c r="U15" s="19">
-        <v>0.99894400000000005</v>
+        <v>0.99899199999999999</v>
       </c>
       <c r="V15" s="13">
-        <v>0.99996399999999996</v>
+        <v>0.99996799999999997</v>
       </c>
       <c r="W15" s="13">
         <v>1</v>
@@ -5274,7 +5270,7 @@
         <v>12</v>
       </c>
       <c r="AB15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:28">
@@ -5285,62 +5281,49 @@
         <v>99996</v>
       </c>
       <c r="D16" s="10">
-        <v>216248</v>
+        <v>226325</v>
       </c>
       <c r="E16" s="10">
-        <v>2535625</v>
+        <v>2609919</v>
       </c>
       <c r="F16" s="10">
-        <v>81413133</v>
+        <v>81532060</v>
       </c>
       <c r="G16" s="10">
-        <v>19173</v>
+        <v>19200</v>
       </c>
       <c r="H16" s="10">
-        <v>76940</v>
-      </c>
-      <c r="I16" s="17">
-        <f t="shared" si="11"/>
-        <v>25.357264290571624</v>
-      </c>
-      <c r="J16" s="18">
-        <f t="shared" si="12"/>
-        <v>2.1625665026601064</v>
-      </c>
-      <c r="K16" s="17">
-        <f t="shared" si="13"/>
-        <v>814.16389655586227</v>
-      </c>
-      <c r="L16" s="18">
-        <f t="shared" si="14"/>
-        <v>3.1145159344254693E-2</v>
-      </c>
-      <c r="M16" s="18">
-        <f t="shared" si="15"/>
-        <v>2.656180790880508E-3</v>
-      </c>
+        <v>102136</v>
+      </c>
+      <c r="I16" s="17"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
       <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
+      <c r="O16" s="13">
+        <v>1.0000000000000001E-5</v>
+      </c>
       <c r="P16" s="13">
-        <v>2.9940999999999999E-2</v>
+        <v>3.0190999999999999E-2</v>
       </c>
       <c r="Q16" s="13">
-        <v>0.40700599999999998</v>
+        <v>0.40543600000000002</v>
       </c>
       <c r="R16" s="13">
-        <v>0.83407299999999995</v>
+        <v>0.83413300000000001</v>
       </c>
       <c r="S16" s="13">
-        <v>0.97155899999999995</v>
+        <v>0.97299899999999995</v>
       </c>
       <c r="T16" s="13">
-        <v>0.99673</v>
+        <v>0.99690000000000001</v>
       </c>
       <c r="U16" s="13">
-        <v>0.99977000000000005</v>
+        <v>0.99973999999999996</v>
       </c>
       <c r="V16" s="13">
-        <v>1</v>
+        <v>0.99999000000000005</v>
       </c>
       <c r="W16" s="13">
         <v>1</v>
@@ -5358,7 +5341,7 @@
         <v>12</v>
       </c>
       <c r="AB16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:28">
@@ -5369,58 +5352,43 @@
         <v>49992</v>
       </c>
       <c r="D17" s="16">
-        <v>369062</v>
+        <v>698510</v>
       </c>
       <c r="E17" s="16">
-        <v>4370251</v>
+        <v>8294349</v>
       </c>
       <c r="F17" s="16">
-        <v>60425721</v>
+        <v>60816952</v>
       </c>
       <c r="G17" s="16">
-        <v>30969</v>
+        <v>31197</v>
       </c>
       <c r="H17" s="16">
-        <v>126820</v>
-      </c>
-      <c r="I17" s="17">
-        <f t="shared" si="11"/>
-        <v>87.419007041126576</v>
-      </c>
-      <c r="J17" s="18">
-        <f t="shared" si="12"/>
-        <v>7.3824211873899825</v>
-      </c>
-      <c r="K17" s="17">
-        <f t="shared" si="13"/>
-        <v>1208.7078132501201</v>
-      </c>
-      <c r="L17" s="18">
-        <f t="shared" si="14"/>
-        <v>7.2324350089260817E-2</v>
-      </c>
-      <c r="M17" s="18">
-        <f t="shared" si="15"/>
-        <v>6.1076970848225375E-3</v>
-      </c>
+        <v>127980</v>
+      </c>
+      <c r="I17" s="17"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
       <c r="N17" s="13"/>
       <c r="O17" s="19">
-        <v>1.8400000000000001E-3</v>
+        <v>2.0600000000000002E-3</v>
       </c>
       <c r="P17" s="19">
-        <v>0.208313</v>
+        <v>0.21221400000000001</v>
       </c>
       <c r="Q17" s="19">
-        <v>0.73457799999999995</v>
+        <v>0.73603799999999997</v>
       </c>
       <c r="R17" s="19">
-        <v>0.95361300000000004</v>
+        <v>0.95509299999999997</v>
       </c>
       <c r="S17" s="19">
-        <v>0.995479</v>
+        <v>0.99567899999999998</v>
       </c>
       <c r="T17" s="19">
-        <v>0.99960000000000004</v>
+        <v>0.99982000000000004</v>
       </c>
       <c r="U17" s="19">
         <v>1</v>
@@ -5444,7 +5412,7 @@
         <v>12</v>
       </c>
       <c r="AB17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="2:28">
@@ -5455,55 +5423,40 @@
         <v>15000</v>
       </c>
       <c r="D18" s="10">
-        <v>1587241</v>
+        <v>1110281</v>
       </c>
       <c r="E18" s="10">
-        <v>18981224</v>
+        <v>13195739</v>
       </c>
       <c r="F18" s="10">
-        <v>19499363</v>
+        <v>19615817</v>
       </c>
       <c r="G18" s="10">
-        <v>33687</v>
+        <v>33889</v>
       </c>
       <c r="H18" s="10">
-        <v>140860</v>
-      </c>
-      <c r="I18" s="17">
-        <f t="shared" si="11"/>
-        <v>1265.4149333333332</v>
-      </c>
-      <c r="J18" s="18">
-        <f t="shared" si="12"/>
-        <v>105.81606666666667</v>
-      </c>
-      <c r="K18" s="17">
-        <f t="shared" si="13"/>
-        <v>1299.9575333333332</v>
-      </c>
-      <c r="L18" s="18">
-        <f t="shared" si="14"/>
-        <v>0.97342790120887535</v>
-      </c>
-      <c r="M18" s="18">
-        <f t="shared" si="15"/>
-        <v>8.1399633413665878E-2</v>
-      </c>
+        <v>128052</v>
+      </c>
+      <c r="I18" s="17"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
       <c r="N18" s="13"/>
       <c r="O18" s="13">
-        <v>3.0000000000000001E-3</v>
+        <v>3.2669999999999999E-3</v>
       </c>
       <c r="P18" s="13">
-        <v>0.25640000000000002</v>
+        <v>0.255467</v>
       </c>
       <c r="Q18" s="13">
-        <v>0.78226700000000005</v>
+        <v>0.78813299999999997</v>
       </c>
       <c r="R18" s="13">
-        <v>0.97246699999999997</v>
+        <v>0.96993300000000005</v>
       </c>
       <c r="S18" s="13">
-        <v>0.99746699999999999</v>
+        <v>0.99733300000000003</v>
       </c>
       <c r="T18" s="13">
         <v>1</v>
@@ -5530,7 +5483,7 @@
         <v>12</v>
       </c>
       <c r="AB18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="2:28">
@@ -5541,19 +5494,19 @@
         <v>4992</v>
       </c>
       <c r="D19" s="16">
-        <v>1144277</v>
+        <v>2310406</v>
       </c>
       <c r="E19" s="16">
-        <v>13574233</v>
+        <v>27264893</v>
       </c>
       <c r="F19" s="16">
-        <v>9309472</v>
+        <v>9298590</v>
       </c>
       <c r="G19" s="16">
-        <v>51209</v>
+        <v>51079</v>
       </c>
       <c r="H19" s="16">
-        <v>159256</v>
+        <v>167360</v>
       </c>
       <c r="I19" s="17"/>
       <c r="J19" s="18"/>
@@ -5562,22 +5515,22 @@
       <c r="M19" s="18"/>
       <c r="N19" s="13"/>
       <c r="O19" s="19">
-        <v>4.2067E-2</v>
+        <v>4.0264000000000001E-2</v>
       </c>
       <c r="P19" s="19">
-        <v>0.57211500000000004</v>
+        <v>0.56690700000000005</v>
       </c>
       <c r="Q19" s="19">
-        <v>0.93429499999999999</v>
+        <v>0.93529600000000002</v>
       </c>
       <c r="R19" s="19">
         <v>0.99419100000000005</v>
       </c>
       <c r="S19" s="19">
-        <v>0.99859799999999999</v>
+        <v>0.99980000000000002</v>
       </c>
       <c r="T19" s="19">
-        <v>0.99980000000000002</v>
+        <v>1</v>
       </c>
       <c r="U19" s="13">
         <v>1</v>
@@ -5601,7 +5554,7 @@
         <v>12</v>
       </c>
       <c r="AB19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="2:28">
@@ -5612,19 +5565,19 @@
         <v>996</v>
       </c>
       <c r="D20" s="10">
-        <v>3271445</v>
+        <v>2561291</v>
       </c>
       <c r="E20" s="10">
-        <v>38366544</v>
+        <v>29787648</v>
       </c>
       <c r="F20" s="10">
-        <v>1942471</v>
+        <v>2013448</v>
       </c>
       <c r="G20" s="10">
-        <v>53842</v>
+        <v>56078</v>
       </c>
       <c r="H20" s="10">
-        <v>153196</v>
+        <v>149496</v>
       </c>
       <c r="I20" s="17"/>
       <c r="J20" s="18"/>
@@ -5633,16 +5586,16 @@
       <c r="M20" s="18"/>
       <c r="N20" s="13"/>
       <c r="O20" s="13">
-        <v>5.5220999999999999E-2</v>
+        <v>6.4256999999999995E-2</v>
       </c>
       <c r="P20" s="13">
-        <v>0.59738999999999998</v>
+        <v>0.64457799999999998</v>
       </c>
       <c r="Q20" s="13">
-        <v>0.95281099999999996</v>
+        <v>0.96184700000000001</v>
       </c>
       <c r="R20" s="13">
-        <v>0.998996</v>
+        <v>1</v>
       </c>
       <c r="S20" s="13">
         <v>1</v>
@@ -5672,21 +5625,21 @@
         <v>12</v>
       </c>
       <c r="AB20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="2:28">
       <c r="G22" s="24">
         <f>SUM(G15:G20)</f>
-        <v>203974</v>
+        <v>206416</v>
       </c>
       <c r="H22" s="24">
         <f>SUM(H15:H20)</f>
-        <v>733848</v>
-      </c>
-      <c r="M22" s="32">
+        <v>751824</v>
+      </c>
+      <c r="M22" s="38">
         <f>SUM(M15:M20)</f>
-        <v>9.0783154674781874E-2</v>
+        <v>0</v>
       </c>
       <c r="N22" s="26">
         <f>SUM(N15:N20)/6</f>
@@ -5694,46 +5647,46 @@
       </c>
       <c r="O22" s="26">
         <f>SUM(O15:O20)/6</f>
-        <v>1.7021333333333333E-2</v>
+        <v>1.8309666666666665E-2</v>
       </c>
       <c r="P22" s="26">
-        <f t="shared" ref="P22:Y22" si="16">SUM(P15:P20)/6</f>
-        <v>0.27878316666666669</v>
-      </c>
-      <c r="Q22" s="33">
-        <f t="shared" si="16"/>
-        <v>0.67804549999999997</v>
+        <f t="shared" ref="P22:Y22" si="11">SUM(P15:P20)/6</f>
+        <v>0.28625950000000006</v>
+      </c>
+      <c r="Q22" s="39">
+        <f t="shared" si="11"/>
+        <v>0.67940433333333328</v>
       </c>
       <c r="R22" s="26">
-        <f t="shared" si="16"/>
-        <v>0.91235733333333335</v>
+        <f t="shared" si="11"/>
+        <v>0.9116008333333333</v>
       </c>
       <c r="S22" s="26">
-        <f t="shared" si="16"/>
-        <v>0.9835976666666667</v>
+        <f t="shared" si="11"/>
+        <v>0.98379633333333327</v>
       </c>
       <c r="T22" s="26">
-        <f t="shared" si="16"/>
-        <v>0.99773699999999999</v>
+        <f t="shared" si="11"/>
+        <v>0.99779800000000007</v>
       </c>
       <c r="U22" s="26">
-        <f t="shared" si="16"/>
-        <v>0.99978566666666657</v>
+        <f t="shared" si="11"/>
+        <v>0.99978866666666677</v>
       </c>
       <c r="V22" s="26">
-        <f t="shared" si="16"/>
-        <v>0.99999400000000005</v>
+        <f t="shared" si="11"/>
+        <v>0.99999299999999991</v>
       </c>
       <c r="W22" s="26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X22" s="26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="Y22" s="26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update to version 2.4.2
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -315,8 +315,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="547">
+  <cellStyleXfs count="549">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -950,7 +952,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="547">
+  <cellStyles count="549">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1224,6 +1226,7 @@
     <cellStyle name="Followed Hyperlink" xfId="542" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="544" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="546" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="548" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1497,6 +1500,7 @@
     <cellStyle name="Hyperlink" xfId="541" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="543" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="545" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="547" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -1860,7 +1864,7 @@
   <dimension ref="A1:AE64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Update to version 2.4.6
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="47020" windowHeight="18620" tabRatio="500"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="29">
   <si>
     <t>Method</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>2.3.16</t>
+  </si>
+  <si>
+    <t>2.4.5</t>
   </si>
 </sst>
 </file>
@@ -315,8 +318,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="549">
+  <cellStyleXfs count="575">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -911,12 +940,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -925,12 +948,6 @@
     <xf numFmtId="166" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -939,20 +956,32 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="549">
+  <cellStyles count="575">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1227,6 +1256,19 @@
     <cellStyle name="Followed Hyperlink" xfId="544" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="546" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="548" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="550" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="552" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="554" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="556" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="560" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="572" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="574" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1501,29 +1543,22 @@
     <cellStyle name="Hyperlink" xfId="543" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="545" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="547" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="549" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="551" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="553" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="555" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="559" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="571" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="573" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1863,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1872,7 +1907,7 @@
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
     <col min="5" max="5" width="12.5" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="9.5" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" customWidth="1"/>
     <col min="10" max="10" width="14.6640625" customWidth="1"/>
     <col min="12" max="12" width="13.6640625" customWidth="1"/>
@@ -1898,24 +1933,24 @@
       <c r="K1" s="22"/>
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
-      <c r="N1" s="42" t="s">
+      <c r="N1" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="42"/>
-      <c r="V1" s="42"/>
-      <c r="W1" s="42"/>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="42"/>
-      <c r="Z1" s="42"/>
-      <c r="AA1" s="43"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="42"/>
+      <c r="AC1" s="42"/>
     </row>
     <row r="2" spans="1:31" s="1" customFormat="1" ht="56" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -1974,7 +2009,7 @@
       <c r="R2" s="7">
         <v>4096</v>
       </c>
-      <c r="S2" s="40">
+      <c r="S2" s="36">
         <v>2048</v>
       </c>
       <c r="T2" s="7">
@@ -2184,22 +2219,22 @@
       <c r="C5" s="24"/>
     </row>
     <row r="6" spans="1:31">
-      <c r="N6" s="42" t="s">
+      <c r="N6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="42"/>
-      <c r="V6" s="42"/>
-      <c r="W6" s="42"/>
-      <c r="X6" s="42"/>
-      <c r="Y6" s="42"/>
-      <c r="Z6" s="42"/>
-      <c r="AA6" s="43"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="45"/>
+      <c r="U6" s="45"/>
+      <c r="V6" s="45"/>
+      <c r="W6" s="45"/>
+      <c r="X6" s="45"/>
+      <c r="Y6" s="45"/>
+      <c r="Z6" s="45"/>
+      <c r="AA6" s="46"/>
     </row>
     <row r="7" spans="1:31" ht="45">
       <c r="A7" s="2" t="s">
@@ -2258,7 +2293,7 @@
       <c r="R7" s="7">
         <v>4096</v>
       </c>
-      <c r="S7" s="40">
+      <c r="S7" s="36">
         <v>2048</v>
       </c>
       <c r="T7" s="7">
@@ -2465,7 +2500,7 @@
       <c r="AE9" s="20"/>
     </row>
     <row r="10" spans="1:31">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="43" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="15">
@@ -2554,7 +2589,7 @@
       </c>
     </row>
     <row r="11" spans="1:31">
-      <c r="A11" s="37"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="9">
         <v>2</v>
       </c>
@@ -2641,7 +2676,7 @@
       </c>
     </row>
     <row r="12" spans="1:31">
-      <c r="A12" s="37"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="15">
         <v>3</v>
       </c>
@@ -2730,7 +2765,7 @@
       </c>
     </row>
     <row r="13" spans="1:31">
-      <c r="A13" s="37"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="9">
         <v>4</v>
       </c>
@@ -2819,7 +2854,7 @@
       </c>
     </row>
     <row r="14" spans="1:31">
-      <c r="A14" s="37"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="15">
         <v>5</v>
       </c>
@@ -2908,7 +2943,7 @@
       </c>
     </row>
     <row r="15" spans="1:31">
-      <c r="A15" s="37"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="9">
         <v>6</v>
       </c>
@@ -2997,7 +3032,7 @@
       </c>
     </row>
     <row r="16" spans="1:31">
-      <c r="A16" s="37"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="15">
         <v>7</v>
       </c>
@@ -3088,7 +3123,7 @@
       </c>
     </row>
     <row r="17" spans="1:31">
-      <c r="A17" s="37"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="9">
         <v>8</v>
       </c>
@@ -3177,53 +3212,53 @@
       </c>
     </row>
     <row r="18" spans="1:31">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="44"/>
-      <c r="O18" s="44"/>
-      <c r="P18" s="45"/>
-      <c r="Q18" s="45"/>
-      <c r="R18" s="45"/>
-      <c r="S18" s="45"/>
-      <c r="T18" s="45"/>
-      <c r="U18" s="45"/>
-      <c r="V18" s="45"/>
-      <c r="W18" s="45"/>
-      <c r="X18" s="45"/>
-      <c r="Y18" s="45"/>
-      <c r="Z18" s="45"/>
-      <c r="AA18" s="46"/>
-      <c r="AB18" s="35"/>
-      <c r="AC18" s="31"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="39"/>
+      <c r="Q18" s="39"/>
+      <c r="R18" s="39"/>
+      <c r="S18" s="39"/>
+      <c r="T18" s="39"/>
+      <c r="U18" s="39"/>
+      <c r="V18" s="39"/>
+      <c r="W18" s="39"/>
+      <c r="X18" s="39"/>
+      <c r="Y18" s="39"/>
+      <c r="Z18" s="39"/>
+      <c r="AA18" s="40"/>
+      <c r="AB18" s="33"/>
+      <c r="AC18" s="29"/>
     </row>
     <row r="19" spans="1:31">
-      <c r="N19" s="42" t="s">
+      <c r="N19" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="O19" s="42"/>
-      <c r="P19" s="42"/>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="42"/>
-      <c r="S19" s="42"/>
-      <c r="T19" s="42"/>
-      <c r="U19" s="42"/>
-      <c r="V19" s="42"/>
-      <c r="W19" s="42"/>
-      <c r="X19" s="42"/>
-      <c r="Y19" s="42"/>
-      <c r="Z19" s="42"/>
-      <c r="AA19" s="43"/>
+      <c r="O19" s="45"/>
+      <c r="P19" s="45"/>
+      <c r="Q19" s="45"/>
+      <c r="R19" s="45"/>
+      <c r="S19" s="45"/>
+      <c r="T19" s="45"/>
+      <c r="U19" s="45"/>
+      <c r="V19" s="45"/>
+      <c r="W19" s="45"/>
+      <c r="X19" s="45"/>
+      <c r="Y19" s="45"/>
+      <c r="Z19" s="45"/>
+      <c r="AA19" s="46"/>
     </row>
     <row r="20" spans="1:31" ht="45">
       <c r="A20" s="2" t="s">
@@ -3282,7 +3317,7 @@
       <c r="R20" s="7">
         <v>4096</v>
       </c>
-      <c r="S20" s="40">
+      <c r="S20" s="36">
         <v>2048</v>
       </c>
       <c r="T20" s="7">
@@ -3489,7 +3524,7 @@
       <c r="AE22" s="20"/>
     </row>
     <row r="23" spans="1:31">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="43" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="15">
@@ -3513,11 +3548,26 @@
       <c r="H23" s="16">
         <v>76068</v>
       </c>
-      <c r="I23" s="11"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
+      <c r="I23" s="11">
+        <f t="shared" ref="I23" si="20">E23/C23</f>
+        <v>8.9498167882744504</v>
+      </c>
+      <c r="J23" s="12">
+        <f t="shared" ref="J23" si="21">D23/C23</f>
+        <v>0.29773505504352277</v>
+      </c>
+      <c r="K23" s="11">
+        <f t="shared" ref="K23" si="22">F23/C23</f>
+        <v>666.25878456221199</v>
+      </c>
+      <c r="L23" s="12">
+        <f t="shared" ref="L23" si="23">I23/K23</f>
+        <v>1.3432943768471635E-2</v>
+      </c>
+      <c r="M23" s="12">
+        <f t="shared" ref="M23" si="24">J23/K23</f>
+        <v>4.4687599164513786E-4</v>
+      </c>
       <c r="N23" s="12"/>
       <c r="O23" s="12"/>
       <c r="P23" s="13"/>
@@ -3563,7 +3613,7 @@
       </c>
     </row>
     <row r="24" spans="1:31">
-      <c r="A24" s="37"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="9">
         <v>2</v>
       </c>
@@ -3585,11 +3635,26 @@
       <c r="H24" s="10">
         <v>93348</v>
       </c>
-      <c r="I24" s="11"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
+      <c r="I24" s="11">
+        <f t="shared" ref="I24:I30" si="25">E24/C24</f>
+        <v>70.758532389068932</v>
+      </c>
+      <c r="J24" s="12">
+        <f t="shared" ref="J24:J30" si="26">D24/C24</f>
+        <v>2.0811427199615893</v>
+      </c>
+      <c r="K24" s="11">
+        <f t="shared" ref="K24:K30" si="27">F24/C24</f>
+        <v>817.61108110270879</v>
+      </c>
+      <c r="L24" s="12">
+        <f t="shared" ref="L24:L30" si="28">I24/K24</f>
+        <v>8.6543020299623616E-2</v>
+      </c>
+      <c r="M24" s="12">
+        <f t="shared" ref="M24:M30" si="29">J24/K24</f>
+        <v>2.5453944645108775E-3</v>
+      </c>
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
       <c r="P24" s="13"/>
@@ -3637,7 +3702,7 @@
       </c>
     </row>
     <row r="25" spans="1:31">
-      <c r="A25" s="37"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="15">
         <v>3</v>
       </c>
@@ -3659,11 +3724,26 @@
       <c r="H25" s="16">
         <v>127768</v>
       </c>
-      <c r="I25" s="11"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
+      <c r="I25" s="11">
+        <f t="shared" si="25"/>
+        <v>119.47580451488953</v>
+      </c>
+      <c r="J25" s="12">
+        <f t="shared" si="26"/>
+        <v>3.5041026256804355</v>
+      </c>
+      <c r="K25" s="11">
+        <f t="shared" si="27"/>
+        <v>1210.6780339417228</v>
+      </c>
+      <c r="L25" s="12">
+        <f t="shared" si="28"/>
+        <v>9.8685035298691659E-2</v>
+      </c>
+      <c r="M25" s="12">
+        <f t="shared" si="29"/>
+        <v>2.8943307200113197E-3</v>
+      </c>
       <c r="N25" s="12"/>
       <c r="O25" s="12"/>
       <c r="P25" s="13"/>
@@ -3711,7 +3791,7 @@
       </c>
     </row>
     <row r="26" spans="1:31">
-      <c r="A26" s="37"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="9">
         <v>4</v>
       </c>
@@ -3733,11 +3813,26 @@
       <c r="H26" s="10">
         <v>129124</v>
       </c>
-      <c r="I26" s="11"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
+      <c r="I26" s="11">
+        <f t="shared" si="25"/>
+        <v>2613.3407451923076</v>
+      </c>
+      <c r="J26" s="12">
+        <f t="shared" si="26"/>
+        <v>74.483774038461533</v>
+      </c>
+      <c r="K26" s="11">
+        <f t="shared" si="27"/>
+        <v>1299.7485977564102</v>
+      </c>
+      <c r="L26" s="12">
+        <f t="shared" si="28"/>
+        <v>2.0106509441159495</v>
+      </c>
+      <c r="M26" s="12">
+        <f t="shared" si="29"/>
+        <v>5.7306293053159166E-2</v>
+      </c>
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
       <c r="P26" s="13"/>
@@ -3785,7 +3880,7 @@
       </c>
     </row>
     <row r="27" spans="1:31">
-      <c r="A27" s="37"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="15">
         <v>5</v>
       </c>
@@ -3807,11 +3902,26 @@
       <c r="H27" s="16">
         <v>153232</v>
       </c>
-      <c r="I27" s="11"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
+      <c r="I27" s="11">
+        <f t="shared" si="25"/>
+        <v>4304.3486312399355</v>
+      </c>
+      <c r="J27" s="12">
+        <f t="shared" si="26"/>
+        <v>124.64110305958133</v>
+      </c>
+      <c r="K27" s="11">
+        <f t="shared" si="27"/>
+        <v>1829.4609500805152</v>
+      </c>
+      <c r="L27" s="12">
+        <f t="shared" si="28"/>
+        <v>2.3527961233884218</v>
+      </c>
+      <c r="M27" s="12">
+        <f t="shared" si="29"/>
+        <v>6.8129960934173436E-2</v>
+      </c>
       <c r="N27" s="12"/>
       <c r="O27" s="12"/>
       <c r="P27" s="13"/>
@@ -3859,7 +3969,7 @@
       </c>
     </row>
     <row r="28" spans="1:31">
-      <c r="A28" s="37"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="9">
         <v>6</v>
       </c>
@@ -3881,11 +3991,26 @@
       <c r="H28" s="10">
         <v>145168</v>
       </c>
-      <c r="I28" s="11"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
+      <c r="I28" s="11">
+        <f t="shared" si="25"/>
+        <v>84211.419753086418</v>
+      </c>
+      <c r="J28" s="12">
+        <f t="shared" si="26"/>
+        <v>2455.2633744855966</v>
+      </c>
+      <c r="K28" s="11">
+        <f t="shared" si="27"/>
+        <v>1925.2448559670781</v>
+      </c>
+      <c r="L28" s="12">
+        <f t="shared" si="28"/>
+        <v>43.740628363235288</v>
+      </c>
+      <c r="M28" s="12">
+        <f t="shared" si="29"/>
+        <v>1.2752992778429124</v>
+      </c>
       <c r="N28" s="12"/>
       <c r="O28" s="12"/>
       <c r="P28" s="13"/>
@@ -3933,7 +4058,7 @@
       </c>
     </row>
     <row r="29" spans="1:31">
-      <c r="A29" s="37"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="15">
         <v>7</v>
       </c>
@@ -3955,11 +4080,26 @@
       <c r="H29" s="16">
         <v>159720</v>
       </c>
-      <c r="I29" s="11"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
+      <c r="I29" s="11">
+        <f t="shared" si="25"/>
+        <v>127159.45277777778</v>
+      </c>
+      <c r="J29" s="12">
+        <f t="shared" si="26"/>
+        <v>3764.4291666666668</v>
+      </c>
+      <c r="K29" s="11">
+        <f t="shared" si="27"/>
+        <v>2337.6361111111109</v>
+      </c>
+      <c r="L29" s="12">
+        <f t="shared" si="28"/>
+        <v>54.396598415540872</v>
+      </c>
+      <c r="M29" s="12">
+        <f t="shared" si="29"/>
+        <v>1.6103572103347519</v>
+      </c>
       <c r="N29" s="12"/>
       <c r="O29" s="12"/>
       <c r="P29" s="13"/>
@@ -4007,7 +4147,7 @@
       </c>
     </row>
     <row r="30" spans="1:31">
-      <c r="A30" s="37"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="9">
         <v>8</v>
       </c>
@@ -4029,11 +4169,26 @@
       <c r="H30" s="10">
         <v>151736</v>
       </c>
-      <c r="I30" s="11"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
+      <c r="I30" s="11">
+        <f t="shared" si="25"/>
+        <v>2336001.2453703703</v>
+      </c>
+      <c r="J30" s="12">
+        <f t="shared" si="26"/>
+        <v>69477.277777777781</v>
+      </c>
+      <c r="K30" s="11">
+        <f t="shared" si="27"/>
+        <v>2457.3611111111113</v>
+      </c>
+      <c r="L30" s="12">
+        <f t="shared" si="28"/>
+        <v>950.6137436651029</v>
+      </c>
+      <c r="M30" s="12">
+        <f t="shared" si="29"/>
+        <v>28.273124964675294</v>
+      </c>
       <c r="N30" s="12"/>
       <c r="O30" s="12"/>
       <c r="P30" s="13"/>
@@ -4083,9 +4238,9 @@
     <row r="32" spans="1:31">
       <c r="G32" s="24"/>
       <c r="H32" s="24"/>
-      <c r="M32" s="38"/>
-      <c r="N32" s="38"/>
-      <c r="O32" s="38"/>
+      <c r="M32" s="34"/>
+      <c r="N32" s="34"/>
+      <c r="O32" s="34"/>
       <c r="P32" s="26"/>
       <c r="Q32" s="26"/>
       <c r="R32" s="26"/>
@@ -4104,63 +4259,63 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>249984</v>
+        <v>99996</v>
       </c>
       <c r="D33">
-        <v>74429</v>
+        <v>33331</v>
       </c>
       <c r="E33">
-        <v>2237311</v>
+        <v>303064</v>
       </c>
       <c r="F33">
-        <v>166554036</v>
+        <v>67148229</v>
       </c>
       <c r="G33">
-        <v>15037</v>
+        <v>15202</v>
       </c>
       <c r="H33">
-        <v>76068</v>
+        <v>73332</v>
       </c>
       <c r="I33" s="11">
-        <f t="shared" ref="I33:I34" si="20">E33/C33</f>
-        <v>8.9498167882744504</v>
+        <f t="shared" ref="I33:I40" si="30">E33/C33</f>
+        <v>3.030761230449218</v>
       </c>
       <c r="J33" s="12">
-        <f t="shared" ref="J33:J34" si="21">D33/C33</f>
-        <v>0.29773505504352277</v>
+        <f t="shared" ref="J33:J40" si="31">D33/C33</f>
+        <v>0.33332333293331734</v>
       </c>
       <c r="K33" s="11">
-        <f t="shared" ref="K33:K34" si="22">F33/C33</f>
-        <v>666.25878456221199</v>
+        <f t="shared" ref="K33:K40" si="32">F33/C33</f>
+        <v>671.50915036601464</v>
       </c>
       <c r="L33" s="12">
-        <f t="shared" ref="L33:L34" si="23">I33/K33</f>
-        <v>1.3432943768471635E-2</v>
+        <f t="shared" ref="L33:L40" si="33">I33/K33</f>
+        <v>4.513358051483383E-3</v>
       </c>
       <c r="M33" s="12">
-        <f t="shared" ref="M33:M34" si="24">J33/K33</f>
-        <v>4.4687599164513786E-4</v>
+        <f t="shared" ref="M33:M40" si="34">J33/K33</f>
+        <v>4.9637943541295778E-4</v>
       </c>
       <c r="R33" s="26">
-        <v>8.1810000000000008E-3</v>
+        <v>7.6899999999999998E-3</v>
       </c>
       <c r="S33" s="26">
-        <v>0.25541999999999998</v>
+        <v>0.26456099999999999</v>
       </c>
       <c r="T33" s="26">
-        <v>0.71959399999999996</v>
+        <v>0.73008899999999999</v>
       </c>
       <c r="U33" s="26">
-        <v>0.93702399999999997</v>
+        <v>0.93991800000000003</v>
       </c>
       <c r="V33" s="26">
-        <v>0.98983900000000002</v>
+        <v>0.99068000000000001</v>
       </c>
       <c r="W33" s="26">
-        <v>0.99878</v>
+        <v>0.99902999999999997</v>
       </c>
       <c r="X33" s="26">
-        <v>0.99995599999999996</v>
+        <v>0.99995000000000001</v>
       </c>
       <c r="Y33" s="27">
         <v>1</v>
@@ -4172,13 +4327,13 @@
         <v>1</v>
       </c>
       <c r="AB33" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="AC33">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="AD33" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="2:30" ht="18" customHeight="1">
@@ -4186,111 +4341,598 @@
         <v>2</v>
       </c>
       <c r="C34">
-        <v>99972</v>
+        <v>49992</v>
       </c>
       <c r="D34">
-        <v>208056</v>
+        <v>116281</v>
       </c>
       <c r="E34">
-        <v>7073872</v>
+        <v>1342565</v>
       </c>
       <c r="F34">
-        <v>81738215</v>
+        <v>41000965</v>
       </c>
       <c r="G34">
-        <v>19275</v>
+        <v>19381</v>
       </c>
       <c r="H34">
-        <v>93348</v>
+        <v>104388</v>
       </c>
       <c r="I34" s="11">
-        <f t="shared" si="20"/>
-        <v>70.758532389068932</v>
+        <f t="shared" si="30"/>
+        <v>26.855596895503279</v>
       </c>
       <c r="J34" s="12">
-        <f t="shared" si="21"/>
-        <v>2.0811427199615893</v>
+        <f t="shared" si="31"/>
+        <v>2.3259921587453993</v>
       </c>
       <c r="K34" s="11">
-        <f t="shared" si="22"/>
-        <v>817.61108110270879</v>
+        <f t="shared" si="32"/>
+        <v>820.15052408385338</v>
       </c>
       <c r="L34" s="12">
-        <f t="shared" si="23"/>
-        <v>8.6543020299623616E-2</v>
+        <f t="shared" si="33"/>
+        <v>3.27447171060486E-2</v>
       </c>
       <c r="M34" s="12">
-        <f t="shared" si="24"/>
-        <v>2.5453944645108775E-3</v>
+        <f t="shared" si="34"/>
+        <v>2.8360552001641913E-3</v>
       </c>
       <c r="Q34" s="26">
-        <v>1.0000000000000001E-5</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="R34" s="26">
-        <v>3.0328000000000001E-2</v>
+        <v>3.1605000000000001E-2</v>
       </c>
       <c r="S34" s="26">
-        <v>0.41298600000000002</v>
+        <v>0.42150700000000002</v>
       </c>
       <c r="T34" s="26">
-        <v>0.835094</v>
+        <v>0.83889400000000003</v>
       </c>
       <c r="U34" s="26">
-        <v>0.97238199999999997</v>
+        <v>0.972916</v>
       </c>
       <c r="V34" s="26">
-        <v>0.99698900000000001</v>
+        <v>0.99707999999999997</v>
       </c>
       <c r="W34" s="26">
-        <v>0.99978999999999996</v>
+        <v>0.99980000000000002</v>
       </c>
       <c r="X34" s="26">
-        <v>0.99999000000000005</v>
-      </c>
-      <c r="Y34" s="47">
-        <v>1</v>
-      </c>
-      <c r="Z34" s="47">
-        <v>1</v>
-      </c>
-      <c r="AA34" s="47">
+        <v>1</v>
+      </c>
+      <c r="Y34" s="41">
+        <v>1</v>
+      </c>
+      <c r="Z34" s="41">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="41">
         <v>1</v>
       </c>
       <c r="AB34" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="AC34">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="AD34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="2:30" ht="17" customHeight="1">
-      <c r="Y35" s="25"/>
-      <c r="Z35" s="25"/>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>24996</v>
+      </c>
+      <c r="D35">
+        <v>167124</v>
+      </c>
+      <c r="E35">
+        <v>1959317</v>
+      </c>
+      <c r="F35">
+        <v>29904421</v>
+      </c>
+      <c r="G35">
+        <v>30615</v>
+      </c>
+      <c r="H35">
+        <v>126960</v>
+      </c>
+      <c r="I35" s="11">
+        <f t="shared" si="30"/>
+        <v>78.385221635461676</v>
+      </c>
+      <c r="J35" s="12">
+        <f t="shared" si="31"/>
+        <v>6.6860297647623623</v>
+      </c>
+      <c r="K35" s="11">
+        <f t="shared" si="32"/>
+        <v>1196.3682589214275</v>
+      </c>
+      <c r="L35" s="12">
+        <f t="shared" si="33"/>
+        <v>6.5519309001167425E-2</v>
+      </c>
+      <c r="M35" s="12">
+        <f t="shared" si="34"/>
+        <v>5.5886051095923239E-3</v>
+      </c>
+      <c r="Q35" s="26">
+        <v>1.1199999999999999E-3</v>
+      </c>
+      <c r="R35" s="26">
+        <v>0.203233</v>
+      </c>
+      <c r="S35" s="26">
+        <v>0.72839699999999996</v>
+      </c>
+      <c r="T35" s="26">
+        <v>0.95127200000000001</v>
+      </c>
+      <c r="U35" s="26">
+        <v>0.99459900000000001</v>
+      </c>
+      <c r="V35" s="26">
+        <v>0.99972000000000005</v>
+      </c>
+      <c r="W35" s="26">
+        <v>0.99995999999999996</v>
+      </c>
+      <c r="X35" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y35" s="25">
+        <v>1</v>
+      </c>
+      <c r="Z35" s="25">
+        <v>1</v>
+      </c>
+      <c r="AA35" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC35">
+        <v>12</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="36" spans="2:30">
-      <c r="Y36" s="25"/>
-      <c r="Z36" s="25"/>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>15000</v>
+      </c>
+      <c r="D36">
+        <v>1370228</v>
+      </c>
+      <c r="E36">
+        <v>16333695</v>
+      </c>
+      <c r="F36">
+        <v>19279774</v>
+      </c>
+      <c r="G36">
+        <v>33235</v>
+      </c>
+      <c r="H36">
+        <v>127012</v>
+      </c>
+      <c r="I36" s="11">
+        <f t="shared" si="30"/>
+        <v>1088.913</v>
+      </c>
+      <c r="J36" s="12">
+        <f t="shared" si="31"/>
+        <v>91.348533333333336</v>
+      </c>
+      <c r="K36" s="11">
+        <f t="shared" si="32"/>
+        <v>1285.3182666666667</v>
+      </c>
+      <c r="L36" s="12">
+        <f t="shared" si="33"/>
+        <v>0.8471932814150207</v>
+      </c>
+      <c r="M36" s="12">
+        <f t="shared" si="34"/>
+        <v>7.1070750103191041E-2</v>
+      </c>
+      <c r="Q36" s="26">
+        <v>2E-3</v>
+      </c>
+      <c r="R36" s="26">
+        <v>0.24773300000000001</v>
+      </c>
+      <c r="S36" s="26">
+        <v>0.77793299999999999</v>
+      </c>
+      <c r="T36" s="26">
+        <v>0.96846699999999997</v>
+      </c>
+      <c r="U36" s="26">
+        <v>0.99719999999999998</v>
+      </c>
+      <c r="V36" s="26">
+        <v>0.99980000000000002</v>
+      </c>
+      <c r="W36" s="27">
+        <v>1</v>
+      </c>
+      <c r="X36" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y36" s="25">
+        <v>1</v>
+      </c>
+      <c r="Z36" s="25">
+        <v>1</v>
+      </c>
+      <c r="AA36" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC36">
+        <v>12</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="37" spans="2:30">
-      <c r="Y37" s="25"/>
-      <c r="Z37" s="25"/>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <v>4992</v>
+      </c>
+      <c r="D37">
+        <v>1090481</v>
+      </c>
+      <c r="E37">
+        <v>12790402</v>
+      </c>
+      <c r="F37">
+        <v>9129459</v>
+      </c>
+      <c r="G37">
+        <v>50074</v>
+      </c>
+      <c r="H37">
+        <v>167856</v>
+      </c>
+      <c r="I37" s="11">
+        <f t="shared" si="30"/>
+        <v>2562.1798878205127</v>
+      </c>
+      <c r="J37" s="12">
+        <f t="shared" si="31"/>
+        <v>218.44571314102564</v>
+      </c>
+      <c r="K37" s="11">
+        <f t="shared" si="32"/>
+        <v>1828.8179086538462</v>
+      </c>
+      <c r="L37" s="12">
+        <f t="shared" si="33"/>
+        <v>1.4010032796028766</v>
+      </c>
+      <c r="M37" s="12">
+        <f t="shared" si="34"/>
+        <v>0.11944639874060445</v>
+      </c>
+      <c r="Q37" s="26">
+        <v>4.1667000000000003E-2</v>
+      </c>
+      <c r="R37" s="26">
+        <v>0.54787699999999995</v>
+      </c>
+      <c r="S37" s="26">
+        <v>0.92888599999999999</v>
+      </c>
+      <c r="T37" s="26">
+        <v>0.992788</v>
+      </c>
+      <c r="U37" s="27">
+        <v>1</v>
+      </c>
+      <c r="V37" s="27">
+        <v>1</v>
+      </c>
+      <c r="W37" s="27">
+        <v>1</v>
+      </c>
+      <c r="X37" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y37" s="25">
+        <v>1</v>
+      </c>
+      <c r="Z37" s="25">
+        <v>1</v>
+      </c>
+      <c r="AA37" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC37">
+        <v>12</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="38" spans="2:30">
-      <c r="Y38" s="25"/>
-      <c r="Z38" s="25"/>
+      <c r="B38">
+        <v>6</v>
+      </c>
+      <c r="C38">
+        <v>996</v>
+      </c>
+      <c r="D38">
+        <v>3237741</v>
+      </c>
+      <c r="E38">
+        <v>38160186</v>
+      </c>
+      <c r="F38">
+        <v>1955009</v>
+      </c>
+      <c r="G38">
+        <v>54299</v>
+      </c>
+      <c r="H38">
+        <v>150544</v>
+      </c>
+      <c r="I38" s="11">
+        <f t="shared" si="30"/>
+        <v>38313.439759036148</v>
+      </c>
+      <c r="J38" s="12">
+        <f t="shared" si="31"/>
+        <v>3250.7439759036147</v>
+      </c>
+      <c r="K38" s="11">
+        <f t="shared" si="32"/>
+        <v>1962.8604417670683</v>
+      </c>
+      <c r="L38" s="12">
+        <f t="shared" si="33"/>
+        <v>19.519186868193447</v>
+      </c>
+      <c r="M38" s="12">
+        <f t="shared" si="34"/>
+        <v>1.6561258797274079</v>
+      </c>
+      <c r="Q38" s="26">
+        <v>5.2208999999999998E-2</v>
+      </c>
+      <c r="R38" s="26">
+        <v>0.625502</v>
+      </c>
+      <c r="S38" s="26">
+        <v>0.95682699999999998</v>
+      </c>
+      <c r="T38" s="26">
+        <v>0.99598399999999998</v>
+      </c>
+      <c r="U38" s="27">
+        <v>1</v>
+      </c>
+      <c r="V38" s="27">
+        <v>1</v>
+      </c>
+      <c r="W38" s="27">
+        <v>1</v>
+      </c>
+      <c r="X38" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y38" s="25">
+        <v>1</v>
+      </c>
+      <c r="Z38" s="25">
+        <v>1</v>
+      </c>
+      <c r="AA38" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC38">
+        <v>12</v>
+      </c>
+      <c r="AD38" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="39" spans="2:30">
-      <c r="Y39" s="25"/>
-      <c r="Z39" s="25"/>
+      <c r="B39">
+        <v>7</v>
+      </c>
+      <c r="C39">
+        <v>744</v>
+      </c>
+      <c r="D39">
+        <v>4698521</v>
+      </c>
+      <c r="E39">
+        <v>54432674</v>
+      </c>
+      <c r="F39">
+        <v>1727792</v>
+      </c>
+      <c r="G39">
+        <v>65857</v>
+      </c>
+      <c r="H39">
+        <v>161692</v>
+      </c>
+      <c r="I39" s="11">
+        <f t="shared" si="30"/>
+        <v>73162.196236559146</v>
+      </c>
+      <c r="J39" s="12">
+        <f t="shared" si="31"/>
+        <v>6315.2163978494627</v>
+      </c>
+      <c r="K39" s="11">
+        <f t="shared" si="32"/>
+        <v>2322.3010752688174</v>
+      </c>
+      <c r="L39" s="12">
+        <f t="shared" si="33"/>
+        <v>31.504182216377899</v>
+      </c>
+      <c r="M39" s="12">
+        <f t="shared" si="34"/>
+        <v>2.719378837267449</v>
+      </c>
+      <c r="Q39" s="26">
+        <v>0.137097</v>
+      </c>
+      <c r="R39" s="26">
+        <v>0.74731199999999998</v>
+      </c>
+      <c r="S39" s="26">
+        <v>0.97311800000000004</v>
+      </c>
+      <c r="T39" s="26">
+        <v>0.99865599999999999</v>
+      </c>
+      <c r="U39" s="27">
+        <v>1</v>
+      </c>
+      <c r="V39" s="27">
+        <v>1</v>
+      </c>
+      <c r="W39" s="27">
+        <v>1</v>
+      </c>
+      <c r="X39" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y39" s="25">
+        <v>1</v>
+      </c>
+      <c r="Z39" s="25">
+        <v>1</v>
+      </c>
+      <c r="AA39" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC39">
+        <v>12</v>
+      </c>
+      <c r="AD39" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="40" spans="2:30">
-      <c r="Y40" s="25"/>
-      <c r="Z40" s="25"/>
+      <c r="B40">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>240</v>
+      </c>
+      <c r="D40">
+        <v>21036856</v>
+      </c>
+      <c r="E40">
+        <v>245116942</v>
+      </c>
+      <c r="F40">
+        <v>566226</v>
+      </c>
+      <c r="G40">
+        <v>67156</v>
+      </c>
+      <c r="H40">
+        <v>150316</v>
+      </c>
+      <c r="I40" s="11">
+        <f t="shared" si="30"/>
+        <v>1021320.5916666667</v>
+      </c>
+      <c r="J40" s="12">
+        <f t="shared" si="31"/>
+        <v>87653.566666666666</v>
+      </c>
+      <c r="K40" s="11">
+        <f t="shared" si="32"/>
+        <v>2359.2750000000001</v>
+      </c>
+      <c r="L40" s="12">
+        <f t="shared" si="33"/>
+        <v>432.89594967380515</v>
+      </c>
+      <c r="M40" s="12">
+        <f t="shared" si="34"/>
+        <v>37.152755260267099</v>
+      </c>
+      <c r="Q40" s="26">
+        <v>0.14583299999999999</v>
+      </c>
+      <c r="R40" s="26">
+        <v>0.77083299999999999</v>
+      </c>
+      <c r="S40" s="26">
+        <v>0.96666700000000005</v>
+      </c>
+      <c r="T40" s="26">
+        <v>0.99583299999999997</v>
+      </c>
+      <c r="U40" s="27">
+        <v>1</v>
+      </c>
+      <c r="V40" s="27">
+        <v>1</v>
+      </c>
+      <c r="W40" s="27">
+        <v>1</v>
+      </c>
+      <c r="X40" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y40" s="25">
+        <v>1</v>
+      </c>
+      <c r="Z40" s="25">
+        <v>1</v>
+      </c>
+      <c r="AA40" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC40">
+        <v>12</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="41" spans="2:30">
+      <c r="G41" s="24"/>
       <c r="Y41" s="25"/>
       <c r="Z41" s="25"/>
     </row>
@@ -4355,15 +4997,15 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="A10:A17"/>
     <mergeCell ref="A23:A30"/>
     <mergeCell ref="N1:AA1"/>
     <mergeCell ref="N6:AA6"/>
     <mergeCell ref="N19:AA19"/>
-    <mergeCell ref="AB1:AC1"/>
   </mergeCells>
   <conditionalFormatting sqref="F68:F73">
-    <cfRule type="cellIs" dxfId="1" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="37" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4846,20 +5488,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
-      <c r="N1" s="28" t="s">
+      <c r="N1" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
     </row>
     <row r="2" spans="1:28" ht="60">
       <c r="A2" s="2" t="s">
@@ -4910,7 +5552,7 @@
       <c r="P2" s="7">
         <v>4096</v>
       </c>
-      <c r="Q2" s="41">
+      <c r="Q2" s="37">
         <v>2048</v>
       </c>
       <c r="R2" s="7">
@@ -4948,7 +5590,7 @@
       </c>
     </row>
     <row r="3" spans="1:28">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="43" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="15">
@@ -5035,7 +5677,7 @@
       </c>
     </row>
     <row r="4" spans="1:28">
-      <c r="A4" s="37"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="9">
         <v>2</v>
       </c>
@@ -5120,7 +5762,7 @@
       </c>
     </row>
     <row r="5" spans="1:28">
-      <c r="A5" s="37"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="15">
         <v>3</v>
       </c>
@@ -5207,7 +5849,7 @@
       </c>
     </row>
     <row r="6" spans="1:28">
-      <c r="A6" s="37"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="9">
         <v>4</v>
       </c>
@@ -5294,7 +5936,7 @@
       </c>
     </row>
     <row r="7" spans="1:28">
-      <c r="A7" s="37"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="15">
         <v>5</v>
       </c>
@@ -5381,7 +6023,7 @@
       </c>
     </row>
     <row r="8" spans="1:28">
-      <c r="A8" s="37"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="9">
         <v>6</v>
       </c>
@@ -5476,7 +6118,7 @@
         <f>SUM(H3:H8)</f>
         <v>745476</v>
       </c>
-      <c r="M10" s="38">
+      <c r="M10" s="34">
         <f>SUM(M3:M8)</f>
         <v>1.8940001014309742</v>
       </c>
@@ -5492,7 +6134,7 @@
         <f t="shared" ref="P10:Y10" si="10">SUM(P3:P8)/6</f>
         <v>0.28283700000000001</v>
       </c>
-      <c r="Q10" s="39">
+      <c r="Q10" s="35">
         <f t="shared" si="10"/>
         <v>0.68294349999999993</v>
       </c>
@@ -5581,7 +6223,7 @@
       <c r="P14" s="7">
         <v>4096</v>
       </c>
-      <c r="Q14" s="40">
+      <c r="Q14" s="36">
         <v>2048</v>
       </c>
       <c r="R14" s="7">
@@ -6051,7 +6693,7 @@
         <f>SUM(H15:H20)</f>
         <v>751824</v>
       </c>
-      <c r="M22" s="38">
+      <c r="M22" s="34">
         <f>SUM(M15:M20)</f>
         <v>0</v>
       </c>
@@ -6067,7 +6709,7 @@
         <f t="shared" ref="P22:Y22" si="11">SUM(P15:P20)/6</f>
         <v>0.28625950000000006</v>
       </c>
-      <c r="Q22" s="39">
+      <c r="Q22" s="35">
         <f t="shared" si="11"/>
         <v>0.67940433333333328</v>
       </c>

</xml_diff>

<commit_message>
Latest results (version 2.4.7)
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="49980" windowHeight="25020" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="49980" windowHeight="25020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Random7" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="39">
   <si>
     <t>Method</t>
   </si>
@@ -104,12 +104,6 @@
     <t>1.0.0</t>
   </si>
   <si>
-    <t>2.3.16</t>
-  </si>
-  <si>
-    <t>2.4.5</t>
-  </si>
-  <si>
     <t>EVALUATION_TOUCHER_WEIGHT</t>
   </si>
   <si>
@@ -141,6 +135,9 @@
   </si>
   <si>
     <t>EVALUATION_CLOSE_WEIGHTS[1]</t>
+  </si>
+  <si>
+    <t>2.4.7</t>
   </si>
 </sst>
 </file>
@@ -352,8 +349,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="589">
+  <cellStyleXfs count="593">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1029,7 +1030,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="589">
+  <cellStyles count="593">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1324,6 +1325,8 @@
     <cellStyle name="Followed Hyperlink" xfId="584" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="586" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="592" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1618,6 +1621,8 @@
     <cellStyle name="Hyperlink" xfId="583" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="585" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="591" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -1990,11 +1995,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2088652520"/>
-        <c:axId val="-2085348936"/>
+        <c:axId val="-2056010296"/>
+        <c:axId val="-2056814552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2088652520"/>
+        <c:axId val="-2056010296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2003,7 +2008,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2085348936"/>
+        <c:crossAx val="-2056814552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2011,7 +2016,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2085348936"/>
+        <c:axId val="-2056814552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2022,7 +2027,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2088652520"/>
+        <c:crossAx val="-2056010296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2410,11 +2415,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2087070712"/>
-        <c:axId val="-2087067704"/>
+        <c:axId val="-2056788184"/>
+        <c:axId val="-2056785176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2087070712"/>
+        <c:axId val="-2056788184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2423,7 +2428,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2087067704"/>
+        <c:crossAx val="-2056785176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2431,7 +2436,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2087067704"/>
+        <c:axId val="-2056785176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2442,7 +2447,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2087070712"/>
+        <c:crossAx val="-2056788184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2570,11 +2575,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2087042968"/>
-        <c:axId val="-2087039960"/>
+        <c:axId val="-2056760440"/>
+        <c:axId val="-2056757432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2087042968"/>
+        <c:axId val="-2056760440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2583,7 +2588,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2087039960"/>
+        <c:crossAx val="-2056757432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2591,7 +2596,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2087039960"/>
+        <c:axId val="-2056757432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2602,7 +2607,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2087042968"/>
+        <c:crossAx val="-2056760440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2973,11 +2978,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2087015624"/>
-        <c:axId val="-2087012616"/>
+        <c:axId val="-2056733096"/>
+        <c:axId val="-2056730088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2087015624"/>
+        <c:axId val="-2056733096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2986,7 +2991,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2087012616"/>
+        <c:crossAx val="-2056730088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2994,7 +2999,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2087012616"/>
+        <c:axId val="-2056730088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3005,7 +3010,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2087015624"/>
+        <c:crossAx val="-2056733096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3391,11 +3396,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2078672504"/>
-        <c:axId val="2078675512"/>
+        <c:axId val="-2056718216"/>
+        <c:axId val="-2056715160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2078672504"/>
+        <c:axId val="-2056718216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3404,7 +3409,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2078675512"/>
+        <c:crossAx val="-2056715160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3412,7 +3417,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2078675512"/>
+        <c:axId val="-2056715160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3423,7 +3428,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2078672504"/>
+        <c:crossAx val="-2056718216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3921,8 +3926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5557,64 +5562,64 @@
         <v>249984</v>
       </c>
       <c r="D23" s="16">
-        <v>74429</v>
+        <v>75355</v>
       </c>
       <c r="E23" s="16">
-        <v>2237311</v>
+        <v>2186606</v>
       </c>
       <c r="F23" s="16">
-        <v>166554036</v>
+        <v>168136184</v>
       </c>
       <c r="G23" s="16">
-        <v>15037</v>
+        <v>15277</v>
       </c>
       <c r="H23" s="16">
-        <v>76068</v>
+        <v>75616</v>
       </c>
       <c r="I23" s="11">
-        <f t="shared" ref="I23" si="20">E23/C23</f>
-        <v>8.9498167882744504</v>
+        <f t="shared" ref="I23:I30" si="20">E23/C23</f>
+        <v>8.7469838069636463</v>
       </c>
       <c r="J23" s="12">
-        <f t="shared" ref="J23" si="21">D23/C23</f>
-        <v>0.29773505504352277</v>
+        <f t="shared" ref="J23:J30" si="21">D23/C23</f>
+        <v>0.30143929211469533</v>
       </c>
       <c r="K23" s="11">
-        <f t="shared" ref="K23" si="22">F23/C23</f>
-        <v>666.25878456221199</v>
+        <f t="shared" ref="K23:K30" si="22">F23/C23</f>
+        <v>672.58778161802354</v>
       </c>
       <c r="L23" s="12">
-        <f t="shared" ref="L23" si="23">I23/K23</f>
-        <v>1.3432943768471635E-2</v>
+        <f t="shared" ref="L23:L30" si="23">I23/K23</f>
+        <v>1.3004969828505209E-2</v>
       </c>
       <c r="M23" s="12">
-        <f t="shared" ref="M23" si="24">J23/K23</f>
-        <v>4.4687599164513786E-4</v>
+        <f t="shared" ref="M23:M30" si="24">J23/K23</f>
+        <v>4.4817836474747162E-4</v>
       </c>
       <c r="N23" s="12"/>
       <c r="O23" s="12"/>
       <c r="P23" s="13"/>
       <c r="Q23" s="13"/>
       <c r="R23" s="19">
-        <v>8.1810000000000008E-3</v>
+        <v>9.0570000000000008E-3</v>
       </c>
       <c r="S23" s="19">
-        <v>0.25541999999999998</v>
+        <v>0.27066099999999998</v>
       </c>
       <c r="T23" s="19">
-        <v>0.71959399999999996</v>
+        <v>0.729603</v>
       </c>
       <c r="U23" s="19">
-        <v>0.93702399999999997</v>
+        <v>0.93745999999999996</v>
       </c>
       <c r="V23" s="19">
-        <v>0.98983900000000002</v>
+        <v>0.98980699999999999</v>
       </c>
       <c r="W23" s="19">
-        <v>0.99878</v>
+        <v>0.99891200000000002</v>
       </c>
       <c r="X23" s="13">
-        <v>0.99995599999999996</v>
+        <v>0.99997999999999998</v>
       </c>
       <c r="Y23" s="13">
         <v>1</v>
@@ -5632,7 +5637,7 @@
         <v>36</v>
       </c>
       <c r="AD23" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:31">
@@ -5644,66 +5649,66 @@
         <v>99972</v>
       </c>
       <c r="D24" s="10">
-        <v>208056</v>
+        <v>197092</v>
       </c>
       <c r="E24" s="10">
-        <v>7073872</v>
+        <v>6497060</v>
       </c>
       <c r="F24" s="10">
-        <v>81738215</v>
+        <v>81875960</v>
       </c>
       <c r="G24" s="10">
-        <v>19275</v>
+        <v>19391</v>
       </c>
       <c r="H24" s="10">
-        <v>93348</v>
+        <v>106568</v>
       </c>
       <c r="I24" s="11">
-        <f t="shared" ref="I24:I30" si="25">E24/C24</f>
-        <v>70.758532389068932</v>
+        <f t="shared" si="20"/>
+        <v>64.988796863121678</v>
       </c>
       <c r="J24" s="12">
-        <f t="shared" ref="J24:J30" si="26">D24/C24</f>
-        <v>2.0811427199615893</v>
+        <f t="shared" si="21"/>
+        <v>1.9714720121634057</v>
       </c>
       <c r="K24" s="11">
-        <f t="shared" ref="K24:K30" si="27">F24/C24</f>
-        <v>817.61108110270879</v>
+        <f t="shared" si="22"/>
+        <v>818.9889168967311</v>
       </c>
       <c r="L24" s="12">
-        <f t="shared" ref="L24:L30" si="28">I24/K24</f>
-        <v>8.6543020299623616E-2</v>
+        <f t="shared" si="23"/>
+        <v>7.9352474157249581E-2</v>
       </c>
       <c r="M24" s="12">
-        <f t="shared" ref="M24:M30" si="29">J24/K24</f>
-        <v>2.5453944645108775E-3</v>
+        <f t="shared" si="24"/>
+        <v>2.4072023094446771E-3</v>
       </c>
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
       <c r="P24" s="13"/>
       <c r="Q24" s="13">
-        <v>1.0000000000000001E-5</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="R24" s="13">
-        <v>3.0328000000000001E-2</v>
+        <v>3.3409000000000001E-2</v>
       </c>
       <c r="S24" s="13">
-        <v>0.41298600000000002</v>
+        <v>0.42209799999999997</v>
       </c>
       <c r="T24" s="13">
-        <v>0.835094</v>
+        <v>0.83774499999999996</v>
       </c>
       <c r="U24" s="13">
-        <v>0.97238199999999997</v>
+        <v>0.97228199999999998</v>
       </c>
       <c r="V24" s="13">
-        <v>0.99698900000000001</v>
+        <v>0.99663900000000005</v>
       </c>
       <c r="W24" s="13">
-        <v>0.99978999999999996</v>
+        <v>0.99973999999999996</v>
       </c>
       <c r="X24" s="13">
-        <v>0.99999000000000005</v>
+        <v>1</v>
       </c>
       <c r="Y24" s="13">
         <v>1</v>
@@ -5721,7 +5726,7 @@
         <v>36</v>
       </c>
       <c r="AD24" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:31">
@@ -5733,63 +5738,63 @@
         <v>49968</v>
       </c>
       <c r="D25" s="16">
-        <v>175093</v>
+        <v>169641</v>
       </c>
       <c r="E25" s="16">
-        <v>5969967</v>
+        <v>5820172</v>
       </c>
       <c r="F25" s="16">
-        <v>60495160</v>
+        <v>62198115</v>
       </c>
       <c r="G25" s="16">
-        <v>31016</v>
+        <v>32119</v>
       </c>
       <c r="H25" s="16">
-        <v>127768</v>
+        <v>150192</v>
       </c>
       <c r="I25" s="11">
-        <f t="shared" si="25"/>
-        <v>119.47580451488953</v>
+        <f t="shared" si="20"/>
+        <v>116.47798591098302</v>
       </c>
       <c r="J25" s="12">
-        <f t="shared" si="26"/>
-        <v>3.5041026256804355</v>
+        <f t="shared" si="21"/>
+        <v>3.3949927953890491</v>
       </c>
       <c r="K25" s="11">
-        <f t="shared" si="27"/>
-        <v>1210.6780339417228</v>
+        <f t="shared" si="22"/>
+        <v>1244.7589457252641</v>
       </c>
       <c r="L25" s="12">
-        <f t="shared" si="28"/>
-        <v>9.8685035298691659E-2</v>
+        <f t="shared" si="23"/>
+        <v>9.3574732932018928E-2</v>
       </c>
       <c r="M25" s="12">
-        <f t="shared" si="29"/>
-        <v>2.8943307200113197E-3</v>
+        <f t="shared" si="24"/>
+        <v>2.7274299229164745E-3</v>
       </c>
       <c r="N25" s="12"/>
       <c r="O25" s="12"/>
       <c r="P25" s="13"/>
       <c r="Q25" s="19">
-        <v>1.781E-3</v>
+        <v>1.9610000000000001E-3</v>
       </c>
       <c r="R25" s="19">
-        <v>0.20961399999999999</v>
+        <v>0.23539099999999999</v>
       </c>
       <c r="S25" s="19">
-        <v>0.733209</v>
+        <v>0.74938000000000005</v>
       </c>
       <c r="T25" s="19">
-        <v>0.95485100000000001</v>
+        <v>0.95360999999999996</v>
       </c>
       <c r="U25" s="19">
-        <v>0.99557700000000005</v>
+        <v>0.99363599999999996</v>
       </c>
       <c r="V25" s="19">
-        <v>0.99987999999999999</v>
+        <v>0.99956</v>
       </c>
       <c r="W25" s="19">
-        <v>1</v>
+        <v>0.99997999999999998</v>
       </c>
       <c r="X25" s="13">
         <v>1</v>
@@ -5810,7 +5815,7 @@
         <v>36</v>
       </c>
       <c r="AD25" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:31">
@@ -5822,60 +5827,60 @@
         <v>14976</v>
       </c>
       <c r="D26" s="10">
-        <v>1115469</v>
+        <v>1400556</v>
       </c>
       <c r="E26" s="10">
-        <v>39137391</v>
+        <v>49110282</v>
       </c>
       <c r="F26" s="10">
-        <v>19465035</v>
+        <v>20272960</v>
       </c>
       <c r="G26" s="10">
-        <v>33646</v>
+        <v>35333</v>
       </c>
       <c r="H26" s="10">
-        <v>129124</v>
+        <v>126908</v>
       </c>
       <c r="I26" s="11">
-        <f t="shared" si="25"/>
-        <v>2613.3407451923076</v>
+        <f t="shared" si="20"/>
+        <v>3279.265625</v>
       </c>
       <c r="J26" s="12">
-        <f t="shared" si="26"/>
-        <v>74.483774038461533</v>
+        <f t="shared" si="21"/>
+        <v>93.520032051282058</v>
       </c>
       <c r="K26" s="11">
-        <f t="shared" si="27"/>
-        <v>1299.7485977564102</v>
+        <f t="shared" si="22"/>
+        <v>1353.6965811965813</v>
       </c>
       <c r="L26" s="12">
-        <f t="shared" si="28"/>
-        <v>2.0106509441159495</v>
+        <f t="shared" si="23"/>
+        <v>2.4224524687070854</v>
       </c>
       <c r="M26" s="12">
-        <f t="shared" si="29"/>
-        <v>5.7306293053159166E-2</v>
+        <f t="shared" si="24"/>
+        <v>6.9084928890502426E-2</v>
       </c>
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
       <c r="P26" s="13"/>
       <c r="Q26" s="13">
-        <v>2.003E-3</v>
+        <v>4.1399999999999996E-3</v>
       </c>
       <c r="R26" s="13">
-        <v>0.25240400000000002</v>
+        <v>0.28772700000000001</v>
       </c>
       <c r="S26" s="13">
-        <v>0.78632500000000005</v>
+        <v>0.80401999999999996</v>
       </c>
       <c r="T26" s="13">
-        <v>0.969418</v>
+        <v>0.97175500000000004</v>
       </c>
       <c r="U26" s="13">
-        <v>0.99773000000000001</v>
+        <v>0.99826400000000004</v>
       </c>
       <c r="V26" s="13">
-        <v>0.99993299999999996</v>
+        <v>0.99986600000000003</v>
       </c>
       <c r="W26" s="13">
         <v>1</v>
@@ -5899,7 +5904,7 @@
         <v>36</v>
       </c>
       <c r="AD26" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:31">
@@ -5911,57 +5916,57 @@
         <v>4968</v>
       </c>
       <c r="D27" s="16">
-        <v>619217</v>
+        <v>726499</v>
       </c>
       <c r="E27" s="16">
-        <v>21384004</v>
+        <v>25240930</v>
       </c>
       <c r="F27" s="16">
-        <v>9088762</v>
+        <v>9007970</v>
       </c>
       <c r="G27" s="16">
-        <v>50068</v>
+        <v>49641</v>
       </c>
       <c r="H27" s="16">
-        <v>153232</v>
+        <v>165508</v>
       </c>
       <c r="I27" s="11">
-        <f t="shared" si="25"/>
-        <v>4304.3486312399355</v>
+        <f t="shared" si="20"/>
+        <v>5080.7024959742348</v>
       </c>
       <c r="J27" s="12">
-        <f t="shared" si="26"/>
-        <v>124.64110305958133</v>
+        <f t="shared" si="21"/>
+        <v>146.23570853462158</v>
       </c>
       <c r="K27" s="11">
-        <f t="shared" si="27"/>
-        <v>1829.4609500805152</v>
+        <f t="shared" si="22"/>
+        <v>1813.1984702093398</v>
       </c>
       <c r="L27" s="12">
-        <f t="shared" si="28"/>
-        <v>2.3527961233884218</v>
+        <f t="shared" si="23"/>
+        <v>2.8020663923170259</v>
       </c>
       <c r="M27" s="12">
-        <f t="shared" si="29"/>
-        <v>6.8129960934173436E-2</v>
+        <f t="shared" si="24"/>
+        <v>8.0650690444128925E-2</v>
       </c>
       <c r="N27" s="12"/>
       <c r="O27" s="12"/>
       <c r="P27" s="13"/>
       <c r="Q27" s="19">
-        <v>3.6836000000000001E-2</v>
+        <v>3.8043E-2</v>
       </c>
       <c r="R27" s="19">
-        <v>0.55515300000000001</v>
+        <v>0.54488700000000001</v>
       </c>
       <c r="S27" s="19">
-        <v>0.93095799999999995</v>
+        <v>0.92491900000000005</v>
       </c>
       <c r="T27" s="19">
         <v>0.99214999999999998</v>
       </c>
       <c r="U27" s="19">
-        <v>0.99959699999999996</v>
+        <v>0.99919500000000006</v>
       </c>
       <c r="V27" s="19">
         <v>1</v>
@@ -5988,7 +5993,7 @@
         <v>36</v>
       </c>
       <c r="AD27" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:31">
@@ -6000,48 +6005,48 @@
         <v>972</v>
       </c>
       <c r="D28" s="10">
-        <v>2386516</v>
+        <v>3251211</v>
       </c>
       <c r="E28" s="10">
-        <v>81853500</v>
+        <v>112464906</v>
       </c>
       <c r="F28" s="10">
-        <v>1871338</v>
+        <v>1853485</v>
       </c>
       <c r="G28" s="10">
-        <v>52991</v>
+        <v>52293</v>
       </c>
       <c r="H28" s="10">
-        <v>145168</v>
+        <v>160308</v>
       </c>
       <c r="I28" s="11">
-        <f t="shared" si="25"/>
-        <v>84211.419753086418</v>
+        <f t="shared" si="20"/>
+        <v>115704.63580246913</v>
       </c>
       <c r="J28" s="12">
-        <f t="shared" si="26"/>
-        <v>2455.2633744855966</v>
+        <f t="shared" si="21"/>
+        <v>3344.8672839506171</v>
       </c>
       <c r="K28" s="11">
-        <f t="shared" si="27"/>
-        <v>1925.2448559670781</v>
+        <f t="shared" si="22"/>
+        <v>1906.8775720164608</v>
       </c>
       <c r="L28" s="12">
-        <f t="shared" si="28"/>
-        <v>43.740628363235288</v>
+        <f t="shared" si="23"/>
+        <v>60.677537719485187</v>
       </c>
       <c r="M28" s="12">
-        <f t="shared" si="29"/>
-        <v>1.2752992778429124</v>
+        <f t="shared" si="24"/>
+        <v>1.7541069930428355</v>
       </c>
       <c r="N28" s="12"/>
       <c r="O28" s="12"/>
       <c r="P28" s="13"/>
       <c r="Q28" s="13">
-        <v>4.2181000000000003E-2</v>
+        <v>3.1892999999999998E-2</v>
       </c>
       <c r="R28" s="13">
-        <v>0.59876499999999999</v>
+        <v>0.59465000000000001</v>
       </c>
       <c r="S28" s="13">
         <v>0.94547300000000001</v>
@@ -6077,7 +6082,7 @@
         <v>36</v>
       </c>
       <c r="AD28" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:31">
@@ -6089,54 +6094,54 @@
         <v>720</v>
       </c>
       <c r="D29" s="16">
-        <v>2710389</v>
+        <v>3400010</v>
       </c>
       <c r="E29" s="16">
-        <v>91554806</v>
+        <v>115540911</v>
       </c>
       <c r="F29" s="16">
-        <v>1683098</v>
+        <v>1665247</v>
       </c>
       <c r="G29" s="16">
-        <v>66354</v>
+        <v>65571</v>
       </c>
       <c r="H29" s="16">
-        <v>159720</v>
+        <v>164952</v>
       </c>
       <c r="I29" s="11">
-        <f t="shared" si="25"/>
-        <v>127159.45277777778</v>
+        <f t="shared" si="20"/>
+        <v>160473.48749999999</v>
       </c>
       <c r="J29" s="12">
-        <f t="shared" si="26"/>
-        <v>3764.4291666666668</v>
+        <f t="shared" si="21"/>
+        <v>4722.2361111111113</v>
       </c>
       <c r="K29" s="11">
-        <f t="shared" si="27"/>
-        <v>2337.6361111111109</v>
+        <f t="shared" si="22"/>
+        <v>2312.8430555555556</v>
       </c>
       <c r="L29" s="12">
-        <f t="shared" si="28"/>
-        <v>54.396598415540872</v>
+        <f t="shared" si="23"/>
+        <v>69.383647591018018</v>
       </c>
       <c r="M29" s="12">
-        <f t="shared" si="29"/>
-        <v>1.6103572103347519</v>
+        <f t="shared" si="24"/>
+        <v>2.0417451585260324</v>
       </c>
       <c r="N29" s="12"/>
       <c r="O29" s="12"/>
       <c r="P29" s="13"/>
       <c r="Q29" s="19">
-        <v>0.13333300000000001</v>
+        <v>0.129167</v>
       </c>
       <c r="R29" s="19">
-        <v>0.77083299999999999</v>
+        <v>0.76666699999999999</v>
       </c>
       <c r="S29" s="19">
-        <v>0.97777800000000004</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="T29" s="19">
-        <v>0.99861100000000003</v>
+        <v>1</v>
       </c>
       <c r="U29" s="19">
         <v>1</v>
@@ -6166,7 +6171,7 @@
         <v>36</v>
       </c>
       <c r="AD29" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:31">
@@ -6178,57 +6183,57 @@
         <v>216</v>
       </c>
       <c r="D30" s="10">
-        <v>15007092</v>
+        <v>20841656</v>
       </c>
       <c r="E30" s="10">
-        <v>504576269</v>
+        <v>699303228</v>
       </c>
       <c r="F30" s="10">
-        <v>530790</v>
+        <v>519822</v>
       </c>
       <c r="G30" s="10">
-        <v>70358</v>
+        <v>68518</v>
       </c>
       <c r="H30" s="10">
-        <v>151736</v>
+        <v>149308</v>
       </c>
       <c r="I30" s="11">
-        <f t="shared" si="25"/>
-        <v>2336001.2453703703</v>
+        <f t="shared" si="20"/>
+        <v>3237514.9444444445</v>
       </c>
       <c r="J30" s="12">
-        <f t="shared" si="26"/>
-        <v>69477.277777777781</v>
+        <f t="shared" si="21"/>
+        <v>96489.148148148146</v>
       </c>
       <c r="K30" s="11">
-        <f t="shared" si="27"/>
-        <v>2457.3611111111113</v>
+        <f t="shared" si="22"/>
+        <v>2406.5833333333335</v>
       </c>
       <c r="L30" s="12">
-        <f t="shared" si="28"/>
-        <v>950.6137436651029</v>
+        <f t="shared" si="23"/>
+        <v>1345.2743977746227</v>
       </c>
       <c r="M30" s="12">
-        <f t="shared" si="29"/>
-        <v>28.273124964675294</v>
+        <f t="shared" si="24"/>
+        <v>40.093832119456273</v>
       </c>
       <c r="N30" s="12"/>
       <c r="O30" s="12"/>
       <c r="P30" s="13"/>
       <c r="Q30" s="13">
-        <v>0.175926</v>
+        <v>0.148148</v>
       </c>
       <c r="R30" s="13">
-        <v>0.796296</v>
+        <v>0.79166700000000001</v>
       </c>
       <c r="S30" s="13">
-        <v>0.97685200000000005</v>
+        <v>0.99536999999999998</v>
       </c>
       <c r="T30" s="13">
-        <v>0.99536999999999998</v>
+        <v>1</v>
       </c>
       <c r="U30" s="13">
-        <v>0.99536999999999998</v>
+        <v>1</v>
       </c>
       <c r="V30" s="13">
         <v>1</v>
@@ -6255,7 +6260,7 @@
         <v>36</v>
       </c>
       <c r="AD30" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:31">
@@ -6277,697 +6282,163 @@
       <c r="Z32" s="26"/>
       <c r="AA32" s="26"/>
     </row>
-    <row r="33" spans="2:30">
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>99996</v>
-      </c>
-      <c r="D33">
-        <v>33331</v>
-      </c>
-      <c r="E33">
-        <v>303064</v>
-      </c>
-      <c r="F33">
-        <v>67148229</v>
-      </c>
-      <c r="G33">
-        <v>15202</v>
-      </c>
-      <c r="H33">
-        <v>73332</v>
-      </c>
-      <c r="I33" s="11">
-        <f t="shared" ref="I33:I40" si="30">E33/C33</f>
-        <v>3.030761230449218</v>
-      </c>
-      <c r="J33" s="12">
-        <f t="shared" ref="J33:J40" si="31">D33/C33</f>
-        <v>0.33332333293331734</v>
-      </c>
-      <c r="K33" s="11">
-        <f t="shared" ref="K33:K40" si="32">F33/C33</f>
-        <v>671.50915036601464</v>
-      </c>
-      <c r="L33" s="12">
-        <f t="shared" ref="L33:L40" si="33">I33/K33</f>
-        <v>4.513358051483383E-3</v>
-      </c>
-      <c r="M33" s="12">
-        <f t="shared" ref="M33:M40" si="34">J33/K33</f>
-        <v>4.9637943541295778E-4</v>
-      </c>
-      <c r="R33" s="26">
-        <v>7.6899999999999998E-3</v>
-      </c>
-      <c r="S33" s="26">
-        <v>0.26456099999999999</v>
-      </c>
-      <c r="T33" s="26">
-        <v>0.73008899999999999</v>
-      </c>
-      <c r="U33" s="26">
-        <v>0.93991800000000003</v>
-      </c>
-      <c r="V33" s="26">
-        <v>0.99068000000000001</v>
-      </c>
-      <c r="W33" s="26">
-        <v>0.99902999999999997</v>
-      </c>
-      <c r="X33" s="26">
-        <v>0.99995000000000001</v>
-      </c>
-      <c r="Y33" s="27">
-        <v>1</v>
-      </c>
-      <c r="Z33" s="27">
-        <v>1</v>
-      </c>
-      <c r="AA33" s="27">
-        <v>1</v>
-      </c>
-      <c r="AB33" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC33">
-        <v>12</v>
-      </c>
-      <c r="AD33" t="s">
-        <v>28</v>
-      </c>
+    <row r="33" spans="7:27">
+      <c r="I33" s="11"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="R33" s="26"/>
+      <c r="S33" s="26"/>
+      <c r="T33" s="26"/>
+      <c r="U33" s="26"/>
+      <c r="V33" s="26"/>
+      <c r="W33" s="26"/>
+      <c r="X33" s="26"/>
+      <c r="Y33" s="27"/>
+      <c r="Z33" s="27"/>
+      <c r="AA33" s="27"/>
     </row>
-    <row r="34" spans="2:30" ht="18" customHeight="1">
-      <c r="B34">
-        <v>2</v>
-      </c>
-      <c r="C34">
-        <v>49992</v>
-      </c>
-      <c r="D34">
-        <v>116281</v>
-      </c>
-      <c r="E34">
-        <v>1342565</v>
-      </c>
-      <c r="F34">
-        <v>41000965</v>
-      </c>
-      <c r="G34">
-        <v>19381</v>
-      </c>
-      <c r="H34">
-        <v>104388</v>
-      </c>
-      <c r="I34" s="11">
-        <f t="shared" si="30"/>
-        <v>26.855596895503279</v>
-      </c>
-      <c r="J34" s="12">
-        <f t="shared" si="31"/>
-        <v>2.3259921587453993</v>
-      </c>
-      <c r="K34" s="11">
-        <f t="shared" si="32"/>
-        <v>820.15052408385338</v>
-      </c>
-      <c r="L34" s="12">
-        <f t="shared" si="33"/>
-        <v>3.27447171060486E-2</v>
-      </c>
-      <c r="M34" s="12">
-        <f t="shared" si="34"/>
-        <v>2.8360552001641913E-3</v>
-      </c>
-      <c r="Q34" s="26">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="R34" s="26">
-        <v>3.1605000000000001E-2</v>
-      </c>
-      <c r="S34" s="26">
-        <v>0.42150700000000002</v>
-      </c>
-      <c r="T34" s="26">
-        <v>0.83889400000000003</v>
-      </c>
-      <c r="U34" s="26">
-        <v>0.972916</v>
-      </c>
-      <c r="V34" s="26">
-        <v>0.99707999999999997</v>
-      </c>
-      <c r="W34" s="26">
-        <v>0.99980000000000002</v>
-      </c>
-      <c r="X34" s="26">
-        <v>1</v>
-      </c>
-      <c r="Y34" s="41">
-        <v>1</v>
-      </c>
-      <c r="Z34" s="41">
-        <v>1</v>
-      </c>
-      <c r="AA34" s="41">
-        <v>1</v>
-      </c>
-      <c r="AB34" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC34">
-        <v>12</v>
-      </c>
-      <c r="AD34" t="s">
-        <v>28</v>
-      </c>
+    <row r="34" spans="7:27" ht="18" customHeight="1">
+      <c r="I34" s="11"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="Q34" s="26"/>
+      <c r="R34" s="26"/>
+      <c r="S34" s="26"/>
+      <c r="T34" s="26"/>
+      <c r="U34" s="26"/>
+      <c r="V34" s="26"/>
+      <c r="W34" s="26"/>
+      <c r="X34" s="26"/>
+      <c r="Y34" s="41"/>
+      <c r="Z34" s="41"/>
+      <c r="AA34" s="41"/>
     </row>
-    <row r="35" spans="2:30" ht="17" customHeight="1">
-      <c r="B35">
-        <v>3</v>
-      </c>
-      <c r="C35">
-        <v>24996</v>
-      </c>
-      <c r="D35">
-        <v>167124</v>
-      </c>
-      <c r="E35">
-        <v>1959317</v>
-      </c>
-      <c r="F35">
-        <v>29904421</v>
-      </c>
-      <c r="G35">
-        <v>30615</v>
-      </c>
-      <c r="H35">
-        <v>126960</v>
-      </c>
-      <c r="I35" s="11">
-        <f t="shared" si="30"/>
-        <v>78.385221635461676</v>
-      </c>
-      <c r="J35" s="12">
-        <f t="shared" si="31"/>
-        <v>6.6860297647623623</v>
-      </c>
-      <c r="K35" s="11">
-        <f t="shared" si="32"/>
-        <v>1196.3682589214275</v>
-      </c>
-      <c r="L35" s="12">
-        <f t="shared" si="33"/>
-        <v>6.5519309001167425E-2</v>
-      </c>
-      <c r="M35" s="12">
-        <f t="shared" si="34"/>
-        <v>5.5886051095923239E-3</v>
-      </c>
-      <c r="Q35" s="26">
-        <v>1.1199999999999999E-3</v>
-      </c>
-      <c r="R35" s="26">
-        <v>0.203233</v>
-      </c>
-      <c r="S35" s="26">
-        <v>0.72839699999999996</v>
-      </c>
-      <c r="T35" s="26">
-        <v>0.95127200000000001</v>
-      </c>
-      <c r="U35" s="26">
-        <v>0.99459900000000001</v>
-      </c>
-      <c r="V35" s="26">
-        <v>0.99972000000000005</v>
-      </c>
-      <c r="W35" s="26">
-        <v>0.99995999999999996</v>
-      </c>
-      <c r="X35" s="27">
-        <v>1</v>
-      </c>
-      <c r="Y35" s="25">
-        <v>1</v>
-      </c>
-      <c r="Z35" s="25">
-        <v>1</v>
-      </c>
-      <c r="AA35" s="27">
-        <v>1</v>
-      </c>
-      <c r="AB35" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC35">
-        <v>12</v>
-      </c>
-      <c r="AD35" t="s">
-        <v>28</v>
-      </c>
+    <row r="35" spans="7:27" ht="17" customHeight="1">
+      <c r="I35" s="11"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="Q35" s="26"/>
+      <c r="R35" s="26"/>
+      <c r="S35" s="26"/>
+      <c r="T35" s="26"/>
+      <c r="U35" s="26"/>
+      <c r="V35" s="26"/>
+      <c r="W35" s="26"/>
+      <c r="X35" s="27"/>
+      <c r="Y35" s="25"/>
+      <c r="Z35" s="25"/>
+      <c r="AA35" s="27"/>
     </row>
-    <row r="36" spans="2:30">
-      <c r="B36">
-        <v>4</v>
-      </c>
-      <c r="C36">
-        <v>15000</v>
-      </c>
-      <c r="D36">
-        <v>1370228</v>
-      </c>
-      <c r="E36">
-        <v>16333695</v>
-      </c>
-      <c r="F36">
-        <v>19279774</v>
-      </c>
-      <c r="G36">
-        <v>33235</v>
-      </c>
-      <c r="H36">
-        <v>127012</v>
-      </c>
-      <c r="I36" s="11">
-        <f t="shared" si="30"/>
-        <v>1088.913</v>
-      </c>
-      <c r="J36" s="12">
-        <f t="shared" si="31"/>
-        <v>91.348533333333336</v>
-      </c>
-      <c r="K36" s="11">
-        <f t="shared" si="32"/>
-        <v>1285.3182666666667</v>
-      </c>
-      <c r="L36" s="12">
-        <f t="shared" si="33"/>
-        <v>0.8471932814150207</v>
-      </c>
-      <c r="M36" s="12">
-        <f t="shared" si="34"/>
-        <v>7.1070750103191041E-2</v>
-      </c>
-      <c r="Q36" s="26">
-        <v>2E-3</v>
-      </c>
-      <c r="R36" s="26">
-        <v>0.24773300000000001</v>
-      </c>
-      <c r="S36" s="26">
-        <v>0.77793299999999999</v>
-      </c>
-      <c r="T36" s="26">
-        <v>0.96846699999999997</v>
-      </c>
-      <c r="U36" s="26">
-        <v>0.99719999999999998</v>
-      </c>
-      <c r="V36" s="26">
-        <v>0.99980000000000002</v>
-      </c>
-      <c r="W36" s="27">
-        <v>1</v>
-      </c>
-      <c r="X36" s="27">
-        <v>1</v>
-      </c>
-      <c r="Y36" s="25">
-        <v>1</v>
-      </c>
-      <c r="Z36" s="25">
-        <v>1</v>
-      </c>
-      <c r="AA36" s="27">
-        <v>1</v>
-      </c>
-      <c r="AB36" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC36">
-        <v>12</v>
-      </c>
-      <c r="AD36" t="s">
-        <v>28</v>
-      </c>
+    <row r="36" spans="7:27">
+      <c r="I36" s="11"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="Q36" s="26"/>
+      <c r="R36" s="26"/>
+      <c r="S36" s="26"/>
+      <c r="T36" s="26"/>
+      <c r="U36" s="26"/>
+      <c r="V36" s="26"/>
+      <c r="W36" s="27"/>
+      <c r="X36" s="27"/>
+      <c r="Y36" s="25"/>
+      <c r="Z36" s="25"/>
+      <c r="AA36" s="27"/>
     </row>
-    <row r="37" spans="2:30">
-      <c r="B37">
-        <v>5</v>
-      </c>
-      <c r="C37">
-        <v>4992</v>
-      </c>
-      <c r="D37">
-        <v>1090481</v>
-      </c>
-      <c r="E37">
-        <v>12790402</v>
-      </c>
-      <c r="F37">
-        <v>9129459</v>
-      </c>
-      <c r="G37">
-        <v>50074</v>
-      </c>
-      <c r="H37">
-        <v>167856</v>
-      </c>
-      <c r="I37" s="11">
-        <f t="shared" si="30"/>
-        <v>2562.1798878205127</v>
-      </c>
-      <c r="J37" s="12">
-        <f t="shared" si="31"/>
-        <v>218.44571314102564</v>
-      </c>
-      <c r="K37" s="11">
-        <f t="shared" si="32"/>
-        <v>1828.8179086538462</v>
-      </c>
-      <c r="L37" s="12">
-        <f t="shared" si="33"/>
-        <v>1.4010032796028766</v>
-      </c>
-      <c r="M37" s="12">
-        <f t="shared" si="34"/>
-        <v>0.11944639874060445</v>
-      </c>
-      <c r="Q37" s="26">
-        <v>4.1667000000000003E-2</v>
-      </c>
-      <c r="R37" s="26">
-        <v>0.54787699999999995</v>
-      </c>
-      <c r="S37" s="26">
-        <v>0.92888599999999999</v>
-      </c>
-      <c r="T37" s="26">
-        <v>0.992788</v>
-      </c>
-      <c r="U37" s="27">
-        <v>1</v>
-      </c>
-      <c r="V37" s="27">
-        <v>1</v>
-      </c>
-      <c r="W37" s="27">
-        <v>1</v>
-      </c>
-      <c r="X37" s="27">
-        <v>1</v>
-      </c>
-      <c r="Y37" s="25">
-        <v>1</v>
-      </c>
-      <c r="Z37" s="25">
-        <v>1</v>
-      </c>
-      <c r="AA37" s="27">
-        <v>1</v>
-      </c>
-      <c r="AB37" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC37">
-        <v>12</v>
-      </c>
-      <c r="AD37" t="s">
-        <v>28</v>
-      </c>
+    <row r="37" spans="7:27">
+      <c r="I37" s="11"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
+      <c r="Q37" s="26"/>
+      <c r="R37" s="26"/>
+      <c r="S37" s="26"/>
+      <c r="T37" s="26"/>
+      <c r="U37" s="27"/>
+      <c r="V37" s="27"/>
+      <c r="W37" s="27"/>
+      <c r="X37" s="27"/>
+      <c r="Y37" s="25"/>
+      <c r="Z37" s="25"/>
+      <c r="AA37" s="27"/>
     </row>
-    <row r="38" spans="2:30">
-      <c r="B38">
-        <v>6</v>
-      </c>
-      <c r="C38">
-        <v>996</v>
-      </c>
-      <c r="D38">
-        <v>3237741</v>
-      </c>
-      <c r="E38">
-        <v>38160186</v>
-      </c>
-      <c r="F38">
-        <v>1955009</v>
-      </c>
-      <c r="G38">
-        <v>54299</v>
-      </c>
-      <c r="H38">
-        <v>150544</v>
-      </c>
-      <c r="I38" s="11">
-        <f t="shared" si="30"/>
-        <v>38313.439759036148</v>
-      </c>
-      <c r="J38" s="12">
-        <f t="shared" si="31"/>
-        <v>3250.7439759036147</v>
-      </c>
-      <c r="K38" s="11">
-        <f t="shared" si="32"/>
-        <v>1962.8604417670683</v>
-      </c>
-      <c r="L38" s="12">
-        <f t="shared" si="33"/>
-        <v>19.519186868193447</v>
-      </c>
-      <c r="M38" s="12">
-        <f t="shared" si="34"/>
-        <v>1.6561258797274079</v>
-      </c>
-      <c r="Q38" s="26">
-        <v>5.2208999999999998E-2</v>
-      </c>
-      <c r="R38" s="26">
-        <v>0.625502</v>
-      </c>
-      <c r="S38" s="26">
-        <v>0.95682699999999998</v>
-      </c>
-      <c r="T38" s="26">
-        <v>0.99598399999999998</v>
-      </c>
-      <c r="U38" s="27">
-        <v>1</v>
-      </c>
-      <c r="V38" s="27">
-        <v>1</v>
-      </c>
-      <c r="W38" s="27">
-        <v>1</v>
-      </c>
-      <c r="X38" s="27">
-        <v>1</v>
-      </c>
-      <c r="Y38" s="25">
-        <v>1</v>
-      </c>
-      <c r="Z38" s="25">
-        <v>1</v>
-      </c>
-      <c r="AA38" s="27">
-        <v>1</v>
-      </c>
-      <c r="AB38" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC38">
-        <v>12</v>
-      </c>
-      <c r="AD38" t="s">
-        <v>28</v>
-      </c>
+    <row r="38" spans="7:27">
+      <c r="I38" s="11"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="Q38" s="26"/>
+      <c r="R38" s="26"/>
+      <c r="S38" s="26"/>
+      <c r="T38" s="26"/>
+      <c r="U38" s="27"/>
+      <c r="V38" s="27"/>
+      <c r="W38" s="27"/>
+      <c r="X38" s="27"/>
+      <c r="Y38" s="25"/>
+      <c r="Z38" s="25"/>
+      <c r="AA38" s="27"/>
     </row>
-    <row r="39" spans="2:30">
-      <c r="B39">
-        <v>7</v>
-      </c>
-      <c r="C39">
-        <v>744</v>
-      </c>
-      <c r="D39">
-        <v>4698521</v>
-      </c>
-      <c r="E39">
-        <v>54432674</v>
-      </c>
-      <c r="F39">
-        <v>1727792</v>
-      </c>
-      <c r="G39">
-        <v>65857</v>
-      </c>
-      <c r="H39">
-        <v>161692</v>
-      </c>
-      <c r="I39" s="11">
-        <f t="shared" si="30"/>
-        <v>73162.196236559146</v>
-      </c>
-      <c r="J39" s="12">
-        <f t="shared" si="31"/>
-        <v>6315.2163978494627</v>
-      </c>
-      <c r="K39" s="11">
-        <f t="shared" si="32"/>
-        <v>2322.3010752688174</v>
-      </c>
-      <c r="L39" s="12">
-        <f t="shared" si="33"/>
-        <v>31.504182216377899</v>
-      </c>
-      <c r="M39" s="12">
-        <f t="shared" si="34"/>
-        <v>2.719378837267449</v>
-      </c>
-      <c r="Q39" s="26">
-        <v>0.137097</v>
-      </c>
-      <c r="R39" s="26">
-        <v>0.74731199999999998</v>
-      </c>
-      <c r="S39" s="26">
-        <v>0.97311800000000004</v>
-      </c>
-      <c r="T39" s="26">
-        <v>0.99865599999999999</v>
-      </c>
-      <c r="U39" s="27">
-        <v>1</v>
-      </c>
-      <c r="V39" s="27">
-        <v>1</v>
-      </c>
-      <c r="W39" s="27">
-        <v>1</v>
-      </c>
-      <c r="X39" s="27">
-        <v>1</v>
-      </c>
-      <c r="Y39" s="25">
-        <v>1</v>
-      </c>
-      <c r="Z39" s="25">
-        <v>1</v>
-      </c>
-      <c r="AA39" s="27">
-        <v>1</v>
-      </c>
-      <c r="AB39" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC39">
-        <v>12</v>
-      </c>
-      <c r="AD39" t="s">
-        <v>28</v>
-      </c>
+    <row r="39" spans="7:27">
+      <c r="I39" s="11"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="12"/>
+      <c r="Q39" s="26"/>
+      <c r="R39" s="26"/>
+      <c r="S39" s="26"/>
+      <c r="T39" s="26"/>
+      <c r="U39" s="27"/>
+      <c r="V39" s="27"/>
+      <c r="W39" s="27"/>
+      <c r="X39" s="27"/>
+      <c r="Y39" s="25"/>
+      <c r="Z39" s="25"/>
+      <c r="AA39" s="27"/>
     </row>
-    <row r="40" spans="2:30">
-      <c r="B40">
-        <v>8</v>
-      </c>
-      <c r="C40">
-        <v>240</v>
-      </c>
-      <c r="D40">
-        <v>21036856</v>
-      </c>
-      <c r="E40">
-        <v>245116942</v>
-      </c>
-      <c r="F40">
-        <v>566226</v>
-      </c>
-      <c r="G40">
-        <v>67156</v>
-      </c>
-      <c r="H40">
-        <v>150316</v>
-      </c>
-      <c r="I40" s="11">
-        <f t="shared" si="30"/>
-        <v>1021320.5916666667</v>
-      </c>
-      <c r="J40" s="12">
-        <f t="shared" si="31"/>
-        <v>87653.566666666666</v>
-      </c>
-      <c r="K40" s="11">
-        <f t="shared" si="32"/>
-        <v>2359.2750000000001</v>
-      </c>
-      <c r="L40" s="12">
-        <f t="shared" si="33"/>
-        <v>432.89594967380515</v>
-      </c>
-      <c r="M40" s="12">
-        <f t="shared" si="34"/>
-        <v>37.152755260267099</v>
-      </c>
-      <c r="Q40" s="26">
-        <v>0.14583299999999999</v>
-      </c>
-      <c r="R40" s="26">
-        <v>0.77083299999999999</v>
-      </c>
-      <c r="S40" s="26">
-        <v>0.96666700000000005</v>
-      </c>
-      <c r="T40" s="26">
-        <v>0.99583299999999997</v>
-      </c>
-      <c r="U40" s="27">
-        <v>1</v>
-      </c>
-      <c r="V40" s="27">
-        <v>1</v>
-      </c>
-      <c r="W40" s="27">
-        <v>1</v>
-      </c>
-      <c r="X40" s="27">
-        <v>1</v>
-      </c>
-      <c r="Y40" s="25">
-        <v>1</v>
-      </c>
-      <c r="Z40" s="25">
-        <v>1</v>
-      </c>
-      <c r="AA40" s="27">
-        <v>1</v>
-      </c>
-      <c r="AB40" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC40">
-        <v>12</v>
-      </c>
-      <c r="AD40" t="s">
-        <v>28</v>
-      </c>
+    <row r="40" spans="7:27">
+      <c r="I40" s="11"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="12"/>
+      <c r="M40" s="12"/>
+      <c r="Q40" s="26"/>
+      <c r="R40" s="26"/>
+      <c r="S40" s="26"/>
+      <c r="T40" s="26"/>
+      <c r="U40" s="27"/>
+      <c r="V40" s="27"/>
+      <c r="W40" s="27"/>
+      <c r="X40" s="27"/>
+      <c r="Y40" s="25"/>
+      <c r="Z40" s="25"/>
+      <c r="AA40" s="27"/>
     </row>
-    <row r="41" spans="2:30">
+    <row r="41" spans="7:27">
       <c r="G41" s="24"/>
       <c r="Y41" s="25"/>
       <c r="Z41" s="25"/>
     </row>
-    <row r="42" spans="2:30">
+    <row r="42" spans="7:27">
       <c r="Y42" s="25"/>
       <c r="Z42" s="25"/>
     </row>
-    <row r="43" spans="2:30">
+    <row r="43" spans="7:27">
       <c r="Y43" s="25"/>
       <c r="Z43" s="25"/>
     </row>
-    <row r="48" spans="2:30">
+    <row r="48" spans="7:27">
       <c r="Z48" s="25"/>
     </row>
     <row r="51" spans="25:26">
@@ -8968,7 +8439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CZ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
@@ -8976,10 +8447,10 @@
   <sheetData>
     <row r="1" spans="1:104">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -8987,10 +8458,10 @@
     </row>
     <row r="2" spans="1:104">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -9298,10 +8769,10 @@
     </row>
     <row r="3" spans="1:104">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -9609,10 +9080,10 @@
     </row>
     <row r="4" spans="1:104">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -9677,10 +9148,10 @@
     </row>
     <row r="5" spans="1:104">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -9991,10 +9462,10 @@
     </row>
     <row r="6" spans="1:104">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6">
         <v>2</v>

</xml_diff>